<commit_message>
Add latest NIST AI frameworks to compliance mapping
New NIST Frameworks Added:
- NIST AI 600-1: Generative AI Profile (July 2024)
  200+ actions for GenAI risks including hallucination, data privacy,
  content provenance, and harmful bias mitigation

- NIST IR 8596: Cybersecurity AI Profile (Draft Jan 2026)
  AI-specific cybersecurity controls mapping CSF 2.0 to AI/ML systems

Updated Existing Entries:
- NIST AI RMF: Now references GenAI Profile companion document
- NIST CSF 2.0: Now references AI Profile draft

Framework count updated: 8 → 10 compliance frameworks

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/AI_Security_Risk_Draft1.xlsx
+++ b/AI_Security_Risk_Draft1.xlsx
@@ -2001,7 +2001,7 @@
       </c>
       <c r="C31" s="100" t="inlineStr">
         <is>
-          <t>46 guardrails → 8 frameworks</t>
+          <t>46 guardrails → 10 frameworks (incl. NIST GenAI Profile)</t>
         </is>
       </c>
       <c r="D31" s="129" t="inlineStr">
@@ -2171,7 +2171,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:J101"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="19" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
@@ -2192,6 +2192,7 @@
     <col width="8.6640625" bestFit="1" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2" ht="21" customHeight="1">
       <c r="B2" s="9" t="inlineStr">
         <is>
@@ -2206,6 +2207,7 @@
         </is>
       </c>
     </row>
+    <row r="4"/>
     <row r="5" ht="16" customHeight="1">
       <c r="B5" s="15" t="inlineStr">
         <is>
@@ -2316,12 +2318,12 @@
       </c>
       <c r="C11" s="65" t="inlineStr">
         <is>
-          <t>AI Risk Management Framework 1.0 (2023)</t>
+          <t>AI Risk Management Framework 1.0 (2023) + GenAI Profile (2024)</t>
         </is>
       </c>
       <c r="D11" s="70" t="inlineStr">
         <is>
-          <t>GOVERN, MAP, MEASURE, MANAGE</t>
+          <t>GOVERN, MAP, MEASURE, MANAGE; AI 600-1 adds 200+ GenAI-specific actions</t>
         </is>
       </c>
       <c r="G11" s="1" t="n"/>
@@ -2335,2517 +2337,2500 @@
       </c>
       <c r="C12" s="65" t="inlineStr">
         <is>
-          <t>Cybersecurity Framework v2.0 (2024)</t>
+          <t>Cybersecurity Framework v2.0 (2024) + AI Profile (Draft 2025)</t>
         </is>
       </c>
       <c r="D12" s="70" t="inlineStr">
         <is>
-          <t>GOVERN, IDENTIFY, PROTECT, DETECT, RESPOND, RECOVER</t>
+          <t>GOVERN, IDENTIFY, PROTECT, DETECT, RESPOND, RECOVER; IR 8596 adds AI-specific controls</t>
         </is>
       </c>
       <c r="G12" s="1" t="n"/>
       <c r="H12" s="1" t="n"/>
     </row>
     <row r="13" ht="22" customHeight="1">
-      <c r="B13" s="192" t="inlineStr">
+      <c r="B13" s="259" t="inlineStr">
+        <is>
+          <t>NIST AI 600-1</t>
+        </is>
+      </c>
+      <c r="C13" s="259" t="inlineStr">
+        <is>
+          <t>Generative AI Profile (July 2024)</t>
+        </is>
+      </c>
+      <c r="D13" s="259" t="inlineStr">
+        <is>
+          <t>200+ actions for GenAI risks: hallucination, data privacy, content provenance, harmful bias</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="22" customHeight="1">
+      <c r="B14" s="259" t="inlineStr">
+        <is>
+          <t>NIST IR 8596</t>
+        </is>
+      </c>
+      <c r="C14" s="259" t="inlineStr">
+        <is>
+          <t>Cybersecurity AI Profile (Draft Jan 2026)</t>
+        </is>
+      </c>
+      <c r="D14" s="259" t="inlineStr">
+        <is>
+          <t>AI-specific cybersecurity controls; maps CSF 2.0 to AI/ML systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="192" t="inlineStr">
         <is>
           <t>OWASP LLM Top 10</t>
         </is>
       </c>
-      <c r="C13" s="65" t="inlineStr">
+      <c r="C15" s="65" t="inlineStr">
         <is>
           <t>LLM Application Security Risks (2025)</t>
         </is>
       </c>
-      <c r="D13" s="70" t="inlineStr">
+      <c r="D15" s="70" t="inlineStr">
         <is>
           <t>LLM01-LLM10: Prompt Injection, Sensitive Info, Supply Chain, Data Poisoning, Output Handling, Excessive Agency, System Prompt Leak, Vector/Embedding, Misinformation, Unbounded Consumption</t>
         </is>
       </c>
-      <c r="G13" s="1" t="n"/>
-      <c r="H13" s="1" t="n"/>
-    </row>
-    <row r="14" ht="22" customHeight="1">
-      <c r="B14" s="192" t="inlineStr">
+      <c r="G15" s="1" t="n"/>
+      <c r="H15" s="1" t="n"/>
+    </row>
+    <row r="16" ht="16" customHeight="1">
+      <c r="B16" s="192" t="inlineStr">
         <is>
           <t>SOC 2</t>
         </is>
       </c>
-      <c r="C14" s="65" t="inlineStr">
+      <c r="C16" s="65" t="inlineStr">
         <is>
           <t>Service Organization Control 2 (AICPA)</t>
         </is>
       </c>
-      <c r="D14" s="70" t="inlineStr">
+      <c r="D16" s="70" t="inlineStr">
         <is>
           <t>Trust Service Criteria: CC, A, PI, C, P</t>
         </is>
       </c>
-      <c r="G14" s="1" t="n"/>
-      <c r="H14" s="1" t="n"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="149" t="n"/>
-      <c r="C15" s="149" t="n"/>
-      <c r="D15" s="149" t="n"/>
-    </row>
-    <row r="16" ht="16" customHeight="1">
-      <c r="B16" s="15" t="inlineStr">
+      <c r="G16" s="1" t="n"/>
+      <c r="H16" s="1" t="n"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="149" t="n"/>
+      <c r="C17" s="149" t="n"/>
+      <c r="D17" s="149" t="n"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="15" t="inlineStr">
         <is>
           <t>Guardrail → Framework Control Mapping</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" s="25" t="inlineStr">
+    <row r="19">
+      <c r="B19" s="25" t="inlineStr">
         <is>
           <t>Guardrails align with the Guardrail Checklist tab. Each maps to specific controls across frameworks.</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="B19" s="52" t="inlineStr">
+    <row r="20" ht="22" customHeight="1"/>
+    <row r="21" ht="42" customHeight="1">
+      <c r="B21" s="52" t="inlineStr">
         <is>
           <t>Guardrail</t>
         </is>
       </c>
-      <c r="C19" s="52" t="inlineStr">
+      <c r="C21" s="52" t="inlineStr">
         <is>
           <t>CSA AI</t>
         </is>
       </c>
-      <c r="D19" s="52" t="inlineStr">
+      <c r="D21" s="52" t="inlineStr">
         <is>
           <t>EU AI Act</t>
         </is>
       </c>
-      <c r="E19" s="52" t="inlineStr">
+      <c r="E21" s="52" t="inlineStr">
         <is>
           <t>ISO 42001</t>
         </is>
       </c>
-      <c r="F19" s="52" t="inlineStr">
+      <c r="F21" s="52" t="inlineStr">
         <is>
           <t>MITRE ATLAS</t>
         </is>
       </c>
-      <c r="G19" s="52" t="inlineStr">
+      <c r="G21" s="52" t="inlineStr">
         <is>
           <t>NIST AI RMF</t>
         </is>
       </c>
-      <c r="H19" s="52" t="inlineStr">
+      <c r="H21" s="52" t="inlineStr">
         <is>
           <t>NIST CSF 2.0</t>
         </is>
       </c>
-      <c r="I19" s="52" t="inlineStr">
+      <c r="I21" s="52" t="inlineStr">
         <is>
           <t>OWASP LLM</t>
         </is>
       </c>
-      <c r="J19" s="52" t="inlineStr">
+      <c r="J21" s="52" t="inlineStr">
         <is>
           <t>SOC 2</t>
         </is>
       </c>
     </row>
-    <row r="20" ht="22" customHeight="1">
-      <c r="B20" s="250" t="inlineStr">
+    <row r="22" ht="42" customHeight="1">
+      <c r="B22" s="250" t="inlineStr">
         <is>
           <t>AI POSTURE &amp; GOVERNANCE</t>
         </is>
       </c>
-      <c r="C20" s="251" t="n"/>
-      <c r="D20" s="251" t="n"/>
-      <c r="E20" s="251" t="n"/>
-      <c r="F20" s="251" t="n"/>
-      <c r="G20" s="251" t="n"/>
-      <c r="H20" s="251" t="n"/>
-      <c r="I20" s="251" t="n"/>
-      <c r="J20" s="26" t="n"/>
-    </row>
-    <row r="21" ht="42" customHeight="1">
-      <c r="B21" s="193" t="inlineStr">
+      <c r="C22" s="251" t="n"/>
+      <c r="D22" s="251" t="n"/>
+      <c r="E22" s="251" t="n"/>
+      <c r="F22" s="251" t="n"/>
+      <c r="G22" s="251" t="n"/>
+      <c r="H22" s="251" t="n"/>
+      <c r="I22" s="251" t="n"/>
+      <c r="J22" s="26" t="n"/>
+    </row>
+    <row r="23" ht="42" customHeight="1">
+      <c r="B23" s="193" t="inlineStr">
         <is>
           <t>Tool Registration</t>
         </is>
       </c>
-      <c r="C21" s="148" t="inlineStr">
+      <c r="C23" s="148" t="inlineStr">
         <is>
           <t>Asset Mgmt
 Inventory</t>
         </is>
       </c>
-      <c r="D21" s="148" t="inlineStr">
+      <c r="D23" s="148" t="inlineStr">
         <is>
           <t>Art. 9(2)(a)
 Art. 11</t>
         </is>
       </c>
-      <c r="E21" s="148" t="inlineStr">
+      <c r="E23" s="148" t="inlineStr">
         <is>
           <t>A.2 AI Policy
 A.4 AI Inventory</t>
         </is>
       </c>
-      <c r="F21" s="148" t="inlineStr">
+      <c r="F23" s="148" t="inlineStr">
         <is>
           <t>Reconnaissance
 defense</t>
         </is>
       </c>
-      <c r="G21" s="148" t="inlineStr">
+      <c r="G23" s="148" t="inlineStr">
         <is>
           <t>GOVERN 1.1, 1.2
 MAP 1.1, 1.5</t>
         </is>
       </c>
-      <c r="H21" s="148" t="inlineStr">
+      <c r="H23" s="148" t="inlineStr">
         <is>
           <t>ID.AM-1, ID.AM-2
 GV.OC-1</t>
         </is>
       </c>
-      <c r="I21" s="148" t="inlineStr">
+      <c r="I23" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain</t>
         </is>
       </c>
-      <c r="J21" s="148" t="inlineStr">
+      <c r="J23" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC6.6
 CC7.1</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="42" customHeight="1">
-      <c r="B22" s="193" t="inlineStr">
+    <row r="24" ht="42" customHeight="1">
+      <c r="B24" s="193" t="inlineStr">
         <is>
           <t>Risk Classification</t>
         </is>
       </c>
-      <c r="C22" s="148" t="inlineStr">
+      <c r="C24" s="148" t="inlineStr">
         <is>
           <t>Risk Assessment
 Threat Modeling</t>
         </is>
       </c>
-      <c r="D22" s="148" t="inlineStr">
+      <c r="D24" s="148" t="inlineStr">
         <is>
           <t>Art. 9(1)(2)
 Art. 9(5)</t>
         </is>
       </c>
-      <c r="E22" s="148" t="inlineStr">
+      <c r="E24" s="148" t="inlineStr">
         <is>
           <t>6.1 Risk Assessment
 A.3 Risk Mgmt</t>
         </is>
       </c>
-      <c r="F22" s="148" t="inlineStr">
+      <c r="F24" s="148" t="inlineStr">
         <is>
           <t>Initial Access
 defense</t>
         </is>
       </c>
-      <c r="G22" s="148" t="inlineStr">
+      <c r="G24" s="148" t="inlineStr">
         <is>
           <t>MAP 1.1-1.6
 MAP 2.1-2.3</t>
         </is>
       </c>
-      <c r="H22" s="148" t="inlineStr">
+      <c r="H24" s="148" t="inlineStr">
         <is>
           <t>ID.RA-1 to ID.RA-6
 GV.RM-1</t>
         </is>
       </c>
-      <c r="I22" s="148" t="inlineStr">
+      <c r="I24" s="148" t="inlineStr">
         <is>
           <t>All: Risk-based
 approach</t>
         </is>
       </c>
-      <c r="J22" s="148" t="inlineStr">
+      <c r="J24" s="148" t="inlineStr">
         <is>
           <t>CC3.1, CC3.2
 CC3.4</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="42" customHeight="1">
-      <c r="B23" s="193" t="inlineStr">
+    <row r="25" ht="42" customHeight="1">
+      <c r="B25" s="193" t="inlineStr">
         <is>
           <t>Approval Obtained</t>
         </is>
       </c>
-      <c r="C23" s="148" t="inlineStr">
+      <c r="C25" s="148" t="inlineStr">
         <is>
           <t>Governance
 Approval Workflows</t>
         </is>
       </c>
-      <c r="D23" s="148" t="inlineStr">
+      <c r="D25" s="148" t="inlineStr">
         <is>
           <t>Art. 17(1)
 Quality Mgmt</t>
         </is>
       </c>
-      <c r="E23" s="148" t="inlineStr">
+      <c r="E25" s="148" t="inlineStr">
         <is>
           <t>5.1 Leadership
 7.1 Resources</t>
         </is>
       </c>
-      <c r="F23" s="148" t="inlineStr">
+      <c r="F25" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G23" s="148" t="inlineStr">
+      <c r="G25" s="148" t="inlineStr">
         <is>
           <t>GOVERN 1.4, 1.6
 GOVERN 2.1-2.3</t>
         </is>
       </c>
-      <c r="H23" s="148" t="inlineStr">
+      <c r="H25" s="148" t="inlineStr">
         <is>
           <t>GV.PO-1, GV.PO-2
 GV.RR-1</t>
         </is>
       </c>
-      <c r="I23" s="148" t="inlineStr">
+      <c r="I25" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="J23" s="148" t="inlineStr">
+      <c r="J25" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC6.2
 CC6.7</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="42" customHeight="1">
-      <c r="B24" s="193" t="inlineStr">
+    <row r="26" ht="42" customHeight="1">
+      <c r="B26" s="193" t="inlineStr">
         <is>
           <t>Policy Alignment</t>
         </is>
       </c>
-      <c r="C24" s="148" t="inlineStr">
+      <c r="C26" s="148" t="inlineStr">
         <is>
           <t>Policy Controls
 Governance</t>
         </is>
       </c>
-      <c r="D24" s="148" t="inlineStr">
+      <c r="D26" s="148" t="inlineStr">
         <is>
           <t>Art. 17(1)
 Quality Mgmt</t>
         </is>
       </c>
-      <c r="E24" s="148" t="inlineStr">
+      <c r="E26" s="148" t="inlineStr">
         <is>
           <t>5.2 AI Policy
 A.2 AI Policy</t>
         </is>
       </c>
-      <c r="F24" s="148" t="inlineStr">
+      <c r="F26" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G24" s="148" t="inlineStr">
+      <c r="G26" s="148" t="inlineStr">
         <is>
           <t>GOVERN 1.1-1.7
 GOVERN 2.1-2.3</t>
         </is>
       </c>
-      <c r="H24" s="148" t="inlineStr">
+      <c r="H26" s="148" t="inlineStr">
         <is>
           <t>GV.PO-1, GV.PO-2
 GV.OV-1</t>
         </is>
       </c>
-      <c r="I24" s="148" t="inlineStr">
+      <c r="I26" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="J24" s="148" t="inlineStr">
+      <c r="J26" s="148" t="inlineStr">
         <is>
           <t>CC1.1, CC1.2
 CC5.1</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="42" customHeight="1">
-      <c r="B25" s="193" t="inlineStr">
+    <row r="27" ht="42" customHeight="1">
+      <c r="B27" s="193" t="inlineStr">
         <is>
           <t>Owner Assignment</t>
         </is>
       </c>
-      <c r="C25" s="148" t="inlineStr">
+      <c r="C27" s="148" t="inlineStr">
         <is>
           <t>Accountability
 RBAC</t>
         </is>
       </c>
-      <c r="D25" s="148" t="inlineStr">
+      <c r="D27" s="148" t="inlineStr">
         <is>
           <t>Art. 17(1)(j)
 Responsibility</t>
         </is>
       </c>
-      <c r="E25" s="148" t="inlineStr">
+      <c r="E27" s="148" t="inlineStr">
         <is>
           <t>5.3 Roles
 7.2 Competence</t>
         </is>
       </c>
-      <c r="F25" s="148" t="inlineStr">
+      <c r="F27" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G25" s="148" t="inlineStr">
+      <c r="G27" s="148" t="inlineStr">
         <is>
           <t>GOVERN 2.1, 2.3
 MANAGE 1.1</t>
         </is>
       </c>
-      <c r="H25" s="148" t="inlineStr">
+      <c r="H27" s="148" t="inlineStr">
         <is>
           <t>GV.RR-1, GV.RR-2
 ID.AM-5</t>
         </is>
       </c>
-      <c r="I25" s="148" t="inlineStr">
+      <c r="I27" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="J25" s="148" t="inlineStr">
+      <c r="J27" s="148" t="inlineStr">
         <is>
           <t>CC1.3, CC1.4
 CC2.2</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="42" customHeight="1">
-      <c r="B26" s="193" t="inlineStr">
+    <row r="28" ht="22" customHeight="1">
+      <c r="B28" s="193" t="inlineStr">
         <is>
           <t>Vendor Assessment</t>
         </is>
       </c>
-      <c r="C26" s="148" t="inlineStr">
+      <c r="C28" s="148" t="inlineStr">
         <is>
           <t>Vendor Mgmt
 Shared Resp.</t>
         </is>
       </c>
-      <c r="D26" s="148" t="inlineStr">
+      <c r="D28" s="148" t="inlineStr">
         <is>
           <t>Art. 9(4)(d)
 Art. 25</t>
         </is>
       </c>
-      <c r="E26" s="148" t="inlineStr">
+      <c r="E28" s="148" t="inlineStr">
         <is>
           <t>A.10 Third Party
 8.4 Outsourcing</t>
         </is>
       </c>
-      <c r="F26" s="148" t="inlineStr">
+      <c r="F28" s="148" t="inlineStr">
         <is>
           <t>Supply Chain
 Compromise</t>
         </is>
       </c>
-      <c r="G26" s="148" t="inlineStr">
+      <c r="G28" s="148" t="inlineStr">
         <is>
           <t>GOVERN 6.1, 6.2
 MAP 3.4, 3.5</t>
         </is>
       </c>
-      <c r="H26" s="148" t="inlineStr">
+      <c r="H28" s="148" t="inlineStr">
         <is>
           <t>GV.SC-1 to GV.SC-10
 ID.RA-9</t>
         </is>
       </c>
-      <c r="I26" s="148" t="inlineStr">
+      <c r="I28" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain</t>
         </is>
       </c>
-      <c r="J26" s="148" t="inlineStr">
+      <c r="J28" s="148" t="inlineStr">
         <is>
           <t>CC9.1, CC9.2
 CC3.4</t>
         </is>
       </c>
     </row>
-    <row r="27" ht="42" customHeight="1">
-      <c r="B27" s="193" t="inlineStr">
+    <row r="29" ht="42" customHeight="1">
+      <c r="B29" s="193" t="inlineStr">
         <is>
           <t>Compliance Mapping</t>
         </is>
       </c>
-      <c r="C27" s="148" t="inlineStr">
+      <c r="C29" s="148" t="inlineStr">
         <is>
           <t>Compliance
 Regulatory</t>
         </is>
       </c>
-      <c r="D27" s="148" t="inlineStr">
+      <c r="D29" s="148" t="inlineStr">
         <is>
           <t>Art. 17(1)(h)
 Conformity</t>
         </is>
       </c>
-      <c r="E27" s="148" t="inlineStr">
+      <c r="E29" s="148" t="inlineStr">
         <is>
           <t>9.2 Internal Audit
 10.2 Continual</t>
         </is>
       </c>
-      <c r="F27" s="148" t="inlineStr">
+      <c r="F29" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G27" s="148" t="inlineStr">
+      <c r="G29" s="148" t="inlineStr">
         <is>
           <t>GOVERN 1.2, 1.5
 MAP 5.1, 5.2</t>
         </is>
       </c>
-      <c r="H27" s="148" t="inlineStr">
+      <c r="H29" s="148" t="inlineStr">
         <is>
           <t>GV.OC-1 to GV.OC-5
 ID.GV-1</t>
         </is>
       </c>
-      <c r="I27" s="148" t="inlineStr">
+      <c r="I29" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="J27" s="148" t="inlineStr">
+      <c r="J29" s="148" t="inlineStr">
         <is>
           <t>CC4.1, CC4.2
 CC2.1</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="22" customHeight="1">
-      <c r="B28" s="252" t="inlineStr">
+    <row r="30" ht="42" customHeight="1">
+      <c r="B30" s="252" t="inlineStr">
         <is>
           <t>RUNTIME PROTECTION &amp; GUARDRAILS</t>
         </is>
       </c>
-      <c r="C28" s="251" t="n"/>
-      <c r="D28" s="251" t="n"/>
-      <c r="E28" s="251" t="n"/>
-      <c r="F28" s="251" t="n"/>
-      <c r="G28" s="251" t="n"/>
-      <c r="H28" s="251" t="n"/>
-      <c r="I28" s="251" t="n"/>
-      <c r="J28" s="26" t="n"/>
-    </row>
-    <row r="29" ht="42" customHeight="1">
-      <c r="B29" s="193" t="inlineStr">
+      <c r="C30" s="251" t="n"/>
+      <c r="D30" s="251" t="n"/>
+      <c r="E30" s="251" t="n"/>
+      <c r="F30" s="251" t="n"/>
+      <c r="G30" s="251" t="n"/>
+      <c r="H30" s="251" t="n"/>
+      <c r="I30" s="251" t="n"/>
+      <c r="J30" s="26" t="n"/>
+    </row>
+    <row r="31" ht="42" customHeight="1">
+      <c r="B31" s="193" t="inlineStr">
         <is>
           <t>Input Validation</t>
         </is>
       </c>
-      <c r="C29" s="148" t="inlineStr">
+      <c r="C31" s="148" t="inlineStr">
         <is>
           <t>Input Validation
 Injection Prev.</t>
         </is>
       </c>
-      <c r="D29" s="148" t="inlineStr">
+      <c r="D31" s="148" t="inlineStr">
         <is>
           <t>Art. 15(4)
 Robustness</t>
         </is>
       </c>
-      <c r="E29" s="148" t="inlineStr">
+      <c r="E31" s="148" t="inlineStr">
         <is>
           <t>A.6 Data Quality
 A.8 Operation</t>
         </is>
       </c>
-      <c r="F29" s="148" t="inlineStr">
+      <c r="F31" s="148" t="inlineStr">
         <is>
           <t>AML.T0051
 Prompt Injection</t>
         </is>
       </c>
-      <c r="G29" s="148" t="inlineStr">
+      <c r="G31" s="148" t="inlineStr">
         <is>
           <t>MEASURE 2.6, 2.7
 MANAGE 2.2</t>
         </is>
       </c>
-      <c r="H29" s="148" t="inlineStr">
+      <c r="H31" s="148" t="inlineStr">
         <is>
           <t>PR.DS-1, PR.DS-2
 DE.CM-1</t>
         </is>
       </c>
-      <c r="I29" s="148" t="inlineStr">
+      <c r="I31" s="148" t="inlineStr">
         <is>
           <t>LLM01: Prompt Inj.
 LLM07: Sys Prompt</t>
         </is>
       </c>
-      <c r="J29" s="148" t="inlineStr">
+      <c r="J31" s="148" t="inlineStr">
         <is>
           <t>CC6.6, CC6.7
 PI1.4</t>
         </is>
       </c>
     </row>
-    <row r="30" ht="42" customHeight="1">
-      <c r="B30" s="193" t="inlineStr">
+    <row r="32" ht="42" customHeight="1">
+      <c r="B32" s="193" t="inlineStr">
         <is>
           <t>Output Filtering</t>
         </is>
       </c>
-      <c r="C30" s="148" t="inlineStr">
+      <c r="C32" s="148" t="inlineStr">
         <is>
           <t>Output Sanitization
 Content Filter</t>
         </is>
       </c>
-      <c r="D30" s="148" t="inlineStr">
+      <c r="D32" s="148" t="inlineStr">
         <is>
           <t>Art. 15(3)
 Accuracy</t>
         </is>
       </c>
-      <c r="E30" s="148" t="inlineStr">
+      <c r="E32" s="148" t="inlineStr">
         <is>
           <t>A.7 Objectives
 A.8.4 Output</t>
         </is>
       </c>
-      <c r="F30" s="148" t="inlineStr">
+      <c r="F32" s="148" t="inlineStr">
         <is>
           <t>AML.T0047
 Evade Model</t>
         </is>
       </c>
-      <c r="G30" s="148" t="inlineStr">
+      <c r="G32" s="148" t="inlineStr">
         <is>
           <t>MEASURE 2.5, 2.11
 MANAGE 2.3</t>
         </is>
       </c>
-      <c r="H30" s="148" t="inlineStr">
+      <c r="H32" s="148" t="inlineStr">
         <is>
           <t>PR.DS-5, PR.DS-6
 PR.PS-1</t>
         </is>
       </c>
-      <c r="I30" s="148" t="inlineStr">
+      <c r="I32" s="148" t="inlineStr">
         <is>
           <t>LLM05: Output Hdlg
 LLM09: Misinfo</t>
         </is>
       </c>
-      <c r="J30" s="148" t="inlineStr">
+      <c r="J32" s="148" t="inlineStr">
         <is>
           <t>CC6.7, CC7.2
 PI1.5</t>
         </is>
       </c>
     </row>
-    <row r="31" ht="42" customHeight="1">
-      <c r="B31" s="193" t="inlineStr">
+    <row r="33" ht="42" customHeight="1">
+      <c r="B33" s="193" t="inlineStr">
         <is>
           <t>Rate Limiting</t>
         </is>
       </c>
-      <c r="C31" s="148" t="inlineStr">
+      <c r="C33" s="148" t="inlineStr">
         <is>
           <t>Availability
 Throttling</t>
         </is>
       </c>
-      <c r="D31" s="148" t="inlineStr">
+      <c r="D33" s="148" t="inlineStr">
         <is>
           <t>Art. 15(5)
 Cybersecurity</t>
         </is>
       </c>
-      <c r="E31" s="148" t="inlineStr">
+      <c r="E33" s="148" t="inlineStr">
         <is>
           <t>8.1 Operational
 A.8.2 Monitoring</t>
         </is>
       </c>
-      <c r="F31" s="148" t="inlineStr">
+      <c r="F33" s="148" t="inlineStr">
         <is>
           <t>AML.T0029
 Denial of Service</t>
         </is>
       </c>
-      <c r="G31" s="148" t="inlineStr">
+      <c r="G33" s="148" t="inlineStr">
         <is>
           <t>MANAGE 2.4
 MAP 5.2</t>
         </is>
       </c>
-      <c r="H31" s="148" t="inlineStr">
+      <c r="H33" s="148" t="inlineStr">
         <is>
           <t>PR.IR-1
 DE.AE-1</t>
         </is>
       </c>
-      <c r="I31" s="148" t="inlineStr">
+      <c r="I33" s="148" t="inlineStr">
         <is>
           <t>LLM10: Unbounded
 Consumption</t>
         </is>
       </c>
-      <c r="J31" s="148" t="inlineStr">
+      <c r="J33" s="148" t="inlineStr">
         <is>
           <t>CC6.1, A1.2
 CC7.2</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="42" customHeight="1">
-      <c r="B32" s="193" t="inlineStr">
+    <row r="34" ht="22" customHeight="1">
+      <c r="B34" s="193" t="inlineStr">
         <is>
           <t>Content Safety</t>
         </is>
       </c>
-      <c r="C32" s="148" t="inlineStr">
+      <c r="C34" s="148" t="inlineStr">
         <is>
           <t>Content Filtering
 Safety Controls</t>
         </is>
       </c>
-      <c r="D32" s="148" t="inlineStr">
+      <c r="D34" s="148" t="inlineStr">
         <is>
           <t>Art. 15(3)
 Art. 15(4)</t>
         </is>
       </c>
-      <c r="E32" s="148" t="inlineStr">
+      <c r="E34" s="148" t="inlineStr">
         <is>
           <t>A.7.3 AI Objectives
 A.8.4 Output</t>
         </is>
       </c>
-      <c r="F32" s="148" t="inlineStr">
+      <c r="F34" s="148" t="inlineStr">
         <is>
           <t>AML.T0048
 DoS ML Model</t>
         </is>
       </c>
-      <c r="G32" s="148" t="inlineStr">
+      <c r="G34" s="148" t="inlineStr">
         <is>
           <t>MEASURE 2.5, 2.11
 MANAGE 1.3</t>
         </is>
       </c>
-      <c r="H32" s="148" t="inlineStr">
+      <c r="H34" s="148" t="inlineStr">
         <is>
           <t>PR.DS-5
 DE.CM-1</t>
         </is>
       </c>
-      <c r="I32" s="148" t="inlineStr">
+      <c r="I34" s="148" t="inlineStr">
         <is>
           <t>LLM05: Output Hdlg
 LLM09: Misinfo</t>
         </is>
       </c>
-      <c r="J32" s="148" t="inlineStr">
+      <c r="J34" s="148" t="inlineStr">
         <is>
           <t>CC6.7, CC7.2
 PI1.5</t>
         </is>
       </c>
     </row>
-    <row r="33" ht="42" customHeight="1">
-      <c r="B33" s="193" t="inlineStr">
+    <row r="35" ht="42" customHeight="1">
+      <c r="B35" s="193" t="inlineStr">
         <is>
           <t>Domain Restrictions</t>
         </is>
       </c>
-      <c r="C33" s="148" t="inlineStr">
+      <c r="C35" s="148" t="inlineStr">
         <is>
           <t>Network Controls
 Egress Filter</t>
         </is>
       </c>
-      <c r="D33" s="148" t="inlineStr">
+      <c r="D35" s="148" t="inlineStr">
         <is>
           <t>Art. 15(5)
 Cybersecurity</t>
         </is>
       </c>
-      <c r="E33" s="148" t="inlineStr">
+      <c r="E35" s="148" t="inlineStr">
         <is>
           <t>A.8.3 Protection
 8.1 Security</t>
         </is>
       </c>
-      <c r="F33" s="148" t="inlineStr">
+      <c r="F35" s="148" t="inlineStr">
         <is>
           <t>Exfiltration
 defense</t>
         </is>
       </c>
-      <c r="G33" s="148" t="inlineStr">
+      <c r="G35" s="148" t="inlineStr">
         <is>
           <t>MANAGE 2.4
 MAP 4.2</t>
         </is>
       </c>
-      <c r="H33" s="148" t="inlineStr">
+      <c r="H35" s="148" t="inlineStr">
         <is>
           <t>PR.DS-2
 PR.AC-5</t>
         </is>
       </c>
-      <c r="I33" s="148" t="inlineStr">
+      <c r="I35" s="148" t="inlineStr">
         <is>
           <t>LLM06: Excessive
 Agency</t>
         </is>
       </c>
-      <c r="J33" s="148" t="inlineStr">
+      <c r="J35" s="148" t="inlineStr">
         <is>
           <t>CC6.6, CC6.7
 CC7.2</t>
         </is>
       </c>
     </row>
-    <row r="34" ht="22" customHeight="1">
-      <c r="B34" s="253" t="inlineStr">
+    <row r="36" ht="42" customHeight="1">
+      <c r="B36" s="253" t="inlineStr">
         <is>
           <t>SHADOW AI &amp; USAGE DISCOVERY</t>
         </is>
       </c>
-      <c r="C34" s="251" t="n"/>
-      <c r="D34" s="251" t="n"/>
-      <c r="E34" s="251" t="n"/>
-      <c r="F34" s="251" t="n"/>
-      <c r="G34" s="251" t="n"/>
-      <c r="H34" s="251" t="n"/>
-      <c r="I34" s="251" t="n"/>
-      <c r="J34" s="26" t="n"/>
-    </row>
-    <row r="35" ht="42" customHeight="1">
-      <c r="B35" s="193" t="inlineStr">
+      <c r="C36" s="251" t="n"/>
+      <c r="D36" s="251" t="n"/>
+      <c r="E36" s="251" t="n"/>
+      <c r="F36" s="251" t="n"/>
+      <c r="G36" s="251" t="n"/>
+      <c r="H36" s="251" t="n"/>
+      <c r="I36" s="251" t="n"/>
+      <c r="J36" s="26" t="n"/>
+    </row>
+    <row r="37" ht="42" customHeight="1">
+      <c r="B37" s="193" t="inlineStr">
         <is>
           <t>Tool Visibility</t>
         </is>
       </c>
-      <c r="C35" s="148" t="inlineStr">
+      <c r="C37" s="148" t="inlineStr">
         <is>
           <t>Shadow IT
 Discovery</t>
         </is>
       </c>
-      <c r="D35" s="148" t="inlineStr">
+      <c r="D37" s="148" t="inlineStr">
         <is>
           <t>Art. 9(2)(a)
 Inventory</t>
         </is>
       </c>
-      <c r="E35" s="148" t="inlineStr">
+      <c r="E37" s="148" t="inlineStr">
         <is>
           <t>A.4 AI Inventory
 9.1 Monitoring</t>
         </is>
       </c>
-      <c r="F35" s="148" t="inlineStr">
+      <c r="F37" s="148" t="inlineStr">
         <is>
           <t>AML.T0000
 Reconnaissance</t>
         </is>
       </c>
-      <c r="G35" s="148" t="inlineStr">
+      <c r="G37" s="148" t="inlineStr">
         <is>
           <t>GOVERN 1.5
 MAP 1.5</t>
         </is>
       </c>
-      <c r="H35" s="148" t="inlineStr">
+      <c r="H37" s="148" t="inlineStr">
         <is>
           <t>ID.AM-1, ID.AM-2
 DE.CM-7</t>
         </is>
       </c>
-      <c r="I35" s="148" t="inlineStr">
+      <c r="I37" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain</t>
         </is>
       </c>
-      <c r="J35" s="148" t="inlineStr">
+      <c r="J37" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC7.1
 CC3.2</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="42" customHeight="1">
-      <c r="B36" s="193" t="inlineStr">
+    <row r="38" ht="42" customHeight="1">
+      <c r="B38" s="193" t="inlineStr">
         <is>
           <t>Sanctioned Status</t>
         </is>
       </c>
-      <c r="C36" s="148" t="inlineStr">
+      <c r="C38" s="148" t="inlineStr">
         <is>
           <t>Asset Mgmt
 Sanctioning</t>
         </is>
       </c>
-      <c r="D36" s="148" t="inlineStr">
+      <c r="D38" s="148" t="inlineStr">
         <is>
           <t>Art. 9(2)(a)
 Art. 17(1)</t>
         </is>
       </c>
-      <c r="E36" s="148" t="inlineStr">
+      <c r="E38" s="148" t="inlineStr">
         <is>
           <t>A.4 AI Inventory
 A.2 AI Policy</t>
         </is>
       </c>
-      <c r="F36" s="148" t="inlineStr">
+      <c r="F38" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G36" s="148" t="inlineStr">
+      <c r="G38" s="148" t="inlineStr">
         <is>
           <t>GOVERN 1.4, 1.6
 MAP 1.1</t>
         </is>
       </c>
-      <c r="H36" s="148" t="inlineStr">
+      <c r="H38" s="148" t="inlineStr">
         <is>
           <t>ID.AM-1
 GV.PO-1</t>
         </is>
       </c>
-      <c r="I36" s="148" t="inlineStr">
+      <c r="I38" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain</t>
         </is>
       </c>
-      <c r="J36" s="148" t="inlineStr">
+      <c r="J38" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC6.2
 CC7.1</t>
         </is>
       </c>
     </row>
-    <row r="37" ht="42" customHeight="1">
-      <c r="B37" s="193" t="inlineStr">
+    <row r="39" ht="22" customHeight="1">
+      <c r="B39" s="193" t="inlineStr">
         <is>
           <t>User Access Tracked</t>
         </is>
       </c>
-      <c r="C37" s="148" t="inlineStr">
+      <c r="C39" s="148" t="inlineStr">
         <is>
           <t>Access Logging
 Monitoring</t>
         </is>
       </c>
-      <c r="D37" s="148" t="inlineStr">
+      <c r="D39" s="148" t="inlineStr">
         <is>
           <t>Art. 12(1)
 Record-keeping</t>
         </is>
       </c>
-      <c r="E37" s="148" t="inlineStr">
+      <c r="E39" s="148" t="inlineStr">
         <is>
           <t>9.1 Monitoring
 A.8.2 Monitoring</t>
         </is>
       </c>
-      <c r="F37" s="148" t="inlineStr">
+      <c r="F39" s="148" t="inlineStr">
         <is>
           <t>Collection
 defense</t>
         </is>
       </c>
-      <c r="G37" s="148" t="inlineStr">
+      <c r="G39" s="148" t="inlineStr">
         <is>
           <t>MEASURE 1.1, 1.3
 MANAGE 4.1</t>
         </is>
       </c>
-      <c r="H37" s="148" t="inlineStr">
+      <c r="H39" s="148" t="inlineStr">
         <is>
           <t>DE.CM-1, DE.CM-3
 PR.AC-1</t>
         </is>
       </c>
-      <c r="I37" s="148" t="inlineStr">
+      <c r="I39" s="148" t="inlineStr">
         <is>
           <t>LLM02: Sensitive
 Info Disclosure</t>
         </is>
       </c>
-      <c r="J37" s="148" t="inlineStr">
+      <c r="J39" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC6.2
 CC7.2</t>
         </is>
       </c>
     </row>
-    <row r="38" ht="42" customHeight="1">
-      <c r="B38" s="193" t="inlineStr">
+    <row r="40" ht="42" customHeight="1">
+      <c r="B40" s="193" t="inlineStr">
         <is>
           <t>Usage Analytics</t>
         </is>
       </c>
-      <c r="C38" s="148" t="inlineStr">
+      <c r="C40" s="148" t="inlineStr">
         <is>
           <t>Analytics
 Anomalies</t>
         </is>
       </c>
-      <c r="D38" s="148" t="inlineStr">
+      <c r="D40" s="148" t="inlineStr">
         <is>
           <t>Art. 12(1)
 Art. 9(9)</t>
         </is>
       </c>
-      <c r="E38" s="148" t="inlineStr">
+      <c r="E40" s="148" t="inlineStr">
         <is>
           <t>9.1 Monitoring
 9.3 Mgmt Review</t>
         </is>
       </c>
-      <c r="F38" s="148" t="inlineStr">
+      <c r="F40" s="148" t="inlineStr">
         <is>
           <t>ML Model Access
 defense</t>
         </is>
       </c>
-      <c r="G38" s="148" t="inlineStr">
+      <c r="G40" s="148" t="inlineStr">
         <is>
           <t>MEASURE 1.1-1.3
 MANAGE 4.2</t>
         </is>
       </c>
-      <c r="H38" s="148" t="inlineStr">
+      <c r="H40" s="148" t="inlineStr">
         <is>
           <t>DE.AE-2, DE.AE-3
 ID.IM-1</t>
         </is>
       </c>
-      <c r="I38" s="148" t="inlineStr">
+      <c r="I40" s="148" t="inlineStr">
         <is>
           <t>LLM10: Unbounded
 Consumption</t>
         </is>
       </c>
-      <c r="J38" s="148" t="inlineStr">
+      <c r="J40" s="148" t="inlineStr">
         <is>
           <t>CC7.1, CC7.2
 CC4.1</t>
         </is>
       </c>
     </row>
-    <row r="39" ht="22" customHeight="1">
-      <c r="B39" s="254" t="inlineStr">
+    <row r="41" ht="42" customHeight="1">
+      <c r="B41" s="254" t="inlineStr">
         <is>
           <t>OBSERVABILITY &amp; EVALUATION</t>
         </is>
       </c>
-      <c r="C39" s="251" t="n"/>
-      <c r="D39" s="251" t="n"/>
-      <c r="E39" s="251" t="n"/>
-      <c r="F39" s="251" t="n"/>
-      <c r="G39" s="251" t="n"/>
-      <c r="H39" s="251" t="n"/>
-      <c r="I39" s="26" t="n"/>
-      <c r="J39" s="152" t="n"/>
-    </row>
-    <row r="40" ht="42" customHeight="1">
-      <c r="B40" s="193" t="inlineStr">
+      <c r="C41" s="251" t="n"/>
+      <c r="D41" s="251" t="n"/>
+      <c r="E41" s="251" t="n"/>
+      <c r="F41" s="251" t="n"/>
+      <c r="G41" s="251" t="n"/>
+      <c r="H41" s="251" t="n"/>
+      <c r="I41" s="26" t="n"/>
+      <c r="J41" s="152" t="n"/>
+    </row>
+    <row r="42" ht="42" customHeight="1">
+      <c r="B42" s="193" t="inlineStr">
         <is>
           <t>Audit Logging</t>
         </is>
       </c>
-      <c r="C40" s="148" t="inlineStr">
+      <c r="C42" s="148" t="inlineStr">
         <is>
           <t>Audit Logging
 Traceability</t>
         </is>
       </c>
-      <c r="D40" s="148" t="inlineStr">
+      <c r="D42" s="148" t="inlineStr">
         <is>
           <t>Art. 12(2)(3)
 Automatic Logs</t>
         </is>
       </c>
-      <c r="E40" s="148" t="inlineStr">
+      <c r="E42" s="148" t="inlineStr">
         <is>
           <t>A.8.5 Recording
 9.2 Internal Audit</t>
         </is>
       </c>
-      <c r="F40" s="148" t="inlineStr">
+      <c r="F42" s="148" t="inlineStr">
         <is>
           <t>All tactics
 defense</t>
         </is>
       </c>
-      <c r="G40" s="148" t="inlineStr">
+      <c r="G42" s="148" t="inlineStr">
         <is>
           <t>MEASURE 2.1-2.3
 GOVERN 4.1</t>
         </is>
       </c>
-      <c r="H40" s="148" t="inlineStr">
+      <c r="H42" s="148" t="inlineStr">
         <is>
           <t>DE.CM-1, DE.CM-9
 PR.PS-4</t>
         </is>
       </c>
-      <c r="I40" s="148" t="inlineStr">
+      <c r="I42" s="148" t="inlineStr">
         <is>
           <t>All: Supports
 detection</t>
         </is>
       </c>
-      <c r="J40" s="148" t="inlineStr">
+      <c r="J42" s="148" t="inlineStr">
         <is>
           <t>CC7.2, CC7.3
 CC4.1</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="42" customHeight="1">
-      <c r="B41" s="193" t="inlineStr">
+    <row r="43" ht="42" customHeight="1">
+      <c r="B43" s="193" t="inlineStr">
         <is>
           <t>Log Retention</t>
         </is>
       </c>
-      <c r="C41" s="148" t="inlineStr">
+      <c r="C43" s="148" t="inlineStr">
         <is>
           <t>Retention
 Archival</t>
         </is>
       </c>
-      <c r="D41" s="148" t="inlineStr">
+      <c r="D43" s="148" t="inlineStr">
         <is>
           <t>Art. 12(3)
 5+ years</t>
         </is>
       </c>
-      <c r="E41" s="148" t="inlineStr">
+      <c r="E43" s="148" t="inlineStr">
         <is>
           <t>7.5 Doc Info
 A.8.5 Recording</t>
         </is>
       </c>
-      <c r="F41" s="148" t="inlineStr">
+      <c r="F43" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G41" s="148" t="inlineStr">
+      <c r="G43" s="148" t="inlineStr">
         <is>
           <t>GOVERN 4.1
 MANAGE 4.1</t>
         </is>
       </c>
-      <c r="H41" s="148" t="inlineStr">
+      <c r="H43" s="148" t="inlineStr">
         <is>
           <t>PR.DS-3
 GV.DP-4</t>
         </is>
       </c>
-      <c r="I41" s="148" t="inlineStr">
+      <c r="I43" s="148" t="inlineStr">
         <is>
           <t>All: Evidence
 retention</t>
         </is>
       </c>
-      <c r="J41" s="148" t="inlineStr">
+      <c r="J43" s="148" t="inlineStr">
         <is>
           <t>CC7.3, CC7.4
 C1.1</t>
         </is>
       </c>
     </row>
-    <row r="42" ht="42" customHeight="1">
-      <c r="B42" s="193" t="inlineStr">
+    <row r="44" ht="42" customHeight="1">
+      <c r="B44" s="193" t="inlineStr">
         <is>
           <t>SIEM Integration</t>
         </is>
       </c>
-      <c r="C42" s="148" t="inlineStr">
+      <c r="C44" s="148" t="inlineStr">
         <is>
           <t>Central Logging
 Correlation</t>
         </is>
       </c>
-      <c r="D42" s="148" t="inlineStr">
+      <c r="D44" s="148" t="inlineStr">
         <is>
           <t>Art. 17(1)(i)
 Incident</t>
         </is>
       </c>
-      <c r="E42" s="148" t="inlineStr">
+      <c r="E44" s="148" t="inlineStr">
         <is>
           <t>9.1 Monitoring
 10.1 Nonconform.</t>
         </is>
       </c>
-      <c r="F42" s="148" t="inlineStr">
+      <c r="F44" s="148" t="inlineStr">
         <is>
           <t>Detection
 tactics</t>
         </is>
       </c>
-      <c r="G42" s="148" t="inlineStr">
+      <c r="G44" s="148" t="inlineStr">
         <is>
           <t>MANAGE 3.1, 3.2
 MEASURE 3.3</t>
         </is>
       </c>
-      <c r="H42" s="148" t="inlineStr">
+      <c r="H44" s="148" t="inlineStr">
         <is>
           <t>DE.CM-1
 DE.AE-5</t>
         </is>
       </c>
-      <c r="I42" s="148" t="inlineStr">
+      <c r="I44" s="148" t="inlineStr">
         <is>
           <t>All: Central
 monitoring</t>
         </is>
       </c>
-      <c r="J42" s="148" t="inlineStr">
+      <c r="J44" s="148" t="inlineStr">
         <is>
           <t>CC7.2, CC7.3
 CC4.2</t>
         </is>
       </c>
     </row>
-    <row r="43" ht="42" customHeight="1">
-      <c r="B43" s="193" t="inlineStr">
+    <row r="45" ht="22" customHeight="1">
+      <c r="B45" s="193" t="inlineStr">
         <is>
           <t>Alerting Configured</t>
         </is>
       </c>
-      <c r="C43" s="148" t="inlineStr">
+      <c r="C45" s="148" t="inlineStr">
         <is>
           <t>Alerting
 Thresholds</t>
         </is>
       </c>
-      <c r="D43" s="148" t="inlineStr">
+      <c r="D45" s="148" t="inlineStr">
         <is>
           <t>Art. 17(1)(i)
 Incident</t>
         </is>
       </c>
-      <c r="E43" s="148" t="inlineStr">
+      <c r="E45" s="148" t="inlineStr">
         <is>
           <t>10.1 Nonconform.
 A.8.2 Monitoring</t>
         </is>
       </c>
-      <c r="F43" s="148" t="inlineStr">
+      <c r="F45" s="148" t="inlineStr">
         <is>
           <t>All Detection
 tactics</t>
         </is>
       </c>
-      <c r="G43" s="148" t="inlineStr">
+      <c r="G45" s="148" t="inlineStr">
         <is>
           <t>MANAGE 3.1, 3.2
 MEASURE 3.3</t>
         </is>
       </c>
-      <c r="H43" s="148" t="inlineStr">
+      <c r="H45" s="148" t="inlineStr">
         <is>
           <t>DE.AE-1 to DE.AE-8
 RS.AN-1</t>
         </is>
       </c>
-      <c r="I43" s="148" t="inlineStr">
+      <c r="I45" s="148" t="inlineStr">
         <is>
           <t>All: Real-time
 detection</t>
         </is>
       </c>
-      <c r="J43" s="148" t="inlineStr">
+      <c r="J45" s="148" t="inlineStr">
         <is>
           <t>CC7.2, CC7.4
 A1.2</t>
         </is>
       </c>
     </row>
-    <row r="44" ht="42" customHeight="1">
-      <c r="B44" s="193" t="inlineStr">
+    <row r="46" ht="42" customHeight="1">
+      <c r="B46" s="193" t="inlineStr">
         <is>
           <t>Performance Monitoring</t>
         </is>
       </c>
-      <c r="C44" s="148" t="inlineStr">
+      <c r="C46" s="148" t="inlineStr">
         <is>
           <t>Performance
 Drift Detection</t>
         </is>
       </c>
-      <c r="D44" s="148" t="inlineStr">
+      <c r="D46" s="148" t="inlineStr">
         <is>
           <t>Art. 15(3)
 Accuracy</t>
         </is>
       </c>
-      <c r="E44" s="148" t="inlineStr">
+      <c r="E46" s="148" t="inlineStr">
         <is>
           <t>9.1 Monitoring
 A.8.4 Output</t>
         </is>
       </c>
-      <c r="F44" s="148" t="inlineStr">
+      <c r="F46" s="148" t="inlineStr">
         <is>
           <t>AML.T0024
 Model Drift</t>
         </is>
       </c>
-      <c r="G44" s="148" t="inlineStr">
+      <c r="G46" s="148" t="inlineStr">
         <is>
           <t>MEASURE 1.1-1.3
 MEASURE 2.5-2.11</t>
         </is>
       </c>
-      <c r="H44" s="148" t="inlineStr">
+      <c r="H46" s="148" t="inlineStr">
         <is>
           <t>DE.CM-1
 ID.IM-2</t>
         </is>
       </c>
-      <c r="I44" s="148" t="inlineStr">
+      <c r="I46" s="148" t="inlineStr">
         <is>
           <t>LLM09: Misinfo
 (drift)</t>
         </is>
       </c>
-      <c r="J44" s="148" t="inlineStr">
+      <c r="J46" s="148" t="inlineStr">
         <is>
           <t>CC7.1, A1.1
 PI1.3</t>
         </is>
       </c>
     </row>
-    <row r="45" ht="22" customHeight="1">
-      <c r="B45" s="255" t="inlineStr">
+    <row r="47" ht="42" customHeight="1">
+      <c r="B47" s="255" t="inlineStr">
         <is>
           <t>DATA PROTECTION FOR AI</t>
         </is>
       </c>
-      <c r="C45" s="251" t="n"/>
-      <c r="D45" s="251" t="n"/>
-      <c r="E45" s="251" t="n"/>
-      <c r="F45" s="251" t="n"/>
-      <c r="G45" s="251" t="n"/>
-      <c r="H45" s="251" t="n"/>
-      <c r="I45" s="251" t="n"/>
-      <c r="J45" s="26" t="n"/>
-    </row>
-    <row r="46" ht="42" customHeight="1">
-      <c r="B46" s="193" t="inlineStr">
+      <c r="C47" s="251" t="n"/>
+      <c r="D47" s="251" t="n"/>
+      <c r="E47" s="251" t="n"/>
+      <c r="F47" s="251" t="n"/>
+      <c r="G47" s="251" t="n"/>
+      <c r="H47" s="251" t="n"/>
+      <c r="I47" s="251" t="n"/>
+      <c r="J47" s="26" t="n"/>
+    </row>
+    <row r="48" ht="42" customHeight="1">
+      <c r="B48" s="193" t="inlineStr">
         <is>
           <t>DLP Rules Active</t>
         </is>
       </c>
-      <c r="C46" s="148" t="inlineStr">
+      <c r="C48" s="148" t="inlineStr">
         <is>
           <t>Data Loss Prev.
 Classification</t>
         </is>
       </c>
-      <c r="D46" s="148" t="inlineStr">
+      <c r="D48" s="148" t="inlineStr">
         <is>
           <t>Art. 10(1-5)
 Data Gov.</t>
         </is>
       </c>
-      <c r="E46" s="148" t="inlineStr">
+      <c r="E48" s="148" t="inlineStr">
         <is>
           <t>A.6 Data for AI
 A.8.3 Protection</t>
         </is>
       </c>
-      <c r="F46" s="148" t="inlineStr">
+      <c r="F48" s="148" t="inlineStr">
         <is>
           <t>AML.T0037
 Exfiltration</t>
         </is>
       </c>
-      <c r="G46" s="148" t="inlineStr">
+      <c r="G48" s="148" t="inlineStr">
         <is>
           <t>MAP 4.1, 4.2
 MANAGE 2.4</t>
         </is>
       </c>
-      <c r="H46" s="148" t="inlineStr">
+      <c r="H48" s="148" t="inlineStr">
         <is>
           <t>PR.DS-1 to PR.DS-5
 PR.PS-4</t>
         </is>
       </c>
-      <c r="I46" s="148" t="inlineStr">
+      <c r="I48" s="148" t="inlineStr">
         <is>
           <t>LLM02: Sensitive
 Info Disclosure</t>
         </is>
       </c>
-      <c r="J46" s="148" t="inlineStr">
+      <c r="J48" s="148" t="inlineStr">
         <is>
           <t>CC6.7, C1.1
 C1.2</t>
         </is>
       </c>
     </row>
-    <row r="47" ht="42" customHeight="1">
-      <c r="B47" s="193" t="inlineStr">
+    <row r="49" ht="42" customHeight="1">
+      <c r="B49" s="193" t="inlineStr">
         <is>
           <t>PII Detection</t>
         </is>
       </c>
-      <c r="C47" s="148" t="inlineStr">
+      <c r="C49" s="148" t="inlineStr">
         <is>
           <t>PII Handling
 Privacy</t>
         </is>
       </c>
-      <c r="D47" s="148" t="inlineStr">
+      <c r="D49" s="148" t="inlineStr">
         <is>
           <t>Art. 10(5)
 GDPR</t>
         </is>
       </c>
-      <c r="E47" s="148" t="inlineStr">
+      <c r="E49" s="148" t="inlineStr">
         <is>
           <t>A.6.3 Acquisition
 A.6.5 Bias</t>
         </is>
       </c>
-      <c r="F47" s="148" t="inlineStr">
+      <c r="F49" s="148" t="inlineStr">
         <is>
           <t>Collection
 defense</t>
         </is>
       </c>
-      <c r="G47" s="148" t="inlineStr">
+      <c r="G49" s="148" t="inlineStr">
         <is>
           <t>MAP 4.1
 GOVERN 5.1, 5.2</t>
         </is>
       </c>
-      <c r="H47" s="148" t="inlineStr">
+      <c r="H49" s="148" t="inlineStr">
         <is>
           <t>PR.DS-3, PR.DS-5
 GV.DP-1</t>
         </is>
       </c>
-      <c r="I47" s="148" t="inlineStr">
+      <c r="I49" s="148" t="inlineStr">
         <is>
           <t>LLM02: Sensitive
 Info Disclosure</t>
         </is>
       </c>
-      <c r="J47" s="148" t="inlineStr">
+      <c r="J49" s="148" t="inlineStr">
         <is>
           <t>P1.1, P3.1
 C1.1</t>
         </is>
       </c>
     </row>
-    <row r="48" ht="42" customHeight="1">
-      <c r="B48" s="193" t="inlineStr">
+    <row r="50" ht="42" customHeight="1">
+      <c r="B50" s="193" t="inlineStr">
         <is>
           <t>Data Classification</t>
         </is>
       </c>
-      <c r="C48" s="148" t="inlineStr">
+      <c r="C50" s="148" t="inlineStr">
         <is>
           <t>Classification
 Labeling</t>
         </is>
       </c>
-      <c r="D48" s="148" t="inlineStr">
+      <c r="D50" s="148" t="inlineStr">
         <is>
           <t>Art. 10(2)
 Data Gov.</t>
         </is>
       </c>
-      <c r="E48" s="148" t="inlineStr">
+      <c r="E50" s="148" t="inlineStr">
         <is>
           <t>A.6.2 Data Source
 A.6.4 Data Prep</t>
         </is>
       </c>
-      <c r="F48" s="148" t="inlineStr">
+      <c r="F50" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G48" s="148" t="inlineStr">
+      <c r="G50" s="148" t="inlineStr">
         <is>
           <t>MAP 4.1, 4.2
 GOVERN 5.2</t>
         </is>
       </c>
-      <c r="H48" s="148" t="inlineStr">
+      <c r="H50" s="148" t="inlineStr">
         <is>
           <t>PR.DS-1
 ID.AM-5</t>
         </is>
       </c>
-      <c r="I48" s="148" t="inlineStr">
+      <c r="I50" s="148" t="inlineStr">
         <is>
           <t>LLM02: Sensitive
 Info Disclosure</t>
         </is>
       </c>
-      <c r="J48" s="148" t="inlineStr">
+      <c r="J50" s="148" t="inlineStr">
         <is>
           <t>CC6.1, C1.1
 P1.1</t>
         </is>
       </c>
     </row>
-    <row r="49" ht="42" customHeight="1">
-      <c r="B49" s="193" t="inlineStr">
+    <row r="51" ht="42" customHeight="1">
+      <c r="B51" s="193" t="inlineStr">
         <is>
           <t>Encryption - Transit</t>
         </is>
       </c>
-      <c r="C49" s="148" t="inlineStr">
+      <c r="C51" s="148" t="inlineStr">
         <is>
           <t>Encryption
 TLS</t>
         </is>
       </c>
-      <c r="D49" s="148" t="inlineStr">
+      <c r="D51" s="148" t="inlineStr">
         <is>
           <t>Art. 15(5)
 Cybersecurity</t>
         </is>
       </c>
-      <c r="E49" s="148" t="inlineStr">
+      <c r="E51" s="148" t="inlineStr">
         <is>
           <t>A.8.3 Protection
 8.1 Security</t>
         </is>
       </c>
-      <c r="F49" s="148" t="inlineStr">
+      <c r="F51" s="148" t="inlineStr">
         <is>
           <t>Exfiltration
 defense</t>
         </is>
       </c>
-      <c r="G49" s="148" t="inlineStr">
+      <c r="G51" s="148" t="inlineStr">
         <is>
           <t>MANAGE 2.4
 MAP 4.2</t>
         </is>
       </c>
-      <c r="H49" s="148" t="inlineStr">
+      <c r="H51" s="148" t="inlineStr">
         <is>
           <t>PR.DS-1, PR.DS-2
 PR.DS-5</t>
         </is>
       </c>
-      <c r="I49" s="148" t="inlineStr">
+      <c r="I51" s="148" t="inlineStr">
         <is>
           <t>LLM02: Sensitive
 Info Disclosure</t>
         </is>
       </c>
-      <c r="J49" s="148" t="inlineStr">
+      <c r="J51" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC6.7
 C1.2</t>
         </is>
       </c>
     </row>
-    <row r="50" ht="42" customHeight="1">
-      <c r="B50" s="193" t="inlineStr">
+    <row r="52" ht="42" customHeight="1">
+      <c r="B52" s="193" t="inlineStr">
         <is>
           <t>Encryption - Rest</t>
         </is>
       </c>
-      <c r="C50" s="148" t="inlineStr">
+      <c r="C52" s="148" t="inlineStr">
         <is>
           <t>Encryption
 Key Mgmt</t>
         </is>
       </c>
-      <c r="D50" s="148" t="inlineStr">
+      <c r="D52" s="148" t="inlineStr">
         <is>
           <t>Art. 15(5)
 Cybersecurity</t>
         </is>
       </c>
-      <c r="E50" s="148" t="inlineStr">
+      <c r="E52" s="148" t="inlineStr">
         <is>
           <t>A.8.3 Protection
 8.1 Security</t>
         </is>
       </c>
-      <c r="F50" s="148" t="inlineStr">
+      <c r="F52" s="148" t="inlineStr">
         <is>
           <t>Exfiltration
 defense</t>
         </is>
       </c>
-      <c r="G50" s="148" t="inlineStr">
+      <c r="G52" s="148" t="inlineStr">
         <is>
           <t>MANAGE 2.4
 MAP 4.2</t>
         </is>
       </c>
-      <c r="H50" s="148" t="inlineStr">
+      <c r="H52" s="148" t="inlineStr">
         <is>
           <t>PR.DS-1
 PR.DS-5</t>
         </is>
       </c>
-      <c r="I50" s="148" t="inlineStr">
+      <c r="I52" s="148" t="inlineStr">
         <is>
           <t>LLM02: Sensitive
 Info Disclosure</t>
         </is>
       </c>
-      <c r="J50" s="148" t="inlineStr">
+      <c r="J52" s="148" t="inlineStr">
         <is>
           <t>CC6.1, C1.1
 C1.2</t>
         </is>
       </c>
     </row>
-    <row r="51" ht="42" customHeight="1">
-      <c r="B51" s="193" t="inlineStr">
+    <row r="53" ht="22" customHeight="1">
+      <c r="B53" s="193" t="inlineStr">
         <is>
           <t>Data Masking</t>
         </is>
       </c>
-      <c r="C51" s="148" t="inlineStr">
+      <c r="C53" s="148" t="inlineStr">
         <is>
           <t>Masking
 Redaction</t>
         </is>
       </c>
-      <c r="D51" s="148" t="inlineStr">
+      <c r="D53" s="148" t="inlineStr">
         <is>
           <t>Art. 10(5)
 GDPR</t>
         </is>
       </c>
-      <c r="E51" s="148" t="inlineStr">
+      <c r="E53" s="148" t="inlineStr">
         <is>
           <t>A.6.5 Data Prep
 A.8.5 Recording</t>
         </is>
       </c>
-      <c r="F51" s="148" t="inlineStr">
+      <c r="F53" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G51" s="148" t="inlineStr">
+      <c r="G53" s="148" t="inlineStr">
         <is>
           <t>MAP 4.1
 MANAGE 2.4</t>
         </is>
       </c>
-      <c r="H51" s="148" t="inlineStr">
+      <c r="H53" s="148" t="inlineStr">
         <is>
           <t>PR.DS-3, PR.DS-5
 PR.PS-4</t>
         </is>
       </c>
-      <c r="I51" s="148" t="inlineStr">
+      <c r="I53" s="148" t="inlineStr">
         <is>
           <t>LLM02: Sensitive
 Info Disclosure</t>
         </is>
       </c>
-      <c r="J51" s="148" t="inlineStr">
+      <c r="J53" s="148" t="inlineStr">
         <is>
           <t>C1.1, C1.2
 P3.2</t>
         </is>
       </c>
     </row>
-    <row r="52" ht="42" customHeight="1">
-      <c r="B52" s="193" t="inlineStr">
+    <row r="54" ht="42" customHeight="1">
+      <c r="B54" s="193" t="inlineStr">
         <is>
           <t>Retention Policies</t>
         </is>
       </c>
-      <c r="C52" s="148" t="inlineStr">
+      <c r="C54" s="148" t="inlineStr">
         <is>
           <t>Data Lifecycle
 Retention</t>
         </is>
       </c>
-      <c r="D52" s="148" t="inlineStr">
+      <c r="D54" s="148" t="inlineStr">
         <is>
           <t>Art. 10(5)
 Minimization</t>
         </is>
       </c>
-      <c r="E52" s="148" t="inlineStr">
+      <c r="E54" s="148" t="inlineStr">
         <is>
           <t>A.6.5 Data Prep
 A.10 Third Party</t>
         </is>
       </c>
-      <c r="F52" s="148" t="inlineStr">
+      <c r="F54" s="148" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G52" s="148" t="inlineStr">
+      <c r="G54" s="148" t="inlineStr">
         <is>
           <t>MAP 4.1
 GOVERN 5.2</t>
         </is>
       </c>
-      <c r="H52" s="148" t="inlineStr">
+      <c r="H54" s="148" t="inlineStr">
         <is>
           <t>PR.DS-3
 GV.DP-4</t>
         </is>
       </c>
-      <c r="I52" s="148" t="inlineStr">
+      <c r="I54" s="148" t="inlineStr">
         <is>
           <t>LLM02: Sensitive
 Info Disclosure</t>
         </is>
       </c>
-      <c r="J52" s="148" t="inlineStr">
+      <c r="J54" s="148" t="inlineStr">
         <is>
           <t>C1.1, P4.2
 CC7.4</t>
         </is>
       </c>
     </row>
-    <row r="53" ht="22" customHeight="1">
-      <c r="B53" s="256" t="inlineStr">
+    <row r="55" ht="42" customHeight="1">
+      <c r="B55" s="256" t="inlineStr">
         <is>
           <t>NHI &amp; AGENTIC ACCESS</t>
         </is>
       </c>
-      <c r="C53" s="251" t="n"/>
-      <c r="D53" s="251" t="n"/>
-      <c r="E53" s="251" t="n"/>
-      <c r="F53" s="251" t="n"/>
-      <c r="G53" s="251" t="n"/>
-      <c r="H53" s="251" t="n"/>
-      <c r="I53" s="26" t="n"/>
-      <c r="J53" s="153" t="n"/>
-    </row>
-    <row r="54" ht="42" customHeight="1">
-      <c r="B54" s="193" t="inlineStr">
+      <c r="C55" s="251" t="n"/>
+      <c r="D55" s="251" t="n"/>
+      <c r="E55" s="251" t="n"/>
+      <c r="F55" s="251" t="n"/>
+      <c r="G55" s="251" t="n"/>
+      <c r="H55" s="251" t="n"/>
+      <c r="I55" s="26" t="n"/>
+      <c r="J55" s="153" t="n"/>
+    </row>
+    <row r="56" ht="42" customHeight="1">
+      <c r="B56" s="193" t="inlineStr">
         <is>
           <t>Service Account Scoping</t>
         </is>
       </c>
-      <c r="C54" s="148" t="inlineStr">
+      <c r="C56" s="148" t="inlineStr">
         <is>
           <t>Identity Mgmt
 Service Accts</t>
         </is>
       </c>
-      <c r="D54" s="148" t="inlineStr">
+      <c r="D56" s="148" t="inlineStr">
         <is>
           <t>Art. 14(4)(d)
 Access Control</t>
         </is>
       </c>
-      <c r="E54" s="148" t="inlineStr">
+      <c r="E56" s="148" t="inlineStr">
         <is>
           <t>A.8.1 Operation
 8.1 Access Control</t>
         </is>
       </c>
-      <c r="F54" s="148" t="inlineStr">
+      <c r="F56" s="148" t="inlineStr">
         <is>
           <t>AML.T0012
 Valid Accounts</t>
         </is>
       </c>
-      <c r="G54" s="148" t="inlineStr">
+      <c r="G56" s="148" t="inlineStr">
         <is>
           <t>GOVERN 1.3
 MAP 3.3</t>
         </is>
       </c>
-      <c r="H54" s="148" t="inlineStr">
+      <c r="H56" s="148" t="inlineStr">
         <is>
           <t>PR.AA-1 to PR.AA-5
 PR.PS-2</t>
         </is>
       </c>
-      <c r="I54" s="148" t="inlineStr">
+      <c r="I56" s="148" t="inlineStr">
         <is>
           <t>LLM06: Excessive
 Agency</t>
         </is>
       </c>
-      <c r="J54" s="148" t="inlineStr">
+      <c r="J56" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC6.2
 CC6.3</t>
         </is>
       </c>
     </row>
-    <row r="55" ht="42" customHeight="1">
-      <c r="B55" s="193" t="inlineStr">
+    <row r="57" ht="42" customHeight="1">
+      <c r="B57" s="193" t="inlineStr">
         <is>
           <t>Secrets Management</t>
         </is>
       </c>
-      <c r="C55" s="148" t="inlineStr">
+      <c r="C57" s="148" t="inlineStr">
         <is>
           <t>Secrets Mgmt
 Vault</t>
         </is>
       </c>
-      <c r="D55" s="148" t="inlineStr">
+      <c r="D57" s="148" t="inlineStr">
         <is>
           <t>Art. 15(5)
 Cybersecurity</t>
         </is>
       </c>
-      <c r="E55" s="148" t="inlineStr">
+      <c r="E57" s="148" t="inlineStr">
         <is>
           <t>A.8.3 Protection
 8.1 Security</t>
         </is>
       </c>
-      <c r="F55" s="148" t="inlineStr">
+      <c r="F57" s="148" t="inlineStr">
         <is>
           <t>Credential Access
 defense</t>
         </is>
       </c>
-      <c r="G55" s="148" t="inlineStr">
+      <c r="G57" s="148" t="inlineStr">
         <is>
           <t>MANAGE 2.4
 GOVERN 6.1</t>
         </is>
       </c>
-      <c r="H55" s="148" t="inlineStr">
+      <c r="H57" s="148" t="inlineStr">
         <is>
           <t>PR.AA-2, PR.AA-5
 PR.DS-1</t>
         </is>
       </c>
-      <c r="I55" s="148" t="inlineStr">
+      <c r="I57" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain</t>
         </is>
       </c>
-      <c r="J55" s="148" t="inlineStr">
+      <c r="J57" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC6.6
 C1.2</t>
         </is>
       </c>
     </row>
-    <row r="56" ht="42" customHeight="1">
-      <c r="B56" s="193" t="inlineStr">
+    <row r="58" ht="42" customHeight="1">
+      <c r="B58" s="193" t="inlineStr">
         <is>
           <t>Credential Rotation</t>
         </is>
       </c>
-      <c r="C56" s="148" t="inlineStr">
+      <c r="C58" s="148" t="inlineStr">
         <is>
           <t>Credential Hygiene
 Rotation</t>
         </is>
       </c>
-      <c r="D56" s="148" t="inlineStr">
+      <c r="D58" s="148" t="inlineStr">
         <is>
           <t>Art. 15(5)
 Cybersecurity</t>
         </is>
       </c>
-      <c r="E56" s="148" t="inlineStr">
+      <c r="E58" s="148" t="inlineStr">
         <is>
           <t>A.8.3 Protection
 8.1 Security</t>
         </is>
       </c>
-      <c r="F56" s="148" t="inlineStr">
+      <c r="F58" s="148" t="inlineStr">
         <is>
           <t>Credential Access
 defense</t>
         </is>
       </c>
-      <c r="G56" s="148" t="inlineStr">
+      <c r="G58" s="148" t="inlineStr">
         <is>
           <t>MANAGE 2.4
 GOVERN 6.1</t>
         </is>
       </c>
-      <c r="H56" s="148" t="inlineStr">
+      <c r="H58" s="148" t="inlineStr">
         <is>
           <t>PR.AA-2, PR.AA-5
 PR.PS-1</t>
         </is>
       </c>
-      <c r="I56" s="148" t="inlineStr">
+      <c r="I58" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain</t>
         </is>
       </c>
-      <c r="J56" s="148" t="inlineStr">
+      <c r="J58" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC6.2
 CC6.6</t>
         </is>
       </c>
     </row>
-    <row r="57" ht="42" customHeight="1">
-      <c r="B57" s="193" t="inlineStr">
+    <row r="59" ht="42" customHeight="1">
+      <c r="B59" s="193" t="inlineStr">
         <is>
           <t>Short-Lived Tokens</t>
         </is>
       </c>
-      <c r="C57" s="148" t="inlineStr">
+      <c r="C59" s="148" t="inlineStr">
         <is>
           <t>Token Mgmt
 Expiry</t>
         </is>
       </c>
-      <c r="D57" s="148" t="inlineStr">
+      <c r="D59" s="148" t="inlineStr">
         <is>
           <t>Art. 15(5)
 Cybersecurity</t>
         </is>
       </c>
-      <c r="E57" s="148" t="inlineStr">
+      <c r="E59" s="148" t="inlineStr">
         <is>
           <t>A.8.1 Operation
 8.1 Access Control</t>
         </is>
       </c>
-      <c r="F57" s="148" t="inlineStr">
+      <c r="F59" s="148" t="inlineStr">
         <is>
           <t>Persistence
 defense</t>
         </is>
       </c>
-      <c r="G57" s="148" t="inlineStr">
+      <c r="G59" s="148" t="inlineStr">
         <is>
           <t>MANAGE 2.4
 MAP 3.3</t>
         </is>
       </c>
-      <c r="H57" s="148" t="inlineStr">
+      <c r="H59" s="148" t="inlineStr">
         <is>
           <t>PR.AA-2, PR.AA-5
 PR.DS-1</t>
         </is>
       </c>
-      <c r="I57" s="148" t="inlineStr">
+      <c r="I59" s="148" t="inlineStr">
         <is>
           <t>LLM06: Excessive
 Agency</t>
         </is>
       </c>
-      <c r="J57" s="148" t="inlineStr">
+      <c r="J59" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC6.2
 CC6.6</t>
         </is>
       </c>
     </row>
-    <row r="58" ht="42" customHeight="1">
-      <c r="B58" s="193" t="inlineStr">
+    <row r="60" ht="22" customHeight="1">
+      <c r="B60" s="193" t="inlineStr">
         <is>
           <t>Agent Authentication</t>
         </is>
       </c>
-      <c r="C58" s="148" t="inlineStr">
+      <c r="C60" s="148" t="inlineStr">
         <is>
           <t>Machine Identity
 mTLS</t>
         </is>
       </c>
-      <c r="D58" s="148" t="inlineStr">
+      <c r="D60" s="148" t="inlineStr">
         <is>
           <t>Art. 14(1)
 Human Oversight</t>
         </is>
       </c>
-      <c r="E58" s="148" t="inlineStr">
+      <c r="E60" s="148" t="inlineStr">
         <is>
           <t>A.8.1 Operation
 8.4 External</t>
         </is>
       </c>
-      <c r="F58" s="148" t="inlineStr">
+      <c r="F60" s="148" t="inlineStr">
         <is>
           <t>Initial Access
 defense</t>
         </is>
       </c>
-      <c r="G58" s="148" t="inlineStr">
+      <c r="G60" s="148" t="inlineStr">
         <is>
           <t>MAP 3.3
 GOVERN 1.3</t>
         </is>
       </c>
-      <c r="H58" s="148" t="inlineStr">
+      <c r="H60" s="148" t="inlineStr">
         <is>
           <t>PR.AA-1, PR.AA-3
 PR.AA-5</t>
         </is>
       </c>
-      <c r="I58" s="148" t="inlineStr">
+      <c r="I60" s="148" t="inlineStr">
         <is>
           <t>LLM06: Excessive
 Agency</t>
         </is>
       </c>
-      <c r="J58" s="148" t="inlineStr">
+      <c r="J60" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC6.2
 CC6.3</t>
         </is>
       </c>
     </row>
-    <row r="59" ht="42" customHeight="1">
-      <c r="B59" s="193" t="inlineStr">
+    <row r="61" ht="42" customHeight="1">
+      <c r="B61" s="193" t="inlineStr">
         <is>
           <t>Intent Validation</t>
         </is>
       </c>
-      <c r="C59" s="148" t="inlineStr">
+      <c r="C61" s="148" t="inlineStr">
         <is>
           <t>Behavior Monitor
 Intent Validation</t>
         </is>
       </c>
-      <c r="D59" s="148" t="inlineStr">
+      <c r="D61" s="148" t="inlineStr">
         <is>
           <t>Art. 14(1-4)
 Human Oversight</t>
         </is>
       </c>
-      <c r="E59" s="148" t="inlineStr">
+      <c r="E61" s="148" t="inlineStr">
         <is>
           <t>A.7.3 Objectives
 A.8.4 Output</t>
         </is>
       </c>
-      <c r="F59" s="148" t="inlineStr">
+      <c r="F61" s="148" t="inlineStr">
         <is>
           <t>Execution
 defense</t>
         </is>
       </c>
-      <c r="G59" s="148" t="inlineStr">
+      <c r="G61" s="148" t="inlineStr">
         <is>
           <t>GOVERN 1.7
 MANAGE 1.3</t>
         </is>
       </c>
-      <c r="H59" s="148" t="inlineStr">
+      <c r="H61" s="148" t="inlineStr">
         <is>
           <t>PR.AA-5
 PR.PS-1, PR.PS-2</t>
         </is>
       </c>
-      <c r="I59" s="148" t="inlineStr">
+      <c r="I61" s="148" t="inlineStr">
         <is>
           <t>LLM06: Excessive
 Agency</t>
         </is>
       </c>
-      <c r="J59" s="148" t="inlineStr">
+      <c r="J61" s="148" t="inlineStr">
         <is>
           <t>CC6.7, CC7.2
 PI1.4</t>
         </is>
       </c>
     </row>
-    <row r="60" ht="22" customHeight="1">
-      <c r="B60" s="257" t="inlineStr">
+    <row r="62" ht="42" customHeight="1">
+      <c r="B62" s="257" t="inlineStr">
         <is>
           <t>AI SUPPLY CHAIN</t>
         </is>
       </c>
-      <c r="C60" s="251" t="n"/>
-      <c r="D60" s="251" t="n"/>
-      <c r="E60" s="251" t="n"/>
-      <c r="F60" s="251" t="n"/>
-      <c r="G60" s="251" t="n"/>
-      <c r="H60" s="251" t="n"/>
-      <c r="I60" s="251" t="n"/>
-      <c r="J60" s="26" t="n"/>
-    </row>
-    <row r="61" ht="42" customHeight="1">
-      <c r="B61" s="193" t="inlineStr">
+      <c r="C62" s="251" t="n"/>
+      <c r="D62" s="251" t="n"/>
+      <c r="E62" s="251" t="n"/>
+      <c r="F62" s="251" t="n"/>
+      <c r="G62" s="251" t="n"/>
+      <c r="H62" s="251" t="n"/>
+      <c r="I62" s="251" t="n"/>
+      <c r="J62" s="26" t="n"/>
+    </row>
+    <row r="63" ht="42" customHeight="1">
+      <c r="B63" s="193" t="inlineStr">
         <is>
           <t>Model Provenance</t>
         </is>
       </c>
-      <c r="C61" s="148" t="inlineStr">
+      <c r="C63" s="148" t="inlineStr">
         <is>
           <t>Model Security
 Provenance</t>
         </is>
       </c>
-      <c r="D61" s="148" t="inlineStr">
+      <c r="D63" s="148" t="inlineStr">
         <is>
           <t>Art. 9(4)(d)
 Art. 11</t>
         </is>
       </c>
-      <c r="E61" s="148" t="inlineStr">
+      <c r="E63" s="148" t="inlineStr">
         <is>
           <t>A.10 Third Party
 8.4 Outsourcing</t>
         </is>
       </c>
-      <c r="F61" s="148" t="inlineStr">
+      <c r="F63" s="148" t="inlineStr">
         <is>
           <t>Supply Chain
 Compromise</t>
         </is>
       </c>
-      <c r="G61" s="148" t="inlineStr">
+      <c r="G63" s="148" t="inlineStr">
         <is>
           <t>GOVERN 6.1, 6.2
 MAP 3.4, 3.5</t>
         </is>
       </c>
-      <c r="H61" s="148" t="inlineStr">
+      <c r="H63" s="148" t="inlineStr">
         <is>
           <t>GV.SC-4, GV.SC-7
 ID.AM-2</t>
         </is>
       </c>
-      <c r="I61" s="148" t="inlineStr">
+      <c r="I63" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain
 LLM04: Poisoning</t>
         </is>
       </c>
-      <c r="J61" s="148" t="inlineStr">
+      <c r="J63" s="148" t="inlineStr">
         <is>
           <t>CC9.1, CC9.2
 CC3.4</t>
         </is>
       </c>
     </row>
-    <row r="62" ht="42" customHeight="1">
-      <c r="B62" s="193" t="inlineStr">
+    <row r="64" ht="42" customHeight="1">
+      <c r="B64" s="193" t="inlineStr">
         <is>
           <t>Training Data Lineage</t>
         </is>
       </c>
-      <c r="C62" s="148" t="inlineStr">
+      <c r="C64" s="148" t="inlineStr">
         <is>
           <t>Data Lineage
 Provenance</t>
         </is>
       </c>
-      <c r="D62" s="148" t="inlineStr">
+      <c r="D64" s="148" t="inlineStr">
         <is>
           <t>Art. 10(2)(3)
 Data Gov.</t>
         </is>
       </c>
-      <c r="E62" s="148" t="inlineStr">
+      <c r="E64" s="148" t="inlineStr">
         <is>
           <t>A.6.2 Data Source
 A.6.3 Acquisition</t>
         </is>
       </c>
-      <c r="F62" s="148" t="inlineStr">
+      <c r="F64" s="148" t="inlineStr">
         <is>
           <t>Data Poisoning
 defense</t>
         </is>
       </c>
-      <c r="G62" s="148" t="inlineStr">
+      <c r="G64" s="148" t="inlineStr">
         <is>
           <t>MAP 4.1, 4.2
 GOVERN 5.2</t>
         </is>
       </c>
-      <c r="H62" s="148" t="inlineStr">
+      <c r="H64" s="148" t="inlineStr">
         <is>
           <t>GV.SC-5
 ID.AM-7</t>
         </is>
       </c>
-      <c r="I62" s="148" t="inlineStr">
+      <c r="I64" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain
 LLM04: Poisoning</t>
         </is>
       </c>
-      <c r="J62" s="148" t="inlineStr">
+      <c r="J64" s="148" t="inlineStr">
         <is>
           <t>CC9.1, PI1.2
 P1.1</t>
         </is>
       </c>
     </row>
-    <row r="63" ht="42" customHeight="1">
-      <c r="B63" s="193" t="inlineStr">
+    <row r="65" ht="42" customHeight="1">
+      <c r="B65" s="193" t="inlineStr">
         <is>
           <t>ML Pipeline Security</t>
         </is>
       </c>
-      <c r="C63" s="148" t="inlineStr">
+      <c r="C65" s="148" t="inlineStr">
         <is>
           <t>Pipeline Security
 DevSecOps</t>
         </is>
       </c>
-      <c r="D63" s="148" t="inlineStr">
+      <c r="D65" s="148" t="inlineStr">
         <is>
           <t>Art. 15(5)
 Cybersecurity</t>
         </is>
       </c>
-      <c r="E63" s="148" t="inlineStr">
+      <c r="E65" s="148" t="inlineStr">
         <is>
           <t>A.9 AI Lifecycle
 8.1 Security</t>
         </is>
       </c>
-      <c r="F63" s="148" t="inlineStr">
+      <c r="F65" s="148" t="inlineStr">
         <is>
           <t>CI/CD defense
 Pipeline attacks</t>
         </is>
       </c>
-      <c r="G63" s="148" t="inlineStr">
+      <c r="G65" s="148" t="inlineStr">
         <is>
           <t>GOVERN 6.1
 MANAGE 2.4</t>
         </is>
       </c>
-      <c r="H63" s="148" t="inlineStr">
+      <c r="H65" s="148" t="inlineStr">
         <is>
           <t>PR.DS-1, PR.DS-6
 PR.PS-1</t>
         </is>
       </c>
-      <c r="I63" s="148" t="inlineStr">
+      <c r="I65" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain</t>
         </is>
       </c>
-      <c r="J63" s="148" t="inlineStr">
+      <c r="J65" s="148" t="inlineStr">
         <is>
           <t>CC6.6, CC7.1
 CC8.1</t>
         </is>
       </c>
     </row>
-    <row r="64" ht="42" customHeight="1">
-      <c r="B64" s="193" t="inlineStr">
+    <row r="66" ht="42" customHeight="1">
+      <c r="B66" s="193" t="inlineStr">
         <is>
           <t>Model Integrity Verification</t>
         </is>
       </c>
-      <c r="C64" s="148" t="inlineStr">
+      <c r="C66" s="148" t="inlineStr">
         <is>
           <t>Integrity
 Signing</t>
         </is>
       </c>
-      <c r="D64" s="148" t="inlineStr">
+      <c r="D66" s="148" t="inlineStr">
         <is>
           <t>Art. 15(1)
 Robustness</t>
         </is>
       </c>
-      <c r="E64" s="148" t="inlineStr">
+      <c r="E66" s="148" t="inlineStr">
         <is>
           <t>A.8.1 Operation
 A.9 Lifecycle</t>
         </is>
       </c>
-      <c r="F64" s="148" t="inlineStr">
+      <c r="F66" s="148" t="inlineStr">
         <is>
           <t>Model Tampering
 defense</t>
         </is>
       </c>
-      <c r="G64" s="148" t="inlineStr">
+      <c r="G66" s="148" t="inlineStr">
         <is>
           <t>MANAGE 1.1, 1.4
 MAP 2.3</t>
         </is>
       </c>
-      <c r="H64" s="148" t="inlineStr">
+      <c r="H66" s="148" t="inlineStr">
         <is>
           <t>PR.DS-6, PR.DS-8
 DE.CM-1</t>
         </is>
       </c>
-      <c r="I64" s="148" t="inlineStr">
+      <c r="I66" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain
 LLM04: Poisoning</t>
         </is>
       </c>
-      <c r="J64" s="148" t="inlineStr">
+      <c r="J66" s="148" t="inlineStr">
         <is>
           <t>CC7.1, CC8.1
 PI1.4</t>
         </is>
       </c>
     </row>
-    <row r="65" ht="42" customHeight="1">
-      <c r="B65" s="193" t="inlineStr">
+    <row r="67" ht="28" customHeight="1">
+      <c r="B67" s="193" t="inlineStr">
         <is>
           <t>Third-Party Model Assessment</t>
         </is>
       </c>
-      <c r="C65" s="148" t="inlineStr">
+      <c r="C67" s="148" t="inlineStr">
         <is>
           <t>Vendor Mgmt
 Assessment</t>
         </is>
       </c>
-      <c r="D65" s="148" t="inlineStr">
+      <c r="D67" s="148" t="inlineStr">
         <is>
           <t>Art. 9(4)(d)
 Art. 25</t>
         </is>
       </c>
-      <c r="E65" s="148" t="inlineStr">
+      <c r="E67" s="148" t="inlineStr">
         <is>
           <t>A.10 Third Party
 8.4 Outsourcing</t>
         </is>
       </c>
-      <c r="F65" s="148" t="inlineStr">
+      <c r="F67" s="148" t="inlineStr">
         <is>
           <t>Supply Chain
 Compromise</t>
         </is>
       </c>
-      <c r="G65" s="148" t="inlineStr">
+      <c r="G67" s="148" t="inlineStr">
         <is>
           <t>GOVERN 6.1, 6.2
 MAP 3.4</t>
         </is>
       </c>
-      <c r="H65" s="148" t="inlineStr">
+      <c r="H67" s="148" t="inlineStr">
         <is>
           <t>GV.SC-1 to GV.SC-10
 ID.RA-9</t>
         </is>
       </c>
-      <c r="I65" s="148" t="inlineStr">
+      <c r="I67" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain</t>
         </is>
       </c>
-      <c r="J65" s="148" t="inlineStr">
+      <c r="J67" s="148" t="inlineStr">
         <is>
           <t>CC9.1, CC9.2
 CC3.4</t>
         </is>
       </c>
     </row>
-    <row r="66" ht="42" customHeight="1">
-      <c r="B66" s="193" t="inlineStr">
+    <row r="68" ht="28" customHeight="1">
+      <c r="B68" s="193" t="inlineStr">
         <is>
           <t>Plugin/Extension Validation</t>
         </is>
       </c>
-      <c r="C66" s="148" t="inlineStr">
+      <c r="C68" s="148" t="inlineStr">
         <is>
           <t>Extension Mgmt
 Validation</t>
         </is>
       </c>
-      <c r="D66" s="148" t="inlineStr">
+      <c r="D68" s="148" t="inlineStr">
         <is>
           <t>Art. 9(4)(d)
 Art. 15</t>
         </is>
       </c>
-      <c r="E66" s="148" t="inlineStr">
+      <c r="E68" s="148" t="inlineStr">
         <is>
           <t>A.10 Third Party
 8.4 External</t>
         </is>
       </c>
-      <c r="F66" s="148" t="inlineStr">
+      <c r="F68" s="148" t="inlineStr">
         <is>
           <t>Plugin attacks
 defense</t>
         </is>
       </c>
-      <c r="G66" s="148" t="inlineStr">
+      <c r="G68" s="148" t="inlineStr">
         <is>
           <t>GOVERN 6.2
 MAP 3.5</t>
         </is>
       </c>
-      <c r="H66" s="148" t="inlineStr">
+      <c r="H68" s="148" t="inlineStr">
         <is>
           <t>GV.SC-7
 PR.PS-2</t>
         </is>
       </c>
-      <c r="I66" s="148" t="inlineStr">
+      <c r="I68" s="148" t="inlineStr">
         <is>
           <t>LLM03: Supply Chain
 LLM06: Agency</t>
         </is>
       </c>
-      <c r="J66" s="148" t="inlineStr">
+      <c r="J68" s="148" t="inlineStr">
         <is>
           <t>CC9.1, CC6.6
 CC7.1</t>
         </is>
       </c>
     </row>
-    <row r="67" ht="28" customHeight="1"/>
-    <row r="68" ht="28" customHeight="1">
-      <c r="B68" s="73" t="inlineStr">
+    <row r="69" ht="28" customHeight="1"/>
+    <row r="70" ht="28" customHeight="1">
+      <c r="B70" s="73" t="inlineStr">
         <is>
           <t>OWASP LLM Top 10 (2025) Quick Reference</t>
         </is>
       </c>
-      <c r="C68" s="74" t="n"/>
-      <c r="D68" s="74" t="n"/>
-      <c r="E68" s="74" t="n"/>
-      <c r="F68" s="74" t="n"/>
-      <c r="G68" s="74" t="n"/>
-      <c r="H68" s="74" t="n"/>
-      <c r="I68" s="74" t="n"/>
-    </row>
-    <row r="69" ht="28" customHeight="1">
-      <c r="B69" s="75" t="inlineStr">
+      <c r="C70" s="74" t="n"/>
+      <c r="D70" s="74" t="n"/>
+      <c r="E70" s="74" t="n"/>
+      <c r="F70" s="74" t="n"/>
+      <c r="G70" s="74" t="n"/>
+      <c r="H70" s="74" t="n"/>
+      <c r="I70" s="74" t="n"/>
+    </row>
+    <row r="71" ht="28" customHeight="1">
+      <c r="B71" s="75" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C69" s="75" t="inlineStr">
+      <c r="C71" s="75" t="inlineStr">
         <is>
           <t>Key Guardrails</t>
         </is>
       </c>
-      <c r="D69" s="75" t="inlineStr">
+      <c r="D71" s="75" t="inlineStr">
         <is>
           <t>Risk</t>
         </is>
       </c>
-      <c r="E69" s="75" t="inlineStr">
+      <c r="E71" s="75" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F69" s="74" t="n"/>
-      <c r="G69" s="271" t="n"/>
-      <c r="H69" s="271" t="n"/>
-      <c r="I69" s="74" t="n"/>
-    </row>
-    <row r="70" ht="28" customHeight="1">
-      <c r="B70" s="194" t="inlineStr">
-        <is>
-          <t>LLM01</t>
-        </is>
-      </c>
-      <c r="C70" s="70" t="inlineStr">
-        <is>
-          <t>Input Validation, Content Safety</t>
-        </is>
-      </c>
-      <c r="D70" s="70" t="inlineStr">
-        <is>
-          <t>Prompt Injection</t>
-        </is>
-      </c>
-      <c r="E70" s="70" t="inlineStr">
-        <is>
-          <t>Direct/indirect manipulation of prompts to bypass controls</t>
-        </is>
-      </c>
-      <c r="F70" s="74" t="n"/>
-      <c r="G70" s="77" t="n"/>
-      <c r="H70" s="77" t="n"/>
-      <c r="I70" s="74" t="n"/>
-    </row>
-    <row r="71" ht="28" customHeight="1">
-      <c r="B71" s="194" t="inlineStr">
-        <is>
-          <t>LLM02</t>
-        </is>
-      </c>
-      <c r="C71" s="70" t="inlineStr">
-        <is>
-          <t>DLP, PII Detection, Data Masking</t>
-        </is>
-      </c>
-      <c r="D71" s="70" t="inlineStr">
-        <is>
-          <t>Sensitive Information</t>
-        </is>
-      </c>
-      <c r="E71" s="70" t="inlineStr">
-        <is>
-          <t>Leakage of PII, secrets, or confidential data</t>
-        </is>
-      </c>
       <c r="F71" s="74" t="n"/>
-      <c r="G71" s="77" t="n"/>
-      <c r="H71" s="77" t="n"/>
+      <c r="G71" s="271" t="n"/>
+      <c r="H71" s="271" t="n"/>
       <c r="I71" s="74" t="n"/>
     </row>
     <row r="72" ht="28" customHeight="1">
       <c r="B72" s="194" t="inlineStr">
         <is>
-          <t>LLM03</t>
+          <t>LLM01</t>
         </is>
       </c>
       <c r="C72" s="70" t="inlineStr">
         <is>
-          <t>Vendor Assessment, Tool Registration</t>
+          <t>Input Validation, Content Safety</t>
         </is>
       </c>
       <c r="D72" s="70" t="inlineStr">
         <is>
-          <t>Supply Chain</t>
+          <t>Prompt Injection</t>
         </is>
       </c>
       <c r="E72" s="70" t="inlineStr">
         <is>
-          <t>Compromised models, training data, or pipelines</t>
+          <t>Direct/indirect manipulation of prompts to bypass controls</t>
         </is>
       </c>
       <c r="F72" s="74" t="n"/>
@@ -4856,22 +4841,22 @@
     <row r="73" ht="28" customHeight="1">
       <c r="B73" s="194" t="inlineStr">
         <is>
-          <t>LLM04</t>
+          <t>LLM02</t>
         </is>
       </c>
       <c r="C73" s="70" t="inlineStr">
         <is>
-          <t>Vendor Assessment, Input Validation</t>
+          <t>DLP, PII Detection, Data Masking</t>
         </is>
       </c>
       <c r="D73" s="70" t="inlineStr">
         <is>
-          <t>Data &amp; Model Poisoning</t>
+          <t>Sensitive Information</t>
         </is>
       </c>
       <c r="E73" s="70" t="inlineStr">
         <is>
-          <t>Manipulation of training data to corrupt model</t>
+          <t>Leakage of PII, secrets, or confidential data</t>
         </is>
       </c>
       <c r="F73" s="74" t="n"/>
@@ -4882,22 +4867,22 @@
     <row r="74" ht="28" customHeight="1">
       <c r="B74" s="194" t="inlineStr">
         <is>
-          <t>LLM05</t>
+          <t>LLM03</t>
         </is>
       </c>
       <c r="C74" s="70" t="inlineStr">
         <is>
-          <t>Output Filtering, Content Safety</t>
+          <t>Vendor Assessment, Tool Registration</t>
         </is>
       </c>
       <c r="D74" s="70" t="inlineStr">
         <is>
-          <t>Improper Output Handling</t>
+          <t>Supply Chain</t>
         </is>
       </c>
       <c r="E74" s="70" t="inlineStr">
         <is>
-          <t>Unsafe handling of model outputs</t>
+          <t>Compromised models, training data, or pipelines</t>
         </is>
       </c>
       <c r="F74" s="74" t="n"/>
@@ -4908,22 +4893,22 @@
     <row r="75" ht="28" customHeight="1">
       <c r="B75" s="194" t="inlineStr">
         <is>
-          <t>LLM06</t>
+          <t>LLM04</t>
         </is>
       </c>
       <c r="C75" s="70" t="inlineStr">
         <is>
-          <t>Intent Validation, Service Account Scoping</t>
+          <t>Vendor Assessment, Input Validation</t>
         </is>
       </c>
       <c r="D75" s="70" t="inlineStr">
         <is>
-          <t>Excessive Agency</t>
+          <t>Data &amp; Model Poisoning</t>
         </is>
       </c>
       <c r="E75" s="70" t="inlineStr">
         <is>
-          <t>Uncontrolled actions by AI agents</t>
+          <t>Manipulation of training data to corrupt model</t>
         </is>
       </c>
       <c r="F75" s="74" t="n"/>
@@ -4934,22 +4919,22 @@
     <row r="76" ht="28" customHeight="1">
       <c r="B76" s="194" t="inlineStr">
         <is>
-          <t>LLM07</t>
+          <t>LLM05</t>
         </is>
       </c>
       <c r="C76" s="70" t="inlineStr">
         <is>
-          <t>Input Validation, Output Filtering</t>
+          <t>Output Filtering, Content Safety</t>
         </is>
       </c>
       <c r="D76" s="70" t="inlineStr">
         <is>
-          <t>System Prompt Leakage</t>
+          <t>Improper Output Handling</t>
         </is>
       </c>
       <c r="E76" s="70" t="inlineStr">
         <is>
-          <t>Exposure of system prompts</t>
+          <t>Unsafe handling of model outputs</t>
         </is>
       </c>
       <c r="F76" s="74" t="n"/>
@@ -4960,22 +4945,22 @@
     <row r="77" ht="28" customHeight="1">
       <c r="B77" s="194" t="inlineStr">
         <is>
-          <t>LLM08</t>
+          <t>LLM06</t>
         </is>
       </c>
       <c r="C77" s="70" t="inlineStr">
         <is>
-          <t>Data Classification, Data Lineage</t>
+          <t>Intent Validation, Service Account Scoping</t>
         </is>
       </c>
       <c r="D77" s="70" t="inlineStr">
         <is>
-          <t>Vector &amp; Embedding Weaknesses</t>
+          <t>Excessive Agency</t>
         </is>
       </c>
       <c r="E77" s="70" t="inlineStr">
         <is>
-          <t>RAG/embedding vulnerabilities</t>
+          <t>Uncontrolled actions by AI agents</t>
         </is>
       </c>
       <c r="F77" s="74" t="n"/>
@@ -4986,22 +4971,22 @@
     <row r="78" ht="28" customHeight="1">
       <c r="B78" s="194" t="inlineStr">
         <is>
-          <t>LLM09</t>
+          <t>LLM07</t>
         </is>
       </c>
       <c r="C78" s="70" t="inlineStr">
         <is>
-          <t>Output Filtering, Performance Monitoring</t>
+          <t>Input Validation, Output Filtering</t>
         </is>
       </c>
       <c r="D78" s="70" t="inlineStr">
         <is>
-          <t>Misinformation</t>
+          <t>System Prompt Leakage</t>
         </is>
       </c>
       <c r="E78" s="70" t="inlineStr">
         <is>
-          <t>Hallucinations, false information</t>
+          <t>Exposure of system prompts</t>
         </is>
       </c>
       <c r="F78" s="74" t="n"/>
@@ -5012,22 +4997,22 @@
     <row r="79" ht="28" customHeight="1">
       <c r="B79" s="194" t="inlineStr">
         <is>
-          <t>LLM10</t>
+          <t>LLM08</t>
         </is>
       </c>
       <c r="C79" s="70" t="inlineStr">
         <is>
-          <t>Rate Limiting, Usage Analytics</t>
+          <t>Data Classification, Data Lineage</t>
         </is>
       </c>
       <c r="D79" s="70" t="inlineStr">
         <is>
-          <t>Unbounded Consumption</t>
+          <t>Vector &amp; Embedding Weaknesses</t>
         </is>
       </c>
       <c r="E79" s="70" t="inlineStr">
         <is>
-          <t>Resource exhaustion</t>
+          <t>RAG/embedding vulnerabilities</t>
         </is>
       </c>
       <c r="F79" s="74" t="n"/>
@@ -5036,343 +5021,398 @@
       <c r="I79" s="74" t="n"/>
     </row>
     <row r="80" ht="22" customHeight="1">
-      <c r="B80" s="74" t="n"/>
-      <c r="C80" s="74" t="n"/>
-      <c r="D80" s="74" t="n"/>
-      <c r="E80" s="74" t="n"/>
+      <c r="B80" s="194" t="inlineStr">
+        <is>
+          <t>LLM09</t>
+        </is>
+      </c>
+      <c r="C80" s="70" t="inlineStr">
+        <is>
+          <t>Output Filtering, Performance Monitoring</t>
+        </is>
+      </c>
+      <c r="D80" s="70" t="inlineStr">
+        <is>
+          <t>Misinformation</t>
+        </is>
+      </c>
+      <c r="E80" s="70" t="inlineStr">
+        <is>
+          <t>Hallucinations, false information</t>
+        </is>
+      </c>
       <c r="F80" s="74" t="n"/>
-      <c r="G80" s="74" t="n"/>
-      <c r="H80" s="74" t="n"/>
+      <c r="G80" s="77" t="n"/>
+      <c r="H80" s="77" t="n"/>
       <c r="I80" s="74" t="n"/>
     </row>
-    <row r="81" ht="22" customHeight="1"/>
+    <row r="81" ht="22" customHeight="1">
+      <c r="B81" s="194" t="inlineStr">
+        <is>
+          <t>LLM10</t>
+        </is>
+      </c>
+      <c r="C81" s="70" t="inlineStr">
+        <is>
+          <t>Rate Limiting, Usage Analytics</t>
+        </is>
+      </c>
+      <c r="D81" s="70" t="inlineStr">
+        <is>
+          <t>Unbounded Consumption</t>
+        </is>
+      </c>
+      <c r="E81" s="70" t="inlineStr">
+        <is>
+          <t>Resource exhaustion</t>
+        </is>
+      </c>
+      <c r="F81" s="74" t="n"/>
+      <c r="G81" s="77" t="n"/>
+      <c r="H81" s="77" t="n"/>
+      <c r="I81" s="74" t="n"/>
+    </row>
     <row r="82" ht="16" customHeight="1">
-      <c r="B82" s="15" t="inlineStr">
+      <c r="B82" s="74" t="n"/>
+      <c r="C82" s="74" t="n"/>
+      <c r="D82" s="74" t="n"/>
+      <c r="E82" s="74" t="n"/>
+      <c r="F82" s="74" t="n"/>
+      <c r="G82" s="74" t="n"/>
+      <c r="H82" s="74" t="n"/>
+      <c r="I82" s="74" t="n"/>
+    </row>
+    <row r="83" ht="32" customHeight="1"/>
+    <row r="84" ht="32" customHeight="1">
+      <c r="B84" s="15" t="inlineStr">
         <is>
           <t>Usage Notes</t>
-        </is>
-      </c>
-    </row>
-    <row r="83" ht="32" customHeight="1">
-      <c r="B83" s="5" t="inlineStr">
-        <is>
-          <t>• CSA AI Safety: Cloud-specific guidance for AI workloads; complements CSA CCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="84" ht="32" customHeight="1">
-      <c r="B84" s="5" t="inlineStr">
-        <is>
-          <t>• EU AI Act: Mandatory for high-risk AI in EU market; Articles 9-17 define technical requirements</t>
         </is>
       </c>
     </row>
     <row r="85" ht="32" customHeight="1">
       <c r="B85" s="5" t="inlineStr">
         <is>
-          <t>• ISO 42001: Required for AI management system certification; Annex A controls are normative requirements</t>
+          <t>• CSA AI Safety: Cloud-specific guidance for AI workloads; complements CSA CCM</t>
         </is>
       </c>
     </row>
     <row r="86" ht="32" customHeight="1">
       <c r="B86" s="5" t="inlineStr">
         <is>
-          <t>• MITRE ATLAS: Adversarial techniques for ML; useful for red team planning and threat modeling</t>
-        </is>
-      </c>
-      <c r="J86" s="7" t="n"/>
+          <t>• EU AI Act: Mandatory for high-risk AI in EU market; Articles 9-17 define technical requirements</t>
+        </is>
+      </c>
     </row>
     <row r="87" ht="32" customHeight="1">
       <c r="B87" s="5" t="inlineStr">
         <is>
-          <t>• NIST AI RMF: Core AI risk management for federal agencies and enterprises; integrates with NIST CSF</t>
+          <t>• ISO 42001: Required for AI management system certification; Annex A controls are normative requirements</t>
         </is>
       </c>
     </row>
     <row r="88" ht="32" customHeight="1">
       <c r="B88" s="5" t="inlineStr">
         <is>
-          <t>• NIST CSF 2.0: Cross-reference with existing cybersecurity controls; new GOVERN function added</t>
-        </is>
-      </c>
+          <t>• MITRE ATLAS: Adversarial techniques for ML; useful for red team planning and threat modeling</t>
+        </is>
+      </c>
+      <c r="J88" s="7" t="n"/>
     </row>
     <row r="89" ht="32" customHeight="1">
       <c r="B89" s="5" t="inlineStr">
         <is>
-          <t>• OWASP LLM Top 10: Practical application security risks; maps directly to runtime guardrails</t>
+          <t>• NIST AI RMF: Core AI risk management for federal agencies and enterprises; integrates with NIST CSF</t>
         </is>
       </c>
     </row>
     <row r="90" ht="48" customHeight="1">
       <c r="B90" s="5" t="inlineStr">
         <is>
+          <t>• NIST CSF 2.0: Cross-reference with existing cybersecurity controls; new GOVERN function added</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" s="5" t="inlineStr">
+        <is>
+          <t>• OWASP LLM Top 10: Practical application security risks; maps directly to runtime guardrails</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" s="5" t="inlineStr">
+        <is>
           <t>• SOC 2: Trust Service Criteria for vendor assessments; maps to Security (CC), Availability (A), Processing Integrity (PI), Confidentiality (C), Privacy (P)</t>
         </is>
       </c>
     </row>
-    <row r="92">
-      <c r="B92" s="261" t="inlineStr">
+    <row r="93"/>
+    <row r="94" ht="45" customHeight="1">
+      <c r="B94" s="261" t="inlineStr">
         <is>
           <t>AGENTIC AI SECURITY (NEW)</t>
         </is>
       </c>
-      <c r="C92" s="259" t="n"/>
-      <c r="D92" s="259" t="n"/>
-      <c r="E92" s="259" t="n"/>
-      <c r="F92" s="259" t="n"/>
-      <c r="G92" s="259" t="n"/>
-      <c r="H92" s="259" t="n"/>
-      <c r="I92" s="259" t="n"/>
-      <c r="J92" s="259" t="n"/>
-    </row>
-    <row r="93">
-      <c r="B93" s="259" t="inlineStr">
+      <c r="C94" s="259" t="n"/>
+      <c r="D94" s="259" t="n"/>
+      <c r="E94" s="259" t="n"/>
+      <c r="F94" s="259" t="n"/>
+      <c r="G94" s="259" t="n"/>
+      <c r="H94" s="259" t="n"/>
+      <c r="I94" s="259" t="n"/>
+      <c r="J94" s="259" t="n"/>
+    </row>
+    <row r="95" ht="45" customHeight="1">
+      <c r="B95" s="259" t="inlineStr">
         <is>
           <t>Vector Store Security</t>
         </is>
       </c>
-      <c r="C93" s="259" t="inlineStr">
+      <c r="C95" s="259" t="inlineStr">
         <is>
           <t>Data Protection</t>
         </is>
       </c>
-      <c r="D93" s="259" t="inlineStr">
+      <c r="D95" s="259" t="inlineStr">
         <is>
           <t>Art. 10 Data Gov</t>
         </is>
       </c>
-      <c r="E93" s="259" t="inlineStr">
+      <c r="E95" s="259" t="inlineStr">
         <is>
           <t>A.6 Data for AI</t>
         </is>
       </c>
-      <c r="F93" s="259" t="inlineStr">
+      <c r="F95" s="259" t="inlineStr">
         <is>
           <t>AML.T0020 Poison</t>
         </is>
       </c>
-      <c r="G93" s="259" t="inlineStr">
+      <c r="G95" s="259" t="inlineStr">
         <is>
           <t>MAP 4.1, 4.2</t>
         </is>
       </c>
-      <c r="H93" s="259" t="inlineStr">
+      <c r="H95" s="259" t="inlineStr">
         <is>
           <t>PR.DS-1, PR.DS-5</t>
         </is>
       </c>
-      <c r="I93" s="259" t="inlineStr">
+      <c r="I95" s="259" t="inlineStr">
         <is>
           <t>LLM04: Vector DB</t>
         </is>
       </c>
-      <c r="J93" s="259" t="inlineStr">
+      <c r="J95" s="259" t="inlineStr">
         <is>
           <t>CC6.1, CC6.7</t>
-        </is>
-      </c>
-    </row>
-    <row r="94" ht="45" customHeight="1">
-      <c r="B94" s="262" t="inlineStr">
-        <is>
-          <t>System Prompt Protection</t>
-        </is>
-      </c>
-      <c r="C94" s="262" t="inlineStr">
-        <is>
-          <t>Prompt Security</t>
-        </is>
-      </c>
-      <c r="D94" s="262" t="inlineStr">
-        <is>
-          <t>Art. 15(4)</t>
-        </is>
-      </c>
-      <c r="E94" s="262" t="inlineStr">
-        <is>
-          <t>A.8.3 Protection</t>
-        </is>
-      </c>
-      <c r="F94" s="262" t="inlineStr">
-        <is>
-          <t>AML.T0051 Prompt</t>
-        </is>
-      </c>
-      <c r="G94" s="262" t="inlineStr">
-        <is>
-          <t>MANAGE 2.2</t>
-        </is>
-      </c>
-      <c r="H94" s="262" t="inlineStr">
-        <is>
-          <t>PR.DS-5, DE.CM-1</t>
-        </is>
-      </c>
-      <c r="I94" s="262" t="inlineStr">
-        <is>
-          <t>LLM07: Sys Prompt</t>
-        </is>
-      </c>
-      <c r="J94" s="262" t="inlineStr">
-        <is>
-          <t>CC6.6, CC6.7</t>
-        </is>
-      </c>
-    </row>
-    <row r="95" ht="45" customHeight="1">
-      <c r="B95" s="262" t="inlineStr">
-        <is>
-          <t>Agentic Boundary Controls</t>
-        </is>
-      </c>
-      <c r="C95" s="262" t="inlineStr">
-        <is>
-          <t>Agent Governance</t>
-        </is>
-      </c>
-      <c r="D95" s="262" t="inlineStr">
-        <is>
-          <t>Art. 14 Human</t>
-        </is>
-      </c>
-      <c r="E95" s="262" t="inlineStr">
-        <is>
-          <t>A.7 AI Objectives</t>
-        </is>
-      </c>
-      <c r="F95" s="262" t="inlineStr">
-        <is>
-          <t>AML.T0052 Agent</t>
-        </is>
-      </c>
-      <c r="G95" s="262" t="inlineStr">
-        <is>
-          <t>GOVERN 1.4, MAP 1.1</t>
-        </is>
-      </c>
-      <c r="H95" s="262" t="inlineStr">
-        <is>
-          <t>GV.PO-1, PR.AC-4</t>
-        </is>
-      </c>
-      <c r="I95" s="262" t="inlineStr">
-        <is>
-          <t>LLM06: Excessive</t>
-        </is>
-      </c>
-      <c r="J95" s="262" t="inlineStr">
-        <is>
-          <t>CC6.1, CC5.2</t>
         </is>
       </c>
     </row>
     <row r="96" ht="45" customHeight="1">
       <c r="B96" s="262" t="inlineStr">
         <is>
-          <t>Tool/Function Authorization</t>
+          <t>System Prompt Protection</t>
         </is>
       </c>
       <c r="C96" s="262" t="inlineStr">
         <is>
-          <t>Access Control</t>
+          <t>Prompt Security</t>
         </is>
       </c>
       <c r="D96" s="262" t="inlineStr">
         <is>
-          <t>Art. 14(4)(d)</t>
+          <t>Art. 15(4)</t>
         </is>
       </c>
       <c r="E96" s="262" t="inlineStr">
         <is>
-          <t>A.8 Operation</t>
+          <t>A.8.3 Protection</t>
         </is>
       </c>
       <c r="F96" s="262" t="inlineStr">
         <is>
-          <t>AML.T0053 Tool</t>
+          <t>AML.T0051 Prompt</t>
         </is>
       </c>
       <c r="G96" s="262" t="inlineStr">
         <is>
-          <t>MANAGE 2.4</t>
+          <t>MANAGE 2.2</t>
         </is>
       </c>
       <c r="H96" s="262" t="inlineStr">
         <is>
-          <t>PR.AC-1, PR.AC-4</t>
+          <t>PR.DS-5, DE.CM-1</t>
         </is>
       </c>
       <c r="I96" s="262" t="inlineStr">
         <is>
-          <t>LLM06: Excessive</t>
+          <t>LLM07: Sys Prompt</t>
         </is>
       </c>
       <c r="J96" s="262" t="inlineStr">
         <is>
-          <t>CC6.1, CC6.3</t>
+          <t>CC6.6, CC6.7</t>
         </is>
       </c>
     </row>
     <row r="97" ht="45" customHeight="1">
       <c r="B97" s="262" t="inlineStr">
         <is>
+          <t>Agentic Boundary Controls</t>
+        </is>
+      </c>
+      <c r="C97" s="262" t="inlineStr">
+        <is>
+          <t>Agent Governance</t>
+        </is>
+      </c>
+      <c r="D97" s="262" t="inlineStr">
+        <is>
+          <t>Art. 14 Human</t>
+        </is>
+      </c>
+      <c r="E97" s="262" t="inlineStr">
+        <is>
+          <t>A.7 AI Objectives</t>
+        </is>
+      </c>
+      <c r="F97" s="262" t="inlineStr">
+        <is>
+          <t>AML.T0052 Agent</t>
+        </is>
+      </c>
+      <c r="G97" s="262" t="inlineStr">
+        <is>
+          <t>GOVERN 1.4, MAP 1.1</t>
+        </is>
+      </c>
+      <c r="H97" s="262" t="inlineStr">
+        <is>
+          <t>GV.PO-1, PR.AC-4</t>
+        </is>
+      </c>
+      <c r="I97" s="262" t="inlineStr">
+        <is>
+          <t>LLM06: Excessive</t>
+        </is>
+      </c>
+      <c r="J97" s="262" t="inlineStr">
+        <is>
+          <t>CC6.1, CC5.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="98" ht="45" customHeight="1">
+      <c r="B98" s="262" t="inlineStr">
+        <is>
+          <t>Tool/Function Authorization</t>
+        </is>
+      </c>
+      <c r="C98" s="262" t="inlineStr">
+        <is>
+          <t>Access Control</t>
+        </is>
+      </c>
+      <c r="D98" s="262" t="inlineStr">
+        <is>
+          <t>Art. 14(4)(d)</t>
+        </is>
+      </c>
+      <c r="E98" s="262" t="inlineStr">
+        <is>
+          <t>A.8 Operation</t>
+        </is>
+      </c>
+      <c r="F98" s="262" t="inlineStr">
+        <is>
+          <t>AML.T0053 Tool</t>
+        </is>
+      </c>
+      <c r="G98" s="262" t="inlineStr">
+        <is>
+          <t>MANAGE 2.4</t>
+        </is>
+      </c>
+      <c r="H98" s="262" t="inlineStr">
+        <is>
+          <t>PR.AC-1, PR.AC-4</t>
+        </is>
+      </c>
+      <c r="I98" s="262" t="inlineStr">
+        <is>
+          <t>LLM06: Excessive</t>
+        </is>
+      </c>
+      <c r="J98" s="262" t="inlineStr">
+        <is>
+          <t>CC6.1, CC6.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" s="262" t="inlineStr">
+        <is>
           <t>Autonomous Action Limits</t>
         </is>
       </c>
-      <c r="C97" s="262" t="inlineStr">
+      <c r="C99" s="262" t="inlineStr">
         <is>
           <t>Autonomy Limits</t>
         </is>
       </c>
-      <c r="D97" s="262" t="inlineStr">
+      <c r="D99" s="262" t="inlineStr">
         <is>
           <t>Art. 14(1-3)</t>
         </is>
       </c>
-      <c r="E97" s="262" t="inlineStr">
+      <c r="E99" s="262" t="inlineStr">
         <is>
           <t>A.7.3 Objectives</t>
         </is>
       </c>
-      <c r="F97" s="262" t="inlineStr">
+      <c r="F99" s="262" t="inlineStr">
         <is>
           <t>All Agent tactics</t>
         </is>
       </c>
-      <c r="G97" s="262" t="inlineStr">
+      <c r="G99" s="262" t="inlineStr">
         <is>
           <t>GOVERN 1.6, MANAGE 1.3</t>
         </is>
       </c>
-      <c r="H97" s="262" t="inlineStr">
+      <c r="H99" s="262" t="inlineStr">
         <is>
           <t>GV.PO-2, PR.AC-5</t>
         </is>
       </c>
-      <c r="I97" s="262" t="inlineStr">
+      <c r="I99" s="262" t="inlineStr">
         <is>
           <t>LLM06: Excessive</t>
         </is>
       </c>
-      <c r="J97" s="262" t="inlineStr">
+      <c r="J99" s="262" t="inlineStr">
         <is>
           <t>CC5.2, CC6.1</t>
         </is>
       </c>
     </row>
-    <row r="98" ht="45" customHeight="1">
-      <c r="B98" s="265" t="n"/>
-      <c r="C98" s="53" t="n"/>
-      <c r="D98" s="53" t="n"/>
-      <c r="E98" s="53" t="n"/>
-      <c r="F98" s="53" t="n"/>
-      <c r="G98" s="53" t="n"/>
-      <c r="H98" s="53" t="n"/>
-      <c r="I98" s="53" t="n"/>
-      <c r="J98" s="53" t="n"/>
-    </row>
-    <row r="101">
-      <c r="B101" s="24" t="n"/>
+    <row r="100">
+      <c r="B100" s="265" t="n"/>
+      <c r="C100" s="53" t="n"/>
+      <c r="D100" s="53" t="n"/>
+      <c r="E100" s="53" t="n"/>
+      <c r="F100" s="53" t="n"/>
+      <c r="G100" s="53" t="n"/>
+      <c r="H100" s="53" t="n"/>
+      <c r="I100" s="53" t="n"/>
+      <c r="J100" s="53" t="n"/>
+    </row>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103">
+      <c r="B103" s="24" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Fix formatting issues: color coding, spacing, and layout
AI Security Tool Landscape:
- Added proper color coding to all 75 vendor rows by product family:
  • Green (E2EFDA) = AI Posture & Governance
  • Orange (FCE4D6) = Runtime Protection & Guardrails
  • Light Blue (DDEBF7) = Shadow AI & Usage Discovery
  • Yellow (FFF2CC) = Observability & Evaluation
  • Purple (E4DFEC) = Data Protection for AI
  • Blue (B4C6E7) = NHI & Agentic Access
  • Salmon (F8CBAD) = AI Supply Chain
- Set consistent row height (40) for all vendor rows
- Applied consistent font and alignment

Intake Form:
- Removed fill colors from empty cells in section headers (rows 12, 45)
- Fixed AI Supply Chain row (65) to match other product family checkboxes

User Guide & Overview:
- Set proper row heights for readability:
  • Empty/spacer rows: 12pt
  • Section headers: 20pt
  • Title rows: 24pt
  • Content rows: 18pt

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/AI_Security_Risk_Draft1.xlsx
+++ b/AI_Security_Risk_Draft1.xlsx
@@ -325,7 +325,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="43">
+  <fills count="50">
     <fill>
       <patternFill/>
     </fill>
@@ -551,6 +551,48 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E2EFDA"/>
+        <bgColor rgb="00E2EFDA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F8CBAD"/>
+        <bgColor rgb="00F8CBAD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DDEBF7"/>
+        <bgColor rgb="00DDEBF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FCE4D6"/>
+        <bgColor rgb="00FCE4D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E4DFEC"/>
+        <bgColor rgb="00E4DFEC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B4C6E7"/>
+        <bgColor rgb="00B4C6E7"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -672,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6"/>
   </cellStyleXfs>
-  <cellXfs count="276">
+  <cellXfs count="290">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1388,6 +1430,48 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="43" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="43" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="44" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="45" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="46" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="47" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="48" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="49" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="47" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="49" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="45" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="43" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="44" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="46" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="48" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1701,21 +1785,23 @@
     <col width="14.6640625" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="2" ht="29" customHeight="1">
+    <row r="1" ht="12" customHeight="1"/>
+    <row r="2" ht="24" customHeight="1">
       <c r="B2" s="38" t="inlineStr">
         <is>
           <t>Enterprise AI Security</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="19" customHeight="1">
+    <row r="3" ht="24" customHeight="1">
       <c r="B3" s="27" t="inlineStr">
         <is>
           <t>Governance &amp; Tool Landscape Workbook</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="17" customHeight="1">
+    <row r="4" ht="12" customHeight="1"/>
+    <row r="5" ht="20" customHeight="1">
       <c r="B5" s="4" t="inlineStr">
         <is>
           <t>Purpose</t>
@@ -1729,49 +1815,49 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="16" customHeight="1">
+    <row r="7" ht="18" customHeight="1">
       <c r="B7" s="5" t="inlineStr">
         <is>
           <t>• Evaluate and classify AI tool requests by risk level</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="16" customHeight="1">
+    <row r="8" ht="18" customHeight="1">
       <c r="B8" s="5" t="inlineStr">
         <is>
           <t>• Identify required guardrails and security products for each tool</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="16" customHeight="1">
+    <row r="9" ht="18" customHeight="1">
       <c r="B9" s="5" t="inlineStr">
         <is>
           <t>• Track approved tools and their review status</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="32" customHeight="1">
+    <row r="10" ht="18" customHeight="1">
       <c r="B10" s="5" t="inlineStr">
         <is>
           <t>• Maintain ongoing governance through periodic reviews, enforcement, KPIs (Program Metrics), and SLOs (Program Metrics)</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="32" customHeight="1">
+    <row r="11" ht="18" customHeight="1">
       <c r="B11" s="5" t="inlineStr">
         <is>
           <t>• Select security vendors from a curated landscape of 75 enterprise tools</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="32" customHeight="1">
+    <row r="12" ht="18" customHeight="1">
       <c r="B12" s="5" t="inlineStr">
         <is>
           <t>• Map controls to 8 compliance frameworks (CSA AI, EU AI Act, ISO 42001, MITRE ATLAS, NIST AI RMF, NIST CSF 2.0, OWASP LLM, SOC 2)</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="17" customHeight="1">
+    <row r="13" ht="20" customHeight="1">
       <c r="B13" s="4" t="inlineStr">
         <is>
           <t>Getting Started</t>
@@ -1785,45 +1871,45 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="16" customHeight="1">
+    <row r="15" ht="18" customHeight="1">
       <c r="B15" s="5" t="inlineStr">
         <is>
           <t>• Workbook contents and tab descriptions</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="16" customHeight="1">
+    <row r="16" ht="18" customHeight="1">
       <c r="B16" s="5" t="inlineStr">
         <is>
           <t>• Step-by-step scenarios for common tasks</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="16" customHeight="1">
+    <row r="17" ht="18" customHeight="1">
       <c r="B17" s="5" t="inlineStr">
         <is>
           <t>• Key concepts and definitions</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="16" customHeight="1">
+    <row r="18" ht="18" customHeight="1">
       <c r="B18" s="5" t="inlineStr">
         <is>
           <t>• Customization guidance</t>
         </is>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="12" customHeight="1">
       <c r="B19" s="5" t="n"/>
     </row>
-    <row r="20" ht="18" customHeight="1">
+    <row r="20" ht="20" customHeight="1">
       <c r="B20" s="96" t="inlineStr">
         <is>
           <t>Workbook Contents</t>
         </is>
       </c>
     </row>
-    <row r="21">
+    <row r="21" ht="18" customHeight="1">
       <c r="B21" s="99" t="inlineStr">
         <is>
           <t>Tab</t>
@@ -2027,6 +2113,7 @@
         </is>
       </c>
     </row>
+    <row r="33" ht="12" customHeight="1"/>
     <row r="34" ht="17" customHeight="1">
       <c r="B34" s="4" t="inlineStr">
         <is>
@@ -2034,14 +2121,14 @@
         </is>
       </c>
     </row>
-    <row r="35">
+    <row r="35" ht="18" customHeight="1">
       <c r="B35" s="20" t="inlineStr">
         <is>
           <t>Key trends shaping AI security tool selection and governance strategy:</t>
         </is>
       </c>
     </row>
-    <row r="36">
+    <row r="36" ht="18" customHeight="1">
       <c r="B36" s="40" t="inlineStr">
         <is>
           <t>1. Rapid Consolidation</t>
@@ -2055,7 +2142,7 @@
         </is>
       </c>
     </row>
-    <row r="38">
+    <row r="38" ht="18" customHeight="1">
       <c r="B38" s="40" t="inlineStr">
         <is>
           <t>2. Tool Family Overlap is the Norm</t>
@@ -2069,7 +2156,7 @@
         </is>
       </c>
     </row>
-    <row r="40">
+    <row r="40" ht="18" customHeight="1">
       <c r="B40" s="40" t="inlineStr">
         <is>
           <t>3. NHI &amp; Agentic Access is the Emerging Battleground</t>
@@ -2083,7 +2170,7 @@
         </is>
       </c>
     </row>
-    <row r="42">
+    <row r="42" ht="18" customHeight="1">
       <c r="B42" s="40" t="inlineStr">
         <is>
           <t>4. Runtime Protection Became Table Stakes</t>
@@ -2097,7 +2184,7 @@
         </is>
       </c>
     </row>
-    <row r="44">
+    <row r="44" ht="18" customHeight="1">
       <c r="B44" s="40" t="inlineStr">
         <is>
           <t>5. Shadow AI Discovery Revealed Scale of Problem</t>
@@ -2111,7 +2198,7 @@
         </is>
       </c>
     </row>
-    <row r="46">
+    <row r="46" ht="18" customHeight="1">
       <c r="B46" s="40" t="inlineStr">
         <is>
           <t>6. Platform vs Best-of-Breed Decision Point</t>
@@ -2125,7 +2212,7 @@
         </is>
       </c>
     </row>
-    <row r="48">
+    <row r="48" ht="18" customHeight="1">
       <c r="B48" s="40" t="inlineStr">
         <is>
           <t>7. Regulatory Pressure Accelerating</t>
@@ -2139,7 +2226,7 @@
         </is>
       </c>
     </row>
-    <row r="50">
+    <row r="50" ht="20" customHeight="1">
       <c r="B50" s="263" t="inlineStr">
         <is>
           <t>Version History</t>
@@ -2171,7 +2258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J103"/>
+  <dimension ref="B2:J103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="19" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
@@ -2192,7 +2279,6 @@
     <col width="8.6640625" bestFit="1" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1"/>
     <row r="2" ht="21" customHeight="1">
       <c r="B2" s="9" t="inlineStr">
         <is>
@@ -2207,7 +2293,6 @@
         </is>
       </c>
     </row>
-    <row r="4"/>
     <row r="5" ht="16" customHeight="1">
       <c r="B5" s="15" t="inlineStr">
         <is>
@@ -2776,53 +2861,14 @@
           <t>Vendor Assessment</t>
         </is>
       </c>
-      <c r="C28" s="148" t="inlineStr">
-        <is>
-          <t>Vendor Mgmt
-Shared Resp.</t>
-        </is>
-      </c>
-      <c r="D28" s="148" t="inlineStr">
-        <is>
-          <t>Art. 9(4)(d)
-Art. 25</t>
-        </is>
-      </c>
-      <c r="E28" s="148" t="inlineStr">
-        <is>
-          <t>A.10 Third Party
-8.4 Outsourcing</t>
-        </is>
-      </c>
-      <c r="F28" s="148" t="inlineStr">
-        <is>
-          <t>Supply Chain
-Compromise</t>
-        </is>
-      </c>
-      <c r="G28" s="148" t="inlineStr">
-        <is>
-          <t>GOVERN 6.1, 6.2
-MAP 3.4, 3.5</t>
-        </is>
-      </c>
-      <c r="H28" s="148" t="inlineStr">
-        <is>
-          <t>GV.SC-1 to GV.SC-10
-ID.RA-9</t>
-        </is>
-      </c>
-      <c r="I28" s="148" t="inlineStr">
-        <is>
-          <t>LLM03: Supply Chain</t>
-        </is>
-      </c>
-      <c r="J28" s="148" t="inlineStr">
-        <is>
-          <t>CC9.1, CC9.2
-CC3.4</t>
-        </is>
-      </c>
+      <c r="C28" s="251" t="n"/>
+      <c r="D28" s="251" t="n"/>
+      <c r="E28" s="251" t="n"/>
+      <c r="F28" s="251" t="n"/>
+      <c r="G28" s="251" t="n"/>
+      <c r="H28" s="251" t="n"/>
+      <c r="I28" s="251" t="n"/>
+      <c r="J28" s="26" t="n"/>
     </row>
     <row r="29" ht="42" customHeight="1">
       <c r="B29" s="193" t="inlineStr">
@@ -3063,54 +3109,14 @@
           <t>Content Safety</t>
         </is>
       </c>
-      <c r="C34" s="148" t="inlineStr">
-        <is>
-          <t>Content Filtering
-Safety Controls</t>
-        </is>
-      </c>
-      <c r="D34" s="148" t="inlineStr">
-        <is>
-          <t>Art. 15(3)
-Art. 15(4)</t>
-        </is>
-      </c>
-      <c r="E34" s="148" t="inlineStr">
-        <is>
-          <t>A.7.3 AI Objectives
-A.8.4 Output</t>
-        </is>
-      </c>
-      <c r="F34" s="148" t="inlineStr">
-        <is>
-          <t>AML.T0048
-DoS ML Model</t>
-        </is>
-      </c>
-      <c r="G34" s="148" t="inlineStr">
-        <is>
-          <t>MEASURE 2.5, 2.11
-MANAGE 1.3</t>
-        </is>
-      </c>
-      <c r="H34" s="148" t="inlineStr">
-        <is>
-          <t>PR.DS-5
-DE.CM-1</t>
-        </is>
-      </c>
-      <c r="I34" s="148" t="inlineStr">
-        <is>
-          <t>LLM05: Output Hdlg
-LLM09: Misinfo</t>
-        </is>
-      </c>
-      <c r="J34" s="148" t="inlineStr">
-        <is>
-          <t>CC6.7, CC7.2
-PI1.5</t>
-        </is>
-      </c>
+      <c r="C34" s="251" t="n"/>
+      <c r="D34" s="251" t="n"/>
+      <c r="E34" s="251" t="n"/>
+      <c r="F34" s="251" t="n"/>
+      <c r="G34" s="251" t="n"/>
+      <c r="H34" s="251" t="n"/>
+      <c r="I34" s="251" t="n"/>
+      <c r="J34" s="26" t="n"/>
     </row>
     <row r="35" ht="42" customHeight="1">
       <c r="B35" s="193" t="inlineStr">
@@ -3295,48 +3301,13 @@
           <t>User Access Tracked</t>
         </is>
       </c>
-      <c r="C39" s="148" t="inlineStr">
-        <is>
-          <t>Access Logging
-Monitoring</t>
-        </is>
-      </c>
-      <c r="D39" s="148" t="inlineStr">
-        <is>
-          <t>Art. 12(1)
-Record-keeping</t>
-        </is>
-      </c>
-      <c r="E39" s="148" t="inlineStr">
-        <is>
-          <t>9.1 Monitoring
-A.8.2 Monitoring</t>
-        </is>
-      </c>
-      <c r="F39" s="148" t="inlineStr">
-        <is>
-          <t>Collection
-defense</t>
-        </is>
-      </c>
-      <c r="G39" s="148" t="inlineStr">
-        <is>
-          <t>MEASURE 1.1, 1.3
-MANAGE 4.1</t>
-        </is>
-      </c>
-      <c r="H39" s="148" t="inlineStr">
-        <is>
-          <t>DE.CM-1, DE.CM-3
-PR.AC-1</t>
-        </is>
-      </c>
-      <c r="I39" s="148" t="inlineStr">
-        <is>
-          <t>LLM02: Sensitive
-Info Disclosure</t>
-        </is>
-      </c>
+      <c r="C39" s="251" t="n"/>
+      <c r="D39" s="251" t="n"/>
+      <c r="E39" s="251" t="n"/>
+      <c r="F39" s="251" t="n"/>
+      <c r="G39" s="251" t="n"/>
+      <c r="H39" s="251" t="n"/>
+      <c r="I39" s="26" t="n"/>
       <c r="J39" s="148" t="inlineStr">
         <is>
           <t>CC6.1, CC6.2
@@ -3584,54 +3555,14 @@
           <t>Alerting Configured</t>
         </is>
       </c>
-      <c r="C45" s="148" t="inlineStr">
-        <is>
-          <t>Alerting
-Thresholds</t>
-        </is>
-      </c>
-      <c r="D45" s="148" t="inlineStr">
-        <is>
-          <t>Art. 17(1)(i)
-Incident</t>
-        </is>
-      </c>
-      <c r="E45" s="148" t="inlineStr">
-        <is>
-          <t>10.1 Nonconform.
-A.8.2 Monitoring</t>
-        </is>
-      </c>
-      <c r="F45" s="148" t="inlineStr">
-        <is>
-          <t>All Detection
-tactics</t>
-        </is>
-      </c>
-      <c r="G45" s="148" t="inlineStr">
-        <is>
-          <t>MANAGE 3.1, 3.2
-MEASURE 3.3</t>
-        </is>
-      </c>
-      <c r="H45" s="148" t="inlineStr">
-        <is>
-          <t>DE.AE-1 to DE.AE-8
-RS.AN-1</t>
-        </is>
-      </c>
-      <c r="I45" s="148" t="inlineStr">
-        <is>
-          <t>All: Real-time
-detection</t>
-        </is>
-      </c>
-      <c r="J45" s="148" t="inlineStr">
-        <is>
-          <t>CC7.2, CC7.4
-A1.2</t>
-        </is>
-      </c>
+      <c r="C45" s="251" t="n"/>
+      <c r="D45" s="251" t="n"/>
+      <c r="E45" s="251" t="n"/>
+      <c r="F45" s="251" t="n"/>
+      <c r="G45" s="251" t="n"/>
+      <c r="H45" s="251" t="n"/>
+      <c r="I45" s="251" t="n"/>
+      <c r="J45" s="26" t="n"/>
     </row>
     <row r="46" ht="42" customHeight="1">
       <c r="B46" s="193" t="inlineStr">
@@ -3983,47 +3914,13 @@
           <t>Data Masking</t>
         </is>
       </c>
-      <c r="C53" s="148" t="inlineStr">
-        <is>
-          <t>Masking
-Redaction</t>
-        </is>
-      </c>
-      <c r="D53" s="148" t="inlineStr">
-        <is>
-          <t>Art. 10(5)
-GDPR</t>
-        </is>
-      </c>
-      <c r="E53" s="148" t="inlineStr">
-        <is>
-          <t>A.6.5 Data Prep
-A.8.5 Recording</t>
-        </is>
-      </c>
-      <c r="F53" s="148" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="G53" s="148" t="inlineStr">
-        <is>
-          <t>MAP 4.1
-MANAGE 2.4</t>
-        </is>
-      </c>
-      <c r="H53" s="148" t="inlineStr">
-        <is>
-          <t>PR.DS-3, PR.DS-5
-PR.PS-4</t>
-        </is>
-      </c>
-      <c r="I53" s="148" t="inlineStr">
-        <is>
-          <t>LLM02: Sensitive
-Info Disclosure</t>
-        </is>
-      </c>
+      <c r="C53" s="251" t="n"/>
+      <c r="D53" s="251" t="n"/>
+      <c r="E53" s="251" t="n"/>
+      <c r="F53" s="251" t="n"/>
+      <c r="G53" s="251" t="n"/>
+      <c r="H53" s="251" t="n"/>
+      <c r="I53" s="26" t="n"/>
       <c r="J53" s="148" t="inlineStr">
         <is>
           <t>C1.1, C1.2
@@ -4324,54 +4221,14 @@
           <t>Agent Authentication</t>
         </is>
       </c>
-      <c r="C60" s="148" t="inlineStr">
-        <is>
-          <t>Machine Identity
-mTLS</t>
-        </is>
-      </c>
-      <c r="D60" s="148" t="inlineStr">
-        <is>
-          <t>Art. 14(1)
-Human Oversight</t>
-        </is>
-      </c>
-      <c r="E60" s="148" t="inlineStr">
-        <is>
-          <t>A.8.1 Operation
-8.4 External</t>
-        </is>
-      </c>
-      <c r="F60" s="148" t="inlineStr">
-        <is>
-          <t>Initial Access
-defense</t>
-        </is>
-      </c>
-      <c r="G60" s="148" t="inlineStr">
-        <is>
-          <t>MAP 3.3
-GOVERN 1.3</t>
-        </is>
-      </c>
-      <c r="H60" s="148" t="inlineStr">
-        <is>
-          <t>PR.AA-1, PR.AA-3
-PR.AA-5</t>
-        </is>
-      </c>
-      <c r="I60" s="148" t="inlineStr">
-        <is>
-          <t>LLM06: Excessive
-Agency</t>
-        </is>
-      </c>
-      <c r="J60" s="148" t="inlineStr">
-        <is>
-          <t>CC6.1, CC6.2
-CC6.3</t>
-        </is>
-      </c>
+      <c r="C60" s="251" t="n"/>
+      <c r="D60" s="251" t="n"/>
+      <c r="E60" s="251" t="n"/>
+      <c r="F60" s="251" t="n"/>
+      <c r="G60" s="251" t="n"/>
+      <c r="H60" s="251" t="n"/>
+      <c r="I60" s="251" t="n"/>
+      <c r="J60" s="26" t="n"/>
     </row>
     <row r="61" ht="42" customHeight="1">
       <c r="B61" s="193" t="inlineStr">
@@ -5147,7 +5004,6 @@
         </is>
       </c>
     </row>
-    <row r="93"/>
     <row r="94" ht="45" customHeight="1">
       <c r="B94" s="261" t="inlineStr">
         <is>
@@ -5409,8 +5265,6 @@
       <c r="I100" s="53" t="n"/>
       <c r="J100" s="53" t="n"/>
     </row>
-    <row r="101"/>
-    <row r="102"/>
     <row r="103">
       <c r="B103" s="24" t="n"/>
     </row>
@@ -7492,6 +7346,7 @@
     <col width="55" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
+    <row r="1" ht="12" customHeight="1"/>
     <row r="2" ht="24" customHeight="1">
       <c r="B2" s="2" t="inlineStr">
         <is>
@@ -7506,14 +7361,14 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="17" customHeight="1">
+    <row r="4" ht="20" customHeight="1">
       <c r="B4" s="4" t="inlineStr">
         <is>
           <t>Customizing for Your Organization</t>
         </is>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="20" customHeight="1">
       <c r="B5" s="143" t="inlineStr">
         <is>
           <t>Customizing for Your Organization</t>
@@ -7525,7 +7380,7 @@
         </is>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="18" customHeight="1">
       <c r="B6" s="143" t="inlineStr">
         <is>
           <t>Tool Registry</t>
@@ -7537,7 +7392,7 @@
         </is>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="18" customHeight="1">
       <c r="B7" s="143" t="inlineStr">
         <is>
           <t>Intake Form</t>
@@ -7549,7 +7404,7 @@
         </is>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="18" customHeight="1">
       <c r="B8" s="143" t="inlineStr">
         <is>
           <t>Guardrail Checklist</t>
@@ -7561,7 +7416,7 @@
         </is>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="18" customHeight="1">
       <c r="B9" s="143" t="inlineStr">
         <is>
           <t>Tool Function Mapping</t>
@@ -7573,18 +7428,18 @@
         </is>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="12" customHeight="1">
       <c r="B10" s="272" t="n"/>
       <c r="C10" s="197" t="n"/>
     </row>
-    <row r="11" ht="17" customHeight="1">
+    <row r="11" ht="20" customHeight="1">
       <c r="B11" s="4" t="inlineStr">
         <is>
           <t>Workbook Contents</t>
         </is>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="18" customHeight="1">
       <c r="B12" s="10" t="inlineStr">
         <is>
           <t>Tab</t>
@@ -7608,7 +7463,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="30" customHeight="1">
+    <row r="14" ht="24" customHeight="1">
       <c r="B14" s="140" t="inlineStr">
         <is>
           <t>User Guide</t>
@@ -7728,6 +7583,7 @@
         </is>
       </c>
     </row>
+    <row r="24" ht="12" customHeight="1"/>
     <row r="25" ht="17" customHeight="1">
       <c r="B25" s="4" t="inlineStr">
         <is>
@@ -7735,7 +7591,7 @@
         </is>
       </c>
     </row>
-    <row r="26">
+    <row r="26" ht="18" customHeight="1">
       <c r="B26" s="20" t="inlineStr">
         <is>
           <t>Choose your scenario:</t>
@@ -7869,7 +7725,7 @@
       </c>
       <c r="C40" s="26" t="n"/>
     </row>
-    <row r="41">
+    <row r="41" ht="18" customHeight="1">
       <c r="B41" s="39" t="inlineStr">
         <is>
           <t>Preparing for a compliance audit</t>
@@ -7889,7 +7745,7 @@
       </c>
       <c r="C42" s="26" t="n"/>
     </row>
-    <row r="43">
+    <row r="43" ht="18" customHeight="1">
       <c r="B43" s="101" t="inlineStr">
         <is>
           <t>Reporting on program effectiveness</t>
@@ -7906,7 +7762,7 @@
         </is>
       </c>
     </row>
-    <row r="45">
+    <row r="45" ht="12" customHeight="1">
       <c r="B45" s="97" t="n"/>
     </row>
     <row r="46" ht="17" customHeight="1">
@@ -7988,18 +7844,18 @@
         </is>
       </c>
     </row>
-    <row r="53">
+    <row r="53" ht="12" customHeight="1">
       <c r="B53" s="273" t="n"/>
       <c r="C53" s="147" t="n"/>
     </row>
-    <row r="54" ht="17" customHeight="1">
+    <row r="54" ht="20" customHeight="1">
       <c r="B54" s="4" t="inlineStr">
         <is>
           <t>Customizing for Your Organization</t>
         </is>
       </c>
     </row>
-    <row r="55">
+    <row r="55" ht="18" customHeight="1">
       <c r="B55" s="22" t="inlineStr">
         <is>
           <t>Governance Guide</t>
@@ -8011,7 +7867,7 @@
         </is>
       </c>
     </row>
-    <row r="56">
+    <row r="56" ht="18" customHeight="1">
       <c r="B56" s="22" t="inlineStr">
         <is>
           <t>Tool Registry</t>
@@ -8023,7 +7879,7 @@
         </is>
       </c>
     </row>
-    <row r="57">
+    <row r="57" ht="18" customHeight="1">
       <c r="B57" s="22" t="inlineStr">
         <is>
           <t>Intake Form</t>
@@ -8035,7 +7891,7 @@
         </is>
       </c>
     </row>
-    <row r="58">
+    <row r="58" ht="18" customHeight="1">
       <c r="B58" s="22" t="inlineStr">
         <is>
           <t>Guardrail Checklist</t>
@@ -8047,7 +7903,7 @@
         </is>
       </c>
     </row>
-    <row r="59">
+    <row r="59" ht="18" customHeight="1">
       <c r="B59" s="22" t="inlineStr">
         <is>
           <t>Tool Function Mapping</t>
@@ -11481,7 +11337,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:D74"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD15"/>
@@ -11495,6 +11351,7 @@
     <col width="20" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2" ht="21" customHeight="1">
       <c r="B2" s="9" t="inlineStr">
         <is>
@@ -11502,6 +11359,7 @@
         </is>
       </c>
     </row>
+    <row r="3"/>
     <row r="4" ht="28" customHeight="1">
       <c r="B4" s="15" t="inlineStr">
         <is>
@@ -11594,14 +11452,14 @@
         </is>
       </c>
     </row>
+    <row r="10"/>
+    <row r="11"/>
     <row r="12" ht="19" customHeight="1">
       <c r="B12" s="31" t="inlineStr">
         <is>
           <t>PART 1: REQUESTOR COMPLETES</t>
         </is>
       </c>
-      <c r="C12" s="32" t="n"/>
-      <c r="D12" s="32" t="n"/>
     </row>
     <row r="13" ht="17" customHeight="1">
       <c r="B13" s="4" t="inlineStr">
@@ -11634,6 +11492,7 @@
       </c>
       <c r="C16" s="23" t="n"/>
     </row>
+    <row r="17"/>
     <row r="18" ht="28" customHeight="1">
       <c r="B18" s="4" t="inlineStr">
         <is>
@@ -11680,6 +11539,7 @@
         </is>
       </c>
     </row>
+    <row r="22"/>
     <row r="23" ht="28" customHeight="1">
       <c r="B23" s="4" t="inlineStr">
         <is>
@@ -11720,6 +11580,7 @@
         </is>
       </c>
     </row>
+    <row r="27"/>
     <row r="28" ht="17" customHeight="1">
       <c r="B28" s="4" t="inlineStr">
         <is>
@@ -11816,6 +11677,7 @@
         </is>
       </c>
     </row>
+    <row r="36"/>
     <row r="37" ht="17" customHeight="1">
       <c r="B37" s="4" t="inlineStr">
         <is>
@@ -11872,6 +11734,7 @@
         </is>
       </c>
     </row>
+    <row r="42"/>
     <row r="43">
       <c r="B43" s="33" t="inlineStr">
         <is>
@@ -11879,15 +11742,15 @@
         </is>
       </c>
     </row>
+    <row r="44"/>
     <row r="45" ht="19" customHeight="1">
       <c r="B45" s="34" t="inlineStr">
         <is>
           <t>PART 2: SECURITY TEAM COMPLETES</t>
         </is>
       </c>
-      <c r="C45" s="35" t="n"/>
-      <c r="D45" s="35" t="n"/>
-    </row>
+    </row>
+    <row r="46"/>
     <row r="47" ht="17" customHeight="1">
       <c r="B47" s="4" t="inlineStr">
         <is>
@@ -11984,6 +11847,7 @@
         </is>
       </c>
     </row>
+    <row r="55"/>
     <row r="56">
       <c r="B56" s="21" t="inlineStr">
         <is>
@@ -11996,6 +11860,7 @@
         </is>
       </c>
     </row>
+    <row r="57"/>
     <row r="58" ht="17" customHeight="1">
       <c r="B58" s="4" t="inlineStr">
         <is>
@@ -12076,17 +11941,18 @@
       </c>
     </row>
     <row r="65" ht="32" customHeight="1">
-      <c r="B65" s="54" t="inlineStr">
+      <c r="B65" s="22" t="inlineStr">
         <is>
           <t>☐ AI Supply Chain</t>
         </is>
       </c>
-      <c r="C65" s="55" t="inlineStr">
+      <c r="C65" s="1" t="inlineStr">
         <is>
           <t>Model provenance, training data lineage, ML pipeline security, third-party model verification</t>
         </is>
       </c>
     </row>
+    <row r="66"/>
     <row r="67">
       <c r="B67" s="21" t="inlineStr">
         <is>
@@ -12108,6 +11974,7 @@
         </is>
       </c>
     </row>
+    <row r="69"/>
     <row r="70" ht="17" customHeight="1">
       <c r="B70" s="4" t="inlineStr">
         <is>
@@ -16199,2128 +16066,2128 @@
       </c>
     </row>
     <row r="17" ht="40" customHeight="1">
-      <c r="B17" s="269" t="inlineStr">
+      <c r="B17" s="262" t="inlineStr">
         <is>
           <t>Palo Alto Networks (Protect AI)</t>
         </is>
       </c>
-      <c r="C17" s="8" t="inlineStr">
+      <c r="C17" s="262" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D17" s="154" t="inlineStr">
+      <c r="D17" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E17" s="162" t="inlineStr">
+      <c r="E17" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F17" s="159" t="inlineStr">
+      <c r="F17" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G17" s="8" t="inlineStr">
+      <c r="G17" s="262" t="inlineStr">
         <is>
           <t>Full-stack AI security via Protect AI: ML supply chain, model scanning, runtime, red teaming</t>
         </is>
       </c>
-      <c r="H17" s="8" t="inlineStr">
+      <c r="H17" s="262" t="inlineStr">
         <is>
           <t>Palo Alto customers; integrated platform play</t>
         </is>
       </c>
     </row>
     <row r="18" ht="40" customHeight="1">
-      <c r="B18" s="269" t="inlineStr">
+      <c r="B18" s="262" t="inlineStr">
         <is>
           <t>Cisco (Robust Intelligence)</t>
         </is>
       </c>
-      <c r="C18" s="8" t="inlineStr">
+      <c r="C18" s="262" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D18" s="154" t="inlineStr">
+      <c r="D18" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E18" s="162" t="inlineStr">
+      <c r="E18" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F18" s="158" t="inlineStr">
+      <c r="F18" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="G18" s="8" t="inlineStr">
+      <c r="G18" s="262" t="inlineStr">
         <is>
           <t>Network-layer AI security via Robust Intelligence: model validation, supply chain, guardrails</t>
         </is>
       </c>
-      <c r="H18" s="8" t="inlineStr">
+      <c r="H18" s="262" t="inlineStr">
         <is>
           <t>Cisco customers; agentless deployment</t>
         </is>
       </c>
     </row>
     <row r="19" ht="40" customHeight="1">
-      <c r="B19" s="269" t="inlineStr">
+      <c r="B19" s="262" t="inlineStr">
         <is>
           <t>Microsoft Defender for Cloud</t>
         </is>
       </c>
-      <c r="C19" s="8" t="inlineStr">
+      <c r="C19" s="262" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="D19" s="154" t="inlineStr">
+      <c r="D19" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E19" s="157" t="inlineStr">
+      <c r="E19" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F19" s="160" t="inlineStr">
+      <c r="F19" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G19" s="8" t="inlineStr">
+      <c r="G19" s="262" t="inlineStr">
         <is>
           <t>Multi-cloud AI-SPM, OWASP Top 10 for LLMs, Azure AI Content Safety integration</t>
         </is>
       </c>
-      <c r="H19" s="8" t="inlineStr">
+      <c r="H19" s="262" t="inlineStr">
         <is>
           <t>Azure/M365 shops; broadest native coverage</t>
         </is>
       </c>
     </row>
     <row r="20" ht="40" customHeight="1">
-      <c r="B20" s="269" t="inlineStr">
+      <c r="B20" s="262" t="inlineStr">
         <is>
           <t>Wiz</t>
         </is>
       </c>
-      <c r="C20" s="8" t="inlineStr">
+      <c r="C20" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D20" s="154" t="inlineStr">
+      <c r="D20" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E20" s="158" t="inlineStr">
+      <c r="E20" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F20" s="159" t="inlineStr">
+      <c r="F20" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G20" s="8" t="inlineStr">
+      <c r="G20" s="262" t="inlineStr">
         <is>
           <t>CNAPP-native AI-SPM: agentless discovery, risk prioritization, compliance mapping</t>
         </is>
       </c>
-      <c r="H20" s="8" t="inlineStr">
+      <c r="H20" s="262" t="inlineStr">
         <is>
           <t>Wiz customers; cloud-native AI workloads</t>
         </is>
       </c>
     </row>
     <row r="21" ht="40" customHeight="1">
-      <c r="B21" s="269" t="inlineStr">
+      <c r="B21" s="262" t="inlineStr">
         <is>
           <t>CrowdStrike (Pangea)</t>
         </is>
       </c>
-      <c r="C21" s="8" t="inlineStr">
+      <c r="C21" s="262" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D21" s="154" t="inlineStr">
+      <c r="D21" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E21" s="157" t="inlineStr">
+      <c r="E21" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F21" s="162" t="inlineStr">
+      <c r="F21" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="G21" s="8" t="inlineStr">
+      <c r="G21" s="262" t="inlineStr">
         <is>
           <t>Charlotte AI for SOC + Pangea adds guardrails, prompt defense, model security</t>
         </is>
       </c>
-      <c r="H21" s="8" t="inlineStr">
+      <c r="H21" s="262" t="inlineStr">
         <is>
           <t>CrowdStrike customers; endpoint-centric orgs</t>
         </is>
       </c>
     </row>
     <row r="22" ht="40" customHeight="1">
-      <c r="B22" s="269" t="inlineStr">
+      <c r="B22" s="262" t="inlineStr">
         <is>
           <t>ServiceNow</t>
         </is>
       </c>
-      <c r="C22" s="8" t="inlineStr">
+      <c r="C22" s="262" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="D22" s="154" t="inlineStr">
+      <c r="D22" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E22" s="159" t="inlineStr">
+      <c r="E22" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F22" s="161" t="inlineStr">
+      <c r="F22" s="282" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="G22" s="8" t="inlineStr">
+      <c r="G22" s="262" t="inlineStr">
         <is>
           <t>AI Governance for Now Assist: AI Control Tower, usage tracking, compliance workflows</t>
         </is>
       </c>
-      <c r="H22" s="8" t="inlineStr">
+      <c r="H22" s="262" t="inlineStr">
         <is>
           <t>ServiceNow customers; IT/GRC-centric governance</t>
         </is>
       </c>
     </row>
     <row r="23" ht="40" customHeight="1">
-      <c r="B23" s="269" t="inlineStr">
+      <c r="B23" s="262" t="inlineStr">
         <is>
           <t>HiddenLayer</t>
         </is>
       </c>
-      <c r="C23" s="8" t="inlineStr">
+      <c r="C23" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D23" s="162" t="inlineStr">
+      <c r="D23" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E23" s="157" t="inlineStr">
+      <c r="E23" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F23" s="154" t="inlineStr">
+      <c r="F23" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G23" s="8" t="inlineStr">
+      <c r="G23" s="262" t="inlineStr">
         <is>
           <t>AI Supply Chain leader ($56M raised): model scanning, ML supply chain security, model BOM</t>
         </is>
       </c>
-      <c r="H23" s="8" t="inlineStr">
+      <c r="H23" s="262" t="inlineStr">
         <is>
           <t>Multi-cloud AI; wants independent vendor</t>
         </is>
       </c>
     </row>
     <row r="24" ht="40" customHeight="1">
-      <c r="B24" s="269" t="inlineStr">
+      <c r="B24" s="262" t="inlineStr">
         <is>
           <t>Noma Security</t>
         </is>
       </c>
-      <c r="C24" s="8" t="inlineStr">
+      <c r="C24" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D24" s="154" t="inlineStr">
+      <c r="D24" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E24" s="162" t="inlineStr">
+      <c r="E24" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F24" s="159" t="inlineStr">
+      <c r="F24" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G24" s="8" t="inlineStr">
+      <c r="G24" s="262" t="inlineStr">
         <is>
           <t>Fastest-growing ($132M raised): full AI lifecycle including supply chain, agentic AI focus</t>
         </is>
       </c>
-      <c r="H24" s="8" t="inlineStr">
+      <c r="H24" s="262" t="inlineStr">
         <is>
           <t>Comprehensive AI security; agentic deployments</t>
         </is>
       </c>
     </row>
     <row r="25" ht="40" customHeight="1">
-      <c r="B25" s="269" t="inlineStr">
+      <c r="B25" s="262" t="inlineStr">
         <is>
           <t>Credo AI</t>
         </is>
       </c>
-      <c r="C25" s="8" t="inlineStr">
+      <c r="C25" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D25" s="154" t="inlineStr">
+      <c r="D25" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E25" s="159" t="inlineStr">
+      <c r="E25" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F25" s="162" t="inlineStr">
+      <c r="F25" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="G25" s="8" t="inlineStr">
+      <c r="G25" s="262" t="inlineStr">
         <is>
           <t>AI governance platform: centralizes policies, risk assessments, model inventory, supply chain tracking</t>
         </is>
       </c>
-      <c r="H25" s="8" t="inlineStr">
+      <c r="H25" s="262" t="inlineStr">
         <is>
           <t>AI governance and vendor risk management</t>
         </is>
       </c>
     </row>
     <row r="26" ht="40" customHeight="1">
-      <c r="B26" s="269" t="inlineStr">
+      <c r="B26" s="262" t="inlineStr">
         <is>
           <t>WitnessAI</t>
         </is>
       </c>
-      <c r="C26" s="8" t="inlineStr">
+      <c r="C26" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D26" s="154" t="inlineStr">
+      <c r="D26" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E26" s="158" t="inlineStr">
+      <c r="E26" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F26" s="157" t="inlineStr">
+      <c r="F26" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G26" s="8" t="inlineStr">
+      <c r="G26" s="262" t="inlineStr">
         <is>
           <t>Discovers AI usage, enforces policy, coaches users on safe AI practices</t>
         </is>
       </c>
-      <c r="H26" s="8" t="inlineStr">
+      <c r="H26" s="262" t="inlineStr">
         <is>
           <t>Safe AI enablement with visibility and coaching</t>
         </is>
       </c>
     </row>
     <row r="27" ht="40" customHeight="1">
-      <c r="B27" s="269" t="inlineStr">
+      <c r="B27" s="262" t="inlineStr">
         <is>
           <t>Acuvity</t>
         </is>
       </c>
-      <c r="C27" s="8" t="inlineStr">
+      <c r="C27" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D27" s="154" t="inlineStr">
+      <c r="D27" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E27" s="160" t="inlineStr">
+      <c r="E27" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F27" s="158" t="inlineStr">
+      <c r="F27" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="G27" s="8" t="inlineStr">
+      <c r="G27" s="262" t="inlineStr">
         <is>
           <t>Unified discovery, governance, data protection across AI landscape</t>
         </is>
       </c>
-      <c r="H27" s="8" t="inlineStr">
+      <c r="H27" s="262" t="inlineStr">
         <is>
           <t>Consolidating AI security into one platform</t>
         </is>
       </c>
     </row>
     <row r="28" ht="40" customHeight="1">
-      <c r="B28" s="269" t="inlineStr">
+      <c r="B28" s="262" t="inlineStr">
         <is>
           <t>Zenity</t>
         </is>
       </c>
-      <c r="C28" s="8" t="inlineStr">
+      <c r="C28" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D28" s="154" t="inlineStr">
+      <c r="D28" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E28" s="161" t="inlineStr">
+      <c r="E28" s="282" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F28" s="157" t="inlineStr">
+      <c r="F28" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G28" s="8" t="inlineStr">
+      <c r="G28" s="262" t="inlineStr">
         <is>
           <t>Agent-centric posture management; low-code/copilot security specialist</t>
         </is>
       </c>
-      <c r="H28" s="8" t="inlineStr">
+      <c r="H28" s="262" t="inlineStr">
         <is>
           <t>Organizations deploying AI agents at scale</t>
         </is>
       </c>
     </row>
     <row r="29" ht="40" customHeight="1">
-      <c r="B29" s="269" t="inlineStr">
+      <c r="B29" s="262" t="inlineStr">
         <is>
           <t>Cato Networks (AIM Security)</t>
         </is>
       </c>
-      <c r="C29" s="8" t="inlineStr">
+      <c r="C29" s="262" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D29" s="154" t="inlineStr">
+      <c r="D29" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E29" s="157" t="inlineStr">
+      <c r="E29" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F29" s="158" t="inlineStr">
+      <c r="F29" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="G29" s="8" t="inlineStr">
+      <c r="G29" s="262" t="inlineStr">
         <is>
           <t>AI-SPM + agent security via AIM Security acquisition; SASE integration</t>
         </is>
       </c>
-      <c r="H29" s="8" t="inlineStr">
+      <c r="H29" s="262" t="inlineStr">
         <is>
           <t>Cato SASE customers</t>
         </is>
       </c>
     </row>
     <row r="30" ht="40" customHeight="1">
-      <c r="B30" s="269" t="inlineStr">
+      <c r="B30" s="262" t="inlineStr">
         <is>
           <t>Legit Security</t>
         </is>
       </c>
-      <c r="C30" s="8" t="inlineStr">
+      <c r="C30" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D30" s="162" t="inlineStr">
+      <c r="D30" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E30" s="154" t="inlineStr">
+      <c r="E30" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F30" s="157" t="inlineStr">
+      <c r="F30" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G30" s="8" t="inlineStr">
+      <c r="G30" s="262" t="inlineStr">
         <is>
           <t>AI Supply Chain via ASPM: AI code security, model supply chain, SDLC for ML pipelines</t>
         </is>
       </c>
-      <c r="H30" s="8" t="inlineStr">
+      <c r="H30" s="262" t="inlineStr">
         <is>
           <t>DevSecOps teams; AI in software supply chain</t>
         </is>
       </c>
     </row>
     <row r="31" ht="40" customHeight="1">
-      <c r="B31" s="269" t="inlineStr">
+      <c r="B31" s="262" t="inlineStr">
         <is>
           <t>Check Point (Lakera)</t>
         </is>
       </c>
-      <c r="C31" s="8" t="inlineStr">
+      <c r="C31" s="262" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D31" s="157" t="inlineStr">
+      <c r="D31" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E31" s="154" t="inlineStr">
+      <c r="E31" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F31" s="162" t="inlineStr">
+      <c r="F31" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="G31" s="8" t="inlineStr">
+      <c r="G31" s="262" t="inlineStr">
         <is>
           <t>Lakera adds runtime guardrails, prompt injection defense, model security to Infinity</t>
         </is>
       </c>
-      <c r="H31" s="8" t="inlineStr">
+      <c r="H31" s="262" t="inlineStr">
         <is>
           <t>Check Point customers; Infinity stack users</t>
         </is>
       </c>
     </row>
     <row r="32" ht="40" customHeight="1">
-      <c r="B32" s="269" t="inlineStr">
+      <c r="B32" s="262" t="inlineStr">
         <is>
           <t>TrojAI</t>
         </is>
       </c>
-      <c r="C32" s="8" t="inlineStr">
+      <c r="C32" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D32" s="157" t="inlineStr">
+      <c r="D32" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E32" s="162" t="inlineStr">
+      <c r="E32" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F32" s="159" t="inlineStr">
+      <c r="F32" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G32" s="8" t="inlineStr">
+      <c r="G32" s="262" t="inlineStr">
         <is>
           <t>Model threat protection: detects backdoors, adversarial attacks, model poisoning; supply chain focus</t>
         </is>
       </c>
-      <c r="H32" s="8" t="inlineStr">
+      <c r="H32" s="262" t="inlineStr">
         <is>
           <t>Deep model hardening beyond prompt-level</t>
         </is>
       </c>
     </row>
     <row r="33" ht="40" customHeight="1">
-      <c r="B33" s="269" t="inlineStr">
+      <c r="B33" s="262" t="inlineStr">
         <is>
           <t>Arthur AI</t>
         </is>
       </c>
-      <c r="C33" s="8" t="inlineStr">
+      <c r="C33" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D33" s="157" t="inlineStr">
+      <c r="D33" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E33" s="159" t="inlineStr">
+      <c r="E33" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F33" s="154" t="inlineStr">
+      <c r="F33" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G33" s="8" t="inlineStr">
+      <c r="G33" s="262" t="inlineStr">
         <is>
           <t>LLM firewall + observability ($60M raised): federated architecture, data stays local</t>
         </is>
       </c>
-      <c r="H33" s="8" t="inlineStr">
+      <c r="H33" s="262" t="inlineStr">
         <is>
           <t>Regulated industries; data residency requirements</t>
         </is>
       </c>
     </row>
     <row r="34" ht="40" customHeight="1">
-      <c r="B34" s="269" t="inlineStr">
+      <c r="B34" s="262" t="inlineStr">
         <is>
           <t>Mindgard</t>
         </is>
       </c>
-      <c r="C34" s="8" t="inlineStr">
+      <c r="C34" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D34" s="157" t="inlineStr">
+      <c r="D34" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E34" s="159" t="inlineStr">
+      <c r="E34" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F34" s="162" t="inlineStr">
+      <c r="F34" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="G34" s="8" t="inlineStr">
+      <c r="G34" s="262" t="inlineStr">
         <is>
           <t>Offensive AI security: automated red teaming, model vulnerability scanning, supply chain testing</t>
         </is>
       </c>
-      <c r="H34" s="8" t="inlineStr">
+      <c r="H34" s="262" t="inlineStr">
         <is>
           <t>Continuous AI security testing; red team automation</t>
         </is>
       </c>
     </row>
     <row r="35" ht="40" customHeight="1">
-      <c r="B35" s="269" t="inlineStr">
+      <c r="B35" s="262" t="inlineStr">
         <is>
           <t>F5 (CalypsoAI)</t>
         </is>
       </c>
-      <c r="C35" s="8" t="inlineStr">
+      <c r="C35" s="262" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D35" s="157" t="inlineStr">
+      <c r="D35" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E35" s="159" t="inlineStr">
+      <c r="E35" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F35" s="162" t="inlineStr">
+      <c r="F35" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="G35" s="8" t="inlineStr">
+      <c r="G35" s="262" t="inlineStr">
         <is>
           <t>Inference protection + red-teaming via CalypsoAI; model testing, API security</t>
         </is>
       </c>
-      <c r="H35" s="8" t="inlineStr">
+      <c r="H35" s="262" t="inlineStr">
         <is>
           <t>F5 customers; API/app security integration</t>
         </is>
       </c>
     </row>
     <row r="36" ht="40" customHeight="1">
-      <c r="B36" s="269" t="inlineStr">
+      <c r="B36" s="262" t="inlineStr">
         <is>
           <t>Rebuff AI</t>
         </is>
       </c>
-      <c r="C36" s="8" t="inlineStr">
+      <c r="C36" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D36" s="157" t="inlineStr">
+      <c r="D36" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E36" s="159" t="inlineStr">
+      <c r="E36" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F36" s="63" t="inlineStr">
+      <c r="F36" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G36" s="8" t="inlineStr">
+      <c r="G36" s="262" t="inlineStr">
         <is>
           <t>Open source prompt injection detection; self-hardening through attack learning</t>
         </is>
       </c>
-      <c r="H36" s="8" t="inlineStr">
+      <c r="H36" s="262" t="inlineStr">
         <is>
           <t>Teams wanting OSS guardrails; cost-conscious</t>
         </is>
       </c>
     </row>
     <row r="37" ht="40" customHeight="1">
-      <c r="B37" s="269" t="inlineStr">
+      <c r="B37" s="262" t="inlineStr">
         <is>
           <t>LLM Guard</t>
         </is>
       </c>
-      <c r="C37" s="8" t="inlineStr">
+      <c r="C37" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D37" s="157" t="inlineStr">
+      <c r="D37" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E37" s="160" t="inlineStr">
+      <c r="E37" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F37" s="63" t="inlineStr">
+      <c r="F37" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G37" s="8" t="inlineStr">
+      <c r="G37" s="262" t="inlineStr">
         <is>
           <t>Open source input/output scanner; PII detection, toxicity, prompt injection</t>
         </is>
       </c>
-      <c r="H37" s="8" t="inlineStr">
+      <c r="H37" s="262" t="inlineStr">
         <is>
           <t>OSS-first orgs; customizable guardrails</t>
         </is>
       </c>
     </row>
     <row r="38" ht="40" customHeight="1">
-      <c r="B38" s="269" t="inlineStr">
+      <c r="B38" s="262" t="inlineStr">
         <is>
           <t>Prompt Armor</t>
         </is>
       </c>
-      <c r="C38" s="8" t="inlineStr">
+      <c r="C38" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D38" s="157" t="inlineStr">
+      <c r="D38" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E38" s="160" t="inlineStr">
+      <c r="E38" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F38" s="159" t="inlineStr">
+      <c r="F38" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G38" s="8" t="inlineStr">
+      <c r="G38" s="262" t="inlineStr">
         <is>
           <t>Prompt injection firewall; real-time threat detection for LLM applications</t>
         </is>
       </c>
-      <c r="H38" s="8" t="inlineStr">
+      <c r="H38" s="262" t="inlineStr">
         <is>
           <t>Dedicated prompt security; API-first deployment</t>
         </is>
       </c>
     </row>
     <row r="39" ht="40" customHeight="1">
-      <c r="B39" s="269" t="inlineStr">
+      <c r="B39" s="262" t="inlineStr">
         <is>
           <t>Invariant Labs</t>
         </is>
       </c>
-      <c r="C39" s="8" t="inlineStr">
+      <c r="C39" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D39" s="157" t="inlineStr">
+      <c r="D39" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E39" s="161" t="inlineStr">
+      <c r="E39" s="282" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F39" s="159" t="inlineStr">
+      <c r="F39" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G39" s="8" t="inlineStr">
+      <c r="G39" s="262" t="inlineStr">
         <is>
           <t>Agent security testing and guardrails; detects agent vulnerabilities and failures</t>
         </is>
       </c>
-      <c r="H39" s="8" t="inlineStr">
+      <c r="H39" s="262" t="inlineStr">
         <is>
           <t>Agentic AI security testing; agent-specific threats</t>
         </is>
       </c>
     </row>
     <row r="40" ht="40" customHeight="1">
-      <c r="B40" s="269" t="inlineStr">
+      <c r="B40" s="262" t="inlineStr">
         <is>
           <t>SentinelOne (Prompt Security)</t>
         </is>
       </c>
-      <c r="C40" s="8" t="inlineStr">
+      <c r="C40" s="262" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D40" s="158" t="inlineStr">
+      <c r="D40" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E40" s="157" t="inlineStr">
+      <c r="E40" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F40" s="160" t="inlineStr">
+      <c r="F40" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G40" s="8" t="inlineStr">
+      <c r="G40" s="262" t="inlineStr">
         <is>
           <t>Purple AI + Prompt Security acquisition: GenAI visibility, runtime protection</t>
         </is>
       </c>
-      <c r="H40" s="8" t="inlineStr">
+      <c r="H40" s="262" t="inlineStr">
         <is>
           <t>SentinelOne customers; GenAI visibility</t>
         </is>
       </c>
     </row>
     <row r="41" ht="40" customHeight="1">
-      <c r="B41" s="269" t="inlineStr">
+      <c r="B41" s="262" t="inlineStr">
         <is>
           <t>Harmonic Security</t>
         </is>
       </c>
-      <c r="C41" s="8" t="inlineStr">
+      <c r="C41" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D41" s="158" t="inlineStr">
+      <c r="D41" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E41" s="160" t="inlineStr">
+      <c r="E41" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F41" s="154" t="inlineStr">
+      <c r="F41" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G41" s="8" t="inlineStr">
+      <c r="G41" s="262" t="inlineStr">
         <is>
           <t>Shadow AI discovery + GenAI-aware DLP ($26M raised): detects sensitive data in AI</t>
         </is>
       </c>
-      <c r="H41" s="8" t="inlineStr">
+      <c r="H41" s="262" t="inlineStr">
         <is>
           <t>DLP specifically tuned for GenAI workflows</t>
         </is>
       </c>
     </row>
     <row r="42" ht="40" customHeight="1">
-      <c r="B42" s="269" t="inlineStr">
+      <c r="B42" s="262" t="inlineStr">
         <is>
           <t>Nightfall AI</t>
         </is>
       </c>
-      <c r="C42" s="8" t="inlineStr">
+      <c r="C42" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D42" s="158" t="inlineStr">
+      <c r="D42" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E42" s="160" t="inlineStr">
+      <c r="E42" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F42" s="157" t="inlineStr">
+      <c r="F42" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G42" s="8" t="inlineStr">
+      <c r="G42" s="262" t="inlineStr">
         <is>
           <t>AI-native DLP + GenAI firewall: discovers AI usage, prevents data exposure</t>
         </is>
       </c>
-      <c r="H42" s="8" t="inlineStr">
+      <c r="H42" s="262" t="inlineStr">
         <is>
           <t>Cloud-native DLP for AI applications</t>
         </is>
       </c>
     </row>
     <row r="43" ht="40" customHeight="1">
-      <c r="B43" s="269" t="inlineStr">
+      <c r="B43" s="262" t="inlineStr">
         <is>
           <t>Reco.ai</t>
         </is>
       </c>
-      <c r="C43" s="8" t="inlineStr">
+      <c r="C43" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D43" s="158" t="inlineStr">
+      <c r="D43" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E43" s="160" t="inlineStr">
+      <c r="E43" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F43" s="154" t="inlineStr">
+      <c r="F43" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G43" s="8" t="inlineStr">
+      <c r="G43" s="262" t="inlineStr">
         <is>
           <t>SaaS security + AI discovery: finds AI apps, tracks data flows, enforces policy</t>
         </is>
       </c>
-      <c r="H43" s="8" t="inlineStr">
+      <c r="H43" s="262" t="inlineStr">
         <is>
           <t>SaaS security teams extending to AI</t>
         </is>
       </c>
     </row>
     <row r="44" ht="40" customHeight="1">
-      <c r="B44" s="269" t="inlineStr">
+      <c r="B44" s="262" t="inlineStr">
         <is>
           <t>Arize AI</t>
         </is>
       </c>
-      <c r="C44" s="8" t="inlineStr">
+      <c r="C44" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D44" s="159" t="inlineStr">
+      <c r="D44" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E44" s="154" t="inlineStr">
+      <c r="E44" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F44" s="157" t="inlineStr">
+      <c r="F44" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G44" s="8" t="inlineStr">
+      <c r="G44" s="262" t="inlineStr">
         <is>
           <t>Enterprise AI observability ($131M raised): Phoenix OSS + AX enterprise platform</t>
         </is>
       </c>
-      <c r="H44" s="8" t="inlineStr">
+      <c r="H44" s="262" t="inlineStr">
         <is>
           <t>Production ML/LLM monitoring; Uber, DoorDash</t>
         </is>
       </c>
     </row>
     <row r="45" ht="40" customHeight="1">
-      <c r="B45" s="269" t="inlineStr">
+      <c r="B45" s="262" t="inlineStr">
         <is>
           <t>Patronus AI</t>
         </is>
       </c>
-      <c r="C45" s="8" t="inlineStr">
+      <c r="C45" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D45" s="159" t="inlineStr">
+      <c r="D45" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E45" s="157" t="inlineStr">
+      <c r="E45" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F45" s="154" t="inlineStr">
+      <c r="F45" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G45" s="8" t="inlineStr">
+      <c r="G45" s="262" t="inlineStr">
         <is>
           <t>LLM evaluation platform ($20M raised): hallucination detection, automated testing</t>
         </is>
       </c>
-      <c r="H45" s="8" t="inlineStr">
+      <c r="H45" s="262" t="inlineStr">
         <is>
           <t>LLM quality assurance; hallucination prevention</t>
         </is>
       </c>
     </row>
     <row r="46" ht="40" customHeight="1">
-      <c r="B46" s="269" t="inlineStr">
+      <c r="B46" s="262" t="inlineStr">
         <is>
           <t>Fiddler AI</t>
         </is>
       </c>
-      <c r="C46" s="8" t="inlineStr">
+      <c r="C46" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D46" s="159" t="inlineStr">
+      <c r="D46" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E46" s="154" t="inlineStr">
+      <c r="E46" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F46" s="160" t="inlineStr">
+      <c r="F46" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G46" s="8" t="inlineStr">
+      <c r="G46" s="262" t="inlineStr">
         <is>
           <t>Trust Service for LLMs ($68.6M raised): model scoring, guardrails, explainability</t>
         </is>
       </c>
-      <c r="H46" s="8" t="inlineStr">
+      <c r="H46" s="262" t="inlineStr">
         <is>
           <t>Regulated industries needing explainability</t>
         </is>
       </c>
     </row>
     <row r="47" ht="40" customHeight="1">
-      <c r="B47" s="269" t="inlineStr">
+      <c r="B47" s="262" t="inlineStr">
         <is>
           <t>Datadog LLM Observability</t>
         </is>
       </c>
-      <c r="C47" s="8" t="inlineStr">
+      <c r="C47" s="262" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="D47" s="159" t="inlineStr">
+      <c r="D47" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E47" s="154" t="inlineStr">
+      <c r="E47" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F47" s="63" t="inlineStr">
+      <c r="F47" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G47" s="8" t="inlineStr">
+      <c r="G47" s="262" t="inlineStr">
         <is>
           <t>LLM monitoring: prompt injection detection, PII scanning, cost tracking</t>
         </is>
       </c>
-      <c r="H47" s="8" t="inlineStr">
+      <c r="H47" s="262" t="inlineStr">
         <is>
           <t>Datadog customers; unified observability</t>
         </is>
       </c>
     </row>
     <row r="48" ht="40" customHeight="1">
-      <c r="B48" s="269" t="inlineStr">
+      <c r="B48" s="262" t="inlineStr">
         <is>
           <t>LangSmith (LangChain)</t>
         </is>
       </c>
-      <c r="C48" s="8" t="inlineStr">
+      <c r="C48" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D48" s="159" t="inlineStr">
+      <c r="D48" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E48" s="154" t="inlineStr">
+      <c r="E48" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F48" s="63" t="inlineStr">
+      <c r="F48" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G48" s="8" t="inlineStr">
+      <c r="G48" s="262" t="inlineStr">
         <is>
           <t>LLM app debugging and monitoring; traces, evaluations, prompt management</t>
         </is>
       </c>
-      <c r="H48" s="8" t="inlineStr">
+      <c r="H48" s="262" t="inlineStr">
         <is>
           <t>LangChain users; LLM app developers</t>
         </is>
       </c>
     </row>
     <row r="49" ht="40" customHeight="1">
-      <c r="B49" s="269" t="inlineStr">
+      <c r="B49" s="262" t="inlineStr">
         <is>
           <t>Weights &amp; Biases</t>
         </is>
       </c>
-      <c r="C49" s="8" t="inlineStr">
+      <c r="C49" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D49" s="159" t="inlineStr">
+      <c r="D49" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E49" s="154" t="inlineStr">
+      <c r="E49" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F49" s="63" t="inlineStr">
+      <c r="F49" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G49" s="8" t="inlineStr">
+      <c r="G49" s="262" t="inlineStr">
         <is>
           <t>MLOps platform ($250M raised): experiment tracking, model registry, LLM tracing</t>
         </is>
       </c>
-      <c r="H49" s="8" t="inlineStr">
+      <c r="H49" s="262" t="inlineStr">
         <is>
           <t>ML teams; experiment tracking; model lifecycle</t>
         </is>
       </c>
     </row>
     <row r="50" ht="40" customHeight="1">
-      <c r="B50" s="269" t="inlineStr">
+      <c r="B50" s="262" t="inlineStr">
         <is>
           <t>Galileo AI</t>
         </is>
       </c>
-      <c r="C50" s="8" t="inlineStr">
+      <c r="C50" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D50" s="159" t="inlineStr">
+      <c r="D50" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E50" s="157" t="inlineStr">
+      <c r="E50" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F50" s="160" t="inlineStr">
+      <c r="F50" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G50" s="8" t="inlineStr">
+      <c r="G50" s="262" t="inlineStr">
         <is>
           <t>LLM debugging and evaluation: hallucination detection, data quality, guardrails</t>
         </is>
       </c>
-      <c r="H50" s="8" t="inlineStr">
+      <c r="H50" s="262" t="inlineStr">
         <is>
           <t>LLM debugging; data scientists; quality focus</t>
         </is>
       </c>
     </row>
     <row r="51" ht="40" customHeight="1">
-      <c r="B51" s="269" t="inlineStr">
+      <c r="B51" s="262" t="inlineStr">
         <is>
           <t>Portkey</t>
         </is>
       </c>
-      <c r="C51" s="8" t="inlineStr">
+      <c r="C51" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D51" s="159" t="inlineStr">
+      <c r="D51" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E51" s="157" t="inlineStr">
+      <c r="E51" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F51" s="154" t="inlineStr">
+      <c r="F51" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G51" s="8" t="inlineStr">
+      <c r="G51" s="262" t="inlineStr">
         <is>
           <t>LLM gateway and observability: unified API, caching, fallbacks, cost management</t>
         </is>
       </c>
-      <c r="H51" s="8" t="inlineStr">
+      <c r="H51" s="262" t="inlineStr">
         <is>
           <t>Multi-LLM deployments; cost optimization</t>
         </is>
       </c>
     </row>
     <row r="52" ht="40" customHeight="1">
-      <c r="B52" s="269" t="inlineStr">
+      <c r="B52" s="262" t="inlineStr">
         <is>
           <t>Helicone</t>
         </is>
       </c>
-      <c r="C52" s="8" t="inlineStr">
+      <c r="C52" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D52" s="159" t="inlineStr">
+      <c r="D52" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E52" s="154" t="inlineStr">
+      <c r="E52" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F52" s="63" t="inlineStr">
+      <c r="F52" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G52" s="8" t="inlineStr">
+      <c r="G52" s="262" t="inlineStr">
         <is>
           <t>Open source LLM observability: request logging, caching, rate limiting, analytics</t>
         </is>
       </c>
-      <c r="H52" s="8" t="inlineStr">
+      <c r="H52" s="262" t="inlineStr">
         <is>
           <t>OSS-first teams; LLM monitoring on budget</t>
         </is>
       </c>
     </row>
     <row r="53" ht="40" customHeight="1">
-      <c r="B53" s="269" t="inlineStr">
+      <c r="B53" s="262" t="inlineStr">
         <is>
           <t>Cyera</t>
         </is>
       </c>
-      <c r="C53" s="8" t="inlineStr">
+      <c r="C53" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D53" s="160" t="inlineStr">
+      <c r="D53" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E53" s="154" t="inlineStr">
+      <c r="E53" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F53" s="158" t="inlineStr">
+      <c r="F53" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="G53" s="8" t="inlineStr">
+      <c r="G53" s="262" t="inlineStr">
         <is>
           <t>DSPM leader ($1.3B raised, $6B valuation): AI Guardian, 98% classification accuracy</t>
         </is>
       </c>
-      <c r="H53" s="8" t="inlineStr">
+      <c r="H53" s="262" t="inlineStr">
         <is>
           <t>Enterprise DSPM; AI data governance</t>
         </is>
       </c>
     </row>
     <row r="54" ht="40" customHeight="1">
-      <c r="B54" s="269" t="inlineStr">
+      <c r="B54" s="262" t="inlineStr">
         <is>
           <t>BigID</t>
         </is>
       </c>
-      <c r="C54" s="8" t="inlineStr">
+      <c r="C54" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D54" s="160" t="inlineStr">
+      <c r="D54" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E54" s="154" t="inlineStr">
+      <c r="E54" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F54" s="158" t="inlineStr">
+      <c r="F54" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="G54" s="8" t="inlineStr">
+      <c r="G54" s="262" t="inlineStr">
         <is>
           <t>Shadow AI detection + AI governance ($290M raised): discovers AI data/models, maps to regs</t>
         </is>
       </c>
-      <c r="H54" s="8" t="inlineStr">
+      <c r="H54" s="262" t="inlineStr">
         <is>
           <t>Data discovery and governance for AI</t>
         </is>
       </c>
     </row>
     <row r="55" ht="40" customHeight="1">
-      <c r="B55" s="269" t="inlineStr">
+      <c r="B55" s="262" t="inlineStr">
         <is>
           <t>Netskope</t>
         </is>
       </c>
-      <c r="C55" s="8" t="inlineStr">
+      <c r="C55" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D55" s="160" t="inlineStr">
+      <c r="D55" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E55" s="158" t="inlineStr">
+      <c r="E55" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F55" s="157" t="inlineStr">
+      <c r="F55" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G55" s="8" t="inlineStr">
+      <c r="G55" s="262" t="inlineStr">
         <is>
           <t>SASE + GenAI DLP: real-time coaching, data protection for AI apps</t>
         </is>
       </c>
-      <c r="H55" s="8" t="inlineStr">
+      <c r="H55" s="262" t="inlineStr">
         <is>
           <t>SASE customers; GenAI-aware DLP</t>
         </is>
       </c>
     </row>
     <row r="56" ht="40" customHeight="1">
-      <c r="B56" s="269" t="inlineStr">
+      <c r="B56" s="262" t="inlineStr">
         <is>
           <t>Zscaler</t>
         </is>
       </c>
-      <c r="C56" s="8" t="inlineStr">
+      <c r="C56" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D56" s="160" t="inlineStr">
+      <c r="D56" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E56" s="158" t="inlineStr">
+      <c r="E56" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F56" s="157" t="inlineStr">
+      <c r="F56" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G56" s="8" t="inlineStr">
+      <c r="G56" s="262" t="inlineStr">
         <is>
           <t>Zero trust + AI security: GenAI app control, data protection, shadow AI</t>
         </is>
       </c>
-      <c r="H56" s="8" t="inlineStr">
+      <c r="H56" s="262" t="inlineStr">
         <is>
           <t>Zscaler customers; zero trust AI security</t>
         </is>
       </c>
     </row>
     <row r="57" ht="40" customHeight="1">
-      <c r="B57" s="269" t="inlineStr">
+      <c r="B57" s="262" t="inlineStr">
         <is>
           <t>Island Browser</t>
         </is>
       </c>
-      <c r="C57" s="8" t="inlineStr">
+      <c r="C57" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D57" s="160" t="inlineStr">
+      <c r="D57" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E57" s="158" t="inlineStr">
+      <c r="E57" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F57" s="154" t="inlineStr">
+      <c r="F57" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G57" s="8" t="inlineStr">
+      <c r="G57" s="262" t="inlineStr">
         <is>
           <t>Enterprise browser with AI controls: DLP, session recording, controlled AI access</t>
         </is>
       </c>
-      <c r="H57" s="8" t="inlineStr">
+      <c r="H57" s="262" t="inlineStr">
         <is>
           <t>Browser-based AI control; high-security orgs</t>
         </is>
       </c>
     </row>
     <row r="58" ht="40" customHeight="1">
-      <c r="B58" s="269" t="inlineStr">
+      <c r="B58" s="262" t="inlineStr">
         <is>
           <t>Knostic</t>
         </is>
       </c>
-      <c r="C58" s="8" t="inlineStr">
+      <c r="C58" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D58" s="160" t="inlineStr">
+      <c r="D58" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E58" s="154" t="inlineStr">
+      <c r="E58" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F58" s="157" t="inlineStr">
+      <c r="F58" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G58" s="8" t="inlineStr">
+      <c r="G58" s="262" t="inlineStr">
         <is>
           <t>Need-to-know access for AI: context-aware data protection, RAG security</t>
         </is>
       </c>
-      <c r="H58" s="8" t="inlineStr">
+      <c r="H58" s="262" t="inlineStr">
         <is>
           <t>RAG deployments; need-to-know data access</t>
         </is>
       </c>
     </row>
     <row r="59" ht="40" customHeight="1">
-      <c r="B59" s="269" t="inlineStr">
+      <c r="B59" s="262" t="inlineStr">
         <is>
           <t>AWS Bedrock Guardrails</t>
         </is>
       </c>
-      <c r="C59" s="8" t="inlineStr">
+      <c r="C59" s="262" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="D59" s="160" t="inlineStr">
+      <c r="D59" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E59" s="157" t="inlineStr">
+      <c r="E59" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F59" s="63" t="inlineStr">
+      <c r="F59" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G59" s="8" t="inlineStr">
+      <c r="G59" s="262" t="inlineStr">
         <is>
           <t>Model-agnostic guardrails: Automated Reasoning for 99% hallucination prevention</t>
         </is>
       </c>
-      <c r="H59" s="8" t="inlineStr">
+      <c r="H59" s="262" t="inlineStr">
         <is>
           <t>AWS customers; Bedrock users</t>
         </is>
       </c>
     </row>
     <row r="60" ht="40" customHeight="1">
-      <c r="B60" s="269" t="inlineStr">
+      <c r="B60" s="262" t="inlineStr">
         <is>
           <t>Google Cloud Model Armor</t>
         </is>
       </c>
-      <c r="C60" s="8" t="inlineStr">
+      <c r="C60" s="262" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="D60" s="160" t="inlineStr">
+      <c r="D60" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E60" s="157" t="inlineStr">
+      <c r="E60" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F60" s="63" t="inlineStr">
+      <c r="F60" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G60" s="8" t="inlineStr">
+      <c r="G60" s="262" t="inlineStr">
         <is>
           <t>Runtime security for any LLM: prompt injection, sensitive data, malicious URL blocking</t>
         </is>
       </c>
-      <c r="H60" s="8" t="inlineStr">
+      <c r="H60" s="262" t="inlineStr">
         <is>
           <t>GCP customers; Vertex AI users</t>
         </is>
       </c>
     </row>
     <row r="61" ht="40" customHeight="1">
-      <c r="B61" s="269" t="inlineStr">
+      <c r="B61" s="262" t="inlineStr">
         <is>
           <t>Silverfort</t>
         </is>
       </c>
-      <c r="C61" s="8" t="inlineStr">
+      <c r="C61" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D61" s="161" t="inlineStr">
+      <c r="D61" s="282" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E61" s="158" t="inlineStr">
+      <c r="E61" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F61" s="154" t="inlineStr">
+      <c r="F61" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G61" s="8" t="inlineStr">
+      <c r="G61" s="262" t="inlineStr">
         <is>
           <t>NHI leader ($222M raised, ~$1B valuation): unified human + non-human identity; NHI visibility reveals unauthorized AI service access</t>
         </is>
       </c>
-      <c r="H61" s="8" t="inlineStr">
+      <c r="H61" s="262" t="inlineStr">
         <is>
           <t>Enterprise IAM extending to NHI; MFA everywhere</t>
         </is>
       </c>
     </row>
     <row r="62" ht="40" customHeight="1">
-      <c r="B62" s="269" t="inlineStr">
+      <c r="B62" s="262" t="inlineStr">
         <is>
           <t>Astrix Security</t>
         </is>
       </c>
-      <c r="C62" s="8" t="inlineStr">
+      <c r="C62" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D62" s="161" t="inlineStr">
+      <c r="D62" s="282" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E62" s="158" t="inlineStr">
+      <c r="E62" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F62" s="154" t="inlineStr">
+      <c r="F62" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G62" s="8" t="inlineStr">
+      <c r="G62" s="262" t="inlineStr">
         <is>
           <t>Dedicated NHI platform ($85M raised): agent inventory, least-privilege; token monitoring surfaces shadow AI tools</t>
         </is>
       </c>
-      <c r="H62" s="8" t="inlineStr">
+      <c r="H62" s="262" t="inlineStr">
         <is>
           <t>NHI-first security; agentic AI deployments</t>
         </is>
       </c>
     </row>
     <row r="63" ht="40" customHeight="1">
-      <c r="B63" s="269" t="inlineStr">
+      <c r="B63" s="262" t="inlineStr">
         <is>
           <t>Oasis Security</t>
         </is>
       </c>
-      <c r="C63" s="8" t="inlineStr">
+      <c r="C63" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D63" s="161" t="inlineStr">
+      <c r="D63" s="282" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E63" s="158" t="inlineStr">
+      <c r="E63" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F63" s="154" t="inlineStr">
+      <c r="F63" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G63" s="8" t="inlineStr">
+      <c r="G63" s="262" t="inlineStr">
         <is>
           <t>NHI Security Cloud ($75M raised): Agentic Access Management; identity-based shadow AI discovery via service account monitoring</t>
         </is>
       </c>
-      <c r="H63" s="8" t="inlineStr">
+      <c r="H63" s="262" t="inlineStr">
         <is>
           <t>Agentic AI security; intent-based access control</t>
         </is>
       </c>
     </row>
     <row r="64" ht="40" customHeight="1">
-      <c r="B64" s="269" t="inlineStr">
+      <c r="B64" s="262" t="inlineStr">
         <is>
           <t>Aembit</t>
         </is>
       </c>
-      <c r="C64" s="8" t="inlineStr">
+      <c r="C64" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D64" s="161" t="inlineStr">
+      <c r="D64" s="282" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E64" s="158" t="inlineStr">
+      <c r="E64" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F64" s="160" t="inlineStr">
+      <c r="F64" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G64" s="8" t="inlineStr">
+      <c r="G64" s="262" t="inlineStr">
         <is>
           <t>Secretless workload IAM ($45M raised): workload-to-workload identity; tracks AI service connections revealing shadow AI</t>
         </is>
       </c>
-      <c r="H64" s="8" t="inlineStr">
+      <c r="H64" s="262" t="inlineStr">
         <is>
           <t>Secretless architecture; workload identity</t>
         </is>
       </c>
     </row>
     <row r="65" ht="40" customHeight="1">
-      <c r="B65" s="269" t="inlineStr">
+      <c r="B65" s="262" t="inlineStr">
         <is>
           <t>Entro Security</t>
         </is>
       </c>
-      <c r="C65" s="8" t="inlineStr">
+      <c r="C65" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D65" s="161" t="inlineStr">
+      <c r="D65" s="282" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E65" s="158" t="inlineStr">
+      <c r="E65" s="279" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F65" s="154" t="inlineStr">
+      <c r="F65" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G65" s="8" t="inlineStr">
+      <c r="G65" s="262" t="inlineStr">
         <is>
           <t>Secrets security platform: discovers and monitors exposed secrets; reveals AI API keys indicating shadow AI usage</t>
         </is>
       </c>
-      <c r="H65" s="8" t="inlineStr">
+      <c r="H65" s="262" t="inlineStr">
         <is>
           <t>Secrets sprawl; credential exposure prevention</t>
         </is>
       </c>
     </row>
     <row r="66" ht="40" customHeight="1">
-      <c r="B66" s="269" t="inlineStr">
+      <c r="B66" s="262" t="inlineStr">
         <is>
           <t>CyberArk</t>
         </is>
       </c>
-      <c r="C66" s="8" t="inlineStr">
+      <c r="C66" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D66" s="161" t="inlineStr">
+      <c r="D66" s="282" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E66" s="154" t="inlineStr">
+      <c r="E66" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F66" s="160" t="inlineStr">
+      <c r="F66" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G66" s="8" t="inlineStr">
+      <c r="G66" s="262" t="inlineStr">
         <is>
           <t>PAM leader extending to NHI: machine identity security, secrets management</t>
         </is>
       </c>
-      <c r="H66" s="8" t="inlineStr">
+      <c r="H66" s="262" t="inlineStr">
         <is>
           <t>Enterprise PAM; extending to machine identities</t>
         </is>
       </c>
     </row>
     <row r="67" ht="40" customHeight="1">
-      <c r="B67" s="269" t="inlineStr">
+      <c r="B67" s="262" t="inlineStr">
         <is>
           <t>HashiCorp Vault</t>
         </is>
       </c>
-      <c r="C67" s="8" t="inlineStr">
+      <c r="C67" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D67" s="161" t="inlineStr">
+      <c r="D67" s="282" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E67" s="160" t="inlineStr">
+      <c r="E67" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F67" s="63" t="inlineStr">
+      <c r="F67" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G67" s="8" t="inlineStr">
+      <c r="G67" s="262" t="inlineStr">
         <is>
           <t>Secrets management leader: dynamic secrets, encryption, identity-based access</t>
         </is>
       </c>
-      <c r="H67" s="8" t="inlineStr">
+      <c r="H67" s="262" t="inlineStr">
         <is>
           <t>Secrets management; dynamic credentials; DevOps</t>
         </is>
       </c>
     </row>
-    <row r="68" ht="32" customHeight="1">
-      <c r="B68" s="269" t="inlineStr">
+    <row r="68" ht="40" customHeight="1">
+      <c r="B68" s="262" t="inlineStr">
         <is>
           <t>Spec</t>
         </is>
       </c>
-      <c r="C68" s="8" t="inlineStr">
+      <c r="C68" s="262" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D68" s="161" t="inlineStr">
+      <c r="D68" s="282" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E68" s="157" t="inlineStr">
+      <c r="E68" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F68" s="154" t="inlineStr">
+      <c r="F68" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G68" s="8" t="inlineStr">
+      <c r="G68" s="262" t="inlineStr">
         <is>
           <t>Agentic security platform: agent identity, behavior monitoring, automated response</t>
         </is>
       </c>
-      <c r="H68" s="8" t="inlineStr">
+      <c r="H68" s="262" t="inlineStr">
         <is>
           <t>Organizations with production AI agents</t>
         </is>
       </c>
     </row>
-    <row r="69" ht="45" customHeight="1">
-      <c r="B69" s="269" t="inlineStr">
+    <row r="69" ht="40" customHeight="1">
+      <c r="B69" s="262" t="inlineStr">
         <is>
           <t>Sonatype</t>
         </is>
       </c>
-      <c r="C69" s="63" t="inlineStr">
+      <c r="C69" s="262" t="inlineStr">
         <is>
           <t>sonatype.com</t>
         </is>
       </c>
-      <c r="D69" s="162" t="inlineStr">
+      <c r="D69" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E69" s="154" t="inlineStr">
+      <c r="E69" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F69" s="63" t="inlineStr">
+      <c r="F69" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G69" s="8" t="inlineStr">
+      <c r="G69" s="262" t="inlineStr">
         <is>
           <t>Software supply chain leader: SBOM management, AI/ML model scanning from Hugging Face, malware detection in packages</t>
         </is>
       </c>
-      <c r="H69" s="149" t="n"/>
-    </row>
-    <row r="70" ht="45" customHeight="1">
-      <c r="B70" s="269" t="inlineStr">
+      <c r="H69" s="259" t="n"/>
+    </row>
+    <row r="70" ht="40" customHeight="1">
+      <c r="B70" s="262" t="inlineStr">
         <is>
           <t>Chainguard</t>
         </is>
       </c>
-      <c r="C70" s="63" t="inlineStr">
+      <c r="C70" s="262" t="inlineStr">
         <is>
           <t>chainguard.dev</t>
         </is>
       </c>
-      <c r="D70" s="162" t="inlineStr">
+      <c r="D70" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E70" s="160" t="inlineStr">
+      <c r="E70" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F70" s="63" t="inlineStr">
+      <c r="F70" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G70" s="8" t="inlineStr">
+      <c r="G70" s="262" t="inlineStr">
         <is>
           <t>Hardened containers and libraries: SBOM generation, SLSA provenance, secure Python packages for ML pipelines</t>
         </is>
       </c>
-      <c r="H70" s="149" t="n"/>
-    </row>
-    <row r="71" ht="45" customHeight="1">
-      <c r="B71" s="269" t="inlineStr">
+      <c r="H70" s="259" t="n"/>
+    </row>
+    <row r="71" ht="40" customHeight="1">
+      <c r="B71" s="262" t="inlineStr">
         <is>
           <t>JFrog</t>
         </is>
       </c>
-      <c r="C71" s="63" t="inlineStr">
+      <c r="C71" s="262" t="inlineStr">
         <is>
           <t>jfrog.com</t>
         </is>
       </c>
-      <c r="D71" s="162" t="inlineStr">
+      <c r="D71" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E71" s="154" t="inlineStr">
+      <c r="E71" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F71" s="63" t="inlineStr">
+      <c r="F71" s="262" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G71" s="8" t="inlineStr">
+      <c r="G71" s="262" t="inlineStr">
         <is>
           <t>Universal artifact repository: ML model management, SBOM, DevSecOps integration, supply chain security</t>
         </is>
       </c>
-      <c r="H71" s="149" t="n"/>
-    </row>
-    <row r="72" ht="45" customHeight="1">
-      <c r="B72" s="269" t="inlineStr">
+      <c r="H71" s="259" t="n"/>
+    </row>
+    <row r="72" ht="40" customHeight="1">
+      <c r="B72" s="262" t="inlineStr">
         <is>
           <t>Snyk</t>
         </is>
       </c>
-      <c r="C72" s="63" t="inlineStr">
+      <c r="C72" s="262" t="inlineStr">
         <is>
           <t>snyk.io</t>
         </is>
       </c>
-      <c r="D72" s="162" t="inlineStr">
+      <c r="D72" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E72" s="157" t="inlineStr">
+      <c r="E72" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F72" s="154" t="inlineStr">
+      <c r="F72" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G72" s="8" t="inlineStr">
+      <c r="G72" s="262" t="inlineStr">
         <is>
           <t>AI Trust Platform: AI-BOM scanning, Evo agentic security, supply chain for AI-generated code, MCP server security</t>
         </is>
       </c>
-      <c r="H72" s="149" t="n"/>
-    </row>
-    <row r="73" ht="45" customHeight="1">
-      <c r="B73" s="269" t="inlineStr">
+      <c r="H72" s="259" t="n"/>
+    </row>
+    <row r="73" ht="40" customHeight="1">
+      <c r="B73" s="262" t="inlineStr">
         <is>
           <t>Wiz</t>
         </is>
       </c>
-      <c r="C73" s="63" t="inlineStr">
+      <c r="C73" s="262" t="inlineStr">
         <is>
           <t>wiz.io</t>
         </is>
       </c>
-      <c r="D73" s="154" t="inlineStr">
+      <c r="D73" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E73" s="160" t="inlineStr">
+      <c r="E73" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F73" s="162" t="inlineStr">
+      <c r="F73" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="G73" s="8" t="inlineStr">
+      <c r="G73" s="262" t="inlineStr">
         <is>
           <t>AI-SPM leader: training data exposure, model pipeline security, DSPM for AI, attack path analysis to models</t>
         </is>
       </c>
-      <c r="H73" s="149" t="n"/>
-    </row>
-    <row r="74" ht="45" customHeight="1">
-      <c r="B74" s="269" t="inlineStr">
+      <c r="H73" s="259" t="n"/>
+    </row>
+    <row r="74" ht="40" customHeight="1">
+      <c r="B74" s="262" t="inlineStr">
         <is>
           <t>Cycode</t>
         </is>
       </c>
-      <c r="C74" s="63" t="inlineStr">
+      <c r="C74" s="262" t="inlineStr">
         <is>
           <t>cycode.com</t>
         </is>
       </c>
-      <c r="D74" s="154" t="inlineStr">
+      <c r="D74" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E74" s="162" t="inlineStr">
+      <c r="E74" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F74" s="157" t="inlineStr">
+      <c r="F74" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G74" s="8" t="inlineStr">
+      <c r="G74" s="262" t="inlineStr">
         <is>
           <t>ASPM platform: AI-native code security, Risk Intelligence Graph, pipeline security, secrets detection</t>
         </is>
       </c>
-      <c r="H74" s="149" t="n"/>
-    </row>
-    <row r="75">
+      <c r="H74" s="259" t="n"/>
+    </row>
+    <row r="75" ht="40" customHeight="1">
       <c r="B75" s="259" t="inlineStr">
         <is>
           <t>Straiker Defend AI</t>
@@ -18331,17 +18198,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D75" s="259" t="inlineStr">
+      <c r="D75" s="283" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E75" s="259" t="inlineStr">
+      <c r="E75" s="284" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F75" s="259" t="inlineStr">
+      <c r="F75" s="285" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -18357,7 +18224,7 @@
         </is>
       </c>
     </row>
-    <row r="76">
+    <row r="76" ht="40" customHeight="1">
       <c r="B76" s="259" t="inlineStr">
         <is>
           <t>Maxim AI</t>
@@ -18368,17 +18235,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D76" s="259" t="inlineStr">
+      <c r="D76" s="285" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E76" s="259" t="inlineStr">
+      <c r="E76" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F76" s="259" t="inlineStr">
+      <c r="F76" s="283" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -18394,7 +18261,7 @@
         </is>
       </c>
     </row>
-    <row r="77">
+    <row r="77" ht="40" customHeight="1">
       <c r="B77" s="259" t="inlineStr">
         <is>
           <t>Braintrust</t>
@@ -18405,12 +18272,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D77" s="259" t="inlineStr">
+      <c r="D77" s="285" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E77" s="259" t="inlineStr">
+      <c r="E77" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18431,7 +18298,7 @@
         </is>
       </c>
     </row>
-    <row r="78">
+    <row r="78" ht="40" customHeight="1">
       <c r="B78" s="259" t="inlineStr">
         <is>
           <t>LangFuse</t>
@@ -18442,12 +18309,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D78" s="259" t="inlineStr">
+      <c r="D78" s="285" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E78" s="259" t="inlineStr">
+      <c r="E78" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18468,7 +18335,7 @@
         </is>
       </c>
     </row>
-    <row r="79">
+    <row r="79" ht="40" customHeight="1">
       <c r="B79" s="259" t="inlineStr">
         <is>
           <t>Comet Opik</t>
@@ -18479,12 +18346,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D79" s="259" t="inlineStr">
+      <c r="D79" s="285" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E79" s="259" t="inlineStr">
+      <c r="E79" s="283" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -18505,7 +18372,7 @@
         </is>
       </c>
     </row>
-    <row r="80">
+    <row r="80" ht="40" customHeight="1">
       <c r="B80" s="259" t="inlineStr">
         <is>
           <t>Spectra Assure</t>
@@ -18516,17 +18383,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D80" s="259" t="inlineStr">
+      <c r="D80" s="287" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E80" s="259" t="inlineStr">
+      <c r="E80" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F80" s="259" t="inlineStr">
+      <c r="F80" s="283" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -18542,7 +18409,7 @@
         </is>
       </c>
     </row>
-    <row r="81">
+    <row r="81" ht="40" customHeight="1">
       <c r="B81" s="259" t="inlineStr">
         <is>
           <t>OpenSSF Model Signing</t>
@@ -18553,7 +18420,7 @@
           <t>Open Standard</t>
         </is>
       </c>
-      <c r="D81" s="259" t="inlineStr">
+      <c r="D81" s="287" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -18579,7 +18446,7 @@
         </is>
       </c>
     </row>
-    <row r="82">
+    <row r="82" ht="40" customHeight="1">
       <c r="B82" s="259" t="inlineStr">
         <is>
           <t>Torq</t>
@@ -18590,17 +18457,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D82" s="259" t="inlineStr">
+      <c r="D82" s="285" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E82" s="259" t="inlineStr">
+      <c r="E82" s="284" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F82" s="259" t="inlineStr">
+      <c r="F82" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18616,7 +18483,7 @@
         </is>
       </c>
     </row>
-    <row r="83">
+    <row r="83" ht="40" customHeight="1">
       <c r="B83" s="259" t="inlineStr">
         <is>
           <t>Radiant Security</t>
@@ -18627,17 +18494,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D83" s="259" t="inlineStr">
+      <c r="D83" s="285" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E83" s="259" t="inlineStr">
+      <c r="E83" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F83" s="259" t="inlineStr">
+      <c r="F83" s="283" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -18653,7 +18520,7 @@
         </is>
       </c>
     </row>
-    <row r="84">
+    <row r="84" ht="40" customHeight="1">
       <c r="B84" s="259" t="inlineStr">
         <is>
           <t>Stellar Cyber</t>
@@ -18664,17 +18531,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D84" s="259" t="inlineStr">
+      <c r="D84" s="285" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E84" s="259" t="inlineStr">
+      <c r="E84" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F84" s="259" t="inlineStr">
+      <c r="F84" s="288" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
@@ -18690,7 +18557,7 @@
         </is>
       </c>
     </row>
-    <row r="85">
+    <row r="85" ht="40" customHeight="1">
       <c r="B85" s="259" t="inlineStr">
         <is>
           <t>Strata Identity</t>
@@ -18701,12 +18568,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D85" s="259" t="inlineStr">
+      <c r="D85" s="284" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E85" s="259" t="inlineStr">
+      <c r="E85" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18727,7 +18594,7 @@
         </is>
       </c>
     </row>
-    <row r="86">
+    <row r="86" ht="40" customHeight="1">
       <c r="B86" s="259" t="inlineStr">
         <is>
           <t>NVIDIA NeMo Guardrails</t>
@@ -18738,12 +18605,12 @@
           <t>Platform</t>
         </is>
       </c>
-      <c r="D86" s="259" t="inlineStr">
+      <c r="D86" s="283" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E86" s="259" t="inlineStr">
+      <c r="E86" s="285" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -18764,7 +18631,7 @@
         </is>
       </c>
     </row>
-    <row r="87">
+    <row r="87" ht="40" customHeight="1">
       <c r="B87" s="259" t="inlineStr">
         <is>
           <t>Holistic AI</t>
@@ -18775,12 +18642,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D87" s="259" t="inlineStr">
+      <c r="D87" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E87" s="259" t="inlineStr">
+      <c r="E87" s="285" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -18801,7 +18668,7 @@
         </is>
       </c>
     </row>
-    <row r="88">
+    <row r="88" ht="40" customHeight="1">
       <c r="B88" s="259" t="inlineStr">
         <is>
           <t>Airia</t>
@@ -18812,17 +18679,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D88" s="259" t="inlineStr">
+      <c r="D88" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E88" s="259" t="inlineStr">
+      <c r="E88" s="284" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F88" s="259" t="inlineStr">
+      <c r="F88" s="283" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -18838,7 +18705,7 @@
         </is>
       </c>
     </row>
-    <row r="89">
+    <row r="89" ht="40" customHeight="1">
       <c r="B89" s="259" t="inlineStr">
         <is>
           <t>Adri</t>
@@ -18849,17 +18716,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D89" s="259" t="inlineStr">
+      <c r="D89" s="288" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E89" s="259" t="inlineStr">
+      <c r="E89" s="289" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F89" s="259" t="inlineStr">
+      <c r="F89" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18875,7 +18742,7 @@
         </is>
       </c>
     </row>
-    <row r="90">
+    <row r="90" ht="40" customHeight="1">
       <c r="B90" s="259" t="inlineStr">
         <is>
           <t>Prophet Security</t>
@@ -18886,12 +18753,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D90" s="259" t="inlineStr">
+      <c r="D90" s="285" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E90" s="259" t="inlineStr">
+      <c r="E90" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18912,7 +18779,7 @@
         </is>
       </c>
     </row>
-    <row r="91">
+    <row r="91" ht="40" customHeight="1">
       <c r="B91" s="259" t="inlineStr">
         <is>
           <t>Hex Security</t>
@@ -18923,12 +18790,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D91" s="259" t="inlineStr">
+      <c r="D91" s="283" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E91" s="259" t="inlineStr">
+      <c r="E91" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>

</xml_diff>

<commit_message>
Fix Tool Landscape vendor data and complete formatting cleanup
- Fix corrupted vendor rows (Cycode, Chainguard, JFrog, Snyk, Sonatype)
  - Restore proper Status values (were showing website URLs)
  - Add missing Best For descriptions
  - Complete Exec Summary content
- Remove duplicate Wiz entry (row 31)
- Fix Tool Function Mapping SEVERE row colors (rows 56-60)
  - Change from transparent (00) to solid (FF) color prefix
- Verify all 74 vendors have complete data

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/AI_Security_Risk_Draft1.xlsx
+++ b/AI_Security_Risk_Draft1.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="49">
+  <fonts count="54">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -330,8 +330,32 @@
       <i val="1"/>
       <sz val="10"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <color rgb="009C0006"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
-  <fills count="54">
+  <fills count="62">
     <fill>
       <patternFill/>
     </fill>
@@ -623,6 +647,54 @@
         <bgColor rgb="00D6DCE4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9C0006"/>
+        <bgColor rgb="FF9C0006"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2E75B6"/>
+        <bgColor rgb="FF2E75B6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD6DCE4"/>
+        <bgColor rgb="FFD6DCE4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CBAD"/>
+        <bgColor rgb="FFF8CBAD"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -744,7 +816,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6"/>
   </cellStyleXfs>
-  <cellXfs count="307">
+  <cellXfs count="326">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1550,6 +1622,59 @@
     <xf numFmtId="0" fontId="43" fillId="50" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="54" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="42" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="55" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="55" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="56" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="57" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="58" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="59" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="59" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="56" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="54" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="60" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="30" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="61" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="54" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="54" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="54" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="52" fillId="55" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="55" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10019,7 +10144,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F69"/>
+  <dimension ref="B2:H67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="20" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
@@ -11143,7 +11268,7 @@
           <t>MCP Server Integration</t>
         </is>
       </c>
-      <c r="C54" s="306" t="inlineStr">
+      <c r="C54" s="307" t="inlineStr">
         <is>
           <t>High</t>
         </is>
@@ -11191,37 +11316,39 @@
         </is>
       </c>
     </row>
-    <row r="56" ht="24" customHeight="1">
-      <c r="B56" s="8" t="inlineStr">
+    <row r="56" ht="35" customHeight="1">
+      <c r="B56" s="321" t="inlineStr">
         <is>
           <t>Human-in-the-loop approval workflows</t>
         </is>
       </c>
-      <c r="C56" s="13" t="inlineStr">
+      <c r="C56" s="322" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D56" s="8" t="inlineStr">
-        <is>
-          <t>Enforce approval gates; log bypass attempts; audit trail for decisions</t>
-        </is>
-      </c>
-      <c r="E56" s="8" t="inlineStr">
+      <c r="D56" s="322" t="inlineStr">
+        <is>
+          <t>Enforce approval gates; log bypass attempts; escalation procedures</t>
+        </is>
+      </c>
+      <c r="E56" s="322" t="inlineStr">
         <is>
           <t>ServiceNow, Noma, Zenity</t>
         </is>
       </c>
-      <c r="F56" s="8" t="inlineStr">
+      <c r="F56" s="322" t="inlineStr">
         <is>
           <t>AI Posture, NHI</t>
         </is>
       </c>
-    </row>
-    <row r="57" ht="40" customHeight="1">
-      <c r="B57" s="258" t="inlineStr">
-        <is>
-          <t>SEVERE RISK — CISO/executive approval; comprehensive controls required</t>
+      <c r="G56" s="323" t="n"/>
+      <c r="H56" s="323" t="n"/>
+    </row>
+    <row r="57" ht="20" customHeight="1">
+      <c r="B57" s="308" t="inlineStr">
+        <is>
+          <t>SEVERE RISK — CISO/executive approval; continuous monitoring required</t>
         </is>
       </c>
       <c r="C57" s="251" t="n"/>
@@ -11229,283 +11356,286 @@
       <c r="E57" s="251" t="n"/>
       <c r="F57" s="26" t="n"/>
     </row>
-    <row r="58" ht="40" customHeight="1">
-      <c r="B58" s="8" t="inlineStr">
+    <row r="58" ht="35" customHeight="1">
+      <c r="B58" s="324" t="inlineStr">
         <is>
           <t>Autonomous web browsing</t>
         </is>
       </c>
-      <c r="C58" s="14" t="inlineStr">
+      <c r="C58" s="324" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D58" s="8" t="inlineStr">
+      <c r="D58" s="324" t="inlineStr">
         <is>
           <t>Requires formal security exception; high risk of unauthorized data collection</t>
         </is>
       </c>
-      <c r="E58" s="8" t="inlineStr">
+      <c r="E58" s="324" t="inlineStr">
         <is>
           <t>Full stack required + formal review</t>
         </is>
       </c>
-      <c r="F58" s="8" t="inlineStr">
+      <c r="F58" s="324" t="inlineStr">
         <is>
           <t>All 7 families</t>
         </is>
       </c>
-    </row>
-    <row r="59" ht="40" customHeight="1">
-      <c r="B59" s="8" t="inlineStr">
+      <c r="G58" s="325" t="n"/>
+      <c r="H58" s="325" t="n"/>
+    </row>
+    <row r="59" ht="35" customHeight="1">
+      <c r="B59" s="324" t="inlineStr">
         <is>
           <t>Log analysis containing PII/sensitive data</t>
         </is>
       </c>
-      <c r="C59" s="14" t="inlineStr">
+      <c r="C59" s="324" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D59" s="8" t="inlineStr">
+      <c r="D59" s="324" t="inlineStr">
         <is>
           <t>Subject to security review; sensitive data must be masked or redacted</t>
         </is>
       </c>
-      <c r="E59" s="8" t="inlineStr">
+      <c r="E59" s="324" t="inlineStr">
         <is>
           <t>Cyera + Datadog + security review</t>
         </is>
       </c>
-      <c r="F59" s="8" t="inlineStr">
+      <c r="F59" s="324" t="inlineStr">
         <is>
           <t>Data Protection, Observability</t>
         </is>
       </c>
-    </row>
-    <row r="60" ht="40" customHeight="1">
-      <c r="B60" s="8" t="inlineStr">
+      <c r="G59" s="325" t="n"/>
+      <c r="H59" s="325" t="n"/>
+    </row>
+    <row r="60" ht="35" customHeight="1">
+      <c r="B60" s="324" t="inlineStr">
         <is>
           <t>Privileged system automation</t>
         </is>
       </c>
-      <c r="C60" s="14" t="inlineStr">
+      <c r="C60" s="324" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D60" s="8" t="inlineStr">
+      <c r="D60" s="324" t="inlineStr">
         <is>
           <t>Prohibited by default; formal security approval and documented risk mitigation required</t>
         </is>
       </c>
-      <c r="E60" s="8" t="inlineStr">
+      <c r="E60" s="324" t="inlineStr">
         <is>
           <t>Silverfort, Astrix, Oasis + full stack</t>
         </is>
       </c>
-      <c r="F60" s="8" t="inlineStr">
+      <c r="F60" s="324" t="inlineStr">
         <is>
           <t>NHI, AI Posture</t>
         </is>
       </c>
-    </row>
-    <row r="61" ht="40" customHeight="1">
-      <c r="B61" s="8" t="inlineStr">
+      <c r="G60" s="325" t="n"/>
+      <c r="H60" s="325" t="n"/>
+    </row>
+    <row r="61" ht="35" customHeight="1">
+      <c r="B61" s="262" t="inlineStr">
         <is>
           <t>Unrestricted code execution</t>
         </is>
       </c>
-      <c r="C61" s="14" t="inlineStr">
+      <c r="C61" s="309" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D61" s="8" t="inlineStr">
+      <c r="D61" s="262" t="inlineStr">
         <is>
           <t>Blocked by default; tool authorization, sandbox isolation, audit logging, strict containment strategies</t>
         </is>
       </c>
-      <c r="E61" s="8" t="inlineStr">
+      <c r="E61" s="262" t="inlineStr">
         <is>
           <t>Full stack + Zenity, Straiker, Spec</t>
         </is>
       </c>
-      <c r="F61" s="8" t="inlineStr">
+      <c r="F61" s="262" t="inlineStr">
         <is>
           <t>All 7 families</t>
         </is>
       </c>
     </row>
-    <row r="62" ht="40" customHeight="1">
-      <c r="B62" s="8" t="inlineStr">
+    <row r="62" ht="35" customHeight="1">
+      <c r="B62" s="262" t="inlineStr">
         <is>
           <t>Model fine-tuning with production data</t>
         </is>
       </c>
-      <c r="C62" s="14" t="inlineStr">
+      <c r="C62" s="309" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D62" s="8" t="inlineStr">
+      <c r="D62" s="262" t="inlineStr">
         <is>
           <t>Data governance review required; IP protection; formal approval with time limit</t>
         </is>
       </c>
-      <c r="E62" s="8" t="inlineStr">
+      <c r="E62" s="262" t="inlineStr">
         <is>
           <t>Noma, HiddenLayer, Cyera, BigID</t>
         </is>
       </c>
-      <c r="F62" s="8" t="inlineStr">
+      <c r="F62" s="262" t="inlineStr">
         <is>
           <t>AI Supply Chain, Data Protection</t>
         </is>
       </c>
     </row>
-    <row r="63" ht="40" customHeight="1">
-      <c r="B63" s="8" t="inlineStr">
+    <row r="63" ht="35" customHeight="1">
+      <c r="B63" s="262" t="inlineStr">
         <is>
           <t>Infrastructure automation (Terraform, K8s)</t>
         </is>
       </c>
-      <c r="C63" s="14" t="inlineStr">
+      <c r="C63" s="309" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D63" s="8" t="inlineStr">
+      <c r="D63" s="262" t="inlineStr">
         <is>
           <t>Prohibited by default; requires full security review; admin rights must be scoped</t>
         </is>
       </c>
-      <c r="E63" s="8" t="inlineStr">
+      <c r="E63" s="262" t="inlineStr">
         <is>
           <t>Silverfort, Astrix + full review</t>
         </is>
       </c>
-      <c r="F63" s="8" t="inlineStr">
+      <c r="F63" s="262" t="inlineStr">
         <is>
           <t>NHI, AI Posture</t>
         </is>
       </c>
     </row>
-    <row r="64" ht="40" customHeight="1">
-      <c r="B64" s="8" t="inlineStr">
+    <row r="64" ht="35" customHeight="1">
+      <c r="B64" s="262" t="inlineStr">
         <is>
           <t>Autonomous agent with unrestricted API access</t>
         </is>
       </c>
-      <c r="C64" s="14" t="inlineStr">
+      <c r="C64" s="309" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D64" s="8" t="inlineStr">
+      <c r="D64" s="262" t="inlineStr">
         <is>
           <t>Prohibited by default; formal exception with strict monitoring and kill switch</t>
         </is>
       </c>
-      <c r="E64" s="8" t="inlineStr">
+      <c r="E64" s="262" t="inlineStr">
         <is>
           <t>Full stack + continuous monitoring</t>
         </is>
       </c>
-      <c r="F64" s="8" t="inlineStr">
+      <c r="F64" s="262" t="inlineStr">
         <is>
           <t>All 7 families</t>
         </is>
       </c>
     </row>
-    <row r="65" ht="40" customHeight="1">
-      <c r="B65" s="8" t="inlineStr">
+    <row r="65" ht="35" customHeight="1">
+      <c r="B65" s="262" t="inlineStr">
         <is>
           <t>Multi-agent orchestration (autonomous)</t>
         </is>
       </c>
-      <c r="C65" s="14" t="inlineStr">
+      <c r="C65" s="309" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D65" s="8" t="inlineStr">
+      <c r="D65" s="262" t="inlineStr">
         <is>
           <t>Prohibited by default; requires agent inventory, boundary controls, tool authorization, autonomous action limits, kill switches</t>
         </is>
       </c>
-      <c r="E65" s="8" t="inlineStr">
+      <c r="E65" s="262" t="inlineStr">
         <is>
           <t>Zenity, Oasis, Astrix, Straiker, Invariant Labs</t>
         </is>
       </c>
-      <c r="F65" s="8" t="inlineStr">
+      <c r="F65" s="262" t="inlineStr">
         <is>
           <t>NHI, AI Posture</t>
         </is>
       </c>
     </row>
-    <row r="66" ht="40" customHeight="1">
-      <c r="B66" s="8" t="inlineStr">
+    <row r="66" ht="35" customHeight="1">
+      <c r="B66" s="262" t="inlineStr">
         <is>
           <t>Agent task delegation / spawning</t>
         </is>
       </c>
-      <c r="C66" s="14" t="inlineStr">
+      <c r="C66" s="309" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D66" s="8" t="inlineStr">
+      <c r="D66" s="262" t="inlineStr">
         <is>
           <t>Prohibited by default; limit spawn depth; enforce resource quotas; audit lineage</t>
         </is>
       </c>
-      <c r="E66" s="8" t="inlineStr">
+      <c r="E66" s="262" t="inlineStr">
         <is>
           <t>Zenity, Noma, Oasis Security</t>
         </is>
       </c>
-      <c r="F66" s="8" t="inlineStr">
+      <c r="F66" s="262" t="inlineStr">
         <is>
           <t>NHI, AI Posture</t>
         </is>
       </c>
     </row>
-    <row r="67">
-      <c r="B67" s="8" t="inlineStr">
+    <row r="67" ht="35" customHeight="1">
+      <c r="B67" s="262" t="inlineStr">
         <is>
           <t>Autonomous decision-making (no human review)</t>
         </is>
       </c>
-      <c r="C67" s="14" t="inlineStr">
+      <c r="C67" s="309" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D67" s="8" t="inlineStr">
+      <c r="D67" s="262" t="inlineStr">
         <is>
           <t>Prohibited for consequential decisions; requires formal exception and audit trail</t>
         </is>
       </c>
-      <c r="E67" s="8" t="inlineStr">
+      <c r="E67" s="262" t="inlineStr">
         <is>
           <t>Full stack + mandatory logging</t>
         </is>
       </c>
-      <c r="F67" s="8" t="inlineStr">
+      <c r="F67" s="262" t="inlineStr">
         <is>
           <t>All 7 families</t>
         </is>
       </c>
     </row>
-    <row r="68"/>
-    <row r="69"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B27:F27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15118,7 +15248,7 @@
       </c>
     </row>
     <row r="8" ht="25" customHeight="1">
-      <c r="B8" s="296" t="inlineStr">
+      <c r="B8" s="310" t="inlineStr">
         <is>
           <t>Severe Tool</t>
         </is>
@@ -15145,7 +15275,7 @@
       </c>
     </row>
     <row r="9" ht="25" customHeight="1">
-      <c r="B9" s="297" t="inlineStr">
+      <c r="B9" s="311" t="inlineStr">
         <is>
           <t>Guardrail Bypass</t>
         </is>
@@ -15172,7 +15302,7 @@
       </c>
     </row>
     <row r="10" ht="25" customHeight="1">
-      <c r="B10" s="298" t="inlineStr">
+      <c r="B10" s="312" t="inlineStr">
         <is>
           <t>Vendor Risk</t>
         </is>
@@ -15199,7 +15329,7 @@
       </c>
     </row>
     <row r="11" ht="25" customHeight="1">
-      <c r="B11" s="299" t="inlineStr">
+      <c r="B11" s="313" t="inlineStr">
         <is>
           <t>Compliance Gap</t>
         </is>
@@ -15226,7 +15356,7 @@
       </c>
     </row>
     <row r="12" ht="25" customHeight="1">
-      <c r="B12" s="300" t="inlineStr">
+      <c r="B12" s="314" t="inlineStr">
         <is>
           <t>Emergency Use</t>
         </is>
@@ -15271,7 +15401,7 @@
       <c r="F14" s="149" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="301" t="inlineStr">
+      <c r="B15" s="315" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -15286,7 +15416,7 @@
       <c r="F15" s="149" t="n"/>
     </row>
     <row r="16">
-      <c r="B16" s="302" t="inlineStr">
+      <c r="B16" s="316" t="inlineStr">
         <is>
           <t>Renewal Due</t>
         </is>
@@ -15301,7 +15431,7 @@
       <c r="F16" s="149" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="303" t="inlineStr">
+      <c r="B17" s="317" t="inlineStr">
         <is>
           <t>Expired</t>
         </is>
@@ -15316,7 +15446,7 @@
       <c r="F17" s="149" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="304" t="inlineStr">
+      <c r="B18" s="318" t="inlineStr">
         <is>
           <t>Closed</t>
         </is>
@@ -15420,7 +15550,7 @@
           <t>Autonomous Agent X</t>
         </is>
       </c>
-      <c r="D24" s="296" t="inlineStr">
+      <c r="D24" s="310" t="inlineStr">
         <is>
           <t>Severe Tool</t>
         </is>
@@ -15492,7 +15622,7 @@
           <t>Custom ML Pipeline</t>
         </is>
       </c>
-      <c r="D25" s="297" t="inlineStr">
+      <c r="D25" s="311" t="inlineStr">
         <is>
           <t>Guardrail Bypass</t>
         </is>
@@ -15564,7 +15694,7 @@
           <t>Vendor AI Tool Y</t>
         </is>
       </c>
-      <c r="D26" s="298" t="inlineStr">
+      <c r="D26" s="312" t="inlineStr">
         <is>
           <t>Vendor Risk</t>
         </is>
@@ -15636,7 +15766,7 @@
           <t>Emergency Chatbot</t>
         </is>
       </c>
-      <c r="D27" s="300" t="inlineStr">
+      <c r="D27" s="314" t="inlineStr">
         <is>
           <t>Emergency Use</t>
         </is>
@@ -16012,7 +16142,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H158"/>
+  <dimension ref="B2:H157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
@@ -16454,37 +16584,41 @@
       </c>
     </row>
     <row r="23" ht="40" customHeight="1">
-      <c r="B23" s="262" t="inlineStr">
+      <c r="B23" s="319" t="inlineStr">
         <is>
           <t>Cycode</t>
         </is>
       </c>
-      <c r="C23" s="262" t="inlineStr">
-        <is>
-          <t>cycode.com</t>
-        </is>
-      </c>
-      <c r="D23" s="276" t="inlineStr">
+      <c r="C23" s="319" t="inlineStr">
+        <is>
+          <t>Independent</t>
+        </is>
+      </c>
+      <c r="D23" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E23" s="277" t="inlineStr">
+      <c r="E23" s="319" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F23" s="280" t="inlineStr">
+      <c r="F23" s="319" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G23" s="262" t="inlineStr">
-        <is>
-          <t>ASPM platform: AI-native code security, Risk Intelligence Graph, pipeline security, secrets detection</t>
-        </is>
-      </c>
-      <c r="H23" s="262" t="n"/>
+      <c r="G23" s="319" t="inlineStr">
+        <is>
+          <t>ASPM platform with AI-native code security: Risk Intelligence Graph correlates code risks, pipeline security, secrets detection, AI code scanner</t>
+        </is>
+      </c>
+      <c r="H23" s="319" t="inlineStr">
+        <is>
+          <t>Code-to-cloud security; ASPM consolidation; pipeline protection</t>
+        </is>
+      </c>
     </row>
     <row r="24" ht="40" customHeight="1">
       <c r="B24" s="262" t="inlineStr">
@@ -16748,12 +16882,12 @@
     <row r="31" ht="40" customHeight="1">
       <c r="B31" s="262" t="inlineStr">
         <is>
-          <t>Wiz</t>
+          <t>Zenity</t>
         </is>
       </c>
       <c r="C31" s="262" t="inlineStr">
         <is>
-          <t>wiz.io</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D31" s="276" t="inlineStr">
@@ -16761,27 +16895,31 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E31" s="281" t="inlineStr">
-        <is>
-          <t>Data Protection for AI</t>
-        </is>
-      </c>
-      <c r="F31" s="277" t="inlineStr">
-        <is>
-          <t>AI Supply Chain</t>
+      <c r="E31" s="282" t="inlineStr">
+        <is>
+          <t>NHI &amp; Agentic Access</t>
+        </is>
+      </c>
+      <c r="F31" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="G31" s="262" t="inlineStr">
         <is>
-          <t>AI-SPM leader: training data exposure, model pipeline security, DSPM for AI, attack path analysis to models</t>
-        </is>
-      </c>
-      <c r="H31" s="262" t="n"/>
+          <t>Agent-centric posture management; low-code/copilot security specialist</t>
+        </is>
+      </c>
+      <c r="H31" s="262" t="inlineStr">
+        <is>
+          <t>Organizations deploying AI agents at scale</t>
+        </is>
+      </c>
     </row>
     <row r="32" ht="40" customHeight="1">
       <c r="B32" s="262" t="inlineStr">
         <is>
-          <t>Zenity</t>
+          <t>Arthur AI</t>
         </is>
       </c>
       <c r="C32" s="262" t="inlineStr">
@@ -16789,41 +16927,41 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D32" s="276" t="inlineStr">
+      <c r="D32" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
+        </is>
+      </c>
+      <c r="E32" s="278" t="inlineStr">
+        <is>
+          <t>Observability &amp; Evaluation</t>
+        </is>
+      </c>
+      <c r="F32" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E32" s="282" t="inlineStr">
-        <is>
-          <t>NHI &amp; Agentic Access</t>
-        </is>
-      </c>
-      <c r="F32" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
       <c r="G32" s="262" t="inlineStr">
         <is>
-          <t>Agent-centric posture management; low-code/copilot security specialist</t>
+          <t>LLM firewall + observability ($60M raised): federated architecture, data stays local</t>
         </is>
       </c>
       <c r="H32" s="262" t="inlineStr">
         <is>
-          <t>Organizations deploying AI agents at scale</t>
+          <t>Regulated industries; data residency requirements</t>
         </is>
       </c>
     </row>
     <row r="33" ht="40" customHeight="1">
       <c r="B33" s="262" t="inlineStr">
         <is>
-          <t>Arthur AI</t>
+          <t>Check Point (Lakera)</t>
         </is>
       </c>
       <c r="C33" s="262" t="inlineStr">
         <is>
-          <t>Independent</t>
+          <t>Acquired</t>
         </is>
       </c>
       <c r="D33" s="280" t="inlineStr">
@@ -16831,31 +16969,31 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E33" s="278" t="inlineStr">
-        <is>
-          <t>Observability &amp; Evaluation</t>
-        </is>
-      </c>
-      <c r="F33" s="276" t="inlineStr">
+      <c r="E33" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
+      <c r="F33" s="277" t="inlineStr">
+        <is>
+          <t>AI Supply Chain</t>
+        </is>
+      </c>
       <c r="G33" s="262" t="inlineStr">
         <is>
-          <t>LLM firewall + observability ($60M raised): federated architecture, data stays local</t>
+          <t>Lakera adds runtime guardrails, prompt injection defense, model security to Infinity</t>
         </is>
       </c>
       <c r="H33" s="262" t="inlineStr">
         <is>
-          <t>Regulated industries; data residency requirements</t>
+          <t>Check Point customers; Infinity stack users</t>
         </is>
       </c>
     </row>
     <row r="34" ht="40" customHeight="1">
       <c r="B34" s="262" t="inlineStr">
         <is>
-          <t>Check Point (Lakera)</t>
+          <t>F5 (CalypsoAI)</t>
         </is>
       </c>
       <c r="C34" s="262" t="inlineStr">
@@ -16868,9 +17006,9 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E34" s="276" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
+      <c r="E34" s="278" t="inlineStr">
+        <is>
+          <t>Observability &amp; Evaluation</t>
         </is>
       </c>
       <c r="F34" s="277" t="inlineStr">
@@ -16880,24 +17018,24 @@
       </c>
       <c r="G34" s="262" t="inlineStr">
         <is>
-          <t>Lakera adds runtime guardrails, prompt injection defense, model security to Infinity</t>
+          <t>Inference protection + red-teaming via CalypsoAI; model testing, API security</t>
         </is>
       </c>
       <c r="H34" s="262" t="inlineStr">
         <is>
-          <t>Check Point customers; Infinity stack users</t>
+          <t>F5 customers; API/app security integration</t>
         </is>
       </c>
     </row>
     <row r="35" ht="40" customHeight="1">
       <c r="B35" s="262" t="inlineStr">
         <is>
-          <t>F5 (CalypsoAI)</t>
+          <t>Hex Security</t>
         </is>
       </c>
       <c r="C35" s="262" t="inlineStr">
         <is>
-          <t>Acquired</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D35" s="280" t="inlineStr">
@@ -16905,31 +17043,31 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E35" s="278" t="inlineStr">
-        <is>
-          <t>Observability &amp; Evaluation</t>
-        </is>
-      </c>
-      <c r="F35" s="277" t="inlineStr">
-        <is>
-          <t>AI Supply Chain</t>
+      <c r="E35" s="276" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
+        </is>
+      </c>
+      <c r="F35" s="262" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
       <c r="G35" s="262" t="inlineStr">
         <is>
-          <t>Inference protection + red-teaming via CalypsoAI; model testing, API security</t>
+          <t>Y Combinator-backed: AI agents running continuous pen tests; 24/7 vulnerability discovery and verification.</t>
         </is>
       </c>
       <c r="H35" s="262" t="inlineStr">
         <is>
-          <t>F5 customers; API/app security integration</t>
+          <t>Continuous security testing; red team automation</t>
         </is>
       </c>
     </row>
     <row r="36" ht="40" customHeight="1">
       <c r="B36" s="262" t="inlineStr">
         <is>
-          <t>Hex Security</t>
+          <t>Invariant Labs</t>
         </is>
       </c>
       <c r="C36" s="262" t="inlineStr">
@@ -16942,31 +17080,31 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E36" s="276" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
-        </is>
-      </c>
-      <c r="F36" s="262" t="inlineStr">
-        <is>
-          <t>—</t>
+      <c r="E36" s="282" t="inlineStr">
+        <is>
+          <t>NHI &amp; Agentic Access</t>
+        </is>
+      </c>
+      <c r="F36" s="278" t="inlineStr">
+        <is>
+          <t>Observability &amp; Evaluation</t>
         </is>
       </c>
       <c r="G36" s="262" t="inlineStr">
         <is>
-          <t>Y Combinator-backed: AI agents running continuous pen tests; 24/7 vulnerability discovery and verification.</t>
+          <t>Agent security testing and guardrails; detects agent vulnerabilities and failures</t>
         </is>
       </c>
       <c r="H36" s="262" t="inlineStr">
         <is>
-          <t>Continuous security testing; red team automation</t>
+          <t>Agentic AI security testing; agent-specific threats</t>
         </is>
       </c>
     </row>
     <row r="37" ht="40" customHeight="1">
       <c r="B37" s="262" t="inlineStr">
         <is>
-          <t>Invariant Labs</t>
+          <t>LLM Guard</t>
         </is>
       </c>
       <c r="C37" s="262" t="inlineStr">
@@ -16979,31 +17117,31 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E37" s="282" t="inlineStr">
-        <is>
-          <t>NHI &amp; Agentic Access</t>
-        </is>
-      </c>
-      <c r="F37" s="278" t="inlineStr">
-        <is>
-          <t>Observability &amp; Evaluation</t>
+      <c r="E37" s="281" t="inlineStr">
+        <is>
+          <t>Data Protection for AI</t>
+        </is>
+      </c>
+      <c r="F37" s="262" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
       <c r="G37" s="262" t="inlineStr">
         <is>
-          <t>Agent security testing and guardrails; detects agent vulnerabilities and failures</t>
+          <t>Open source input/output scanner; PII detection, toxicity, prompt injection</t>
         </is>
       </c>
       <c r="H37" s="262" t="inlineStr">
         <is>
-          <t>Agentic AI security testing; agent-specific threats</t>
+          <t>OSS-first orgs; customizable guardrails</t>
         </is>
       </c>
     </row>
     <row r="38" ht="40" customHeight="1">
       <c r="B38" s="262" t="inlineStr">
         <is>
-          <t>LLM Guard</t>
+          <t>Mindgard</t>
         </is>
       </c>
       <c r="C38" s="262" t="inlineStr">
@@ -17016,36 +17154,36 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E38" s="281" t="inlineStr">
-        <is>
-          <t>Data Protection for AI</t>
-        </is>
-      </c>
-      <c r="F38" s="262" t="inlineStr">
-        <is>
-          <t>—</t>
+      <c r="E38" s="278" t="inlineStr">
+        <is>
+          <t>Observability &amp; Evaluation</t>
+        </is>
+      </c>
+      <c r="F38" s="277" t="inlineStr">
+        <is>
+          <t>AI Supply Chain</t>
         </is>
       </c>
       <c r="G38" s="262" t="inlineStr">
         <is>
-          <t>Open source input/output scanner; PII detection, toxicity, prompt injection</t>
+          <t>Offensive AI security: automated red teaming, model vulnerability scanning, supply chain testing</t>
         </is>
       </c>
       <c r="H38" s="262" t="inlineStr">
         <is>
-          <t>OSS-first orgs; customizable guardrails</t>
+          <t>Continuous AI security testing; red team automation</t>
         </is>
       </c>
     </row>
     <row r="39" ht="40" customHeight="1">
       <c r="B39" s="262" t="inlineStr">
         <is>
-          <t>Mindgard</t>
+          <t>NVIDIA NeMo Guardrails</t>
         </is>
       </c>
       <c r="C39" s="262" t="inlineStr">
         <is>
-          <t>Independent</t>
+          <t>Platform</t>
         </is>
       </c>
       <c r="D39" s="280" t="inlineStr">
@@ -17058,31 +17196,31 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F39" s="277" t="inlineStr">
-        <is>
-          <t>AI Supply Chain</t>
+      <c r="F39" s="262" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
       <c r="G39" s="262" t="inlineStr">
         <is>
-          <t>Offensive AI security: automated red teaming, model vulnerability scanning, supply chain testing</t>
+          <t>Inference microservices (GA Jan 2025): programmable guardrails for LLMs; safety, security, control for AI applications.</t>
         </is>
       </c>
       <c r="H39" s="262" t="inlineStr">
         <is>
-          <t>Continuous AI security testing; red team automation</t>
+          <t>NVIDIA ecosystem; custom guardrail logic</t>
         </is>
       </c>
     </row>
     <row r="40" ht="40" customHeight="1">
       <c r="B40" s="262" t="inlineStr">
         <is>
-          <t>NVIDIA NeMo Guardrails</t>
+          <t>Prompt Armor</t>
         </is>
       </c>
       <c r="C40" s="262" t="inlineStr">
         <is>
-          <t>Platform</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D40" s="280" t="inlineStr">
@@ -17090,31 +17228,31 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E40" s="278" t="inlineStr">
+      <c r="E40" s="281" t="inlineStr">
+        <is>
+          <t>Data Protection for AI</t>
+        </is>
+      </c>
+      <c r="F40" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F40" s="262" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
       <c r="G40" s="262" t="inlineStr">
         <is>
-          <t>Inference microservices (GA Jan 2025): programmable guardrails for LLMs; safety, security, control for AI applications.</t>
+          <t>Prompt injection firewall; real-time threat detection for LLM applications</t>
         </is>
       </c>
       <c r="H40" s="262" t="inlineStr">
         <is>
-          <t>NVIDIA ecosystem; custom guardrail logic</t>
+          <t>Dedicated prompt security; API-first deployment</t>
         </is>
       </c>
     </row>
     <row r="41" ht="40" customHeight="1">
       <c r="B41" s="262" t="inlineStr">
         <is>
-          <t>Prompt Armor</t>
+          <t>Rebuff AI</t>
         </is>
       </c>
       <c r="C41" s="262" t="inlineStr">
@@ -17127,31 +17265,31 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E41" s="281" t="inlineStr">
-        <is>
-          <t>Data Protection for AI</t>
-        </is>
-      </c>
-      <c r="F41" s="278" t="inlineStr">
+      <c r="E41" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
+      <c r="F41" s="262" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="G41" s="262" t="inlineStr">
         <is>
-          <t>Prompt injection firewall; real-time threat detection for LLM applications</t>
+          <t>Open source prompt injection detection; self-hardening through attack learning</t>
         </is>
       </c>
       <c r="H41" s="262" t="inlineStr">
         <is>
-          <t>Dedicated prompt security; API-first deployment</t>
+          <t>Teams wanting OSS guardrails; cost-conscious</t>
         </is>
       </c>
     </row>
     <row r="42" ht="40" customHeight="1">
       <c r="B42" s="262" t="inlineStr">
         <is>
-          <t>Rebuff AI</t>
+          <t>Straiker Defend AI</t>
         </is>
       </c>
       <c r="C42" s="262" t="inlineStr">
@@ -17164,31 +17302,31 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E42" s="278" t="inlineStr">
+      <c r="E42" s="282" t="inlineStr">
+        <is>
+          <t>NHI &amp; Agentic Access</t>
+        </is>
+      </c>
+      <c r="F42" s="278" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F42" s="262" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
       <c r="G42" s="262" t="inlineStr">
         <is>
-          <t>Open source prompt injection detection; self-hardening through attack learning</t>
+          <t>Agentic AI runtime security ($21M Series A, Lightspeed): fast context-aware guardrails; inspects prompts, reasoning steps, tool calls; stops prompt injection, data leaks, agent manipulation.</t>
         </is>
       </c>
       <c r="H42" s="262" t="inlineStr">
         <is>
-          <t>Teams wanting OSS guardrails; cost-conscious</t>
+          <t>Production agentic AI; real-time agent security</t>
         </is>
       </c>
     </row>
     <row r="43" ht="40" customHeight="1">
       <c r="B43" s="262" t="inlineStr">
         <is>
-          <t>Straiker Defend AI</t>
+          <t>TrojAI</t>
         </is>
       </c>
       <c r="C43" s="262" t="inlineStr">
@@ -17201,9 +17339,9 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E43" s="282" t="inlineStr">
-        <is>
-          <t>NHI &amp; Agentic Access</t>
+      <c r="E43" s="277" t="inlineStr">
+        <is>
+          <t>AI Supply Chain</t>
         </is>
       </c>
       <c r="F43" s="278" t="inlineStr">
@@ -17213,19 +17351,19 @@
       </c>
       <c r="G43" s="262" t="inlineStr">
         <is>
-          <t>Agentic AI runtime security ($21M Series A, Lightspeed): fast context-aware guardrails; inspects prompts, reasoning steps, tool calls; stops prompt injection, data leaks, agent manipulation.</t>
+          <t>Model threat protection: detects backdoors, adversarial attacks, model poisoning; supply chain focus</t>
         </is>
       </c>
       <c r="H43" s="262" t="inlineStr">
         <is>
-          <t>Production agentic AI; real-time agent security</t>
+          <t>Deep model hardening beyond prompt-level</t>
         </is>
       </c>
     </row>
     <row r="44" ht="40" customHeight="1">
       <c r="B44" s="262" t="inlineStr">
         <is>
-          <t>TrojAI</t>
+          <t>Adri</t>
         </is>
       </c>
       <c r="C44" s="262" t="inlineStr">
@@ -17233,36 +17371,36 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D44" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="E44" s="277" t="inlineStr">
-        <is>
-          <t>AI Supply Chain</t>
-        </is>
-      </c>
-      <c r="F44" s="278" t="inlineStr">
-        <is>
-          <t>Observability &amp; Evaluation</t>
+      <c r="D44" s="279" t="inlineStr">
+        <is>
+          <t>Shadow AI &amp; Usage Discovery</t>
+        </is>
+      </c>
+      <c r="E44" s="281" t="inlineStr">
+        <is>
+          <t>Data Protection for AI</t>
+        </is>
+      </c>
+      <c r="F44" s="276" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
         </is>
       </c>
       <c r="G44" s="262" t="inlineStr">
         <is>
-          <t>Model threat protection: detects backdoors, adversarial attacks, model poisoning; supply chain focus</t>
+          <t>Y Combinator-backed: patented technology monitoring AI vendor infrastructure; detects intentional/accidental misuse of proprietary data.</t>
         </is>
       </c>
       <c r="H44" s="262" t="inlineStr">
         <is>
-          <t>Deep model hardening beyond prompt-level</t>
+          <t>IP protection; AI vendor monitoring</t>
         </is>
       </c>
     </row>
     <row r="45" ht="40" customHeight="1">
       <c r="B45" s="262" t="inlineStr">
         <is>
-          <t>Adri</t>
+          <t>Harmonic Security</t>
         </is>
       </c>
       <c r="C45" s="262" t="inlineStr">
@@ -17287,19 +17425,19 @@
       </c>
       <c r="G45" s="262" t="inlineStr">
         <is>
-          <t>Y Combinator-backed: patented technology monitoring AI vendor infrastructure; detects intentional/accidental misuse of proprietary data.</t>
+          <t>Shadow AI discovery + GenAI-aware DLP ($26M raised): detects sensitive data in AI</t>
         </is>
       </c>
       <c r="H45" s="262" t="inlineStr">
         <is>
-          <t>IP protection; AI vendor monitoring</t>
+          <t>DLP specifically tuned for GenAI workflows</t>
         </is>
       </c>
     </row>
     <row r="46" ht="40" customHeight="1">
       <c r="B46" s="262" t="inlineStr">
         <is>
-          <t>Harmonic Security</t>
+          <t>Nightfall AI</t>
         </is>
       </c>
       <c r="C46" s="262" t="inlineStr">
@@ -17317,26 +17455,26 @@
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F46" s="276" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
+      <c r="F46" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="G46" s="262" t="inlineStr">
         <is>
-          <t>Shadow AI discovery + GenAI-aware DLP ($26M raised): detects sensitive data in AI</t>
+          <t>AI-native DLP + GenAI firewall: discovers AI usage, prevents data exposure</t>
         </is>
       </c>
       <c r="H46" s="262" t="inlineStr">
         <is>
-          <t>DLP specifically tuned for GenAI workflows</t>
+          <t>Cloud-native DLP for AI applications</t>
         </is>
       </c>
     </row>
     <row r="47" ht="40" customHeight="1">
       <c r="B47" s="262" t="inlineStr">
         <is>
-          <t>Nightfall AI</t>
+          <t>Reco.ai</t>
         </is>
       </c>
       <c r="C47" s="262" t="inlineStr">
@@ -17354,31 +17492,31 @@
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F47" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
+      <c r="F47" s="276" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
         </is>
       </c>
       <c r="G47" s="262" t="inlineStr">
         <is>
-          <t>AI-native DLP + GenAI firewall: discovers AI usage, prevents data exposure</t>
+          <t>SaaS security + AI discovery: finds AI apps, tracks data flows, enforces policy</t>
         </is>
       </c>
       <c r="H47" s="262" t="inlineStr">
         <is>
-          <t>Cloud-native DLP for AI applications</t>
+          <t>SaaS security teams extending to AI</t>
         </is>
       </c>
     </row>
     <row r="48" ht="40" customHeight="1">
       <c r="B48" s="262" t="inlineStr">
         <is>
-          <t>Reco.ai</t>
+          <t>SentinelOne (Prompt Security)</t>
         </is>
       </c>
       <c r="C48" s="262" t="inlineStr">
         <is>
-          <t>Independent</t>
+          <t>Acquired</t>
         </is>
       </c>
       <c r="D48" s="279" t="inlineStr">
@@ -17386,68 +17524,68 @@
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E48" s="281" t="inlineStr">
+      <c r="E48" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
+        </is>
+      </c>
+      <c r="F48" s="281" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F48" s="276" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
-        </is>
-      </c>
       <c r="G48" s="262" t="inlineStr">
         <is>
-          <t>SaaS security + AI discovery: finds AI apps, tracks data flows, enforces policy</t>
+          <t>Purple AI + Prompt Security acquisition: GenAI visibility, runtime protection</t>
         </is>
       </c>
       <c r="H48" s="262" t="inlineStr">
         <is>
-          <t>SaaS security teams extending to AI</t>
+          <t>SentinelOne customers; GenAI visibility</t>
         </is>
       </c>
     </row>
     <row r="49" ht="40" customHeight="1">
       <c r="B49" s="262" t="inlineStr">
         <is>
-          <t>SentinelOne (Prompt Security)</t>
+          <t>Arize AI</t>
         </is>
       </c>
       <c r="C49" s="262" t="inlineStr">
         <is>
-          <t>Acquired</t>
-        </is>
-      </c>
-      <c r="D49" s="279" t="inlineStr">
-        <is>
-          <t>Shadow AI &amp; Usage Discovery</t>
-        </is>
-      </c>
-      <c r="E49" s="280" t="inlineStr">
+          <t>Independent</t>
+        </is>
+      </c>
+      <c r="D49" s="278" t="inlineStr">
+        <is>
+          <t>Observability &amp; Evaluation</t>
+        </is>
+      </c>
+      <c r="E49" s="276" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
+        </is>
+      </c>
+      <c r="F49" s="280" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F49" s="281" t="inlineStr">
-        <is>
-          <t>Data Protection for AI</t>
-        </is>
-      </c>
       <c r="G49" s="262" t="inlineStr">
         <is>
-          <t>Purple AI + Prompt Security acquisition: GenAI visibility, runtime protection</t>
+          <t>Enterprise AI observability ($131M raised): Phoenix OSS + AX enterprise platform</t>
         </is>
       </c>
       <c r="H49" s="262" t="inlineStr">
         <is>
-          <t>SentinelOne customers; GenAI visibility</t>
+          <t>Production ML/LLM monitoring; Uber, DoorDash</t>
         </is>
       </c>
     </row>
     <row r="50" ht="40" customHeight="1">
       <c r="B50" s="262" t="inlineStr">
         <is>
-          <t>Arize AI</t>
+          <t>Braintrust</t>
         </is>
       </c>
       <c r="C50" s="262" t="inlineStr">
@@ -17465,26 +17603,26 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F50" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
+      <c r="F50" s="262" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
       <c r="G50" s="262" t="inlineStr">
         <is>
-          <t>Enterprise AI observability ($131M raised): Phoenix OSS + AX enterprise platform</t>
+          <t>End-to-end LLM platform connecting observability to improvement: production traces become eval cases; results on PRs; unified PM/engineer interface.</t>
         </is>
       </c>
       <c r="H50" s="262" t="inlineStr">
         <is>
-          <t>Production ML/LLM monitoring; Uber, DoorDash</t>
+          <t>LLM app teams; iterative improvement workflows</t>
         </is>
       </c>
     </row>
     <row r="51" ht="40" customHeight="1">
       <c r="B51" s="262" t="inlineStr">
         <is>
-          <t>Braintrust</t>
+          <t>Comet Opik</t>
         </is>
       </c>
       <c r="C51" s="262" t="inlineStr">
@@ -17497,9 +17635,9 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E51" s="276" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
+      <c r="E51" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="F51" s="262" t="inlineStr">
@@ -17509,24 +17647,24 @@
       </c>
       <c r="G51" s="262" t="inlineStr">
         <is>
-          <t>End-to-end LLM platform connecting observability to improvement: production traces become eval cases; results on PRs; unified PM/engineer interface.</t>
+          <t>LLM evaluation and monitoring platform: tracks AI model quality, performance drift; integrates with major LLM providers.</t>
         </is>
       </c>
       <c r="H51" s="262" t="inlineStr">
         <is>
-          <t>LLM app teams; iterative improvement workflows</t>
+          <t>ML teams; model quality assurance</t>
         </is>
       </c>
     </row>
     <row r="52" ht="40" customHeight="1">
       <c r="B52" s="262" t="inlineStr">
         <is>
-          <t>Comet Opik</t>
+          <t>Datadog LLM Observability</t>
         </is>
       </c>
       <c r="C52" s="262" t="inlineStr">
         <is>
-          <t>Independent</t>
+          <t>Platform</t>
         </is>
       </c>
       <c r="D52" s="278" t="inlineStr">
@@ -17534,9 +17672,9 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E52" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
+      <c r="E52" s="276" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
         </is>
       </c>
       <c r="F52" s="262" t="inlineStr">
@@ -17546,24 +17684,24 @@
       </c>
       <c r="G52" s="262" t="inlineStr">
         <is>
-          <t>LLM evaluation and monitoring platform: tracks AI model quality, performance drift; integrates with major LLM providers.</t>
+          <t>LLM monitoring: prompt injection detection, PII scanning, cost tracking</t>
         </is>
       </c>
       <c r="H52" s="262" t="inlineStr">
         <is>
-          <t>ML teams; model quality assurance</t>
+          <t>Datadog customers; unified observability</t>
         </is>
       </c>
     </row>
     <row r="53" ht="40" customHeight="1">
       <c r="B53" s="262" t="inlineStr">
         <is>
-          <t>Datadog LLM Observability</t>
+          <t>Fiddler AI</t>
         </is>
       </c>
       <c r="C53" s="262" t="inlineStr">
         <is>
-          <t>Platform</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D53" s="278" t="inlineStr">
@@ -17576,26 +17714,26 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F53" s="262" t="inlineStr">
-        <is>
-          <t>—</t>
+      <c r="F53" s="281" t="inlineStr">
+        <is>
+          <t>Data Protection for AI</t>
         </is>
       </c>
       <c r="G53" s="262" t="inlineStr">
         <is>
-          <t>LLM monitoring: prompt injection detection, PII scanning, cost tracking</t>
+          <t>Trust Service for LLMs ($68.6M raised): model scoring, guardrails, explainability</t>
         </is>
       </c>
       <c r="H53" s="262" t="inlineStr">
         <is>
-          <t>Datadog customers; unified observability</t>
+          <t>Regulated industries needing explainability</t>
         </is>
       </c>
     </row>
     <row r="54" ht="40" customHeight="1">
       <c r="B54" s="262" t="inlineStr">
         <is>
-          <t>Fiddler AI</t>
+          <t>Galileo AI</t>
         </is>
       </c>
       <c r="C54" s="262" t="inlineStr">
@@ -17608,9 +17746,9 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E54" s="276" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
+      <c r="E54" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="F54" s="281" t="inlineStr">
@@ -17620,19 +17758,19 @@
       </c>
       <c r="G54" s="262" t="inlineStr">
         <is>
-          <t>Trust Service for LLMs ($68.6M raised): model scoring, guardrails, explainability</t>
+          <t>LLM debugging and evaluation: hallucination detection, data quality, guardrails</t>
         </is>
       </c>
       <c r="H54" s="262" t="inlineStr">
         <is>
-          <t>Regulated industries needing explainability</t>
+          <t>LLM debugging; data scientists; quality focus</t>
         </is>
       </c>
     </row>
     <row r="55" ht="40" customHeight="1">
       <c r="B55" s="262" t="inlineStr">
         <is>
-          <t>Galileo AI</t>
+          <t>Helicone</t>
         </is>
       </c>
       <c r="C55" s="262" t="inlineStr">
@@ -17645,31 +17783,31 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E55" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="F55" s="281" t="inlineStr">
-        <is>
-          <t>Data Protection for AI</t>
+      <c r="E55" s="276" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
+        </is>
+      </c>
+      <c r="F55" s="262" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
       <c r="G55" s="262" t="inlineStr">
         <is>
-          <t>LLM debugging and evaluation: hallucination detection, data quality, guardrails</t>
+          <t>Open source LLM observability: request logging, caching, rate limiting, analytics</t>
         </is>
       </c>
       <c r="H55" s="262" t="inlineStr">
         <is>
-          <t>LLM debugging; data scientists; quality focus</t>
+          <t>OSS-first teams; LLM monitoring on budget</t>
         </is>
       </c>
     </row>
     <row r="56" ht="40" customHeight="1">
       <c r="B56" s="262" t="inlineStr">
         <is>
-          <t>Helicone</t>
+          <t>LangFuse</t>
         </is>
       </c>
       <c r="C56" s="262" t="inlineStr">
@@ -17694,19 +17832,19 @@
       </c>
       <c r="G56" s="262" t="inlineStr">
         <is>
-          <t>Open source LLM observability: request logging, caching, rate limiting, analytics</t>
+          <t>Open-source LLM observability: distributed tracing, prompt management, evaluation; self-hosted or cloud; growing ecosystem.</t>
         </is>
       </c>
       <c r="H56" s="262" t="inlineStr">
         <is>
-          <t>OSS-first teams; LLM monitoring on budget</t>
+          <t>OSS-first teams; cost-conscious LLM monitoring</t>
         </is>
       </c>
     </row>
     <row r="57" ht="40" customHeight="1">
       <c r="B57" s="262" t="inlineStr">
         <is>
-          <t>LangFuse</t>
+          <t>LangSmith (LangChain)</t>
         </is>
       </c>
       <c r="C57" s="262" t="inlineStr">
@@ -17731,19 +17869,19 @@
       </c>
       <c r="G57" s="262" t="inlineStr">
         <is>
-          <t>Open-source LLM observability: distributed tracing, prompt management, evaluation; self-hosted or cloud; growing ecosystem.</t>
+          <t>LLM app debugging and monitoring; traces, evaluations, prompt management</t>
         </is>
       </c>
       <c r="H57" s="262" t="inlineStr">
         <is>
-          <t>OSS-first teams; cost-conscious LLM monitoring</t>
+          <t>LangChain users; LLM app developers</t>
         </is>
       </c>
     </row>
     <row r="58" ht="40" customHeight="1">
       <c r="B58" s="262" t="inlineStr">
         <is>
-          <t>LangSmith (LangChain)</t>
+          <t>Maxim AI</t>
         </is>
       </c>
       <c r="C58" s="262" t="inlineStr">
@@ -17761,26 +17899,26 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F58" s="262" t="inlineStr">
-        <is>
-          <t>—</t>
+      <c r="F58" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="G58" s="262" t="inlineStr">
         <is>
-          <t>LLM app debugging and monitoring; traces, evaluations, prompt management</t>
+          <t>End-to-end AI agent lifecycle platform: experimentation, simulation, evaluation, production observability; unified workflow replacing multiple point tools.</t>
         </is>
       </c>
       <c r="H58" s="262" t="inlineStr">
         <is>
-          <t>LangChain users; LLM app developers</t>
+          <t>Agent development teams; unified agent lifecycle</t>
         </is>
       </c>
     </row>
     <row r="59" ht="40" customHeight="1">
       <c r="B59" s="262" t="inlineStr">
         <is>
-          <t>Maxim AI</t>
+          <t>Patronus AI</t>
         </is>
       </c>
       <c r="C59" s="262" t="inlineStr">
@@ -17793,31 +17931,31 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E59" s="276" t="inlineStr">
+      <c r="E59" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
+        </is>
+      </c>
+      <c r="F59" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F59" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
       <c r="G59" s="262" t="inlineStr">
         <is>
-          <t>End-to-end AI agent lifecycle platform: experimentation, simulation, evaluation, production observability; unified workflow replacing multiple point tools.</t>
+          <t>LLM evaluation platform ($20M raised): hallucination detection, automated testing</t>
         </is>
       </c>
       <c r="H59" s="262" t="inlineStr">
         <is>
-          <t>Agent development teams; unified agent lifecycle</t>
+          <t>LLM quality assurance; hallucination prevention</t>
         </is>
       </c>
     </row>
     <row r="60" ht="40" customHeight="1">
       <c r="B60" s="262" t="inlineStr">
         <is>
-          <t>Patronus AI</t>
+          <t>Portkey</t>
         </is>
       </c>
       <c r="C60" s="262" t="inlineStr">
@@ -17842,19 +17980,19 @@
       </c>
       <c r="G60" s="262" t="inlineStr">
         <is>
-          <t>LLM evaluation platform ($20M raised): hallucination detection, automated testing</t>
+          <t>LLM gateway and observability: unified API, caching, fallbacks, cost management</t>
         </is>
       </c>
       <c r="H60" s="262" t="inlineStr">
         <is>
-          <t>LLM quality assurance; hallucination prevention</t>
+          <t>Multi-LLM deployments; cost optimization</t>
         </is>
       </c>
     </row>
     <row r="61" ht="40" customHeight="1">
       <c r="B61" s="262" t="inlineStr">
         <is>
-          <t>Portkey</t>
+          <t>Prophet Security</t>
         </is>
       </c>
       <c r="C61" s="262" t="inlineStr">
@@ -17867,31 +18005,31 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E61" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="F61" s="276" t="inlineStr">
+      <c r="E61" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
+      <c r="F61" s="262" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="G61" s="262" t="inlineStr">
         <is>
-          <t>LLM gateway and observability: unified API, caching, fallbacks, cost management</t>
+          <t>Agentic SOC: autonomous security investigation; AI-driven threat response; reduces analyst burden.</t>
         </is>
       </c>
       <c r="H61" s="262" t="inlineStr">
         <is>
-          <t>Multi-LLM deployments; cost optimization</t>
+          <t>SOC teams; autonomous investigation</t>
         </is>
       </c>
     </row>
     <row r="62" ht="40" customHeight="1">
       <c r="B62" s="262" t="inlineStr">
         <is>
-          <t>Prophet Security</t>
+          <t>Radiant Security</t>
         </is>
       </c>
       <c r="C62" s="262" t="inlineStr">
@@ -17909,26 +18047,26 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F62" s="262" t="inlineStr">
-        <is>
-          <t>—</t>
+      <c r="F62" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="G62" s="262" t="inlineStr">
         <is>
-          <t>Agentic SOC: autonomous security investigation; AI-driven threat response; reduces analyst burden.</t>
+          <t>Agentic AI SOC platform: handles 100% of alerts; 90% false positive reduction; integrates 100+ data sources; autonomous triage.</t>
         </is>
       </c>
       <c r="H62" s="262" t="inlineStr">
         <is>
-          <t>SOC teams; autonomous investigation</t>
+          <t>SOC teams; alert fatigue reduction</t>
         </is>
       </c>
     </row>
     <row r="63" ht="40" customHeight="1">
       <c r="B63" s="262" t="inlineStr">
         <is>
-          <t>Radiant Security</t>
+          <t>Stellar Cyber</t>
         </is>
       </c>
       <c r="C63" s="262" t="inlineStr">
@@ -17946,26 +18084,26 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F63" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
+      <c r="F63" s="279" t="inlineStr">
+        <is>
+          <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
       <c r="G63" s="262" t="inlineStr">
         <is>
-          <t>Agentic AI SOC platform: handles 100% of alerts; 90% false positive reduction; integrates 100+ data sources; autonomous triage.</t>
+          <t>Open XDR with agentic AI: multi-agent architecture (detection, correlation, scoring, response); 50M+ data points across endpoints/network/cloud.</t>
         </is>
       </c>
       <c r="H63" s="262" t="inlineStr">
         <is>
-          <t>SOC teams; alert fatigue reduction</t>
+          <t>Mid-market; unified security operations</t>
         </is>
       </c>
     </row>
     <row r="64" ht="40" customHeight="1">
       <c r="B64" s="262" t="inlineStr">
         <is>
-          <t>Stellar Cyber</t>
+          <t>Torq</t>
         </is>
       </c>
       <c r="C64" s="262" t="inlineStr">
@@ -17978,31 +18116,31 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E64" s="276" t="inlineStr">
+      <c r="E64" s="282" t="inlineStr">
+        <is>
+          <t>NHI &amp; Agentic Access</t>
+        </is>
+      </c>
+      <c r="F64" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F64" s="279" t="inlineStr">
-        <is>
-          <t>Shadow AI &amp; Usage Discovery</t>
-        </is>
-      </c>
       <c r="G64" s="262" t="inlineStr">
         <is>
-          <t>Open XDR with agentic AI: multi-agent architecture (detection, correlation, scoring, response); 50M+ data points across endpoints/network/cloud.</t>
+          <t>AI-native security hyperautomation ($1.2B valuation): 300% revenue growth; customers include Marriott, PepsiCo, Siemens, Uber.</t>
         </is>
       </c>
       <c r="H64" s="262" t="inlineStr">
         <is>
-          <t>Mid-market; unified security operations</t>
+          <t>Security automation; enterprise SOC</t>
         </is>
       </c>
     </row>
     <row r="65" ht="40" customHeight="1">
       <c r="B65" s="262" t="inlineStr">
         <is>
-          <t>Torq</t>
+          <t>Weights &amp; Biases</t>
         </is>
       </c>
       <c r="C65" s="262" t="inlineStr">
@@ -18015,46 +18153,46 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E65" s="282" t="inlineStr">
-        <is>
-          <t>NHI &amp; Agentic Access</t>
-        </is>
-      </c>
-      <c r="F65" s="276" t="inlineStr">
+      <c r="E65" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
+      <c r="F65" s="262" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="G65" s="262" t="inlineStr">
         <is>
-          <t>AI-native security hyperautomation ($1.2B valuation): 300% revenue growth; customers include Marriott, PepsiCo, Siemens, Uber.</t>
+          <t>MLOps platform ($250M raised): experiment tracking, model registry, LLM tracing</t>
         </is>
       </c>
       <c r="H65" s="262" t="inlineStr">
         <is>
-          <t>Security automation; enterprise SOC</t>
+          <t>ML teams; experiment tracking; model lifecycle</t>
         </is>
       </c>
     </row>
     <row r="66" ht="40" customHeight="1">
       <c r="B66" s="262" t="inlineStr">
         <is>
-          <t>Weights &amp; Biases</t>
+          <t>AWS Bedrock Guardrails</t>
         </is>
       </c>
       <c r="C66" s="262" t="inlineStr">
         <is>
-          <t>Independent</t>
-        </is>
-      </c>
-      <c r="D66" s="278" t="inlineStr">
-        <is>
-          <t>Observability &amp; Evaluation</t>
-        </is>
-      </c>
-      <c r="E66" s="276" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
+          <t>Platform</t>
+        </is>
+      </c>
+      <c r="D66" s="281" t="inlineStr">
+        <is>
+          <t>Data Protection for AI</t>
+        </is>
+      </c>
+      <c r="E66" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="F66" s="262" t="inlineStr">
@@ -18064,24 +18202,24 @@
       </c>
       <c r="G66" s="262" t="inlineStr">
         <is>
-          <t>MLOps platform ($250M raised): experiment tracking, model registry, LLM tracing</t>
+          <t>Model-agnostic guardrails: Automated Reasoning for 99% hallucination prevention</t>
         </is>
       </c>
       <c r="H66" s="262" t="inlineStr">
         <is>
-          <t>ML teams; experiment tracking; model lifecycle</t>
+          <t>AWS customers; Bedrock users</t>
         </is>
       </c>
     </row>
     <row r="67" ht="40" customHeight="1">
       <c r="B67" s="262" t="inlineStr">
         <is>
-          <t>AWS Bedrock Guardrails</t>
+          <t>BigID</t>
         </is>
       </c>
       <c r="C67" s="262" t="inlineStr">
         <is>
-          <t>Platform</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D67" s="281" t="inlineStr">
@@ -18089,31 +18227,31 @@
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E67" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="F67" s="262" t="inlineStr">
-        <is>
-          <t>—</t>
+      <c r="E67" s="276" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
+        </is>
+      </c>
+      <c r="F67" s="279" t="inlineStr">
+        <is>
+          <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
       <c r="G67" s="262" t="inlineStr">
         <is>
-          <t>Model-agnostic guardrails: Automated Reasoning for 99% hallucination prevention</t>
+          <t>Shadow AI detection + AI governance ($290M raised): discovers AI data/models, maps to regs</t>
         </is>
       </c>
       <c r="H67" s="262" t="inlineStr">
         <is>
-          <t>AWS customers; Bedrock users</t>
+          <t>Data discovery and governance for AI</t>
         </is>
       </c>
     </row>
     <row r="68" ht="40" customHeight="1">
       <c r="B68" s="262" t="inlineStr">
         <is>
-          <t>BigID</t>
+          <t>Cyera</t>
         </is>
       </c>
       <c r="C68" s="262" t="inlineStr">
@@ -18138,24 +18276,24 @@
       </c>
       <c r="G68" s="262" t="inlineStr">
         <is>
-          <t>Shadow AI detection + AI governance ($290M raised): discovers AI data/models, maps to regs</t>
-        </is>
-      </c>
-      <c r="H68" s="262" t="inlineStr">
-        <is>
-          <t>Data discovery and governance for AI</t>
+          <t>DSPM leader ($1.3B raised, $6B valuation): AI Guardian, 98% classification accuracy</t>
+        </is>
+      </c>
+      <c r="H68" s="259" t="inlineStr">
+        <is>
+          <t>Enterprise DSPM; AI data governance</t>
         </is>
       </c>
     </row>
     <row r="69" ht="40" customHeight="1">
       <c r="B69" s="262" t="inlineStr">
         <is>
-          <t>Cyera</t>
+          <t>Google Cloud Model Armor</t>
         </is>
       </c>
       <c r="C69" s="262" t="inlineStr">
         <is>
-          <t>Independent</t>
+          <t>Platform</t>
         </is>
       </c>
       <c r="D69" s="281" t="inlineStr">
@@ -18163,36 +18301,36 @@
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E69" s="276" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
-        </is>
-      </c>
-      <c r="F69" s="279" t="inlineStr">
-        <is>
-          <t>Shadow AI &amp; Usage Discovery</t>
+      <c r="E69" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
+        </is>
+      </c>
+      <c r="F69" s="262" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
       <c r="G69" s="262" t="inlineStr">
         <is>
-          <t>DSPM leader ($1.3B raised, $6B valuation): AI Guardian, 98% classification accuracy</t>
+          <t>Runtime security for any LLM: prompt injection, sensitive data, malicious URL blocking</t>
         </is>
       </c>
       <c r="H69" s="259" t="inlineStr">
         <is>
-          <t>Enterprise DSPM; AI data governance</t>
+          <t>GCP customers; Vertex AI users</t>
         </is>
       </c>
     </row>
     <row r="70" ht="40" customHeight="1">
       <c r="B70" s="262" t="inlineStr">
         <is>
-          <t>Google Cloud Model Armor</t>
+          <t>Island Browser</t>
         </is>
       </c>
       <c r="C70" s="262" t="inlineStr">
         <is>
-          <t>Platform</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D70" s="281" t="inlineStr">
@@ -18200,31 +18338,31 @@
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E70" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="F70" s="262" t="inlineStr">
-        <is>
-          <t>—</t>
+      <c r="E70" s="279" t="inlineStr">
+        <is>
+          <t>Shadow AI &amp; Usage Discovery</t>
+        </is>
+      </c>
+      <c r="F70" s="276" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
         </is>
       </c>
       <c r="G70" s="262" t="inlineStr">
         <is>
-          <t>Runtime security for any LLM: prompt injection, sensitive data, malicious URL blocking</t>
+          <t>Enterprise browser with AI controls: DLP, session recording, controlled AI access</t>
         </is>
       </c>
       <c r="H70" s="259" t="inlineStr">
         <is>
-          <t>GCP customers; Vertex AI users</t>
+          <t>Browser-based AI control; high-security orgs</t>
         </is>
       </c>
     </row>
     <row r="71" ht="40" customHeight="1">
       <c r="B71" s="262" t="inlineStr">
         <is>
-          <t>Island Browser</t>
+          <t>Knostic</t>
         </is>
       </c>
       <c r="C71" s="262" t="inlineStr">
@@ -18237,31 +18375,31 @@
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E71" s="279" t="inlineStr">
-        <is>
-          <t>Shadow AI &amp; Usage Discovery</t>
-        </is>
-      </c>
-      <c r="F71" s="276" t="inlineStr">
+      <c r="E71" s="276" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
+      <c r="F71" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
+        </is>
+      </c>
       <c r="G71" s="262" t="inlineStr">
         <is>
-          <t>Enterprise browser with AI controls: DLP, session recording, controlled AI access</t>
+          <t>Need-to-know access for AI: context-aware data protection, RAG security</t>
         </is>
       </c>
       <c r="H71" s="259" t="inlineStr">
         <is>
-          <t>Browser-based AI control; high-security orgs</t>
+          <t>RAG deployments; need-to-know data access</t>
         </is>
       </c>
     </row>
     <row r="72" ht="40" customHeight="1">
       <c r="B72" s="262" t="inlineStr">
         <is>
-          <t>Knostic</t>
+          <t>Netskope</t>
         </is>
       </c>
       <c r="C72" s="262" t="inlineStr">
@@ -18274,9 +18412,9 @@
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E72" s="276" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
+      <c r="E72" s="279" t="inlineStr">
+        <is>
+          <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
       <c r="F72" s="280" t="inlineStr">
@@ -18286,19 +18424,19 @@
       </c>
       <c r="G72" s="262" t="inlineStr">
         <is>
-          <t>Need-to-know access for AI: context-aware data protection, RAG security</t>
+          <t>SASE + GenAI DLP: real-time coaching, data protection for AI apps</t>
         </is>
       </c>
       <c r="H72" s="259" t="inlineStr">
         <is>
-          <t>RAG deployments; need-to-know data access</t>
+          <t>SASE customers; GenAI-aware DLP</t>
         </is>
       </c>
     </row>
     <row r="73" ht="40" customHeight="1">
       <c r="B73" s="262" t="inlineStr">
         <is>
-          <t>Netskope</t>
+          <t>Zscaler</t>
         </is>
       </c>
       <c r="C73" s="262" t="inlineStr">
@@ -18323,56 +18461,56 @@
       </c>
       <c r="G73" s="262" t="inlineStr">
         <is>
-          <t>SASE + GenAI DLP: real-time coaching, data protection for AI apps</t>
+          <t>Zero trust + AI security: GenAI app control, data protection, shadow AI</t>
         </is>
       </c>
       <c r="H73" s="259" t="inlineStr">
         <is>
-          <t>SASE customers; GenAI-aware DLP</t>
+          <t>Zscaler customers; zero trust AI security</t>
         </is>
       </c>
     </row>
     <row r="74" ht="40" customHeight="1">
-      <c r="B74" s="262" t="inlineStr">
-        <is>
-          <t>Zscaler</t>
-        </is>
-      </c>
-      <c r="C74" s="262" t="inlineStr">
+      <c r="B74" s="259" t="inlineStr">
+        <is>
+          <t>Aembit</t>
+        </is>
+      </c>
+      <c r="C74" s="259" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D74" s="281" t="inlineStr">
+      <c r="D74" s="284" t="inlineStr">
+        <is>
+          <t>NHI &amp; Agentic Access</t>
+        </is>
+      </c>
+      <c r="E74" s="288" t="inlineStr">
+        <is>
+          <t>Shadow AI &amp; Usage Discovery</t>
+        </is>
+      </c>
+      <c r="F74" s="289" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E74" s="279" t="inlineStr">
-        <is>
-          <t>Shadow AI &amp; Usage Discovery</t>
-        </is>
-      </c>
-      <c r="F74" s="280" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="G74" s="262" t="inlineStr">
-        <is>
-          <t>Zero trust + AI security: GenAI app control, data protection, shadow AI</t>
+      <c r="G74" s="259" t="inlineStr">
+        <is>
+          <t>Secretless workload IAM ($45M raised): workload-to-workload identity; tracks AI service connections revealing shadow AI</t>
         </is>
       </c>
       <c r="H74" s="259" t="inlineStr">
         <is>
-          <t>Zscaler customers; zero trust AI security</t>
+          <t>Secretless architecture; workload identity</t>
         </is>
       </c>
     </row>
     <row r="75" ht="40" customHeight="1">
       <c r="B75" s="259" t="inlineStr">
         <is>
-          <t>Aembit</t>
+          <t>Astrix Security</t>
         </is>
       </c>
       <c r="C75" s="259" t="inlineStr">
@@ -18390,26 +18528,26 @@
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F75" s="289" t="inlineStr">
-        <is>
-          <t>Data Protection for AI</t>
+      <c r="F75" s="286" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
         </is>
       </c>
       <c r="G75" s="259" t="inlineStr">
         <is>
-          <t>Secretless workload IAM ($45M raised): workload-to-workload identity; tracks AI service connections revealing shadow AI</t>
+          <t>Dedicated NHI platform ($85M raised): agent inventory, least-privilege; token monitoring surfaces shadow AI tools</t>
         </is>
       </c>
       <c r="H75" s="259" t="inlineStr">
         <is>
-          <t>Secretless architecture; workload identity</t>
+          <t>NHI-first security; agentic AI deployments</t>
         </is>
       </c>
     </row>
     <row r="76" ht="40" customHeight="1">
       <c r="B76" s="259" t="inlineStr">
         <is>
-          <t>Astrix Security</t>
+          <t>CyberArk</t>
         </is>
       </c>
       <c r="C76" s="259" t="inlineStr">
@@ -18422,31 +18560,31 @@
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E76" s="288" t="inlineStr">
-        <is>
-          <t>Shadow AI &amp; Usage Discovery</t>
-        </is>
-      </c>
-      <c r="F76" s="286" t="inlineStr">
+      <c r="E76" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
+      <c r="F76" s="289" t="inlineStr">
+        <is>
+          <t>Data Protection for AI</t>
+        </is>
+      </c>
       <c r="G76" s="259" t="inlineStr">
         <is>
-          <t>Dedicated NHI platform ($85M raised): agent inventory, least-privilege; token monitoring surfaces shadow AI tools</t>
+          <t>PAM leader extending to NHI: machine identity security, secrets management</t>
         </is>
       </c>
       <c r="H76" s="259" t="inlineStr">
         <is>
-          <t>NHI-first security; agentic AI deployments</t>
+          <t>Enterprise PAM; extending to machine identities</t>
         </is>
       </c>
     </row>
     <row r="77" ht="40" customHeight="1">
       <c r="B77" s="259" t="inlineStr">
         <is>
-          <t>CyberArk</t>
+          <t>Entro Security</t>
         </is>
       </c>
       <c r="C77" s="259" t="inlineStr">
@@ -18459,31 +18597,31 @@
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E77" s="286" t="inlineStr">
+      <c r="E77" s="288" t="inlineStr">
+        <is>
+          <t>Shadow AI &amp; Usage Discovery</t>
+        </is>
+      </c>
+      <c r="F77" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F77" s="289" t="inlineStr">
-        <is>
-          <t>Data Protection for AI</t>
-        </is>
-      </c>
       <c r="G77" s="259" t="inlineStr">
         <is>
-          <t>PAM leader extending to NHI: machine identity security, secrets management</t>
+          <t>Secrets security platform: discovers and monitors exposed secrets; reveals AI API keys indicating shadow AI usage</t>
         </is>
       </c>
       <c r="H77" s="259" t="inlineStr">
         <is>
-          <t>Enterprise PAM; extending to machine identities</t>
+          <t>Secrets sprawl; credential exposure prevention</t>
         </is>
       </c>
     </row>
     <row r="78" ht="40" customHeight="1">
       <c r="B78" s="259" t="inlineStr">
         <is>
-          <t>Entro Security</t>
+          <t>HashiCorp Vault</t>
         </is>
       </c>
       <c r="C78" s="259" t="inlineStr">
@@ -18496,31 +18634,31 @@
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E78" s="288" t="inlineStr">
-        <is>
-          <t>Shadow AI &amp; Usage Discovery</t>
-        </is>
-      </c>
-      <c r="F78" s="286" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
+      <c r="E78" s="289" t="inlineStr">
+        <is>
+          <t>Data Protection for AI</t>
+        </is>
+      </c>
+      <c r="F78" s="259" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
       <c r="G78" s="259" t="inlineStr">
         <is>
-          <t>Secrets security platform: discovers and monitors exposed secrets; reveals AI API keys indicating shadow AI usage</t>
+          <t>Secrets management leader: dynamic secrets, encryption, identity-based access</t>
         </is>
       </c>
       <c r="H78" s="259" t="inlineStr">
         <is>
-          <t>Secrets sprawl; credential exposure prevention</t>
+          <t>Secrets management; dynamic credentials; DevOps</t>
         </is>
       </c>
     </row>
     <row r="79" ht="40" customHeight="1">
       <c r="B79" s="259" t="inlineStr">
         <is>
-          <t>HashiCorp Vault</t>
+          <t>Oasis Security</t>
         </is>
       </c>
       <c r="C79" s="259" t="inlineStr">
@@ -18533,31 +18671,31 @@
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E79" s="289" t="inlineStr">
-        <is>
-          <t>Data Protection for AI</t>
-        </is>
-      </c>
-      <c r="F79" s="259" t="inlineStr">
-        <is>
-          <t>—</t>
+      <c r="E79" s="288" t="inlineStr">
+        <is>
+          <t>Shadow AI &amp; Usage Discovery</t>
+        </is>
+      </c>
+      <c r="F79" s="286" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
         </is>
       </c>
       <c r="G79" s="259" t="inlineStr">
         <is>
-          <t>Secrets management leader: dynamic secrets, encryption, identity-based access</t>
+          <t>NHI Security Cloud ($75M raised): Agentic Access Management; identity-based shadow AI discovery via service account monitoring</t>
         </is>
       </c>
       <c r="H79" s="259" t="inlineStr">
         <is>
-          <t>Secrets management; dynamic credentials; DevOps</t>
+          <t>Agentic AI security; intent-based access control</t>
         </is>
       </c>
     </row>
     <row r="80" ht="40" customHeight="1">
       <c r="B80" s="259" t="inlineStr">
         <is>
-          <t>Oasis Security</t>
+          <t>Silverfort</t>
         </is>
       </c>
       <c r="C80" s="259" t="inlineStr">
@@ -18582,19 +18720,19 @@
       </c>
       <c r="G80" s="259" t="inlineStr">
         <is>
-          <t>NHI Security Cloud ($75M raised): Agentic Access Management; identity-based shadow AI discovery via service account monitoring</t>
+          <t>NHI leader ($222M raised, ~$1B valuation): unified human + non-human identity; NHI visibility reveals unauthorized AI service access</t>
         </is>
       </c>
       <c r="H80" s="259" t="inlineStr">
         <is>
-          <t>Agentic AI security; intent-based access control</t>
+          <t>Enterprise IAM extending to NHI; MFA everywhere</t>
         </is>
       </c>
     </row>
     <row r="81" ht="40" customHeight="1">
       <c r="B81" s="259" t="inlineStr">
         <is>
-          <t>Silverfort</t>
+          <t>Spec</t>
         </is>
       </c>
       <c r="C81" s="259" t="inlineStr">
@@ -18607,9 +18745,9 @@
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E81" s="288" t="inlineStr">
-        <is>
-          <t>Shadow AI &amp; Usage Discovery</t>
+      <c r="E81" s="283" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="F81" s="286" t="inlineStr">
@@ -18619,19 +18757,19 @@
       </c>
       <c r="G81" s="259" t="inlineStr">
         <is>
-          <t>NHI leader ($222M raised, ~$1B valuation): unified human + non-human identity; NHI visibility reveals unauthorized AI service access</t>
+          <t>Agentic security platform: agent identity, behavior monitoring, automated response</t>
         </is>
       </c>
       <c r="H81" s="259" t="inlineStr">
         <is>
-          <t>Enterprise IAM extending to NHI; MFA everywhere</t>
+          <t>Organizations with production AI agents</t>
         </is>
       </c>
     </row>
     <row r="82" ht="40" customHeight="1">
       <c r="B82" s="259" t="inlineStr">
         <is>
-          <t>Spec</t>
+          <t>Strata Identity</t>
         </is>
       </c>
       <c r="C82" s="259" t="inlineStr">
@@ -18644,73 +18782,73 @@
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E82" s="283" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="F82" s="286" t="inlineStr">
+      <c r="E82" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
+      <c r="F82" s="259" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="G82" s="259" t="inlineStr">
         <is>
-          <t>Agentic security platform: agent identity, behavior monitoring, automated response</t>
+          <t>Agentic identity management: dynamic, autonomous NHI governance; distinct from static machine identities; policy-based agent permissions.</t>
         </is>
       </c>
       <c r="H82" s="259" t="inlineStr">
         <is>
-          <t>Organizations with production AI agents</t>
+          <t>Agentic AI identity; dynamic access control</t>
         </is>
       </c>
     </row>
     <row r="83" ht="40" customHeight="1">
-      <c r="B83" s="259" t="inlineStr">
-        <is>
-          <t>Strata Identity</t>
-        </is>
-      </c>
-      <c r="C83" s="259" t="inlineStr">
+      <c r="B83" s="320" t="inlineStr">
+        <is>
+          <t>Chainguard</t>
+        </is>
+      </c>
+      <c r="C83" s="320" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D83" s="284" t="inlineStr">
-        <is>
-          <t>NHI &amp; Agentic Access</t>
-        </is>
-      </c>
-      <c r="E83" s="286" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
-        </is>
-      </c>
-      <c r="F83" s="259" t="inlineStr">
+      <c r="D83" s="320" t="inlineStr">
+        <is>
+          <t>AI Supply Chain</t>
+        </is>
+      </c>
+      <c r="E83" s="320" t="inlineStr">
+        <is>
+          <t>Data Protection for AI</t>
+        </is>
+      </c>
+      <c r="F83" s="320" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G83" s="259" t="inlineStr">
-        <is>
-          <t>Agentic identity management: dynamic, autonomous NHI governance; distinct from static machine identities; policy-based agent permissions.</t>
-        </is>
-      </c>
-      <c r="H83" s="259" t="inlineStr">
-        <is>
-          <t>Agentic AI identity; dynamic access control</t>
+      <c r="G83" s="320" t="inlineStr">
+        <is>
+          <t>Hardened containers and libraries: SBOM generation, SLSA provenance, secure Python packages for ML pipelines, zero-CVE images</t>
+        </is>
+      </c>
+      <c r="H83" s="320" t="inlineStr">
+        <is>
+          <t>Secure base images; ML pipeline containers; compliance-focused orgs</t>
         </is>
       </c>
     </row>
     <row r="84" ht="40" customHeight="1">
       <c r="B84" s="259" t="inlineStr">
         <is>
-          <t>Chainguard</t>
+          <t>HiddenLayer</t>
         </is>
       </c>
       <c r="C84" s="259" t="inlineStr">
         <is>
-          <t>chainguard.dev</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D84" s="287" t="inlineStr">
@@ -18718,69 +18856,73 @@
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E84" s="289" t="inlineStr">
-        <is>
-          <t>Data Protection for AI</t>
-        </is>
-      </c>
-      <c r="F84" s="259" t="inlineStr">
+      <c r="E84" s="283" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
+        </is>
+      </c>
+      <c r="F84" s="286" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
+        </is>
+      </c>
+      <c r="G84" s="259" t="inlineStr">
+        <is>
+          <t>AI Supply Chain leader ($56M raised): model scanning, ML supply chain security, model BOM</t>
+        </is>
+      </c>
+      <c r="H84" s="259" t="inlineStr">
+        <is>
+          <t>Multi-cloud AI; wants independent vendor</t>
+        </is>
+      </c>
+    </row>
+    <row r="85" ht="40" customHeight="1">
+      <c r="B85" s="320" t="inlineStr">
+        <is>
+          <t>JFrog</t>
+        </is>
+      </c>
+      <c r="C85" s="320" t="inlineStr">
+        <is>
+          <t>Platform</t>
+        </is>
+      </c>
+      <c r="D85" s="320" t="inlineStr">
+        <is>
+          <t>AI Supply Chain</t>
+        </is>
+      </c>
+      <c r="E85" s="320" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
+        </is>
+      </c>
+      <c r="F85" s="320" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G84" s="259" t="inlineStr">
-        <is>
-          <t>Hardened containers and libraries: SBOM generation, SLSA provenance, secure Python packages for ML pipelines</t>
-        </is>
-      </c>
-      <c r="H84" s="259" t="n"/>
-    </row>
-    <row r="85" ht="40" customHeight="1">
-      <c r="B85" s="259" t="inlineStr">
-        <is>
-          <t>HiddenLayer</t>
-        </is>
-      </c>
-      <c r="C85" s="259" t="inlineStr">
-        <is>
-          <t>Independent</t>
-        </is>
-      </c>
-      <c r="D85" s="287" t="inlineStr">
-        <is>
-          <t>AI Supply Chain</t>
-        </is>
-      </c>
-      <c r="E85" s="283" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="F85" s="286" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
-        </is>
-      </c>
-      <c r="G85" s="259" t="inlineStr">
-        <is>
-          <t>AI Supply Chain leader ($56M raised): model scanning, ML supply chain security, model BOM</t>
-        </is>
-      </c>
-      <c r="H85" s="259" t="inlineStr">
-        <is>
-          <t>Multi-cloud AI; wants independent vendor</t>
+      <c r="G85" s="320" t="inlineStr">
+        <is>
+          <t>Universal artifact repository: ML model management, SBOM generation, DevSecOps integration, binary analysis, supply chain security</t>
+        </is>
+      </c>
+      <c r="H85" s="320" t="inlineStr">
+        <is>
+          <t>Artifact management; DevOps integration; ML model versioning</t>
         </is>
       </c>
     </row>
     <row r="86" ht="40" customHeight="1">
       <c r="B86" s="259" t="inlineStr">
         <is>
-          <t>JFrog</t>
+          <t>Legit Security</t>
         </is>
       </c>
       <c r="C86" s="259" t="inlineStr">
         <is>
-          <t>jfrog.com</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D86" s="287" t="inlineStr">
@@ -18793,134 +18935,142 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F86" s="259" t="inlineStr">
-        <is>
-          <t>—</t>
+      <c r="F86" s="283" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="G86" s="259" t="inlineStr">
         <is>
-          <t>Universal artifact repository: ML model management, SBOM, DevSecOps integration, supply chain security</t>
-        </is>
-      </c>
-      <c r="H86" s="259" t="n"/>
+          <t>AI Supply Chain via ASPM: AI code security, model supply chain, SDLC for ML pipelines</t>
+        </is>
+      </c>
+      <c r="H86" s="259" t="inlineStr">
+        <is>
+          <t>DevSecOps teams; AI in software supply chain</t>
+        </is>
+      </c>
     </row>
     <row r="87" ht="40" customHeight="1">
       <c r="B87" s="259" t="inlineStr">
         <is>
-          <t>Legit Security</t>
+          <t>OpenSSF Model Signing</t>
         </is>
       </c>
       <c r="C87" s="259" t="inlineStr">
         <is>
+          <t>Open Standard</t>
+        </is>
+      </c>
+      <c r="D87" s="287" t="inlineStr">
+        <is>
+          <t>AI Supply Chain</t>
+        </is>
+      </c>
+      <c r="E87" s="284" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F87" s="259" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G87" s="259" t="inlineStr">
+        <is>
+          <t>Open Source Security Foundation: model signing specification for cryptographically verifying AI model origin and integrity.</t>
+        </is>
+      </c>
+      <c r="H87" s="259" t="inlineStr">
+        <is>
+          <t>OSS model consumers; provenance verification</t>
+        </is>
+      </c>
+    </row>
+    <row r="88" ht="40" customHeight="1">
+      <c r="B88" s="320" t="inlineStr">
+        <is>
+          <t>Snyk</t>
+        </is>
+      </c>
+      <c r="C88" s="320" t="inlineStr">
+        <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D87" s="287" t="inlineStr">
+      <c r="D88" s="320" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E87" s="286" t="inlineStr">
+      <c r="E88" s="320" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
+        </is>
+      </c>
+      <c r="F88" s="320" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F87" s="283" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="G87" s="259" t="inlineStr">
-        <is>
-          <t>AI Supply Chain via ASPM: AI code security, model supply chain, SDLC for ML pipelines</t>
-        </is>
-      </c>
-      <c r="H87" s="259" t="inlineStr">
-        <is>
-          <t>DevSecOps teams; AI in software supply chain</t>
-        </is>
-      </c>
-    </row>
-    <row r="88" ht="40" customHeight="1">
-      <c r="B88" s="259" t="inlineStr">
-        <is>
-          <t>OpenSSF Model Signing</t>
-        </is>
-      </c>
-      <c r="C88" s="259" t="inlineStr">
-        <is>
-          <t>Open Standard</t>
-        </is>
-      </c>
-      <c r="D88" s="287" t="inlineStr">
+      <c r="G88" s="320" t="inlineStr">
+        <is>
+          <t>AI Trust Platform: AI-BOM scanning, Evo agentic security assistant, supply chain for AI-generated code, MCP server security</t>
+        </is>
+      </c>
+      <c r="H88" s="320" t="inlineStr">
+        <is>
+          <t>Developer-first security; AI-generated code scanning; modern DevSecOps</t>
+        </is>
+      </c>
+    </row>
+    <row r="89" ht="40" customHeight="1">
+      <c r="B89" s="320" t="inlineStr">
+        <is>
+          <t>Sonatype</t>
+        </is>
+      </c>
+      <c r="C89" s="320" t="inlineStr">
+        <is>
+          <t>Independent</t>
+        </is>
+      </c>
+      <c r="D89" s="320" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E88" s="284" t="inlineStr">
+      <c r="E89" s="320" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
+        </is>
+      </c>
+      <c r="F89" s="320" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="F88" s="259" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="G88" s="259" t="inlineStr">
-        <is>
-          <t>Open Source Security Foundation: model signing specification for cryptographically verifying AI model origin and integrity.</t>
-        </is>
-      </c>
-      <c r="H88" s="259" t="inlineStr">
-        <is>
-          <t>OSS model consumers; provenance verification</t>
-        </is>
-      </c>
-    </row>
-    <row r="89" ht="40" customHeight="1">
-      <c r="B89" s="259" t="inlineStr">
-        <is>
-          <t>Snyk</t>
-        </is>
-      </c>
-      <c r="C89" s="259" t="inlineStr">
-        <is>
-          <t>snyk.io</t>
-        </is>
-      </c>
-      <c r="D89" s="287" t="inlineStr">
-        <is>
-          <t>AI Supply Chain</t>
-        </is>
-      </c>
-      <c r="E89" s="283" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="F89" s="286" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
-        </is>
-      </c>
-      <c r="G89" s="259" t="inlineStr">
-        <is>
-          <t>AI Trust Platform: AI-BOM scanning, Evo agentic security, supply chain for AI-generated code, MCP server security</t>
-        </is>
-      </c>
-      <c r="H89" s="259" t="n"/>
+      <c r="G89" s="320" t="inlineStr">
+        <is>
+          <t>Software supply chain leader: SBOM management, AI/ML model scanning from Hugging Face, malware detection in packages, Nexus repository</t>
+        </is>
+      </c>
+      <c r="H89" s="320" t="inlineStr">
+        <is>
+          <t>Supply chain governance; package security; model provenance</t>
+        </is>
+      </c>
     </row>
     <row r="90" ht="40" customHeight="1">
       <c r="B90" s="259" t="inlineStr">
         <is>
-          <t>Sonatype</t>
+          <t>Spectra Assure</t>
         </is>
       </c>
       <c r="C90" s="259" t="inlineStr">
         <is>
-          <t>sonatype.com</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D90" s="287" t="inlineStr">
@@ -18933,54 +19083,29 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F90" s="259" t="inlineStr">
-        <is>
-          <t>—</t>
+      <c r="F90" s="283" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="G90" s="259" t="inlineStr">
         <is>
-          <t>Software supply chain leader: SBOM management, AI/ML model scanning from Hugging Face, malware detection in packages</t>
-        </is>
-      </c>
-      <c r="H90" s="259" t="n"/>
+          <t>Software supply chain security: SAFE reports for AI/ML artifacts; flags poisoning risks; CycloneDX export; NIST/ISO 42001 compliant.</t>
+        </is>
+      </c>
+      <c r="H90" s="259" t="inlineStr">
+        <is>
+          <t>Regulated industries; AI supply chain compliance</t>
+        </is>
+      </c>
     </row>
     <row r="91" ht="40" customHeight="1">
-      <c r="B91" s="259" t="inlineStr">
-        <is>
-          <t>Spectra Assure</t>
-        </is>
-      </c>
-      <c r="C91" s="259" t="inlineStr">
-        <is>
-          <t>Independent</t>
-        </is>
-      </c>
-      <c r="D91" s="287" t="inlineStr">
-        <is>
-          <t>AI Supply Chain</t>
-        </is>
-      </c>
-      <c r="E91" s="286" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
-        </is>
-      </c>
-      <c r="F91" s="283" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="G91" s="259" t="inlineStr">
-        <is>
-          <t>Software supply chain security: SAFE reports for AI/ML artifacts; flags poisoning risks; CycloneDX export; NIST/ISO 42001 compliant.</t>
-        </is>
-      </c>
-      <c r="H91" s="259" t="inlineStr">
-        <is>
-          <t>Regulated industries; AI supply chain compliance</t>
-        </is>
-      </c>
+      <c r="C91" s="190" t="n"/>
+      <c r="D91" s="190" t="n"/>
+      <c r="E91" s="190" t="n"/>
+      <c r="F91" s="190" t="n"/>
+      <c r="G91" s="190" t="n"/>
+      <c r="H91" s="190" t="n"/>
     </row>
     <row r="92">
       <c r="C92" s="190" t="n"/>
@@ -19510,14 +19635,6 @@
       <c r="G157" s="190" t="n"/>
       <c r="H157" s="190" t="n"/>
     </row>
-    <row r="158">
-      <c r="C158" s="190" t="n"/>
-      <c r="D158" s="190" t="n"/>
-      <c r="E158" s="190" t="n"/>
-      <c r="F158" s="190" t="n"/>
-      <c r="G158" s="190" t="n"/>
-      <c r="H158" s="190" t="n"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix formatting across Tool Function Mapping and Tool Landscape
Tool Function Mapping:
- Apply consistent row fills based on risk level (Low/Medium/High/Severe)
- Fix rows 41-67 to have uniform color across all columns
- Severe rows now have white text for readability

AI Security Tool Landscape:
- Change all colors from transparent (00 prefix) to solid (FF prefix)
- Apply primary family color consistently across entire vendor rows
- Clear any color bleed into columns beyond H
- All 74 vendors now have proper solid color fills

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/AI_Security_Risk_Draft1.xlsx
+++ b/AI_Security_Risk_Draft1.xlsx
@@ -355,7 +355,7 @@
       <color rgb="FF000000"/>
     </font>
   </fonts>
-  <fills count="62">
+  <fills count="63">
     <fill>
       <patternFill/>
     </fill>
@@ -695,6 +695,12 @@
         <bgColor rgb="FFF8CBAD"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FFB4C6E7"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -816,7 +822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6"/>
   </cellStyleXfs>
-  <cellXfs count="326">
+  <cellXfs count="337">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1675,6 +1681,37 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="55" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="53" fillId="59" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="59" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="59" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="53" fillId="56" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="54" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="32" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="31" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="34" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="33" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="33" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="62" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10144,7 +10181,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H67"/>
+  <dimension ref="B2:H69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="20" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
@@ -10175,6 +10212,7 @@
         </is>
       </c>
     </row>
+    <row r="4"/>
     <row r="5" ht="16" customHeight="1">
       <c r="B5" s="15" t="inlineStr">
         <is>
@@ -10189,28 +10227,29 @@
         </is>
       </c>
     </row>
+    <row r="7"/>
     <row r="8">
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="326" t="inlineStr">
         <is>
           <t>Risk Factor</t>
         </is>
       </c>
-      <c r="C8" s="186" t="inlineStr">
+      <c r="C8" s="327" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="D8" s="187" t="inlineStr">
+      <c r="D8" s="327" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="E8" s="188" t="inlineStr">
+      <c r="E8" s="327" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="F8" s="204" t="inlineStr">
+      <c r="F8" s="327" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
@@ -10298,27 +10337,27 @@
       </c>
     </row>
     <row r="12" ht="26" customHeight="1">
-      <c r="B12" s="22" t="inlineStr">
+      <c r="B12" s="328" t="inlineStr">
         <is>
           <t>Misuse Potential</t>
         </is>
       </c>
-      <c r="C12" s="17" t="inlineStr">
+      <c r="C12" s="326" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="D12" s="18" t="inlineStr">
+      <c r="D12" s="326" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="E12" s="19" t="inlineStr">
+      <c r="E12" s="326" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="F12" s="205" t="inlineStr">
+      <c r="F12" s="326" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
@@ -10378,6 +10417,8 @@
         </is>
       </c>
     </row>
+    <row r="15"/>
+    <row r="16"/>
     <row r="17" ht="16" customHeight="1">
       <c r="B17" s="15" t="inlineStr">
         <is>
@@ -10392,6 +10433,7 @@
         </is>
       </c>
     </row>
+    <row r="19"/>
     <row r="20">
       <c r="B20" s="10" t="inlineStr">
         <is>
@@ -10431,135 +10473,135 @@
       <c r="F21" s="26" t="n"/>
     </row>
     <row r="22" ht="40" customHeight="1">
-      <c r="B22" s="8" t="inlineStr">
+      <c r="B22" s="326" t="inlineStr">
         <is>
           <t>Time, date, and timezone calculations</t>
         </is>
       </c>
-      <c r="C22" s="11" t="inlineStr">
+      <c r="C22" s="326" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="D22" s="8" t="inlineStr">
+      <c r="D22" s="326" t="inlineStr">
         <is>
           <t>Tool Registration; basic monitoring</t>
         </is>
       </c>
-      <c r="E22" s="8" t="inlineStr">
+      <c r="E22" s="326" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="F22" s="8" t="inlineStr">
+      <c r="F22" s="326" t="inlineStr">
         <is>
           <t>Posture</t>
         </is>
       </c>
     </row>
     <row r="23" ht="40" customHeight="1">
-      <c r="B23" s="8" t="inlineStr">
+      <c r="B23" s="326" t="inlineStr">
         <is>
           <t>Public data lookups (weather, rates, reference)</t>
         </is>
       </c>
-      <c r="C23" s="11" t="inlineStr">
+      <c r="C23" s="326" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="D23" s="8" t="inlineStr">
+      <c r="D23" s="326" t="inlineStr">
         <is>
           <t>Tool Registration; rate limiting recommended</t>
         </is>
       </c>
-      <c r="E23" s="8" t="inlineStr">
+      <c r="E23" s="326" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="F23" s="8" t="inlineStr">
+      <c r="F23" s="326" t="inlineStr">
         <is>
           <t>Posture, Runtime (optional)</t>
         </is>
       </c>
     </row>
     <row r="24" ht="40" customHeight="1">
-      <c r="B24" s="8" t="inlineStr">
+      <c r="B24" s="326" t="inlineStr">
         <is>
           <t>Geographic and mapping information</t>
         </is>
       </c>
-      <c r="C24" s="11" t="inlineStr">
+      <c r="C24" s="326" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="D24" s="8" t="inlineStr">
+      <c r="D24" s="326" t="inlineStr">
         <is>
           <t>Tool Registration; no PII in queries</t>
         </is>
       </c>
-      <c r="E24" s="8" t="inlineStr">
+      <c r="E24" s="326" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="F24" s="8" t="inlineStr">
+      <c r="F24" s="326" t="inlineStr">
         <is>
           <t>Posture</t>
         </is>
       </c>
     </row>
     <row r="25" ht="40" customHeight="1">
-      <c r="B25" s="8" t="inlineStr">
+      <c r="B25" s="326" t="inlineStr">
         <is>
           <t>Basic system health checks (read-only)</t>
         </is>
       </c>
-      <c r="C25" s="11" t="inlineStr">
+      <c r="C25" s="326" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="D25" s="8" t="inlineStr">
+      <c r="D25" s="326" t="inlineStr">
         <is>
           <t>Tool Registration; read-only access verified</t>
         </is>
       </c>
-      <c r="E25" s="8" t="inlineStr">
+      <c r="E25" s="326" t="inlineStr">
         <is>
           <t>Datadog, Arize AI (optional)</t>
         </is>
       </c>
-      <c r="F25" s="8" t="inlineStr">
+      <c r="F25" s="326" t="inlineStr">
         <is>
           <t>Posture, Observability (optional)</t>
         </is>
       </c>
     </row>
     <row r="26" ht="40" customHeight="1">
-      <c r="B26" s="8" t="inlineStr">
+      <c r="B26" s="326" t="inlineStr">
         <is>
           <t>Static file read (public/non-sensitive)</t>
         </is>
       </c>
-      <c r="C26" s="11" t="inlineStr">
+      <c r="C26" s="326" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="D26" s="8" t="inlineStr">
+      <c r="D26" s="326" t="inlineStr">
         <is>
           <t>Tool Registration; scoped to non-sensitive directories</t>
         </is>
       </c>
-      <c r="E26" s="8" t="inlineStr">
+      <c r="E26" s="326" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="F26" s="8" t="inlineStr">
+      <c r="F26" s="326" t="inlineStr">
         <is>
           <t>Posture</t>
         </is>
@@ -10577,324 +10619,324 @@
       <c r="F27" s="26" t="n"/>
     </row>
     <row r="28" ht="40" customHeight="1">
-      <c r="B28" s="8" t="inlineStr">
+      <c r="B28" s="329" t="inlineStr">
         <is>
           <t>Online search interfaces</t>
         </is>
       </c>
-      <c r="C28" s="12" t="inlineStr">
+      <c r="C28" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D28" s="8" t="inlineStr">
+      <c r="D28" s="329" t="inlineStr">
         <is>
           <t>Rate limits; DLP controls to prevent unintentional PII exposure</t>
         </is>
       </c>
-      <c r="E28" s="8" t="inlineStr">
+      <c r="E28" s="329" t="inlineStr">
         <is>
           <t>Harmonic, Nightfall, Netskope</t>
         </is>
       </c>
-      <c r="F28" s="8" t="inlineStr">
+      <c r="F28" s="329" t="inlineStr">
         <is>
           <t>Shadow AI, Data Protection</t>
         </is>
       </c>
     </row>
     <row r="29" ht="40" customHeight="1">
-      <c r="B29" s="8" t="inlineStr">
+      <c r="B29" s="329" t="inlineStr">
         <is>
           <t>Web data extraction / scraping</t>
         </is>
       </c>
-      <c r="C29" s="12" t="inlineStr">
+      <c r="C29" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D29" s="8" t="inlineStr">
+      <c r="D29" s="329" t="inlineStr">
         <is>
           <t>Restrict permitted domains; allowlist trusted sources only</t>
         </is>
       </c>
-      <c r="E29" s="8" t="inlineStr">
+      <c r="E29" s="329" t="inlineStr">
         <is>
           <t>Netskope, Zscaler, Island Browser</t>
         </is>
       </c>
-      <c r="F29" s="8" t="inlineStr">
+      <c r="F29" s="329" t="inlineStr">
         <is>
           <t>Data Protection</t>
         </is>
       </c>
     </row>
     <row r="30" ht="40" customHeight="1">
-      <c r="B30" s="8" t="inlineStr">
+      <c r="B30" s="329" t="inlineStr">
         <is>
           <t>Automated task execution (scoped)</t>
         </is>
       </c>
-      <c r="C30" s="12" t="inlineStr">
+      <c r="C30" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D30" s="8" t="inlineStr">
+      <c r="D30" s="329" t="inlineStr">
         <is>
           <t>Monitor for injection risks and unintended data leakage</t>
         </is>
       </c>
-      <c r="E30" s="8" t="inlineStr">
+      <c r="E30" s="329" t="inlineStr">
         <is>
           <t>Arthur AI, Mindgard, Datadog</t>
         </is>
       </c>
-      <c r="F30" s="8" t="inlineStr">
+      <c r="F30" s="329" t="inlineStr">
         <is>
           <t>Runtime, Observability</t>
         </is>
       </c>
     </row>
     <row r="31" ht="40" customHeight="1">
-      <c r="B31" s="8" t="inlineStr">
+      <c r="B31" s="329" t="inlineStr">
         <is>
           <t>Log processing and event analysis</t>
         </is>
       </c>
-      <c r="C31" s="12" t="inlineStr">
+      <c r="C31" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D31" s="8" t="inlineStr">
+      <c r="D31" s="329" t="inlineStr">
         <is>
           <t>Ensure sensitive details stripped before processing; restrict data access</t>
         </is>
       </c>
-      <c r="E31" s="8" t="inlineStr">
+      <c r="E31" s="329" t="inlineStr">
         <is>
           <t>Datadog, Arize AI, Splunk</t>
         </is>
       </c>
-      <c r="F31" s="8" t="inlineStr">
+      <c r="F31" s="329" t="inlineStr">
         <is>
           <t>Observability</t>
         </is>
       </c>
     </row>
     <row r="32" ht="40" customHeight="1">
-      <c r="B32" s="8" t="inlineStr">
+      <c r="B32" s="329" t="inlineStr">
         <is>
           <t>Enterprise data queries (read-only)</t>
         </is>
       </c>
-      <c r="C32" s="12" t="inlineStr">
+      <c r="C32" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D32" s="8" t="inlineStr">
+      <c r="D32" s="329" t="inlineStr">
         <is>
           <t>Limit permissions to read-only; periodically review access logs</t>
         </is>
       </c>
-      <c r="E32" s="8" t="inlineStr">
+      <c r="E32" s="329" t="inlineStr">
         <is>
           <t>Cyera, BigID, Knostic</t>
         </is>
       </c>
-      <c r="F32" s="8" t="inlineStr">
+      <c r="F32" s="329" t="inlineStr">
         <is>
           <t>Data Protection</t>
         </is>
       </c>
     </row>
     <row r="33" ht="40" customHeight="1">
-      <c r="B33" s="8" t="inlineStr">
+      <c r="B33" s="329" t="inlineStr">
         <is>
           <t>Internal documentation retrieval</t>
         </is>
       </c>
-      <c r="C33" s="12" t="inlineStr">
+      <c r="C33" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D33" s="8" t="inlineStr">
+      <c r="D33" s="329" t="inlineStr">
         <is>
           <t>Read-only access; access logging; scoped permissions</t>
         </is>
       </c>
-      <c r="E33" s="8" t="inlineStr">
+      <c r="E33" s="329" t="inlineStr">
         <is>
           <t>Knostic, Cyera, Reco.ai</t>
         </is>
       </c>
-      <c r="F33" s="8" t="inlineStr">
+      <c r="F33" s="329" t="inlineStr">
         <is>
           <t>Data Protection</t>
         </is>
       </c>
     </row>
     <row r="34" ht="40" customHeight="1">
-      <c r="B34" s="8" t="inlineStr">
+      <c r="B34" s="329" t="inlineStr">
         <is>
           <t>Code repository read access</t>
         </is>
       </c>
-      <c r="C34" s="12" t="inlineStr">
+      <c r="C34" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D34" s="8" t="inlineStr">
+      <c r="D34" s="329" t="inlineStr">
         <is>
           <t>Scoped to specific repos; access logging enabled</t>
         </is>
       </c>
-      <c r="E34" s="8" t="inlineStr">
+      <c r="E34" s="329" t="inlineStr">
         <is>
           <t>Wiz, Noma Security, HiddenLayer</t>
         </is>
       </c>
-      <c r="F34" s="8" t="inlineStr">
+      <c r="F34" s="329" t="inlineStr">
         <is>
           <t>AI Posture</t>
         </is>
       </c>
     </row>
     <row r="35" ht="40" customHeight="1">
-      <c r="B35" s="8" t="inlineStr">
+      <c r="B35" s="329" t="inlineStr">
         <is>
           <t>Email/chat/messaging read access</t>
         </is>
       </c>
-      <c r="C35" s="12" t="inlineStr">
+      <c r="C35" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D35" s="8" t="inlineStr">
+      <c r="D35" s="329" t="inlineStr">
         <is>
           <t>Scoped channels; PII redaction; query logging</t>
         </is>
       </c>
-      <c r="E35" s="8" t="inlineStr">
+      <c r="E35" s="329" t="inlineStr">
         <is>
           <t>Harmonic, Nightfall, Knostic</t>
         </is>
       </c>
-      <c r="F35" s="8" t="inlineStr">
+      <c r="F35" s="329" t="inlineStr">
         <is>
           <t>Shadow AI, Data Protection</t>
         </is>
       </c>
     </row>
     <row r="36" ht="40" customHeight="1">
-      <c r="B36" s="8" t="inlineStr">
+      <c r="B36" s="329" t="inlineStr">
         <is>
           <t>LLM prompt processing</t>
         </is>
       </c>
-      <c r="C36" s="12" t="inlineStr">
+      <c r="C36" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D36" s="8" t="inlineStr">
+      <c r="D36" s="329" t="inlineStr">
         <is>
           <t>Input validation; prompt injection detection; query logging</t>
         </is>
       </c>
-      <c r="E36" s="8" t="inlineStr">
+      <c r="E36" s="329" t="inlineStr">
         <is>
           <t>Arthur AI, Mindgard, Rebuff AI</t>
         </is>
       </c>
-      <c r="F36" s="8" t="inlineStr">
+      <c r="F36" s="329" t="inlineStr">
         <is>
           <t>Runtime Protection</t>
         </is>
       </c>
     </row>
     <row r="37" ht="40" customHeight="1">
-      <c r="B37" s="8" t="inlineStr">
+      <c r="B37" s="329" t="inlineStr">
         <is>
           <t>AI response generation</t>
         </is>
       </c>
-      <c r="C37" s="12" t="inlineStr">
+      <c r="C37" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D37" s="8" t="inlineStr">
+      <c r="D37" s="329" t="inlineStr">
         <is>
           <t>Output filtering for harmful content; hallucination detection</t>
         </is>
       </c>
-      <c r="E37" s="8" t="inlineStr">
+      <c r="E37" s="329" t="inlineStr">
         <is>
           <t>Arthur AI, Patronus AI, Arize AI</t>
         </is>
       </c>
-      <c r="F37" s="8" t="inlineStr">
+      <c r="F37" s="329" t="inlineStr">
         <is>
           <t>Runtime, Observability</t>
         </is>
       </c>
     </row>
     <row r="38" ht="40" customHeight="1">
-      <c r="B38" s="8" t="inlineStr">
+      <c r="B38" s="329" t="inlineStr">
         <is>
           <t>Vector database queries (read-only)</t>
         </is>
       </c>
-      <c r="C38" s="12" t="inlineStr">
+      <c r="C38" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D38" s="8" t="inlineStr">
+      <c r="D38" s="329" t="inlineStr">
         <is>
           <t>Access logging; scope to approved collections; no PII in embeddings</t>
         </is>
       </c>
-      <c r="E38" s="8" t="inlineStr">
+      <c r="E38" s="329" t="inlineStr">
         <is>
           <t>Knostic, Cyera, Wiz</t>
         </is>
       </c>
-      <c r="F38" s="8" t="inlineStr">
+      <c r="F38" s="329" t="inlineStr">
         <is>
           <t>Data Protection, AI Posture</t>
         </is>
       </c>
     </row>
     <row r="39" ht="40" customHeight="1">
-      <c r="B39" s="8" t="inlineStr">
+      <c r="B39" s="329" t="inlineStr">
         <is>
           <t>Prompt chaining / workflow orchestration</t>
         </is>
       </c>
-      <c r="C39" s="12" t="inlineStr">
+      <c r="C39" s="329" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D39" s="8" t="inlineStr">
+      <c r="D39" s="329" t="inlineStr">
         <is>
           <t>Monitor chain depth; log intermediate outputs; timeout limits</t>
         </is>
       </c>
-      <c r="E39" s="8" t="inlineStr">
+      <c r="E39" s="329" t="inlineStr">
         <is>
           <t>Arthur AI, LangSmith, Arize AI</t>
         </is>
       </c>
-      <c r="F39" s="8" t="inlineStr">
+      <c r="F39" s="329" t="inlineStr">
         <is>
           <t>Runtime, Observability</t>
         </is>
@@ -10912,405 +10954,405 @@
       <c r="F40" s="26" t="n"/>
     </row>
     <row r="41" ht="40" customHeight="1">
-      <c r="B41" s="8" t="inlineStr">
+      <c r="B41" s="330" t="inlineStr">
         <is>
           <t>Automated file handling (read/write)</t>
         </is>
       </c>
-      <c r="C41" s="13" t="inlineStr">
+      <c r="C41" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D41" s="8" t="inlineStr">
+      <c r="D41" s="330" t="inlineStr">
         <is>
           <t>Default to read-only; apply restrictions on sensitive directories; approval required</t>
         </is>
       </c>
-      <c r="E41" s="8" t="inlineStr">
+      <c r="E41" s="330" t="inlineStr">
         <is>
           <t>Cyera, BigID, Netskope</t>
         </is>
       </c>
-      <c r="F41" s="8" t="inlineStr">
+      <c r="F41" s="330" t="inlineStr">
         <is>
           <t>Data Protection</t>
         </is>
       </c>
     </row>
     <row r="42" ht="40" customHeight="1">
-      <c r="B42" s="8" t="inlineStr">
+      <c r="B42" s="330" t="inlineStr">
         <is>
           <t>Code repository write access</t>
         </is>
       </c>
-      <c r="C42" s="13" t="inlineStr">
+      <c r="C42" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D42" s="8" t="inlineStr">
+      <c r="D42" s="330" t="inlineStr">
         <is>
           <t>Approval required; maintain logging for AI-generated code changes</t>
         </is>
       </c>
-      <c r="E42" s="8" t="inlineStr">
+      <c r="E42" s="330" t="inlineStr">
         <is>
           <t>Noma, HiddenLayer, Wiz, CrowdStrike</t>
         </is>
       </c>
-      <c r="F42" s="8" t="inlineStr">
+      <c r="F42" s="330" t="inlineStr">
         <is>
           <t>AI Posture, Runtime</t>
         </is>
       </c>
     </row>
     <row r="43" ht="40" customHeight="1">
-      <c r="B43" s="8" t="inlineStr">
+      <c r="B43" s="330" t="inlineStr">
         <is>
           <t>Enterprise file indexing and search</t>
         </is>
       </c>
-      <c r="C43" s="13" t="inlineStr">
+      <c r="C43" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D43" s="8" t="inlineStr">
+      <c r="D43" s="330" t="inlineStr">
         <is>
           <t>Limit access to designated storage areas; read-only unless explicitly permitted</t>
         </is>
       </c>
-      <c r="E43" s="8" t="inlineStr">
+      <c r="E43" s="330" t="inlineStr">
         <is>
           <t>Knostic, Cyera, BigID</t>
         </is>
       </c>
-      <c r="F43" s="8" t="inlineStr">
+      <c r="F43" s="330" t="inlineStr">
         <is>
           <t>Data Protection</t>
         </is>
       </c>
     </row>
     <row r="44" ht="40" customHeight="1">
-      <c r="B44" s="8" t="inlineStr">
+      <c r="B44" s="330" t="inlineStr">
         <is>
           <t>Automated messaging/email send</t>
         </is>
       </c>
-      <c r="C44" s="13" t="inlineStr">
+      <c r="C44" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D44" s="8" t="inlineStr">
+      <c r="D44" s="330" t="inlineStr">
         <is>
           <t>Requires explicit approval; activate logging and monitoring</t>
         </is>
       </c>
-      <c r="E44" s="8" t="inlineStr">
+      <c r="E44" s="330" t="inlineStr">
         <is>
           <t>Arthur AI, Mindgard, Harmonic</t>
         </is>
       </c>
-      <c r="F44" s="8" t="inlineStr">
+      <c r="F44" s="330" t="inlineStr">
         <is>
           <t>Runtime, Data Protection</t>
         </is>
       </c>
     </row>
     <row r="45" ht="40" customHeight="1">
-      <c r="B45" s="8" t="inlineStr">
+      <c r="B45" s="330" t="inlineStr">
         <is>
           <t>AI memory and context storage</t>
         </is>
       </c>
-      <c r="C45" s="13" t="inlineStr">
+      <c r="C45" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D45" s="8" t="inlineStr">
+      <c r="D45" s="330" t="inlineStr">
         <is>
           <t>Encrypt stored data; apply retention policies; approval for confidential info</t>
         </is>
       </c>
-      <c r="E45" s="8" t="inlineStr">
+      <c r="E45" s="330" t="inlineStr">
         <is>
           <t>Knostic, Cyera, Noma, HiddenLayer</t>
         </is>
       </c>
-      <c r="F45" s="8" t="inlineStr">
+      <c r="F45" s="330" t="inlineStr">
         <is>
           <t>Data Protection, AI Posture</t>
         </is>
       </c>
     </row>
     <row r="46" ht="40" customHeight="1">
-      <c r="B46" s="8" t="inlineStr">
+      <c r="B46" s="330" t="inlineStr">
         <is>
           <t>Business intelligence system updates</t>
         </is>
       </c>
-      <c r="C46" s="13" t="inlineStr">
+      <c r="C46" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D46" s="8" t="inlineStr">
+      <c r="D46" s="330" t="inlineStr">
         <is>
           <t>Requires security clearance; strict logging and role-based access</t>
         </is>
       </c>
-      <c r="E46" s="8" t="inlineStr">
+      <c r="E46" s="330" t="inlineStr">
         <is>
           <t>Cyera, BigID, Silverfort</t>
         </is>
       </c>
-      <c r="F46" s="8" t="inlineStr">
+      <c r="F46" s="330" t="inlineStr">
         <is>
           <t>Data Protection, NHI</t>
         </is>
       </c>
     </row>
     <row r="47" ht="40" customHeight="1">
-      <c r="B47" s="8" t="inlineStr">
+      <c r="B47" s="330" t="inlineStr">
         <is>
           <t>HR/Financial/PII system access</t>
         </is>
       </c>
-      <c r="C47" s="13" t="inlineStr">
+      <c r="C47" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D47" s="8" t="inlineStr">
+      <c r="D47" s="330" t="inlineStr">
         <is>
           <t>MFA required; strict RBAC; committee approval; full audit logging</t>
         </is>
       </c>
-      <c r="E47" s="8" t="inlineStr">
+      <c r="E47" s="330" t="inlineStr">
         <is>
           <t>Silverfort, Cyera, ServiceNow</t>
         </is>
       </c>
-      <c r="F47" s="8" t="inlineStr">
+      <c r="F47" s="330" t="inlineStr">
         <is>
           <t>NHI, Data Protection</t>
         </is>
       </c>
     </row>
     <row r="48" ht="40" customHeight="1">
-      <c r="B48" s="8" t="inlineStr">
+      <c r="B48" s="330" t="inlineStr">
         <is>
           <t>Cloud storage access (S3/GCS/Azure)</t>
         </is>
       </c>
-      <c r="C48" s="13" t="inlineStr">
+      <c r="C48" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D48" s="8" t="inlineStr">
+      <c r="D48" s="330" t="inlineStr">
         <is>
           <t>Scoped IAM policies; encryption required; bucket/container policies enforced</t>
         </is>
       </c>
-      <c r="E48" s="8" t="inlineStr">
+      <c r="E48" s="330" t="inlineStr">
         <is>
           <t>Wiz, Cyera, AWS/GCP guardrails</t>
         </is>
       </c>
-      <c r="F48" s="8" t="inlineStr">
+      <c r="F48" s="330" t="inlineStr">
         <is>
           <t>Data Protection, AI Posture</t>
         </is>
       </c>
     </row>
     <row r="49" ht="40" customHeight="1">
-      <c r="B49" s="8" t="inlineStr">
+      <c r="B49" s="330" t="inlineStr">
         <is>
           <t>Agent-to-agent communication</t>
         </is>
       </c>
-      <c r="C49" s="13" t="inlineStr">
+      <c r="C49" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D49" s="8" t="inlineStr">
+      <c r="D49" s="330" t="inlineStr">
         <is>
           <t>mTLS required; short-lived credentials; intent validation</t>
         </is>
       </c>
-      <c r="E49" s="8" t="inlineStr">
+      <c r="E49" s="330" t="inlineStr">
         <is>
           <t>Silverfort, Astrix, Oasis, Aembit</t>
         </is>
       </c>
-      <c r="F49" s="8" t="inlineStr">
+      <c r="F49" s="330" t="inlineStr">
         <is>
           <t>NHI</t>
         </is>
       </c>
     </row>
     <row r="50" ht="40" customHeight="1">
-      <c r="B50" s="8" t="inlineStr">
+      <c r="B50" s="330" t="inlineStr">
         <is>
           <t>External API calls (outbound)</t>
         </is>
       </c>
-      <c r="C50" s="13" t="inlineStr">
+      <c r="C50" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D50" s="8" t="inlineStr">
+      <c r="D50" s="330" t="inlineStr">
         <is>
           <t>Allowlisted endpoints only; egress filtering; full request/response logging</t>
         </is>
       </c>
-      <c r="E50" s="8" t="inlineStr">
+      <c r="E50" s="330" t="inlineStr">
         <is>
           <t>Netskope, Zscaler, Arthur AI</t>
         </is>
       </c>
-      <c r="F50" s="8" t="inlineStr">
+      <c r="F50" s="330" t="inlineStr">
         <is>
           <t>Data Protection, Runtime</t>
         </is>
       </c>
     </row>
     <row r="51" ht="40" customHeight="1">
-      <c r="B51" s="8" t="inlineStr">
+      <c r="B51" s="330" t="inlineStr">
         <is>
           <t>Code execution (sandboxed environment)</t>
         </is>
       </c>
-      <c r="C51" s="13" t="inlineStr">
+      <c r="C51" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D51" s="8" t="inlineStr">
+      <c r="D51" s="330" t="inlineStr">
         <is>
           <t>Container isolation; resource limits; output validation; no network by default</t>
         </is>
       </c>
-      <c r="E51" s="8" t="inlineStr">
+      <c r="E51" s="330" t="inlineStr">
         <is>
           <t>Noma, HiddenLayer, Arthur AI</t>
         </is>
       </c>
-      <c r="F51" s="8" t="inlineStr">
+      <c r="F51" s="330" t="inlineStr">
         <is>
           <t>AI Posture, Runtime</t>
         </is>
       </c>
     </row>
     <row r="52" ht="40" customHeight="1">
-      <c r="B52" s="8" t="inlineStr">
+      <c r="B52" s="330" t="inlineStr">
         <is>
           <t>RAG with confidential documents</t>
         </is>
       </c>
-      <c r="C52" s="13" t="inlineStr">
+      <c r="C52" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D52" s="8" t="inlineStr">
+      <c r="D52" s="330" t="inlineStr">
         <is>
           <t>Access controls on source docs; vector store security; embedding integrity; audit retrieval; prevent data leakage</t>
         </is>
       </c>
-      <c r="E52" s="8" t="inlineStr">
+      <c r="E52" s="330" t="inlineStr">
         <is>
           <t>Knostic, Cyera, BigID, Wiz, Arthur AI</t>
         </is>
       </c>
-      <c r="F52" s="8" t="inlineStr">
+      <c r="F52" s="330" t="inlineStr">
         <is>
           <t>Data Protection, AI Supply Chain</t>
         </is>
       </c>
     </row>
     <row r="53" ht="40" customHeight="1">
-      <c r="B53" s="8" t="inlineStr">
+      <c r="B53" s="330" t="inlineStr">
         <is>
           <t>Tool/function calling by AI agents</t>
         </is>
       </c>
-      <c r="C53" s="13" t="inlineStr">
+      <c r="C53" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D53" s="8" t="inlineStr">
+      <c r="D53" s="330" t="inlineStr">
         <is>
           <t>Allowlist permitted tools; validate parameters; log all invocations; rate limits</t>
         </is>
       </c>
-      <c r="E53" s="8" t="inlineStr">
+      <c r="E53" s="330" t="inlineStr">
         <is>
           <t>Arthur AI, Noma, Oasis Security</t>
         </is>
       </c>
-      <c r="F53" s="8" t="inlineStr">
+      <c r="F53" s="330" t="inlineStr">
         <is>
           <t>Runtime, NHI</t>
         </is>
       </c>
     </row>
     <row r="54" ht="35" customHeight="1">
-      <c r="B54" s="259" t="inlineStr">
+      <c r="B54" s="322" t="inlineStr">
         <is>
           <t>MCP Server Integration</t>
         </is>
       </c>
-      <c r="C54" s="307" t="inlineStr">
+      <c r="C54" s="322" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D54" s="259" t="inlineStr">
+      <c r="D54" s="322" t="inlineStr">
         <is>
           <t>System prompt protection, tool authorization, input validation; secure MCP server configs</t>
         </is>
       </c>
-      <c r="E54" s="259" t="inlineStr">
+      <c r="E54" s="322" t="inlineStr">
         <is>
           <t>Lakera, Prompt Armor, Straiker</t>
         </is>
       </c>
-      <c r="F54" s="259" t="inlineStr">
+      <c r="F54" s="322" t="inlineStr">
         <is>
           <t>Runtime Protection, NHI &amp; Agentic Access</t>
         </is>
       </c>
     </row>
     <row r="55" ht="40" customHeight="1">
-      <c r="B55" s="8" t="inlineStr">
+      <c r="B55" s="330" t="inlineStr">
         <is>
           <t>Vector database write access</t>
         </is>
       </c>
-      <c r="C55" s="13" t="inlineStr">
+      <c r="C55" s="330" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="D55" s="8" t="inlineStr">
+      <c r="D55" s="330" t="inlineStr">
         <is>
           <t>Validate embeddings don't contain PII; access logging; approval for sensitive data</t>
         </is>
       </c>
-      <c r="E55" s="8" t="inlineStr">
+      <c r="E55" s="330" t="inlineStr">
         <is>
           <t>Knostic, Cyera, Wiz</t>
         </is>
       </c>
-      <c r="F55" s="8" t="inlineStr">
+      <c r="F55" s="330" t="inlineStr">
         <is>
           <t>Data Protection, AI Supply Chain</t>
         </is>
@@ -11444,194 +11486,196 @@
       <c r="H60" s="325" t="n"/>
     </row>
     <row r="61" ht="35" customHeight="1">
-      <c r="B61" s="262" t="inlineStr">
+      <c r="B61" s="324" t="inlineStr">
         <is>
           <t>Unrestricted code execution</t>
         </is>
       </c>
-      <c r="C61" s="309" t="inlineStr">
+      <c r="C61" s="324" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D61" s="262" t="inlineStr">
+      <c r="D61" s="324" t="inlineStr">
         <is>
           <t>Blocked by default; tool authorization, sandbox isolation, audit logging, strict containment strategies</t>
         </is>
       </c>
-      <c r="E61" s="262" t="inlineStr">
+      <c r="E61" s="324" t="inlineStr">
         <is>
           <t>Full stack + Zenity, Straiker, Spec</t>
         </is>
       </c>
-      <c r="F61" s="262" t="inlineStr">
+      <c r="F61" s="324" t="inlineStr">
         <is>
           <t>All 7 families</t>
         </is>
       </c>
     </row>
     <row r="62" ht="35" customHeight="1">
-      <c r="B62" s="262" t="inlineStr">
+      <c r="B62" s="324" t="inlineStr">
         <is>
           <t>Model fine-tuning with production data</t>
         </is>
       </c>
-      <c r="C62" s="309" t="inlineStr">
+      <c r="C62" s="324" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D62" s="262" t="inlineStr">
+      <c r="D62" s="324" t="inlineStr">
         <is>
           <t>Data governance review required; IP protection; formal approval with time limit</t>
         </is>
       </c>
-      <c r="E62" s="262" t="inlineStr">
+      <c r="E62" s="324" t="inlineStr">
         <is>
           <t>Noma, HiddenLayer, Cyera, BigID</t>
         </is>
       </c>
-      <c r="F62" s="262" t="inlineStr">
+      <c r="F62" s="324" t="inlineStr">
         <is>
           <t>AI Supply Chain, Data Protection</t>
         </is>
       </c>
     </row>
     <row r="63" ht="35" customHeight="1">
-      <c r="B63" s="262" t="inlineStr">
+      <c r="B63" s="324" t="inlineStr">
         <is>
           <t>Infrastructure automation (Terraform, K8s)</t>
         </is>
       </c>
-      <c r="C63" s="309" t="inlineStr">
+      <c r="C63" s="324" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D63" s="262" t="inlineStr">
+      <c r="D63" s="324" t="inlineStr">
         <is>
           <t>Prohibited by default; requires full security review; admin rights must be scoped</t>
         </is>
       </c>
-      <c r="E63" s="262" t="inlineStr">
+      <c r="E63" s="324" t="inlineStr">
         <is>
           <t>Silverfort, Astrix + full review</t>
         </is>
       </c>
-      <c r="F63" s="262" t="inlineStr">
+      <c r="F63" s="324" t="inlineStr">
         <is>
           <t>NHI, AI Posture</t>
         </is>
       </c>
     </row>
     <row r="64" ht="35" customHeight="1">
-      <c r="B64" s="262" t="inlineStr">
+      <c r="B64" s="324" t="inlineStr">
         <is>
           <t>Autonomous agent with unrestricted API access</t>
         </is>
       </c>
-      <c r="C64" s="309" t="inlineStr">
+      <c r="C64" s="324" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D64" s="262" t="inlineStr">
+      <c r="D64" s="324" t="inlineStr">
         <is>
           <t>Prohibited by default; formal exception with strict monitoring and kill switch</t>
         </is>
       </c>
-      <c r="E64" s="262" t="inlineStr">
+      <c r="E64" s="324" t="inlineStr">
         <is>
           <t>Full stack + continuous monitoring</t>
         </is>
       </c>
-      <c r="F64" s="262" t="inlineStr">
+      <c r="F64" s="324" t="inlineStr">
         <is>
           <t>All 7 families</t>
         </is>
       </c>
     </row>
     <row r="65" ht="35" customHeight="1">
-      <c r="B65" s="262" t="inlineStr">
+      <c r="B65" s="324" t="inlineStr">
         <is>
           <t>Multi-agent orchestration (autonomous)</t>
         </is>
       </c>
-      <c r="C65" s="309" t="inlineStr">
+      <c r="C65" s="324" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D65" s="262" t="inlineStr">
+      <c r="D65" s="324" t="inlineStr">
         <is>
           <t>Prohibited by default; requires agent inventory, boundary controls, tool authorization, autonomous action limits, kill switches</t>
         </is>
       </c>
-      <c r="E65" s="262" t="inlineStr">
+      <c r="E65" s="324" t="inlineStr">
         <is>
           <t>Zenity, Oasis, Astrix, Straiker, Invariant Labs</t>
         </is>
       </c>
-      <c r="F65" s="262" t="inlineStr">
+      <c r="F65" s="324" t="inlineStr">
         <is>
           <t>NHI, AI Posture</t>
         </is>
       </c>
     </row>
     <row r="66" ht="35" customHeight="1">
-      <c r="B66" s="262" t="inlineStr">
+      <c r="B66" s="324" t="inlineStr">
         <is>
           <t>Agent task delegation / spawning</t>
         </is>
       </c>
-      <c r="C66" s="309" t="inlineStr">
+      <c r="C66" s="324" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D66" s="262" t="inlineStr">
+      <c r="D66" s="324" t="inlineStr">
         <is>
           <t>Prohibited by default; limit spawn depth; enforce resource quotas; audit lineage</t>
         </is>
       </c>
-      <c r="E66" s="262" t="inlineStr">
+      <c r="E66" s="324" t="inlineStr">
         <is>
           <t>Zenity, Noma, Oasis Security</t>
         </is>
       </c>
-      <c r="F66" s="262" t="inlineStr">
+      <c r="F66" s="324" t="inlineStr">
         <is>
           <t>NHI, AI Posture</t>
         </is>
       </c>
     </row>
     <row r="67" ht="35" customHeight="1">
-      <c r="B67" s="262" t="inlineStr">
+      <c r="B67" s="324" t="inlineStr">
         <is>
           <t>Autonomous decision-making (no human review)</t>
         </is>
       </c>
-      <c r="C67" s="309" t="inlineStr">
+      <c r="C67" s="324" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D67" s="262" t="inlineStr">
+      <c r="D67" s="324" t="inlineStr">
         <is>
           <t>Prohibited for consequential decisions; requires formal exception and audit trail</t>
         </is>
       </c>
-      <c r="E67" s="262" t="inlineStr">
+      <c r="E67" s="324" t="inlineStr">
         <is>
           <t>Full stack + mandatory logging</t>
         </is>
       </c>
-      <c r="F67" s="262" t="inlineStr">
+      <c r="F67" s="324" t="inlineStr">
         <is>
           <t>All 7 families</t>
         </is>
       </c>
     </row>
+    <row r="68"/>
+    <row r="69"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B21:F21"/>
@@ -16142,7 +16186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H157"/>
+  <dimension ref="B2:K157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
@@ -16362,222 +16406,222 @@
       </c>
     </row>
     <row r="17" ht="40" customHeight="1">
-      <c r="B17" s="262" t="inlineStr">
+      <c r="B17" s="319" t="inlineStr">
         <is>
           <t>Acuvity</t>
         </is>
       </c>
-      <c r="C17" s="262" t="inlineStr">
+      <c r="C17" s="319" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D17" s="276" t="inlineStr">
+      <c r="D17" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E17" s="281" t="inlineStr">
+      <c r="E17" s="319" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F17" s="279" t="inlineStr">
+      <c r="F17" s="319" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="G17" s="262" t="inlineStr">
+      <c r="G17" s="319" t="inlineStr">
         <is>
           <t>Unified discovery, governance, data protection across AI landscape</t>
         </is>
       </c>
-      <c r="H17" s="262" t="inlineStr">
+      <c r="H17" s="319" t="inlineStr">
         <is>
           <t>Consolidating AI security into one platform</t>
         </is>
       </c>
     </row>
     <row r="18" ht="40" customHeight="1">
-      <c r="B18" s="262" t="inlineStr">
+      <c r="B18" s="319" t="inlineStr">
         <is>
           <t>Airia</t>
         </is>
       </c>
-      <c r="C18" s="262" t="inlineStr">
+      <c r="C18" s="319" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D18" s="276" t="inlineStr">
+      <c r="D18" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E18" s="282" t="inlineStr">
+      <c r="E18" s="319" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F18" s="280" t="inlineStr">
+      <c r="F18" s="319" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G18" s="262" t="inlineStr">
+      <c r="G18" s="319" t="inlineStr">
         <is>
           <t>Three-pillar platform (Q1 2026): AI Security, AI Governance, Agent Orchestration; unified enterprise AI management.</t>
         </is>
       </c>
-      <c r="H18" s="262" t="inlineStr">
+      <c r="H18" s="319" t="inlineStr">
         <is>
           <t>Enterprises needing unified AI governance</t>
         </is>
       </c>
     </row>
     <row r="19" ht="40" customHeight="1">
-      <c r="B19" s="262" t="inlineStr">
+      <c r="B19" s="319" t="inlineStr">
         <is>
           <t>Cato Networks (AIM Security)</t>
         </is>
       </c>
-      <c r="C19" s="262" t="inlineStr">
+      <c r="C19" s="319" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D19" s="276" t="inlineStr">
+      <c r="D19" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E19" s="280" t="inlineStr">
+      <c r="E19" s="319" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F19" s="279" t="inlineStr">
+      <c r="F19" s="319" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="G19" s="262" t="inlineStr">
+      <c r="G19" s="319" t="inlineStr">
         <is>
           <t>AI-SPM + agent security via AIM Security acquisition; SASE integration</t>
         </is>
       </c>
-      <c r="H19" s="262" t="inlineStr">
+      <c r="H19" s="319" t="inlineStr">
         <is>
           <t>Cato SASE customers</t>
         </is>
       </c>
     </row>
     <row r="20" ht="40" customHeight="1">
-      <c r="B20" s="262" t="inlineStr">
+      <c r="B20" s="319" t="inlineStr">
         <is>
           <t>Cisco (Robust Intelligence)</t>
         </is>
       </c>
-      <c r="C20" s="262" t="inlineStr">
+      <c r="C20" s="319" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D20" s="276" t="inlineStr">
+      <c r="D20" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E20" s="277" t="inlineStr">
+      <c r="E20" s="319" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F20" s="279" t="inlineStr">
+      <c r="F20" s="319" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="G20" s="262" t="inlineStr">
+      <c r="G20" s="319" t="inlineStr">
         <is>
           <t>Network-layer AI security via Robust Intelligence: model validation, supply chain, guardrails</t>
         </is>
       </c>
-      <c r="H20" s="262" t="inlineStr">
+      <c r="H20" s="319" t="inlineStr">
         <is>
           <t>Cisco customers; agentless deployment</t>
         </is>
       </c>
     </row>
     <row r="21" ht="40" customHeight="1">
-      <c r="B21" s="262" t="inlineStr">
+      <c r="B21" s="319" t="inlineStr">
         <is>
           <t>Credo AI</t>
         </is>
       </c>
-      <c r="C21" s="262" t="inlineStr">
+      <c r="C21" s="319" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D21" s="276" t="inlineStr">
+      <c r="D21" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E21" s="278" t="inlineStr">
+      <c r="E21" s="319" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F21" s="277" t="inlineStr">
+      <c r="F21" s="319" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="G21" s="262" t="inlineStr">
+      <c r="G21" s="319" t="inlineStr">
         <is>
           <t>AI governance platform: centralizes policies, risk assessments, model inventory, supply chain tracking</t>
         </is>
       </c>
-      <c r="H21" s="262" t="inlineStr">
+      <c r="H21" s="319" t="inlineStr">
         <is>
           <t>AI governance and vendor risk management</t>
         </is>
       </c>
     </row>
     <row r="22" ht="40" customHeight="1">
-      <c r="B22" s="262" t="inlineStr">
+      <c r="B22" s="319" t="inlineStr">
         <is>
           <t>CrowdStrike (Pangea)</t>
         </is>
       </c>
-      <c r="C22" s="262" t="inlineStr">
+      <c r="C22" s="319" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D22" s="276" t="inlineStr">
+      <c r="D22" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E22" s="280" t="inlineStr">
+      <c r="E22" s="319" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F22" s="277" t="inlineStr">
+      <c r="F22" s="319" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="G22" s="262" t="inlineStr">
+      <c r="G22" s="319" t="inlineStr">
         <is>
           <t>Charlotte AI for SOC + Pangea adds guardrails, prompt defense, model security</t>
         </is>
       </c>
-      <c r="H22" s="262" t="inlineStr">
+      <c r="H22" s="319" t="inlineStr">
         <is>
           <t>CrowdStrike customers; endpoint-centric orgs</t>
         </is>
@@ -16621,2183 +16665,2183 @@
       </c>
     </row>
     <row r="24" ht="40" customHeight="1">
-      <c r="B24" s="262" t="inlineStr">
+      <c r="B24" s="319" t="inlineStr">
         <is>
           <t>Holistic AI</t>
         </is>
       </c>
-      <c r="C24" s="262" t="inlineStr">
+      <c r="C24" s="319" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D24" s="276" t="inlineStr">
+      <c r="D24" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E24" s="278" t="inlineStr">
+      <c r="E24" s="319" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F24" s="262" t="inlineStr">
+      <c r="F24" s="319" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G24" s="262" t="inlineStr">
+      <c r="G24" s="319" t="inlineStr">
         <is>
           <t>End-to-end AI risk management: live AI system inventory; EU AI Act alignment; bias auditing; regulatory compliance focus.</t>
         </is>
       </c>
-      <c r="H24" s="262" t="inlineStr">
+      <c r="H24" s="319" t="inlineStr">
         <is>
           <t>EU AI Act compliance; risk management</t>
         </is>
       </c>
     </row>
     <row r="25" ht="40" customHeight="1">
-      <c r="B25" s="262" t="inlineStr">
+      <c r="B25" s="319" t="inlineStr">
         <is>
           <t>Microsoft Defender for Cloud</t>
         </is>
       </c>
-      <c r="C25" s="262" t="inlineStr">
+      <c r="C25" s="319" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="D25" s="276" t="inlineStr">
+      <c r="D25" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E25" s="280" t="inlineStr">
+      <c r="E25" s="319" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F25" s="281" t="inlineStr">
+      <c r="F25" s="319" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G25" s="262" t="inlineStr">
+      <c r="G25" s="319" t="inlineStr">
         <is>
           <t>Multi-cloud AI-SPM, OWASP Top 10 for LLMs, Azure AI Content Safety integration</t>
         </is>
       </c>
-      <c r="H25" s="262" t="inlineStr">
+      <c r="H25" s="319" t="inlineStr">
         <is>
           <t>Azure/M365 shops; broadest native coverage</t>
         </is>
       </c>
     </row>
     <row r="26" ht="40" customHeight="1">
-      <c r="B26" s="262" t="inlineStr">
+      <c r="B26" s="319" t="inlineStr">
         <is>
           <t>Noma Security</t>
         </is>
       </c>
-      <c r="C26" s="262" t="inlineStr">
+      <c r="C26" s="319" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D26" s="276" t="inlineStr">
+      <c r="D26" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E26" s="277" t="inlineStr">
+      <c r="E26" s="319" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F26" s="278" t="inlineStr">
+      <c r="F26" s="319" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G26" s="262" t="inlineStr">
+      <c r="G26" s="319" t="inlineStr">
         <is>
           <t>Fastest-growing ($132M raised): full AI lifecycle including supply chain, agentic AI focus</t>
         </is>
       </c>
-      <c r="H26" s="262" t="inlineStr">
+      <c r="H26" s="319" t="inlineStr">
         <is>
           <t>Comprehensive AI security; agentic deployments</t>
         </is>
       </c>
     </row>
     <row r="27" ht="40" customHeight="1">
-      <c r="B27" s="262" t="inlineStr">
+      <c r="B27" s="319" t="inlineStr">
         <is>
           <t>Palo Alto Networks (Protect AI)</t>
         </is>
       </c>
-      <c r="C27" s="262" t="inlineStr">
+      <c r="C27" s="319" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D27" s="276" t="inlineStr">
+      <c r="D27" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E27" s="277" t="inlineStr">
+      <c r="E27" s="319" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F27" s="278" t="inlineStr">
+      <c r="F27" s="319" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G27" s="262" t="inlineStr">
+      <c r="G27" s="319" t="inlineStr">
         <is>
           <t>Full-stack AI security via Protect AI: ML supply chain, model scanning, runtime, red teaming</t>
         </is>
       </c>
-      <c r="H27" s="262" t="inlineStr">
+      <c r="H27" s="319" t="inlineStr">
         <is>
           <t>Palo Alto customers; integrated platform play</t>
         </is>
       </c>
     </row>
     <row r="28" ht="40" customHeight="1">
-      <c r="B28" s="262" t="inlineStr">
+      <c r="B28" s="319" t="inlineStr">
         <is>
           <t>ServiceNow</t>
         </is>
       </c>
-      <c r="C28" s="262" t="inlineStr">
+      <c r="C28" s="319" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="D28" s="276" t="inlineStr">
+      <c r="D28" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E28" s="278" t="inlineStr">
+      <c r="E28" s="319" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F28" s="282" t="inlineStr">
+      <c r="F28" s="319" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="G28" s="262" t="inlineStr">
+      <c r="G28" s="319" t="inlineStr">
         <is>
           <t>AI Governance for Now Assist: AI Control Tower, usage tracking, compliance workflows</t>
         </is>
       </c>
-      <c r="H28" s="262" t="inlineStr">
+      <c r="H28" s="319" t="inlineStr">
         <is>
           <t>ServiceNow customers; IT/GRC-centric governance</t>
         </is>
       </c>
     </row>
     <row r="29" ht="40" customHeight="1">
-      <c r="B29" s="262" t="inlineStr">
+      <c r="B29" s="319" t="inlineStr">
         <is>
           <t>WitnessAI</t>
         </is>
       </c>
-      <c r="C29" s="262" t="inlineStr">
+      <c r="C29" s="319" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D29" s="276" t="inlineStr">
+      <c r="D29" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E29" s="279" t="inlineStr">
+      <c r="E29" s="319" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F29" s="280" t="inlineStr">
+      <c r="F29" s="319" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G29" s="262" t="inlineStr">
+      <c r="G29" s="319" t="inlineStr">
         <is>
           <t>Discovers AI usage, enforces policy, coaches users on safe AI practices</t>
         </is>
       </c>
-      <c r="H29" s="262" t="inlineStr">
+      <c r="H29" s="319" t="inlineStr">
         <is>
           <t>Safe AI enablement with visibility and coaching</t>
         </is>
       </c>
     </row>
     <row r="30" ht="40" customHeight="1">
-      <c r="B30" s="262" t="inlineStr">
+      <c r="B30" s="319" t="inlineStr">
         <is>
           <t>Wiz</t>
         </is>
       </c>
-      <c r="C30" s="262" t="inlineStr">
+      <c r="C30" s="319" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D30" s="276" t="inlineStr">
+      <c r="D30" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E30" s="279" t="inlineStr">
+      <c r="E30" s="319" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F30" s="278" t="inlineStr">
+      <c r="F30" s="319" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G30" s="262" t="inlineStr">
+      <c r="G30" s="319" t="inlineStr">
         <is>
           <t>CNAPP-native AI-SPM: agentless discovery, risk prioritization, compliance mapping</t>
         </is>
       </c>
-      <c r="H30" s="262" t="inlineStr">
+      <c r="H30" s="319" t="inlineStr">
         <is>
           <t>Wiz customers; cloud-native AI workloads</t>
         </is>
       </c>
     </row>
     <row r="31" ht="40" customHeight="1">
-      <c r="B31" s="262" t="inlineStr">
+      <c r="B31" s="319" t="inlineStr">
         <is>
           <t>Zenity</t>
         </is>
       </c>
-      <c r="C31" s="262" t="inlineStr">
+      <c r="C31" s="319" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D31" s="276" t="inlineStr">
+      <c r="D31" s="319" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E31" s="282" t="inlineStr">
+      <c r="E31" s="319" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F31" s="280" t="inlineStr">
+      <c r="F31" s="319" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G31" s="262" t="inlineStr">
+      <c r="G31" s="319" t="inlineStr">
         <is>
           <t>Agent-centric posture management; low-code/copilot security specialist</t>
         </is>
       </c>
-      <c r="H31" s="262" t="inlineStr">
+      <c r="H31" s="319" t="inlineStr">
         <is>
           <t>Organizations deploying AI agents at scale</t>
         </is>
       </c>
     </row>
     <row r="32" ht="40" customHeight="1">
-      <c r="B32" s="262" t="inlineStr">
+      <c r="B32" s="331" t="inlineStr">
         <is>
           <t>Arthur AI</t>
         </is>
       </c>
-      <c r="C32" s="262" t="inlineStr">
+      <c r="C32" s="331" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D32" s="280" t="inlineStr">
+      <c r="D32" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E32" s="278" t="inlineStr">
+      <c r="E32" s="331" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F32" s="276" t="inlineStr">
+      <c r="F32" s="331" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G32" s="262" t="inlineStr">
+      <c r="G32" s="331" t="inlineStr">
         <is>
           <t>LLM firewall + observability ($60M raised): federated architecture, data stays local</t>
         </is>
       </c>
-      <c r="H32" s="262" t="inlineStr">
+      <c r="H32" s="331" t="inlineStr">
         <is>
           <t>Regulated industries; data residency requirements</t>
         </is>
       </c>
     </row>
     <row r="33" ht="40" customHeight="1">
-      <c r="B33" s="262" t="inlineStr">
+      <c r="B33" s="331" t="inlineStr">
         <is>
           <t>Check Point (Lakera)</t>
         </is>
       </c>
-      <c r="C33" s="262" t="inlineStr">
+      <c r="C33" s="331" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D33" s="280" t="inlineStr">
+      <c r="D33" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E33" s="276" t="inlineStr">
+      <c r="E33" s="331" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F33" s="277" t="inlineStr">
+      <c r="F33" s="331" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="G33" s="262" t="inlineStr">
+      <c r="G33" s="331" t="inlineStr">
         <is>
           <t>Lakera adds runtime guardrails, prompt injection defense, model security to Infinity</t>
         </is>
       </c>
-      <c r="H33" s="262" t="inlineStr">
+      <c r="H33" s="331" t="inlineStr">
         <is>
           <t>Check Point customers; Infinity stack users</t>
         </is>
       </c>
     </row>
     <row r="34" ht="40" customHeight="1">
-      <c r="B34" s="262" t="inlineStr">
+      <c r="B34" s="331" t="inlineStr">
         <is>
           <t>F5 (CalypsoAI)</t>
         </is>
       </c>
-      <c r="C34" s="262" t="inlineStr">
+      <c r="C34" s="331" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D34" s="280" t="inlineStr">
+      <c r="D34" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E34" s="278" t="inlineStr">
+      <c r="E34" s="331" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F34" s="277" t="inlineStr">
+      <c r="F34" s="331" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="G34" s="262" t="inlineStr">
+      <c r="G34" s="331" t="inlineStr">
         <is>
           <t>Inference protection + red-teaming via CalypsoAI; model testing, API security</t>
         </is>
       </c>
-      <c r="H34" s="262" t="inlineStr">
+      <c r="H34" s="331" t="inlineStr">
         <is>
           <t>F5 customers; API/app security integration</t>
         </is>
       </c>
     </row>
     <row r="35" ht="40" customHeight="1">
-      <c r="B35" s="262" t="inlineStr">
+      <c r="B35" s="331" t="inlineStr">
         <is>
           <t>Hex Security</t>
         </is>
       </c>
-      <c r="C35" s="262" t="inlineStr">
+      <c r="C35" s="331" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D35" s="280" t="inlineStr">
+      <c r="D35" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E35" s="276" t="inlineStr">
+      <c r="E35" s="331" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F35" s="262" t="inlineStr">
+      <c r="F35" s="331" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G35" s="262" t="inlineStr">
+      <c r="G35" s="331" t="inlineStr">
         <is>
           <t>Y Combinator-backed: AI agents running continuous pen tests; 24/7 vulnerability discovery and verification.</t>
         </is>
       </c>
-      <c r="H35" s="262" t="inlineStr">
+      <c r="H35" s="331" t="inlineStr">
         <is>
           <t>Continuous security testing; red team automation</t>
         </is>
       </c>
     </row>
     <row r="36" ht="40" customHeight="1">
-      <c r="B36" s="262" t="inlineStr">
+      <c r="B36" s="331" t="inlineStr">
         <is>
           <t>Invariant Labs</t>
         </is>
       </c>
-      <c r="C36" s="262" t="inlineStr">
+      <c r="C36" s="331" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D36" s="280" t="inlineStr">
+      <c r="D36" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E36" s="282" t="inlineStr">
+      <c r="E36" s="331" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F36" s="278" t="inlineStr">
+      <c r="F36" s="331" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G36" s="262" t="inlineStr">
+      <c r="G36" s="331" t="inlineStr">
         <is>
           <t>Agent security testing and guardrails; detects agent vulnerabilities and failures</t>
         </is>
       </c>
-      <c r="H36" s="262" t="inlineStr">
+      <c r="H36" s="331" t="inlineStr">
         <is>
           <t>Agentic AI security testing; agent-specific threats</t>
         </is>
       </c>
     </row>
     <row r="37" ht="40" customHeight="1">
-      <c r="B37" s="262" t="inlineStr">
+      <c r="B37" s="331" t="inlineStr">
         <is>
           <t>LLM Guard</t>
         </is>
       </c>
-      <c r="C37" s="262" t="inlineStr">
+      <c r="C37" s="331" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D37" s="280" t="inlineStr">
+      <c r="D37" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E37" s="281" t="inlineStr">
+      <c r="E37" s="331" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F37" s="262" t="inlineStr">
+      <c r="F37" s="331" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G37" s="262" t="inlineStr">
+      <c r="G37" s="331" t="inlineStr">
         <is>
           <t>Open source input/output scanner; PII detection, toxicity, prompt injection</t>
         </is>
       </c>
-      <c r="H37" s="262" t="inlineStr">
+      <c r="H37" s="331" t="inlineStr">
         <is>
           <t>OSS-first orgs; customizable guardrails</t>
         </is>
       </c>
     </row>
     <row r="38" ht="40" customHeight="1">
-      <c r="B38" s="262" t="inlineStr">
+      <c r="B38" s="331" t="inlineStr">
         <is>
           <t>Mindgard</t>
         </is>
       </c>
-      <c r="C38" s="262" t="inlineStr">
+      <c r="C38" s="331" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D38" s="280" t="inlineStr">
+      <c r="D38" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E38" s="278" t="inlineStr">
+      <c r="E38" s="331" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F38" s="277" t="inlineStr">
+      <c r="F38" s="331" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="G38" s="262" t="inlineStr">
+      <c r="G38" s="331" t="inlineStr">
         <is>
           <t>Offensive AI security: automated red teaming, model vulnerability scanning, supply chain testing</t>
         </is>
       </c>
-      <c r="H38" s="262" t="inlineStr">
+      <c r="H38" s="331" t="inlineStr">
         <is>
           <t>Continuous AI security testing; red team automation</t>
         </is>
       </c>
     </row>
     <row r="39" ht="40" customHeight="1">
-      <c r="B39" s="262" t="inlineStr">
+      <c r="B39" s="331" t="inlineStr">
         <is>
           <t>NVIDIA NeMo Guardrails</t>
         </is>
       </c>
-      <c r="C39" s="262" t="inlineStr">
+      <c r="C39" s="331" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="D39" s="280" t="inlineStr">
+      <c r="D39" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E39" s="278" t="inlineStr">
+      <c r="E39" s="331" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F39" s="262" t="inlineStr">
+      <c r="F39" s="331" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G39" s="262" t="inlineStr">
+      <c r="G39" s="331" t="inlineStr">
         <is>
           <t>Inference microservices (GA Jan 2025): programmable guardrails for LLMs; safety, security, control for AI applications.</t>
         </is>
       </c>
-      <c r="H39" s="262" t="inlineStr">
+      <c r="H39" s="331" t="inlineStr">
         <is>
           <t>NVIDIA ecosystem; custom guardrail logic</t>
         </is>
       </c>
     </row>
     <row r="40" ht="40" customHeight="1">
-      <c r="B40" s="262" t="inlineStr">
+      <c r="B40" s="331" t="inlineStr">
         <is>
           <t>Prompt Armor</t>
         </is>
       </c>
-      <c r="C40" s="262" t="inlineStr">
+      <c r="C40" s="331" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D40" s="280" t="inlineStr">
+      <c r="D40" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E40" s="281" t="inlineStr">
+      <c r="E40" s="331" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F40" s="278" t="inlineStr">
+      <c r="F40" s="331" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G40" s="262" t="inlineStr">
+      <c r="G40" s="331" t="inlineStr">
         <is>
           <t>Prompt injection firewall; real-time threat detection for LLM applications</t>
         </is>
       </c>
-      <c r="H40" s="262" t="inlineStr">
+      <c r="H40" s="331" t="inlineStr">
         <is>
           <t>Dedicated prompt security; API-first deployment</t>
         </is>
       </c>
     </row>
     <row r="41" ht="40" customHeight="1">
-      <c r="B41" s="262" t="inlineStr">
+      <c r="B41" s="331" t="inlineStr">
         <is>
           <t>Rebuff AI</t>
         </is>
       </c>
-      <c r="C41" s="262" t="inlineStr">
+      <c r="C41" s="331" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D41" s="280" t="inlineStr">
+      <c r="D41" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E41" s="278" t="inlineStr">
+      <c r="E41" s="331" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F41" s="262" t="inlineStr">
+      <c r="F41" s="331" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G41" s="262" t="inlineStr">
+      <c r="G41" s="331" t="inlineStr">
         <is>
           <t>Open source prompt injection detection; self-hardening through attack learning</t>
         </is>
       </c>
-      <c r="H41" s="262" t="inlineStr">
+      <c r="H41" s="331" t="inlineStr">
         <is>
           <t>Teams wanting OSS guardrails; cost-conscious</t>
         </is>
       </c>
     </row>
     <row r="42" ht="40" customHeight="1">
-      <c r="B42" s="262" t="inlineStr">
+      <c r="B42" s="331" t="inlineStr">
         <is>
           <t>Straiker Defend AI</t>
         </is>
       </c>
-      <c r="C42" s="262" t="inlineStr">
+      <c r="C42" s="331" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D42" s="280" t="inlineStr">
+      <c r="D42" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E42" s="282" t="inlineStr">
+      <c r="E42" s="331" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F42" s="278" t="inlineStr">
+      <c r="F42" s="331" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G42" s="262" t="inlineStr">
+      <c r="G42" s="331" t="inlineStr">
         <is>
           <t>Agentic AI runtime security ($21M Series A, Lightspeed): fast context-aware guardrails; inspects prompts, reasoning steps, tool calls; stops prompt injection, data leaks, agent manipulation.</t>
         </is>
       </c>
-      <c r="H42" s="262" t="inlineStr">
+      <c r="H42" s="331" t="inlineStr">
         <is>
           <t>Production agentic AI; real-time agent security</t>
         </is>
       </c>
     </row>
     <row r="43" ht="40" customHeight="1">
-      <c r="B43" s="262" t="inlineStr">
+      <c r="B43" s="331" t="inlineStr">
         <is>
           <t>TrojAI</t>
         </is>
       </c>
-      <c r="C43" s="262" t="inlineStr">
+      <c r="C43" s="331" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D43" s="280" t="inlineStr">
+      <c r="D43" s="331" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E43" s="277" t="inlineStr">
+      <c r="E43" s="331" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F43" s="278" t="inlineStr">
+      <c r="F43" s="331" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="G43" s="262" t="inlineStr">
+      <c r="G43" s="331" t="inlineStr">
         <is>
           <t>Model threat protection: detects backdoors, adversarial attacks, model poisoning; supply chain focus</t>
         </is>
       </c>
-      <c r="H43" s="262" t="inlineStr">
+      <c r="H43" s="331" t="inlineStr">
         <is>
           <t>Deep model hardening beyond prompt-level</t>
         </is>
       </c>
     </row>
     <row r="44" ht="40" customHeight="1">
-      <c r="B44" s="262" t="inlineStr">
+      <c r="B44" s="332" t="inlineStr">
         <is>
           <t>Adri</t>
         </is>
       </c>
-      <c r="C44" s="262" t="inlineStr">
+      <c r="C44" s="332" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D44" s="279" t="inlineStr">
+      <c r="D44" s="332" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E44" s="281" t="inlineStr">
+      <c r="E44" s="332" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F44" s="276" t="inlineStr">
+      <c r="F44" s="332" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G44" s="262" t="inlineStr">
+      <c r="G44" s="332" t="inlineStr">
         <is>
           <t>Y Combinator-backed: patented technology monitoring AI vendor infrastructure; detects intentional/accidental misuse of proprietary data.</t>
         </is>
       </c>
-      <c r="H44" s="262" t="inlineStr">
+      <c r="H44" s="332" t="inlineStr">
         <is>
           <t>IP protection; AI vendor monitoring</t>
         </is>
       </c>
     </row>
     <row r="45" ht="40" customHeight="1">
-      <c r="B45" s="262" t="inlineStr">
+      <c r="B45" s="332" t="inlineStr">
         <is>
           <t>Harmonic Security</t>
         </is>
       </c>
-      <c r="C45" s="262" t="inlineStr">
+      <c r="C45" s="332" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D45" s="279" t="inlineStr">
+      <c r="D45" s="332" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E45" s="281" t="inlineStr">
+      <c r="E45" s="332" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F45" s="276" t="inlineStr">
+      <c r="F45" s="332" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G45" s="262" t="inlineStr">
+      <c r="G45" s="332" t="inlineStr">
         <is>
           <t>Shadow AI discovery + GenAI-aware DLP ($26M raised): detects sensitive data in AI</t>
         </is>
       </c>
-      <c r="H45" s="262" t="inlineStr">
+      <c r="H45" s="332" t="inlineStr">
         <is>
           <t>DLP specifically tuned for GenAI workflows</t>
         </is>
       </c>
     </row>
     <row r="46" ht="40" customHeight="1">
-      <c r="B46" s="262" t="inlineStr">
+      <c r="B46" s="332" t="inlineStr">
         <is>
           <t>Nightfall AI</t>
         </is>
       </c>
-      <c r="C46" s="262" t="inlineStr">
+      <c r="C46" s="332" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D46" s="279" t="inlineStr">
+      <c r="D46" s="332" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E46" s="281" t="inlineStr">
+      <c r="E46" s="332" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F46" s="280" t="inlineStr">
+      <c r="F46" s="332" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G46" s="262" t="inlineStr">
+      <c r="G46" s="332" t="inlineStr">
         <is>
           <t>AI-native DLP + GenAI firewall: discovers AI usage, prevents data exposure</t>
         </is>
       </c>
-      <c r="H46" s="262" t="inlineStr">
+      <c r="H46" s="332" t="inlineStr">
         <is>
           <t>Cloud-native DLP for AI applications</t>
         </is>
       </c>
     </row>
     <row r="47" ht="40" customHeight="1">
-      <c r="B47" s="262" t="inlineStr">
+      <c r="B47" s="332" t="inlineStr">
         <is>
           <t>Reco.ai</t>
         </is>
       </c>
-      <c r="C47" s="262" t="inlineStr">
+      <c r="C47" s="332" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D47" s="279" t="inlineStr">
+      <c r="D47" s="332" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E47" s="281" t="inlineStr">
+      <c r="E47" s="332" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F47" s="276" t="inlineStr">
+      <c r="F47" s="332" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G47" s="262" t="inlineStr">
+      <c r="G47" s="332" t="inlineStr">
         <is>
           <t>SaaS security + AI discovery: finds AI apps, tracks data flows, enforces policy</t>
         </is>
       </c>
-      <c r="H47" s="262" t="inlineStr">
+      <c r="H47" s="332" t="inlineStr">
         <is>
           <t>SaaS security teams extending to AI</t>
         </is>
       </c>
     </row>
     <row r="48" ht="40" customHeight="1">
-      <c r="B48" s="262" t="inlineStr">
+      <c r="B48" s="332" t="inlineStr">
         <is>
           <t>SentinelOne (Prompt Security)</t>
         </is>
       </c>
-      <c r="C48" s="262" t="inlineStr">
+      <c r="C48" s="332" t="inlineStr">
         <is>
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D48" s="279" t="inlineStr">
+      <c r="D48" s="332" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E48" s="280" t="inlineStr">
+      <c r="E48" s="332" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F48" s="281" t="inlineStr">
+      <c r="F48" s="332" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G48" s="262" t="inlineStr">
+      <c r="G48" s="332" t="inlineStr">
         <is>
           <t>Purple AI + Prompt Security acquisition: GenAI visibility, runtime protection</t>
         </is>
       </c>
-      <c r="H48" s="262" t="inlineStr">
+      <c r="H48" s="332" t="inlineStr">
         <is>
           <t>SentinelOne customers; GenAI visibility</t>
         </is>
       </c>
     </row>
     <row r="49" ht="40" customHeight="1">
-      <c r="B49" s="262" t="inlineStr">
+      <c r="B49" s="333" t="inlineStr">
         <is>
           <t>Arize AI</t>
         </is>
       </c>
-      <c r="C49" s="262" t="inlineStr">
+      <c r="C49" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D49" s="278" t="inlineStr">
+      <c r="D49" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E49" s="276" t="inlineStr">
+      <c r="E49" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F49" s="280" t="inlineStr">
+      <c r="F49" s="333" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G49" s="262" t="inlineStr">
+      <c r="G49" s="333" t="inlineStr">
         <is>
           <t>Enterprise AI observability ($131M raised): Phoenix OSS + AX enterprise platform</t>
         </is>
       </c>
-      <c r="H49" s="262" t="inlineStr">
+      <c r="H49" s="333" t="inlineStr">
         <is>
           <t>Production ML/LLM monitoring; Uber, DoorDash</t>
         </is>
       </c>
     </row>
     <row r="50" ht="40" customHeight="1">
-      <c r="B50" s="262" t="inlineStr">
+      <c r="B50" s="333" t="inlineStr">
         <is>
           <t>Braintrust</t>
         </is>
       </c>
-      <c r="C50" s="262" t="inlineStr">
+      <c r="C50" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D50" s="278" t="inlineStr">
+      <c r="D50" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E50" s="276" t="inlineStr">
+      <c r="E50" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F50" s="262" t="inlineStr">
+      <c r="F50" s="333" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G50" s="262" t="inlineStr">
+      <c r="G50" s="333" t="inlineStr">
         <is>
           <t>End-to-end LLM platform connecting observability to improvement: production traces become eval cases; results on PRs; unified PM/engineer interface.</t>
         </is>
       </c>
-      <c r="H50" s="262" t="inlineStr">
+      <c r="H50" s="333" t="inlineStr">
         <is>
           <t>LLM app teams; iterative improvement workflows</t>
         </is>
       </c>
     </row>
     <row r="51" ht="40" customHeight="1">
-      <c r="B51" s="262" t="inlineStr">
+      <c r="B51" s="333" t="inlineStr">
         <is>
           <t>Comet Opik</t>
         </is>
       </c>
-      <c r="C51" s="262" t="inlineStr">
+      <c r="C51" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D51" s="278" t="inlineStr">
+      <c r="D51" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E51" s="280" t="inlineStr">
+      <c r="E51" s="333" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F51" s="262" t="inlineStr">
+      <c r="F51" s="333" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G51" s="262" t="inlineStr">
+      <c r="G51" s="333" t="inlineStr">
         <is>
           <t>LLM evaluation and monitoring platform: tracks AI model quality, performance drift; integrates with major LLM providers.</t>
         </is>
       </c>
-      <c r="H51" s="262" t="inlineStr">
+      <c r="H51" s="333" t="inlineStr">
         <is>
           <t>ML teams; model quality assurance</t>
         </is>
       </c>
     </row>
     <row r="52" ht="40" customHeight="1">
-      <c r="B52" s="262" t="inlineStr">
+      <c r="B52" s="333" t="inlineStr">
         <is>
           <t>Datadog LLM Observability</t>
         </is>
       </c>
-      <c r="C52" s="262" t="inlineStr">
+      <c r="C52" s="333" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="D52" s="278" t="inlineStr">
+      <c r="D52" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E52" s="276" t="inlineStr">
+      <c r="E52" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F52" s="262" t="inlineStr">
+      <c r="F52" s="333" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G52" s="262" t="inlineStr">
+      <c r="G52" s="333" t="inlineStr">
         <is>
           <t>LLM monitoring: prompt injection detection, PII scanning, cost tracking</t>
         </is>
       </c>
-      <c r="H52" s="262" t="inlineStr">
+      <c r="H52" s="333" t="inlineStr">
         <is>
           <t>Datadog customers; unified observability</t>
         </is>
       </c>
     </row>
     <row r="53" ht="40" customHeight="1">
-      <c r="B53" s="262" t="inlineStr">
+      <c r="B53" s="333" t="inlineStr">
         <is>
           <t>Fiddler AI</t>
         </is>
       </c>
-      <c r="C53" s="262" t="inlineStr">
+      <c r="C53" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D53" s="278" t="inlineStr">
+      <c r="D53" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E53" s="276" t="inlineStr">
+      <c r="E53" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F53" s="281" t="inlineStr">
+      <c r="F53" s="333" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G53" s="262" t="inlineStr">
+      <c r="G53" s="333" t="inlineStr">
         <is>
           <t>Trust Service for LLMs ($68.6M raised): model scoring, guardrails, explainability</t>
         </is>
       </c>
-      <c r="H53" s="262" t="inlineStr">
+      <c r="H53" s="333" t="inlineStr">
         <is>
           <t>Regulated industries needing explainability</t>
         </is>
       </c>
     </row>
     <row r="54" ht="40" customHeight="1">
-      <c r="B54" s="262" t="inlineStr">
+      <c r="B54" s="333" t="inlineStr">
         <is>
           <t>Galileo AI</t>
         </is>
       </c>
-      <c r="C54" s="262" t="inlineStr">
+      <c r="C54" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D54" s="278" t="inlineStr">
+      <c r="D54" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E54" s="280" t="inlineStr">
+      <c r="E54" s="333" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F54" s="281" t="inlineStr">
+      <c r="F54" s="333" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G54" s="262" t="inlineStr">
+      <c r="G54" s="333" t="inlineStr">
         <is>
           <t>LLM debugging and evaluation: hallucination detection, data quality, guardrails</t>
         </is>
       </c>
-      <c r="H54" s="262" t="inlineStr">
+      <c r="H54" s="333" t="inlineStr">
         <is>
           <t>LLM debugging; data scientists; quality focus</t>
         </is>
       </c>
     </row>
     <row r="55" ht="40" customHeight="1">
-      <c r="B55" s="262" t="inlineStr">
+      <c r="B55" s="333" t="inlineStr">
         <is>
           <t>Helicone</t>
         </is>
       </c>
-      <c r="C55" s="262" t="inlineStr">
+      <c r="C55" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D55" s="278" t="inlineStr">
+      <c r="D55" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E55" s="276" t="inlineStr">
+      <c r="E55" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F55" s="262" t="inlineStr">
+      <c r="F55" s="333" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G55" s="262" t="inlineStr">
+      <c r="G55" s="333" t="inlineStr">
         <is>
           <t>Open source LLM observability: request logging, caching, rate limiting, analytics</t>
         </is>
       </c>
-      <c r="H55" s="262" t="inlineStr">
+      <c r="H55" s="333" t="inlineStr">
         <is>
           <t>OSS-first teams; LLM monitoring on budget</t>
         </is>
       </c>
     </row>
     <row r="56" ht="40" customHeight="1">
-      <c r="B56" s="262" t="inlineStr">
+      <c r="B56" s="333" t="inlineStr">
         <is>
           <t>LangFuse</t>
         </is>
       </c>
-      <c r="C56" s="262" t="inlineStr">
+      <c r="C56" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D56" s="278" t="inlineStr">
+      <c r="D56" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E56" s="276" t="inlineStr">
+      <c r="E56" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F56" s="262" t="inlineStr">
+      <c r="F56" s="333" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G56" s="262" t="inlineStr">
+      <c r="G56" s="333" t="inlineStr">
         <is>
           <t>Open-source LLM observability: distributed tracing, prompt management, evaluation; self-hosted or cloud; growing ecosystem.</t>
         </is>
       </c>
-      <c r="H56" s="262" t="inlineStr">
+      <c r="H56" s="333" t="inlineStr">
         <is>
           <t>OSS-first teams; cost-conscious LLM monitoring</t>
         </is>
       </c>
     </row>
     <row r="57" ht="40" customHeight="1">
-      <c r="B57" s="262" t="inlineStr">
+      <c r="B57" s="333" t="inlineStr">
         <is>
           <t>LangSmith (LangChain)</t>
         </is>
       </c>
-      <c r="C57" s="262" t="inlineStr">
+      <c r="C57" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D57" s="278" t="inlineStr">
+      <c r="D57" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E57" s="276" t="inlineStr">
+      <c r="E57" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F57" s="262" t="inlineStr">
+      <c r="F57" s="333" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G57" s="262" t="inlineStr">
+      <c r="G57" s="333" t="inlineStr">
         <is>
           <t>LLM app debugging and monitoring; traces, evaluations, prompt management</t>
         </is>
       </c>
-      <c r="H57" s="262" t="inlineStr">
+      <c r="H57" s="333" t="inlineStr">
         <is>
           <t>LangChain users; LLM app developers</t>
         </is>
       </c>
     </row>
     <row r="58" ht="40" customHeight="1">
-      <c r="B58" s="262" t="inlineStr">
+      <c r="B58" s="333" t="inlineStr">
         <is>
           <t>Maxim AI</t>
         </is>
       </c>
-      <c r="C58" s="262" t="inlineStr">
+      <c r="C58" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D58" s="278" t="inlineStr">
+      <c r="D58" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E58" s="276" t="inlineStr">
+      <c r="E58" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F58" s="280" t="inlineStr">
+      <c r="F58" s="333" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G58" s="262" t="inlineStr">
+      <c r="G58" s="333" t="inlineStr">
         <is>
           <t>End-to-end AI agent lifecycle platform: experimentation, simulation, evaluation, production observability; unified workflow replacing multiple point tools.</t>
         </is>
       </c>
-      <c r="H58" s="262" t="inlineStr">
+      <c r="H58" s="333" t="inlineStr">
         <is>
           <t>Agent development teams; unified agent lifecycle</t>
         </is>
       </c>
     </row>
     <row r="59" ht="40" customHeight="1">
-      <c r="B59" s="262" t="inlineStr">
+      <c r="B59" s="333" t="inlineStr">
         <is>
           <t>Patronus AI</t>
         </is>
       </c>
-      <c r="C59" s="262" t="inlineStr">
+      <c r="C59" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D59" s="278" t="inlineStr">
+      <c r="D59" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E59" s="280" t="inlineStr">
+      <c r="E59" s="333" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F59" s="276" t="inlineStr">
+      <c r="F59" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G59" s="262" t="inlineStr">
+      <c r="G59" s="333" t="inlineStr">
         <is>
           <t>LLM evaluation platform ($20M raised): hallucination detection, automated testing</t>
         </is>
       </c>
-      <c r="H59" s="262" t="inlineStr">
+      <c r="H59" s="333" t="inlineStr">
         <is>
           <t>LLM quality assurance; hallucination prevention</t>
         </is>
       </c>
     </row>
     <row r="60" ht="40" customHeight="1">
-      <c r="B60" s="262" t="inlineStr">
+      <c r="B60" s="333" t="inlineStr">
         <is>
           <t>Portkey</t>
         </is>
       </c>
-      <c r="C60" s="262" t="inlineStr">
+      <c r="C60" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D60" s="278" t="inlineStr">
+      <c r="D60" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E60" s="280" t="inlineStr">
+      <c r="E60" s="333" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F60" s="276" t="inlineStr">
+      <c r="F60" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G60" s="262" t="inlineStr">
+      <c r="G60" s="333" t="inlineStr">
         <is>
           <t>LLM gateway and observability: unified API, caching, fallbacks, cost management</t>
         </is>
       </c>
-      <c r="H60" s="262" t="inlineStr">
+      <c r="H60" s="333" t="inlineStr">
         <is>
           <t>Multi-LLM deployments; cost optimization</t>
         </is>
       </c>
     </row>
     <row r="61" ht="40" customHeight="1">
-      <c r="B61" s="262" t="inlineStr">
+      <c r="B61" s="333" t="inlineStr">
         <is>
           <t>Prophet Security</t>
         </is>
       </c>
-      <c r="C61" s="262" t="inlineStr">
+      <c r="C61" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D61" s="278" t="inlineStr">
+      <c r="D61" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E61" s="276" t="inlineStr">
+      <c r="E61" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F61" s="262" t="inlineStr">
+      <c r="F61" s="333" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G61" s="262" t="inlineStr">
+      <c r="G61" s="333" t="inlineStr">
         <is>
           <t>Agentic SOC: autonomous security investigation; AI-driven threat response; reduces analyst burden.</t>
         </is>
       </c>
-      <c r="H61" s="262" t="inlineStr">
+      <c r="H61" s="333" t="inlineStr">
         <is>
           <t>SOC teams; autonomous investigation</t>
         </is>
       </c>
     </row>
     <row r="62" ht="40" customHeight="1">
-      <c r="B62" s="262" t="inlineStr">
+      <c r="B62" s="333" t="inlineStr">
         <is>
           <t>Radiant Security</t>
         </is>
       </c>
-      <c r="C62" s="262" t="inlineStr">
+      <c r="C62" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D62" s="278" t="inlineStr">
+      <c r="D62" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E62" s="276" t="inlineStr">
+      <c r="E62" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F62" s="280" t="inlineStr">
+      <c r="F62" s="333" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G62" s="262" t="inlineStr">
+      <c r="G62" s="333" t="inlineStr">
         <is>
           <t>Agentic AI SOC platform: handles 100% of alerts; 90% false positive reduction; integrates 100+ data sources; autonomous triage.</t>
         </is>
       </c>
-      <c r="H62" s="262" t="inlineStr">
+      <c r="H62" s="333" t="inlineStr">
         <is>
           <t>SOC teams; alert fatigue reduction</t>
         </is>
       </c>
     </row>
     <row r="63" ht="40" customHeight="1">
-      <c r="B63" s="262" t="inlineStr">
+      <c r="B63" s="333" t="inlineStr">
         <is>
           <t>Stellar Cyber</t>
         </is>
       </c>
-      <c r="C63" s="262" t="inlineStr">
+      <c r="C63" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D63" s="278" t="inlineStr">
+      <c r="D63" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E63" s="276" t="inlineStr">
+      <c r="E63" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F63" s="279" t="inlineStr">
+      <c r="F63" s="333" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="G63" s="262" t="inlineStr">
+      <c r="G63" s="333" t="inlineStr">
         <is>
           <t>Open XDR with agentic AI: multi-agent architecture (detection, correlation, scoring, response); 50M+ data points across endpoints/network/cloud.</t>
         </is>
       </c>
-      <c r="H63" s="262" t="inlineStr">
+      <c r="H63" s="333" t="inlineStr">
         <is>
           <t>Mid-market; unified security operations</t>
         </is>
       </c>
     </row>
     <row r="64" ht="40" customHeight="1">
-      <c r="B64" s="262" t="inlineStr">
+      <c r="B64" s="333" t="inlineStr">
         <is>
           <t>Torq</t>
         </is>
       </c>
-      <c r="C64" s="262" t="inlineStr">
+      <c r="C64" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D64" s="278" t="inlineStr">
+      <c r="D64" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E64" s="282" t="inlineStr">
+      <c r="E64" s="333" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F64" s="276" t="inlineStr">
+      <c r="F64" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G64" s="262" t="inlineStr">
+      <c r="G64" s="333" t="inlineStr">
         <is>
           <t>AI-native security hyperautomation ($1.2B valuation): 300% revenue growth; customers include Marriott, PepsiCo, Siemens, Uber.</t>
         </is>
       </c>
-      <c r="H64" s="262" t="inlineStr">
+      <c r="H64" s="333" t="inlineStr">
         <is>
           <t>Security automation; enterprise SOC</t>
         </is>
       </c>
     </row>
     <row r="65" ht="40" customHeight="1">
-      <c r="B65" s="262" t="inlineStr">
+      <c r="B65" s="333" t="inlineStr">
         <is>
           <t>Weights &amp; Biases</t>
         </is>
       </c>
-      <c r="C65" s="262" t="inlineStr">
+      <c r="C65" s="333" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D65" s="278" t="inlineStr">
+      <c r="D65" s="333" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E65" s="276" t="inlineStr">
+      <c r="E65" s="333" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F65" s="262" t="inlineStr">
+      <c r="F65" s="333" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G65" s="262" t="inlineStr">
+      <c r="G65" s="333" t="inlineStr">
         <is>
           <t>MLOps platform ($250M raised): experiment tracking, model registry, LLM tracing</t>
         </is>
       </c>
-      <c r="H65" s="262" t="inlineStr">
+      <c r="H65" s="333" t="inlineStr">
         <is>
           <t>ML teams; experiment tracking; model lifecycle</t>
         </is>
       </c>
     </row>
     <row r="66" ht="40" customHeight="1">
-      <c r="B66" s="262" t="inlineStr">
+      <c r="B66" s="334" t="inlineStr">
         <is>
           <t>AWS Bedrock Guardrails</t>
         </is>
       </c>
-      <c r="C66" s="262" t="inlineStr">
+      <c r="C66" s="334" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="D66" s="281" t="inlineStr">
+      <c r="D66" s="334" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E66" s="280" t="inlineStr">
+      <c r="E66" s="334" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F66" s="262" t="inlineStr">
+      <c r="F66" s="334" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G66" s="262" t="inlineStr">
+      <c r="G66" s="334" t="inlineStr">
         <is>
           <t>Model-agnostic guardrails: Automated Reasoning for 99% hallucination prevention</t>
         </is>
       </c>
-      <c r="H66" s="262" t="inlineStr">
+      <c r="H66" s="334" t="inlineStr">
         <is>
           <t>AWS customers; Bedrock users</t>
         </is>
       </c>
     </row>
     <row r="67" ht="40" customHeight="1">
-      <c r="B67" s="262" t="inlineStr">
+      <c r="B67" s="334" t="inlineStr">
         <is>
           <t>BigID</t>
         </is>
       </c>
-      <c r="C67" s="262" t="inlineStr">
+      <c r="C67" s="334" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D67" s="281" t="inlineStr">
+      <c r="D67" s="334" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E67" s="276" t="inlineStr">
+      <c r="E67" s="334" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F67" s="279" t="inlineStr">
+      <c r="F67" s="334" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="G67" s="262" t="inlineStr">
+      <c r="G67" s="334" t="inlineStr">
         <is>
           <t>Shadow AI detection + AI governance ($290M raised): discovers AI data/models, maps to regs</t>
         </is>
       </c>
-      <c r="H67" s="262" t="inlineStr">
+      <c r="H67" s="334" t="inlineStr">
         <is>
           <t>Data discovery and governance for AI</t>
         </is>
       </c>
     </row>
     <row r="68" ht="40" customHeight="1">
-      <c r="B68" s="262" t="inlineStr">
+      <c r="B68" s="334" t="inlineStr">
         <is>
           <t>Cyera</t>
         </is>
       </c>
-      <c r="C68" s="262" t="inlineStr">
+      <c r="C68" s="334" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D68" s="281" t="inlineStr">
+      <c r="D68" s="334" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E68" s="276" t="inlineStr">
+      <c r="E68" s="334" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F68" s="279" t="inlineStr">
+      <c r="F68" s="334" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="G68" s="262" t="inlineStr">
+      <c r="G68" s="334" t="inlineStr">
         <is>
           <t>DSPM leader ($1.3B raised, $6B valuation): AI Guardian, 98% classification accuracy</t>
         </is>
       </c>
-      <c r="H68" s="259" t="inlineStr">
+      <c r="H68" s="335" t="inlineStr">
         <is>
           <t>Enterprise DSPM; AI data governance</t>
         </is>
       </c>
     </row>
     <row r="69" ht="40" customHeight="1">
-      <c r="B69" s="262" t="inlineStr">
+      <c r="B69" s="334" t="inlineStr">
         <is>
           <t>Google Cloud Model Armor</t>
         </is>
       </c>
-      <c r="C69" s="262" t="inlineStr">
+      <c r="C69" s="334" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="D69" s="281" t="inlineStr">
+      <c r="D69" s="334" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E69" s="280" t="inlineStr">
+      <c r="E69" s="334" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F69" s="262" t="inlineStr">
+      <c r="F69" s="334" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G69" s="262" t="inlineStr">
+      <c r="G69" s="334" t="inlineStr">
         <is>
           <t>Runtime security for any LLM: prompt injection, sensitive data, malicious URL blocking</t>
         </is>
       </c>
-      <c r="H69" s="259" t="inlineStr">
+      <c r="H69" s="335" t="inlineStr">
         <is>
           <t>GCP customers; Vertex AI users</t>
         </is>
       </c>
     </row>
     <row r="70" ht="40" customHeight="1">
-      <c r="B70" s="262" t="inlineStr">
+      <c r="B70" s="334" t="inlineStr">
         <is>
           <t>Island Browser</t>
         </is>
       </c>
-      <c r="C70" s="262" t="inlineStr">
+      <c r="C70" s="334" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D70" s="281" t="inlineStr">
+      <c r="D70" s="334" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E70" s="279" t="inlineStr">
+      <c r="E70" s="334" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F70" s="276" t="inlineStr">
+      <c r="F70" s="334" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G70" s="262" t="inlineStr">
+      <c r="G70" s="334" t="inlineStr">
         <is>
           <t>Enterprise browser with AI controls: DLP, session recording, controlled AI access</t>
         </is>
       </c>
-      <c r="H70" s="259" t="inlineStr">
+      <c r="H70" s="335" t="inlineStr">
         <is>
           <t>Browser-based AI control; high-security orgs</t>
         </is>
       </c>
     </row>
     <row r="71" ht="40" customHeight="1">
-      <c r="B71" s="262" t="inlineStr">
+      <c r="B71" s="334" t="inlineStr">
         <is>
           <t>Knostic</t>
         </is>
       </c>
-      <c r="C71" s="262" t="inlineStr">
+      <c r="C71" s="334" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D71" s="281" t="inlineStr">
+      <c r="D71" s="334" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E71" s="276" t="inlineStr">
+      <c r="E71" s="334" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F71" s="280" t="inlineStr">
+      <c r="F71" s="334" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G71" s="262" t="inlineStr">
+      <c r="G71" s="334" t="inlineStr">
         <is>
           <t>Need-to-know access for AI: context-aware data protection, RAG security</t>
         </is>
       </c>
-      <c r="H71" s="259" t="inlineStr">
+      <c r="H71" s="335" t="inlineStr">
         <is>
           <t>RAG deployments; need-to-know data access</t>
         </is>
       </c>
     </row>
     <row r="72" ht="40" customHeight="1">
-      <c r="B72" s="262" t="inlineStr">
+      <c r="B72" s="334" t="inlineStr">
         <is>
           <t>Netskope</t>
         </is>
       </c>
-      <c r="C72" s="262" t="inlineStr">
+      <c r="C72" s="334" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D72" s="281" t="inlineStr">
+      <c r="D72" s="334" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E72" s="279" t="inlineStr">
+      <c r="E72" s="334" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F72" s="280" t="inlineStr">
+      <c r="F72" s="334" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G72" s="262" t="inlineStr">
+      <c r="G72" s="334" t="inlineStr">
         <is>
           <t>SASE + GenAI DLP: real-time coaching, data protection for AI apps</t>
         </is>
       </c>
-      <c r="H72" s="259" t="inlineStr">
+      <c r="H72" s="335" t="inlineStr">
         <is>
           <t>SASE customers; GenAI-aware DLP</t>
         </is>
       </c>
     </row>
     <row r="73" ht="40" customHeight="1">
-      <c r="B73" s="262" t="inlineStr">
+      <c r="B73" s="334" t="inlineStr">
         <is>
           <t>Zscaler</t>
         </is>
       </c>
-      <c r="C73" s="262" t="inlineStr">
+      <c r="C73" s="334" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D73" s="281" t="inlineStr">
+      <c r="D73" s="334" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E73" s="279" t="inlineStr">
+      <c r="E73" s="334" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F73" s="280" t="inlineStr">
+      <c r="F73" s="334" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G73" s="262" t="inlineStr">
+      <c r="G73" s="334" t="inlineStr">
         <is>
           <t>Zero trust + AI security: GenAI app control, data protection, shadow AI</t>
         </is>
       </c>
-      <c r="H73" s="259" t="inlineStr">
+      <c r="H73" s="335" t="inlineStr">
         <is>
           <t>Zscaler customers; zero trust AI security</t>
         </is>
       </c>
     </row>
     <row r="74" ht="40" customHeight="1">
-      <c r="B74" s="259" t="inlineStr">
+      <c r="B74" s="336" t="inlineStr">
         <is>
           <t>Aembit</t>
         </is>
       </c>
-      <c r="C74" s="259" t="inlineStr">
+      <c r="C74" s="336" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D74" s="284" t="inlineStr">
+      <c r="D74" s="336" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E74" s="288" t="inlineStr">
+      <c r="E74" s="336" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F74" s="289" t="inlineStr">
+      <c r="F74" s="336" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G74" s="259" t="inlineStr">
+      <c r="G74" s="336" t="inlineStr">
         <is>
           <t>Secretless workload IAM ($45M raised): workload-to-workload identity; tracks AI service connections revealing shadow AI</t>
         </is>
       </c>
-      <c r="H74" s="259" t="inlineStr">
+      <c r="H74" s="336" t="inlineStr">
         <is>
           <t>Secretless architecture; workload identity</t>
         </is>
       </c>
     </row>
     <row r="75" ht="40" customHeight="1">
-      <c r="B75" s="259" t="inlineStr">
+      <c r="B75" s="336" t="inlineStr">
         <is>
           <t>Astrix Security</t>
         </is>
       </c>
-      <c r="C75" s="259" t="inlineStr">
+      <c r="C75" s="336" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D75" s="284" t="inlineStr">
+      <c r="D75" s="336" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E75" s="288" t="inlineStr">
+      <c r="E75" s="336" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F75" s="286" t="inlineStr">
+      <c r="F75" s="336" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G75" s="259" t="inlineStr">
+      <c r="G75" s="336" t="inlineStr">
         <is>
           <t>Dedicated NHI platform ($85M raised): agent inventory, least-privilege; token monitoring surfaces shadow AI tools</t>
         </is>
       </c>
-      <c r="H75" s="259" t="inlineStr">
+      <c r="H75" s="336" t="inlineStr">
         <is>
           <t>NHI-first security; agentic AI deployments</t>
         </is>
       </c>
     </row>
     <row r="76" ht="40" customHeight="1">
-      <c r="B76" s="259" t="inlineStr">
+      <c r="B76" s="336" t="inlineStr">
         <is>
           <t>CyberArk</t>
         </is>
       </c>
-      <c r="C76" s="259" t="inlineStr">
+      <c r="C76" s="336" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D76" s="284" t="inlineStr">
+      <c r="D76" s="336" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E76" s="286" t="inlineStr">
+      <c r="E76" s="336" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F76" s="289" t="inlineStr">
+      <c r="F76" s="336" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="G76" s="259" t="inlineStr">
+      <c r="G76" s="336" t="inlineStr">
         <is>
           <t>PAM leader extending to NHI: machine identity security, secrets management</t>
         </is>
       </c>
-      <c r="H76" s="259" t="inlineStr">
+      <c r="H76" s="336" t="inlineStr">
         <is>
           <t>Enterprise PAM; extending to machine identities</t>
         </is>
       </c>
     </row>
     <row r="77" ht="40" customHeight="1">
-      <c r="B77" s="259" t="inlineStr">
+      <c r="B77" s="336" t="inlineStr">
         <is>
           <t>Entro Security</t>
         </is>
       </c>
-      <c r="C77" s="259" t="inlineStr">
+      <c r="C77" s="336" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D77" s="284" t="inlineStr">
+      <c r="D77" s="336" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E77" s="288" t="inlineStr">
+      <c r="E77" s="336" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F77" s="286" t="inlineStr">
+      <c r="F77" s="336" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G77" s="259" t="inlineStr">
+      <c r="G77" s="336" t="inlineStr">
         <is>
           <t>Secrets security platform: discovers and monitors exposed secrets; reveals AI API keys indicating shadow AI usage</t>
         </is>
       </c>
-      <c r="H77" s="259" t="inlineStr">
+      <c r="H77" s="336" t="inlineStr">
         <is>
           <t>Secrets sprawl; credential exposure prevention</t>
         </is>
       </c>
     </row>
     <row r="78" ht="40" customHeight="1">
-      <c r="B78" s="259" t="inlineStr">
+      <c r="B78" s="336" t="inlineStr">
         <is>
           <t>HashiCorp Vault</t>
         </is>
       </c>
-      <c r="C78" s="259" t="inlineStr">
+      <c r="C78" s="336" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D78" s="284" t="inlineStr">
+      <c r="D78" s="336" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E78" s="289" t="inlineStr">
+      <c r="E78" s="336" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F78" s="259" t="inlineStr">
+      <c r="F78" s="336" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G78" s="259" t="inlineStr">
+      <c r="G78" s="336" t="inlineStr">
         <is>
           <t>Secrets management leader: dynamic secrets, encryption, identity-based access</t>
         </is>
       </c>
-      <c r="H78" s="259" t="inlineStr">
+      <c r="H78" s="336" t="inlineStr">
         <is>
           <t>Secrets management; dynamic credentials; DevOps</t>
         </is>
       </c>
     </row>
     <row r="79" ht="40" customHeight="1">
-      <c r="B79" s="259" t="inlineStr">
+      <c r="B79" s="336" t="inlineStr">
         <is>
           <t>Oasis Security</t>
         </is>
       </c>
-      <c r="C79" s="259" t="inlineStr">
+      <c r="C79" s="336" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D79" s="284" t="inlineStr">
+      <c r="D79" s="336" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E79" s="288" t="inlineStr">
+      <c r="E79" s="336" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F79" s="286" t="inlineStr">
+      <c r="F79" s="336" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G79" s="259" t="inlineStr">
+      <c r="G79" s="336" t="inlineStr">
         <is>
           <t>NHI Security Cloud ($75M raised): Agentic Access Management; identity-based shadow AI discovery via service account monitoring</t>
         </is>
       </c>
-      <c r="H79" s="259" t="inlineStr">
+      <c r="H79" s="336" t="inlineStr">
         <is>
           <t>Agentic AI security; intent-based access control</t>
         </is>
       </c>
     </row>
     <row r="80" ht="40" customHeight="1">
-      <c r="B80" s="259" t="inlineStr">
+      <c r="B80" s="336" t="inlineStr">
         <is>
           <t>Silverfort</t>
         </is>
       </c>
-      <c r="C80" s="259" t="inlineStr">
+      <c r="C80" s="336" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D80" s="284" t="inlineStr">
+      <c r="D80" s="336" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E80" s="288" t="inlineStr">
+      <c r="E80" s="336" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F80" s="286" t="inlineStr">
+      <c r="F80" s="336" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G80" s="259" t="inlineStr">
+      <c r="G80" s="336" t="inlineStr">
         <is>
           <t>NHI leader ($222M raised, ~$1B valuation): unified human + non-human identity; NHI visibility reveals unauthorized AI service access</t>
         </is>
       </c>
-      <c r="H80" s="259" t="inlineStr">
+      <c r="H80" s="336" t="inlineStr">
         <is>
           <t>Enterprise IAM extending to NHI; MFA everywhere</t>
         </is>
       </c>
     </row>
     <row r="81" ht="40" customHeight="1">
-      <c r="B81" s="259" t="inlineStr">
+      <c r="B81" s="336" t="inlineStr">
         <is>
           <t>Spec</t>
         </is>
       </c>
-      <c r="C81" s="259" t="inlineStr">
+      <c r="C81" s="336" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D81" s="284" t="inlineStr">
+      <c r="D81" s="336" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E81" s="283" t="inlineStr">
+      <c r="E81" s="336" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F81" s="286" t="inlineStr">
+      <c r="F81" s="336" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G81" s="259" t="inlineStr">
+      <c r="G81" s="336" t="inlineStr">
         <is>
           <t>Agentic security platform: agent identity, behavior monitoring, automated response</t>
         </is>
       </c>
-      <c r="H81" s="259" t="inlineStr">
+      <c r="H81" s="336" t="inlineStr">
         <is>
           <t>Organizations with production AI agents</t>
         </is>
       </c>
     </row>
     <row r="82" ht="40" customHeight="1">
-      <c r="B82" s="259" t="inlineStr">
+      <c r="B82" s="336" t="inlineStr">
         <is>
           <t>Strata Identity</t>
         </is>
       </c>
-      <c r="C82" s="259" t="inlineStr">
+      <c r="C82" s="336" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D82" s="284" t="inlineStr">
+      <c r="D82" s="336" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E82" s="286" t="inlineStr">
+      <c r="E82" s="336" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F82" s="259" t="inlineStr">
+      <c r="F82" s="336" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G82" s="259" t="inlineStr">
+      <c r="G82" s="336" t="inlineStr">
         <is>
           <t>Agentic identity management: dynamic, autonomous NHI governance; distinct from static machine identities; policy-based agent permissions.</t>
         </is>
       </c>
-      <c r="H82" s="259" t="inlineStr">
+      <c r="H82" s="336" t="inlineStr">
         <is>
           <t>Agentic AI identity; dynamic access control</t>
         </is>
@@ -18841,37 +18885,37 @@
       </c>
     </row>
     <row r="84" ht="40" customHeight="1">
-      <c r="B84" s="259" t="inlineStr">
+      <c r="B84" s="320" t="inlineStr">
         <is>
           <t>HiddenLayer</t>
         </is>
       </c>
-      <c r="C84" s="259" t="inlineStr">
+      <c r="C84" s="320" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D84" s="287" t="inlineStr">
+      <c r="D84" s="320" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E84" s="283" t="inlineStr">
+      <c r="E84" s="320" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F84" s="286" t="inlineStr">
+      <c r="F84" s="320" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="G84" s="259" t="inlineStr">
+      <c r="G84" s="320" t="inlineStr">
         <is>
           <t>AI Supply Chain leader ($56M raised): model scanning, ML supply chain security, model BOM</t>
         </is>
       </c>
-      <c r="H84" s="259" t="inlineStr">
+      <c r="H84" s="320" t="inlineStr">
         <is>
           <t>Multi-cloud AI; wants independent vendor</t>
         </is>
@@ -18915,74 +18959,74 @@
       </c>
     </row>
     <row r="86" ht="40" customHeight="1">
-      <c r="B86" s="259" t="inlineStr">
+      <c r="B86" s="320" t="inlineStr">
         <is>
           <t>Legit Security</t>
         </is>
       </c>
-      <c r="C86" s="259" t="inlineStr">
+      <c r="C86" s="320" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D86" s="287" t="inlineStr">
+      <c r="D86" s="320" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E86" s="286" t="inlineStr">
+      <c r="E86" s="320" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F86" s="283" t="inlineStr">
+      <c r="F86" s="320" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G86" s="259" t="inlineStr">
+      <c r="G86" s="320" t="inlineStr">
         <is>
           <t>AI Supply Chain via ASPM: AI code security, model supply chain, SDLC for ML pipelines</t>
         </is>
       </c>
-      <c r="H86" s="259" t="inlineStr">
+      <c r="H86" s="320" t="inlineStr">
         <is>
           <t>DevSecOps teams; AI in software supply chain</t>
         </is>
       </c>
     </row>
     <row r="87" ht="40" customHeight="1">
-      <c r="B87" s="259" t="inlineStr">
+      <c r="B87" s="320" t="inlineStr">
         <is>
           <t>OpenSSF Model Signing</t>
         </is>
       </c>
-      <c r="C87" s="259" t="inlineStr">
+      <c r="C87" s="320" t="inlineStr">
         <is>
           <t>Open Standard</t>
         </is>
       </c>
-      <c r="D87" s="287" t="inlineStr">
+      <c r="D87" s="320" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E87" s="284" t="inlineStr">
+      <c r="E87" s="320" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="F87" s="259" t="inlineStr">
+      <c r="F87" s="320" t="inlineStr">
         <is>
           <t>—</t>
         </is>
       </c>
-      <c r="G87" s="259" t="inlineStr">
+      <c r="G87" s="320" t="inlineStr">
         <is>
           <t>Open Source Security Foundation: model signing specification for cryptographically verifying AI model origin and integrity.</t>
         </is>
       </c>
-      <c r="H87" s="259" t="inlineStr">
+      <c r="H87" s="320" t="inlineStr">
         <is>
           <t>OSS model consumers; provenance verification</t>
         </is>
@@ -19063,37 +19107,37 @@
       </c>
     </row>
     <row r="90" ht="40" customHeight="1">
-      <c r="B90" s="259" t="inlineStr">
+      <c r="B90" s="320" t="inlineStr">
         <is>
           <t>Spectra Assure</t>
         </is>
       </c>
-      <c r="C90" s="259" t="inlineStr">
+      <c r="C90" s="320" t="inlineStr">
         <is>
           <t>Independent</t>
         </is>
       </c>
-      <c r="D90" s="287" t="inlineStr">
+      <c r="D90" s="320" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E90" s="286" t="inlineStr">
+      <c r="E90" s="320" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F90" s="283" t="inlineStr">
+      <c r="F90" s="320" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G90" s="259" t="inlineStr">
+      <c r="G90" s="320" t="inlineStr">
         <is>
           <t>Software supply chain security: SAFE reports for AI/ML artifacts; flags poisoning risks; CycloneDX export; NIST/ISO 42001 compliant.</t>
         </is>
       </c>
-      <c r="H90" s="259" t="inlineStr">
+      <c r="H90" s="320" t="inlineStr">
         <is>
           <t>Regulated industries; AI supply chain compliance</t>
         </is>

</xml_diff>

<commit_message>
Add Agentic AI KPIs, fix Tool Function Mapping, and Exception Tracker colors
Program Metrics:
- Added 3 new Agentic AI KPIs: Agent Inventory Coverage, Autonomous Action Rate, Agent Incident Rate
- Added corresponding SLOs for the new KPIs
- Removed placeholder note

Tool Function Mapping:
- Moved RAG/Vector Database and MCP Server Integration to correct HIGH risk section
- Removed duplicate entries (Multi-Agent Orchestration, Autonomous Code Execution)
- Fixed merged cell issues

Exception Tracker:
- Applied consistent document colors (matching Guardrail Checklist risk colors)
- Severe Tool = red, Guardrail Bypass = pink, Vendor Risk = yellow, etc.
- Fixed header and status legend styling

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/AI_Security_Risk_Draft1.xlsx
+++ b/AI_Security_Risk_Draft1.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="48">
+  <fonts count="49">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -324,8 +324,12 @@
       <b val="1"/>
       <sz val="11"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
   </fonts>
-  <fills count="50">
+  <fills count="58">
     <fill>
       <patternFill/>
     </fill>
@@ -593,6 +597,54 @@
         <bgColor rgb="00B4C6E7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6B6B"/>
+        <bgColor rgb="FFFF6B6B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF00B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor rgb="FFC00000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -714,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6"/>
   </cellStyleXfs>
-  <cellXfs count="290">
+  <cellXfs count="300">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1472,6 +1524,36 @@
     </xf>
     <xf numFmtId="0" fontId="43" fillId="48" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="29" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="50" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="51" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="52" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="52" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="53" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="54" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="55" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="56" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="57" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5288,7 +5370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:K96"/>
+  <dimension ref="B2:K102"/>
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
@@ -5335,11 +5417,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="266" t="inlineStr">
-        <is>
-          <t>NEW: Consider adding Agentic AI-specific KPIs: Agent Inventory Coverage, Autonomous Action Rate, Agent Incident Rate</t>
-        </is>
-      </c>
+      <c r="B7" s="266" t="n"/>
     </row>
     <row r="8" ht="18" customHeight="1">
       <c r="B8" s="96" t="inlineStr">
@@ -5652,647 +5730,508 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Agent Inventory Coverage</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>% of AI agents registered vs. discovered</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>(Registered Agents / Discovered Agents) × 100</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Agent Registry + Discovery Tools</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Autonomous Action Rate</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>% of agent actions without human approval</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>(Autonomous Actions / Total Agent Actions) × 100</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Agent Logging + Audit Trail</t>
+        </is>
+      </c>
+    </row>
     <row r="23" ht="18" customHeight="1">
-      <c r="B23" s="96" t="inlineStr">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Agent Incident Rate</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Security incidents involving AI agents</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Count of agent-related incidents / Total agents</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>SIEM / Incident Management</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Agent Inventory Coverage</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>≥ 95%</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>&lt; 90% triggers audit</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Security Lead → CISO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Autonomous Action Rate</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>&lt; 20% for High-risk agents</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>&gt; 30% triggers review</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Security Lead</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="25" customHeight="1">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Agent Incident Rate</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>&lt; 2 per quarter</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>&gt; 3 triggers program review</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Committee</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="25" customHeight="1"/>
+    <row r="28" ht="25" customHeight="1"/>
+    <row r="29" ht="25" customHeight="1">
+      <c r="B29" s="96" t="inlineStr">
         <is>
           <t>3. Service Level Objectives (SLOs)</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="B24" s="98" t="inlineStr">
+    <row r="30" ht="25" customHeight="1">
+      <c r="B30" s="98" t="inlineStr">
         <is>
           <t>Performance targets that the AI security program commits to meeting.</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="B25" s="99" t="inlineStr">
+    <row r="31" ht="25" customHeight="1">
+      <c r="B31" s="99" t="inlineStr">
         <is>
           <t>SLO</t>
         </is>
       </c>
-      <c r="C25" s="99" t="inlineStr">
+      <c r="C31" s="99" t="inlineStr">
         <is>
           <t>Target</t>
         </is>
       </c>
-      <c r="D25" s="99" t="inlineStr">
+      <c r="D31" s="99" t="inlineStr">
         <is>
           <t>Threshold</t>
         </is>
       </c>
-      <c r="E25" s="99" t="inlineStr">
+      <c r="E31" s="99" t="inlineStr">
         <is>
           <t>Escalation</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="25" customHeight="1">
-      <c r="B26" s="130" t="inlineStr">
-        <is>
-          <t>Tool Inventory Coverage</t>
-        </is>
-      </c>
-      <c r="C26" s="130" t="inlineStr">
-        <is>
-          <t>≥ 95%</t>
-        </is>
-      </c>
-      <c r="D26" s="130" t="inlineStr">
-        <is>
-          <t>&lt; 90% triggers audit</t>
-        </is>
-      </c>
-      <c r="E26" s="130" t="inlineStr">
-        <is>
-          <t>Security Lead → CISO</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" ht="25" customHeight="1">
-      <c r="B27" s="130" t="inlineStr">
-        <is>
-          <t>Review Completion Rate</t>
-        </is>
-      </c>
-      <c r="C27" s="130" t="inlineStr">
-        <is>
-          <t>≥ 95%</t>
-        </is>
-      </c>
-      <c r="D27" s="130" t="inlineStr">
-        <is>
-          <t>&lt; 85% triggers remediation</t>
-        </is>
-      </c>
-      <c r="E27" s="130" t="inlineStr">
-        <is>
-          <t>Security Lead</t>
-        </is>
-      </c>
-    </row>
-    <row r="28" ht="25" customHeight="1">
-      <c r="B28" s="130" t="inlineStr">
-        <is>
-          <t>Low Risk Approval Time</t>
-        </is>
-      </c>
-      <c r="C28" s="130" t="inlineStr">
-        <is>
-          <t>≤ 2 business days</t>
-        </is>
-      </c>
-      <c r="D28" s="130" t="inlineStr">
-        <is>
-          <t>&gt; 3 days escalates</t>
-        </is>
-      </c>
-      <c r="E28" s="130" t="inlineStr">
-        <is>
-          <t>Security Team</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" ht="25" customHeight="1">
-      <c r="B29" s="130" t="inlineStr">
-        <is>
-          <t>Medium Risk Approval Time</t>
-        </is>
-      </c>
-      <c r="C29" s="130" t="inlineStr">
-        <is>
-          <t>≤ 5 business days</t>
-        </is>
-      </c>
-      <c r="D29" s="130" t="inlineStr">
-        <is>
-          <t>&gt; 7 days escalates</t>
-        </is>
-      </c>
-      <c r="E29" s="130" t="inlineStr">
-        <is>
-          <t>Security Lead</t>
-        </is>
-      </c>
-    </row>
-    <row r="30" ht="25" customHeight="1">
-      <c r="B30" s="130" t="inlineStr">
-        <is>
-          <t>High Risk Approval Time</t>
-        </is>
-      </c>
-      <c r="C30" s="130" t="inlineStr">
-        <is>
-          <t>≤ 10 business days</t>
-        </is>
-      </c>
-      <c r="D30" s="130" t="inlineStr">
-        <is>
-          <t>&gt; 14 days escalates</t>
-        </is>
-      </c>
-      <c r="E30" s="130" t="inlineStr">
-        <is>
-          <t>Committee Chair</t>
-        </is>
-      </c>
-    </row>
-    <row r="31" ht="25" customHeight="1">
-      <c r="B31" s="130" t="inlineStr">
-        <is>
-          <t>Severe Risk Exception Review</t>
-        </is>
-      </c>
-      <c r="C31" s="130" t="inlineStr">
-        <is>
-          <t>≤ 15 business days</t>
-        </is>
-      </c>
-      <c r="D31" s="130" t="inlineStr">
-        <is>
-          <t>&gt; 20 days escalates</t>
-        </is>
-      </c>
-      <c r="E31" s="130" t="inlineStr">
-        <is>
-          <t>CISO</t>
         </is>
       </c>
     </row>
     <row r="32" ht="25" customHeight="1">
       <c r="B32" s="130" t="inlineStr">
         <is>
-          <t>Guardrail Verification Rate</t>
+          <t>Tool Inventory Coverage</t>
         </is>
       </c>
       <c r="C32" s="130" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>≥ 95%</t>
         </is>
       </c>
       <c r="D32" s="130" t="inlineStr">
         <is>
-          <t>&lt; 95% blocks activation</t>
+          <t>&lt; 90% triggers audit</t>
         </is>
       </c>
       <c r="E32" s="130" t="inlineStr">
         <is>
-          <t>Security Team</t>
+          <t>Security Lead → CISO</t>
         </is>
       </c>
     </row>
     <row r="33" ht="25" customHeight="1">
       <c r="B33" s="130" t="inlineStr">
         <is>
-          <t>Tier 1 (Kill Switch) Response</t>
+          <t>Review Completion Rate</t>
         </is>
       </c>
       <c r="C33" s="130" t="inlineStr">
         <is>
-          <t>&lt; 15 minutes</t>
+          <t>≥ 95%</t>
         </is>
       </c>
       <c r="D33" s="130" t="inlineStr">
         <is>
-          <t>Immediate escalation</t>
+          <t>&lt; 85% triggers remediation</t>
         </is>
       </c>
       <c r="E33" s="130" t="inlineStr">
         <is>
-          <t>On-call Security</t>
+          <t>Security Lead</t>
         </is>
       </c>
     </row>
     <row r="34" ht="25" customHeight="1">
       <c r="B34" s="130" t="inlineStr">
         <is>
-          <t>Tier 2 (Rapid Response) Time</t>
+          <t>Low Risk Approval Time</t>
         </is>
       </c>
       <c r="C34" s="130" t="inlineStr">
         <is>
-          <t>&lt; 4 hours</t>
+          <t>≤ 2 business days</t>
         </is>
       </c>
       <c r="D34" s="130" t="inlineStr">
         <is>
-          <t>&gt; 6 hours escalates</t>
+          <t>&gt; 3 days escalates</t>
         </is>
       </c>
       <c r="E34" s="130" t="inlineStr">
         <is>
-          <t>Security Lead</t>
+          <t>Security Team</t>
         </is>
       </c>
     </row>
     <row r="35" ht="25" customHeight="1">
       <c r="B35" s="130" t="inlineStr">
         <is>
-          <t>Tier 3 (Accelerated Review) Time</t>
+          <t>Medium Risk Approval Time</t>
         </is>
       </c>
       <c r="C35" s="130" t="inlineStr">
         <is>
-          <t>&lt; 24 hours</t>
+          <t>≤ 5 business days</t>
         </is>
       </c>
       <c r="D35" s="130" t="inlineStr">
         <is>
-          <t>&gt; 48 hours escalates</t>
+          <t>&gt; 7 days escalates</t>
         </is>
       </c>
       <c r="E35" s="130" t="inlineStr">
         <is>
-          <t>Security Team</t>
+          <t>Security Lead</t>
         </is>
       </c>
     </row>
     <row r="36" ht="25" customHeight="1">
       <c r="B36" s="130" t="inlineStr">
         <is>
-          <t>Non-Compliance Rate</t>
+          <t>High Risk Approval Time</t>
         </is>
       </c>
       <c r="C36" s="130" t="inlineStr">
         <is>
-          <t>&lt; 5%</t>
+          <t>≤ 10 business days</t>
         </is>
       </c>
       <c r="D36" s="130" t="inlineStr">
         <is>
-          <t>&gt; 10% triggers program review</t>
+          <t>&gt; 14 days escalates</t>
         </is>
       </c>
       <c r="E36" s="130" t="inlineStr">
         <is>
-          <t>Committee</t>
+          <t>Committee Chair</t>
         </is>
       </c>
     </row>
     <row r="37" ht="25" customHeight="1">
       <c r="B37" s="130" t="inlineStr">
         <is>
+          <t>Severe Risk Exception Review</t>
+        </is>
+      </c>
+      <c r="C37" s="130" t="inlineStr">
+        <is>
+          <t>≤ 15 business days</t>
+        </is>
+      </c>
+      <c r="D37" s="130" t="inlineStr">
+        <is>
+          <t>&gt; 20 days escalates</t>
+        </is>
+      </c>
+      <c r="E37" s="130" t="inlineStr">
+        <is>
+          <t>CISO</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" s="130" t="inlineStr">
+        <is>
+          <t>Guardrail Verification Rate</t>
+        </is>
+      </c>
+      <c r="C38" s="130" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="D38" s="130" t="inlineStr">
+        <is>
+          <t>&lt; 95% blocks activation</t>
+        </is>
+      </c>
+      <c r="E38" s="130" t="inlineStr">
+        <is>
+          <t>Security Team</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" s="130" t="inlineStr">
+        <is>
+          <t>Tier 1 (Kill Switch) Response</t>
+        </is>
+      </c>
+      <c r="C39" s="130" t="inlineStr">
+        <is>
+          <t>&lt; 15 minutes</t>
+        </is>
+      </c>
+      <c r="D39" s="130" t="inlineStr">
+        <is>
+          <t>Immediate escalation</t>
+        </is>
+      </c>
+      <c r="E39" s="130" t="inlineStr">
+        <is>
+          <t>On-call Security</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="18" customHeight="1">
+      <c r="B40" s="130" t="inlineStr">
+        <is>
+          <t>Tier 2 (Rapid Response) Time</t>
+        </is>
+      </c>
+      <c r="C40" s="130" t="inlineStr">
+        <is>
+          <t>&lt; 4 hours</t>
+        </is>
+      </c>
+      <c r="D40" s="130" t="inlineStr">
+        <is>
+          <t>&gt; 6 hours escalates</t>
+        </is>
+      </c>
+      <c r="E40" s="130" t="inlineStr">
+        <is>
+          <t>Security Lead</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" s="130" t="inlineStr">
+        <is>
+          <t>Tier 3 (Accelerated Review) Time</t>
+        </is>
+      </c>
+      <c r="C41" s="130" t="inlineStr">
+        <is>
+          <t>&lt; 24 hours</t>
+        </is>
+      </c>
+      <c r="D41" s="130" t="inlineStr">
+        <is>
+          <t>&gt; 48 hours escalates</t>
+        </is>
+      </c>
+      <c r="E41" s="130" t="inlineStr">
+        <is>
+          <t>Security Team</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" s="130" t="inlineStr">
+        <is>
+          <t>Non-Compliance Rate</t>
+        </is>
+      </c>
+      <c r="C42" s="130" t="inlineStr">
+        <is>
+          <t>&lt; 5%</t>
+        </is>
+      </c>
+      <c r="D42" s="130" t="inlineStr">
+        <is>
+          <t>&gt; 10% triggers program review</t>
+        </is>
+      </c>
+      <c r="E42" s="130" t="inlineStr">
+        <is>
+          <t>Committee</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" ht="40" customHeight="1">
+      <c r="B43" s="130" t="inlineStr">
+        <is>
           <t>Exception Renewal Processing</t>
         </is>
       </c>
-      <c r="C37" s="130" t="inlineStr">
+      <c r="C43" s="130" t="inlineStr">
         <is>
           <t>≤ 5 business days before expiry</t>
         </is>
       </c>
-      <c r="D37" s="130" t="inlineStr">
+      <c r="D43" s="130" t="inlineStr">
         <is>
           <t>Auto-suspend if missed</t>
         </is>
       </c>
-      <c r="E37" s="130" t="inlineStr">
+      <c r="E43" s="130" t="inlineStr">
         <is>
           <t>Exception Owner</t>
         </is>
       </c>
     </row>
-    <row r="40" ht="18" customHeight="1">
-      <c r="B40" s="103" t="inlineStr">
+    <row r="44" ht="40" customHeight="1"/>
+    <row r="45" ht="40" customHeight="1"/>
+    <row r="46" ht="40" customHeight="1">
+      <c r="B46" s="103" t="inlineStr">
         <is>
           <t>4. Compliance Framework Metrics Matrix</t>
         </is>
       </c>
-      <c r="C40" s="74" t="n"/>
-      <c r="D40" s="74" t="n"/>
-      <c r="E40" s="74" t="n"/>
-      <c r="F40" s="74" t="n"/>
-      <c r="G40" s="74" t="n"/>
-      <c r="H40" s="74" t="n"/>
-      <c r="I40" s="74" t="n"/>
-      <c r="J40" s="74" t="n"/>
-      <c r="K40" s="74" t="n"/>
-    </row>
-    <row r="41">
-      <c r="B41" s="104" t="inlineStr">
-        <is>
-          <t>Matrix showing which metrics each framework requires. Use this to identify gaps and prioritize measurement efforts based on your compliance obligations.</t>
-        </is>
-      </c>
-      <c r="C41" s="74" t="n"/>
-      <c r="D41" s="74" t="n"/>
-      <c r="E41" s="74" t="n"/>
-      <c r="F41" s="74" t="n"/>
-      <c r="G41" s="74" t="n"/>
-      <c r="H41" s="74" t="n"/>
-      <c r="I41" s="74" t="n"/>
-      <c r="J41" s="74" t="n"/>
-      <c r="K41" s="74" t="n"/>
-    </row>
-    <row r="42">
-      <c r="B42" s="105" t="inlineStr">
-        <is>
-          <t>Metric Category</t>
-        </is>
-      </c>
-      <c r="C42" s="106" t="inlineStr">
-        <is>
-          <t>ISO 42001</t>
-        </is>
-      </c>
-      <c r="D42" s="107" t="inlineStr">
-        <is>
-          <t>NIST AI RMF</t>
-        </is>
-      </c>
-      <c r="E42" s="108" t="inlineStr">
-        <is>
-          <t>EU AI Act</t>
-        </is>
-      </c>
-      <c r="F42" s="109" t="inlineStr">
-        <is>
-          <t>SOC 2</t>
-        </is>
-      </c>
-      <c r="G42" s="110" t="inlineStr">
-        <is>
-          <t>CSA AI Safety</t>
-        </is>
-      </c>
-      <c r="H42" s="111" t="inlineStr">
-        <is>
-          <t>NIST CSF 2.0</t>
-        </is>
-      </c>
-      <c r="I42" s="74" t="n"/>
-      <c r="J42" s="74" t="n"/>
-      <c r="K42" s="74" t="n"/>
-    </row>
-    <row r="43" ht="40" customHeight="1">
-      <c r="B43" s="131" t="inlineStr">
-        <is>
-          <t>AI Inventory &amp; Discovery</t>
-        </is>
-      </c>
-      <c r="C43" s="206" t="inlineStr">
-        <is>
-          <t>Annex A.6.2.2
-AI system register</t>
-        </is>
-      </c>
-      <c r="D43" s="207" t="inlineStr">
-        <is>
-          <t>MAP 1.1
-AI system catalog</t>
-        </is>
-      </c>
-      <c r="E43" s="208" t="inlineStr">
-        <is>
-          <t>Art. 60
-EU database registration</t>
-        </is>
-      </c>
-      <c r="F43" s="209" t="inlineStr">
-        <is>
-          <t>CC6.1
-Asset inventory</t>
-        </is>
-      </c>
-      <c r="G43" s="210" t="inlineStr">
-        <is>
-          <t>AIS-01
-AI workload inventory</t>
-        </is>
-      </c>
-      <c r="H43" s="211" t="inlineStr">
-        <is>
-          <t>ID.AM-1
-Hardware/software inventory</t>
-        </is>
-      </c>
-      <c r="I43" s="74" t="n"/>
-      <c r="J43" s="74" t="n"/>
-      <c r="K43" s="74" t="n"/>
-    </row>
-    <row r="44" ht="40" customHeight="1">
-      <c r="B44" s="131" t="inlineStr">
-        <is>
-          <t>Risk Assessment</t>
-        </is>
-      </c>
-      <c r="C44" s="206" t="inlineStr">
-        <is>
-          <t>Annex A.5.4
-AI risk assessment</t>
-        </is>
-      </c>
-      <c r="D44" s="207" t="inlineStr">
-        <is>
-          <t>MAP 2.1-2.3
-Risk identification</t>
-        </is>
-      </c>
-      <c r="E44" s="208" t="inlineStr">
-        <is>
-          <t>Art. 9
-Risk management system</t>
-        </is>
-      </c>
-      <c r="F44" s="209" t="inlineStr">
-        <is>
-          <t>CC3.2
-Risk assessment</t>
-        </is>
-      </c>
-      <c r="G44" s="210" t="inlineStr">
-        <is>
-          <t>AIS-02
-Cloud AI risk assessment</t>
-        </is>
-      </c>
-      <c r="H44" s="211" t="inlineStr">
-        <is>
-          <t>ID.RA-1
-Asset vulnerabilities</t>
-        </is>
-      </c>
-      <c r="I44" s="74" t="n"/>
-      <c r="J44" s="74" t="n"/>
-      <c r="K44" s="74" t="n"/>
-    </row>
-    <row r="45" ht="40" customHeight="1">
-      <c r="B45" s="131" t="inlineStr">
-        <is>
-          <t>Control Verification</t>
-        </is>
-      </c>
-      <c r="C45" s="206" t="inlineStr">
-        <is>
-          <t>Annex A.6.2.4
-Control effectiveness</t>
-        </is>
-      </c>
-      <c r="D45" s="207" t="inlineStr">
-        <is>
-          <t>MEASURE 2.1
-Control evaluation</t>
-        </is>
-      </c>
-      <c r="E45" s="208" t="inlineStr">
-        <is>
-          <t>Art. 9(4)
-Testing &amp; validation</t>
-        </is>
-      </c>
-      <c r="F45" s="209" t="inlineStr">
-        <is>
-          <t>CC5.1
-Control activities</t>
-        </is>
-      </c>
-      <c r="G45" s="210" t="inlineStr">
-        <is>
-          <t>AIS-03
-Security controls</t>
-        </is>
-      </c>
-      <c r="H45" s="211" t="inlineStr">
-        <is>
-          <t>PR.IP-1
-Baseline config</t>
-        </is>
-      </c>
-      <c r="I45" s="74" t="n"/>
-      <c r="J45" s="74" t="n"/>
-      <c r="K45" s="74" t="n"/>
-    </row>
-    <row r="46" ht="40" customHeight="1">
-      <c r="B46" s="131" t="inlineStr">
-        <is>
-          <t>Approval &amp; Change Mgmt</t>
-        </is>
-      </c>
-      <c r="C46" s="206" t="inlineStr">
-        <is>
-          <t>Annex A.7.2
-Change management</t>
-        </is>
-      </c>
-      <c r="D46" s="207" t="inlineStr">
-        <is>
-          <t>GOVERN 1.4
-Approval processes</t>
-        </is>
-      </c>
-      <c r="E46" s="208" t="inlineStr">
-        <is>
-          <t>Art. 17
-Quality mgmt system</t>
-        </is>
-      </c>
-      <c r="F46" s="209" t="inlineStr">
-        <is>
-          <t>CC8.1
-Change management</t>
-        </is>
-      </c>
-      <c r="G46" s="122" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="H46" s="211" t="inlineStr">
-        <is>
-          <t>PR.IP-3
-Change control</t>
-        </is>
-      </c>
+      <c r="C46" s="74" t="n"/>
+      <c r="D46" s="74" t="n"/>
+      <c r="E46" s="74" t="n"/>
+      <c r="F46" s="74" t="n"/>
+      <c r="G46" s="74" t="n"/>
+      <c r="H46" s="74" t="n"/>
       <c r="I46" s="74" t="n"/>
       <c r="J46" s="74" t="n"/>
       <c r="K46" s="74" t="n"/>
     </row>
     <row r="47" ht="40" customHeight="1">
-      <c r="B47" s="131" t="inlineStr">
-        <is>
-          <t>Monitoring &amp; Logging</t>
-        </is>
-      </c>
-      <c r="C47" s="206" t="inlineStr">
-        <is>
-          <t>Annex A.8.3
-Monitoring</t>
-        </is>
-      </c>
-      <c r="D47" s="207" t="inlineStr">
-        <is>
-          <t>MEASURE 1.1
-Performance metrics</t>
-        </is>
-      </c>
-      <c r="E47" s="208" t="inlineStr">
-        <is>
-          <t>Art. 12
-Record-keeping</t>
-        </is>
-      </c>
-      <c r="F47" s="209" t="inlineStr">
-        <is>
-          <t>CC7.2
-System monitoring</t>
-        </is>
-      </c>
-      <c r="G47" s="210" t="inlineStr">
-        <is>
-          <t>AIS-04
-Observability</t>
-        </is>
-      </c>
-      <c r="H47" s="211" t="inlineStr">
-        <is>
-          <t>DE.CM-1
-Network monitoring</t>
-        </is>
-      </c>
+      <c r="B47" s="104" t="inlineStr">
+        <is>
+          <t>Matrix showing which metrics each framework requires. Use this to identify gaps and prioritize measurement efforts based on your compliance obligations.</t>
+        </is>
+      </c>
+      <c r="C47" s="74" t="n"/>
+      <c r="D47" s="74" t="n"/>
+      <c r="E47" s="74" t="n"/>
+      <c r="F47" s="74" t="n"/>
+      <c r="G47" s="74" t="n"/>
+      <c r="H47" s="74" t="n"/>
       <c r="I47" s="74" t="n"/>
       <c r="J47" s="74" t="n"/>
       <c r="K47" s="74" t="n"/>
     </row>
     <row r="48" ht="40" customHeight="1">
-      <c r="B48" s="131" t="inlineStr">
-        <is>
-          <t>Incident Response</t>
-        </is>
-      </c>
-      <c r="C48" s="206" t="inlineStr">
-        <is>
-          <t>Annex A.8.4
-Incident handling</t>
-        </is>
-      </c>
-      <c r="D48" s="207" t="inlineStr">
-        <is>
-          <t>MANAGE 3.1
-Incident response</t>
-        </is>
-      </c>
-      <c r="E48" s="208" t="inlineStr">
-        <is>
-          <t>Art. 62
-Serious incident reporting</t>
-        </is>
-      </c>
-      <c r="F48" s="209" t="inlineStr">
-        <is>
-          <t>CC7.4
-Incident response</t>
-        </is>
-      </c>
-      <c r="G48" s="210" t="inlineStr">
-        <is>
-          <t>AIS-06
-Incident management</t>
-        </is>
-      </c>
-      <c r="H48" s="211" t="inlineStr">
-        <is>
-          <t>RS.RP-1
-Response plan</t>
+      <c r="B48" s="105" t="inlineStr">
+        <is>
+          <t>Metric Category</t>
+        </is>
+      </c>
+      <c r="C48" s="106" t="inlineStr">
+        <is>
+          <t>ISO 42001</t>
+        </is>
+      </c>
+      <c r="D48" s="107" t="inlineStr">
+        <is>
+          <t>NIST AI RMF</t>
+        </is>
+      </c>
+      <c r="E48" s="108" t="inlineStr">
+        <is>
+          <t>EU AI Act</t>
+        </is>
+      </c>
+      <c r="F48" s="109" t="inlineStr">
+        <is>
+          <t>SOC 2</t>
+        </is>
+      </c>
+      <c r="G48" s="110" t="inlineStr">
+        <is>
+          <t>CSA AI Safety</t>
+        </is>
+      </c>
+      <c r="H48" s="111" t="inlineStr">
+        <is>
+          <t>NIST CSF 2.0</t>
         </is>
       </c>
       <c r="I48" s="74" t="n"/>
@@ -6302,43 +6241,43 @@
     <row r="49" ht="40" customHeight="1">
       <c r="B49" s="131" t="inlineStr">
         <is>
-          <t>Third-Party/Vendor</t>
+          <t>AI Inventory &amp; Discovery</t>
         </is>
       </c>
       <c r="C49" s="206" t="inlineStr">
         <is>
-          <t>Annex A.6.2.6
-Supplier management</t>
+          <t>Annex A.6.2.2
+AI system register</t>
         </is>
       </c>
       <c r="D49" s="207" t="inlineStr">
         <is>
-          <t>MAP 4.1
-Third-party assessment</t>
+          <t>MAP 1.1
+AI system catalog</t>
         </is>
       </c>
       <c r="E49" s="208" t="inlineStr">
         <is>
-          <t>Art. 25
-Supply chain diligence</t>
+          <t>Art. 60
+EU database registration</t>
         </is>
       </c>
       <c r="F49" s="209" t="inlineStr">
         <is>
-          <t>CC9.2
-Vendor management</t>
+          <t>CC6.1
+Asset inventory</t>
         </is>
       </c>
       <c r="G49" s="210" t="inlineStr">
         <is>
-          <t>AIS-05
-Third-party AI</t>
+          <t>AIS-01
+AI workload inventory</t>
         </is>
       </c>
       <c r="H49" s="211" t="inlineStr">
         <is>
-          <t>ID.SC-1
-Supply chain risk</t>
+          <t>ID.AM-1
+Hardware/software inventory</t>
         </is>
       </c>
       <c r="I49" s="74" t="n"/>
@@ -6348,40 +6287,43 @@
     <row r="50" ht="40" customHeight="1">
       <c r="B50" s="131" t="inlineStr">
         <is>
-          <t>Human Oversight</t>
+          <t>Risk Assessment</t>
         </is>
       </c>
       <c r="C50" s="206" t="inlineStr">
         <is>
-          <t>Annex A.6.2.3
-Human oversight</t>
+          <t>Annex A.5.4
+AI risk assessment</t>
         </is>
       </c>
       <c r="D50" s="207" t="inlineStr">
         <is>
-          <t>GOVERN 3.1
-Human-AI teaming</t>
+          <t>MAP 2.1-2.3
+Risk identification</t>
         </is>
       </c>
       <c r="E50" s="208" t="inlineStr">
         <is>
-          <t>Art. 14
-Human oversight</t>
-        </is>
-      </c>
-      <c r="F50" s="122" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="G50" s="122" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="H50" s="122" t="inlineStr">
-        <is>
-          <t>—</t>
+          <t>Art. 9
+Risk management system</t>
+        </is>
+      </c>
+      <c r="F50" s="209" t="inlineStr">
+        <is>
+          <t>CC3.2
+Risk assessment</t>
+        </is>
+      </c>
+      <c r="G50" s="210" t="inlineStr">
+        <is>
+          <t>AIS-02
+Cloud AI risk assessment</t>
+        </is>
+      </c>
+      <c r="H50" s="211" t="inlineStr">
+        <is>
+          <t>ID.RA-1
+Asset vulnerabilities</t>
         </is>
       </c>
       <c r="I50" s="74" t="n"/>
@@ -6391,43 +6333,43 @@
     <row r="51" ht="40" customHeight="1">
       <c r="B51" s="131" t="inlineStr">
         <is>
-          <t>Data Protection</t>
+          <t>Control Verification</t>
         </is>
       </c>
       <c r="C51" s="206" t="inlineStr">
         <is>
-          <t>Annex A.7.4
-Data management</t>
+          <t>Annex A.6.2.4
+Control effectiveness</t>
         </is>
       </c>
       <c r="D51" s="207" t="inlineStr">
         <is>
-          <t>MAP 3.1
-Data quality</t>
+          <t>MEASURE 2.1
+Control evaluation</t>
         </is>
       </c>
       <c r="E51" s="208" t="inlineStr">
         <is>
-          <t>Art. 10
-Data governance</t>
+          <t>Art. 9(4)
+Testing &amp; validation</t>
         </is>
       </c>
       <c r="F51" s="209" t="inlineStr">
         <is>
-          <t>CC6.1
-Data protection</t>
+          <t>CC5.1
+Control activities</t>
         </is>
       </c>
       <c r="G51" s="210" t="inlineStr">
         <is>
-          <t>AIS-07
-Data security</t>
+          <t>AIS-03
+Security controls</t>
         </is>
       </c>
       <c r="H51" s="211" t="inlineStr">
         <is>
-          <t>PR.DS-1
-Data protection</t>
+          <t>PR.IP-1
+Baseline config</t>
         </is>
       </c>
       <c r="I51" s="74" t="n"/>
@@ -6435,313 +6377,587 @@
       <c r="K51" s="74" t="n"/>
     </row>
     <row r="52" ht="25" customHeight="1">
-      <c r="B52" s="112" t="n"/>
-      <c r="C52" s="112" t="n"/>
-      <c r="D52" s="112" t="n"/>
-      <c r="E52" s="112" t="n"/>
-      <c r="F52" s="74" t="n"/>
-      <c r="G52" s="74" t="n"/>
-      <c r="H52" s="74" t="n"/>
+      <c r="B52" s="131" t="inlineStr">
+        <is>
+          <t>Approval &amp; Change Mgmt</t>
+        </is>
+      </c>
+      <c r="C52" s="206" t="inlineStr">
+        <is>
+          <t>Annex A.7.2
+Change management</t>
+        </is>
+      </c>
+      <c r="D52" s="207" t="inlineStr">
+        <is>
+          <t>GOVERN 1.4
+Approval processes</t>
+        </is>
+      </c>
+      <c r="E52" s="208" t="inlineStr">
+        <is>
+          <t>Art. 17
+Quality mgmt system</t>
+        </is>
+      </c>
+      <c r="F52" s="209" t="inlineStr">
+        <is>
+          <t>CC8.1
+Change management</t>
+        </is>
+      </c>
+      <c r="G52" s="122" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H52" s="211" t="inlineStr">
+        <is>
+          <t>PR.IP-3
+Change control</t>
+        </is>
+      </c>
       <c r="I52" s="74" t="n"/>
       <c r="J52" s="74" t="n"/>
       <c r="K52" s="74" t="n"/>
     </row>
     <row r="53" ht="25" customHeight="1">
-      <c r="B53" s="113" t="inlineStr">
-        <is>
-          <t>Reading the Matrix:</t>
-        </is>
-      </c>
-      <c r="C53" s="112" t="n"/>
-      <c r="D53" s="112" t="n"/>
-      <c r="E53" s="112" t="n"/>
-      <c r="F53" s="74" t="n"/>
-      <c r="G53" s="74" t="n"/>
-      <c r="H53" s="74" t="n"/>
+      <c r="B53" s="131" t="inlineStr">
+        <is>
+          <t>Monitoring &amp; Logging</t>
+        </is>
+      </c>
+      <c r="C53" s="206" t="inlineStr">
+        <is>
+          <t>Annex A.8.3
+Monitoring</t>
+        </is>
+      </c>
+      <c r="D53" s="207" t="inlineStr">
+        <is>
+          <t>MEASURE 1.1
+Performance metrics</t>
+        </is>
+      </c>
+      <c r="E53" s="208" t="inlineStr">
+        <is>
+          <t>Art. 12
+Record-keeping</t>
+        </is>
+      </c>
+      <c r="F53" s="209" t="inlineStr">
+        <is>
+          <t>CC7.2
+System monitoring</t>
+        </is>
+      </c>
+      <c r="G53" s="210" t="inlineStr">
+        <is>
+          <t>AIS-04
+Observability</t>
+        </is>
+      </c>
+      <c r="H53" s="211" t="inlineStr">
+        <is>
+          <t>DE.CM-1
+Network monitoring</t>
+        </is>
+      </c>
       <c r="I53" s="74" t="n"/>
       <c r="J53" s="74" t="n"/>
       <c r="K53" s="74" t="n"/>
     </row>
     <row r="54" ht="25" customHeight="1">
-      <c r="B54" s="114" t="inlineStr">
-        <is>
-          <t>• Each cell shows the specific clause/control requiring that metric category</t>
-        </is>
-      </c>
-      <c r="C54" s="112" t="n"/>
-      <c r="D54" s="112" t="n"/>
-      <c r="E54" s="112" t="n"/>
-      <c r="F54" s="74" t="n"/>
-      <c r="G54" s="74" t="n"/>
-      <c r="H54" s="74" t="n"/>
+      <c r="B54" s="131" t="inlineStr">
+        <is>
+          <t>Incident Response</t>
+        </is>
+      </c>
+      <c r="C54" s="206" t="inlineStr">
+        <is>
+          <t>Annex A.8.4
+Incident handling</t>
+        </is>
+      </c>
+      <c r="D54" s="207" t="inlineStr">
+        <is>
+          <t>MANAGE 3.1
+Incident response</t>
+        </is>
+      </c>
+      <c r="E54" s="208" t="inlineStr">
+        <is>
+          <t>Art. 62
+Serious incident reporting</t>
+        </is>
+      </c>
+      <c r="F54" s="209" t="inlineStr">
+        <is>
+          <t>CC7.4
+Incident response</t>
+        </is>
+      </c>
+      <c r="G54" s="210" t="inlineStr">
+        <is>
+          <t>AIS-06
+Incident management</t>
+        </is>
+      </c>
+      <c r="H54" s="211" t="inlineStr">
+        <is>
+          <t>RS.RP-1
+Response plan</t>
+        </is>
+      </c>
       <c r="I54" s="74" t="n"/>
       <c r="J54" s="74" t="n"/>
       <c r="K54" s="74" t="n"/>
     </row>
     <row r="55" ht="25" customHeight="1">
-      <c r="B55" s="114" t="inlineStr">
-        <is>
-          <t>• '—' indicates the framework does not explicitly require this metric</t>
-        </is>
-      </c>
-      <c r="C55" s="112" t="n"/>
-      <c r="D55" s="112" t="n"/>
-      <c r="E55" s="112" t="n"/>
-      <c r="F55" s="74" t="n"/>
-      <c r="G55" s="74" t="n"/>
-      <c r="H55" s="74" t="n"/>
+      <c r="B55" s="131" t="inlineStr">
+        <is>
+          <t>Third-Party/Vendor</t>
+        </is>
+      </c>
+      <c r="C55" s="206" t="inlineStr">
+        <is>
+          <t>Annex A.6.2.6
+Supplier management</t>
+        </is>
+      </c>
+      <c r="D55" s="207" t="inlineStr">
+        <is>
+          <t>MAP 4.1
+Third-party assessment</t>
+        </is>
+      </c>
+      <c r="E55" s="208" t="inlineStr">
+        <is>
+          <t>Art. 25
+Supply chain diligence</t>
+        </is>
+      </c>
+      <c r="F55" s="209" t="inlineStr">
+        <is>
+          <t>CC9.2
+Vendor management</t>
+        </is>
+      </c>
+      <c r="G55" s="210" t="inlineStr">
+        <is>
+          <t>AIS-05
+Third-party AI</t>
+        </is>
+      </c>
+      <c r="H55" s="211" t="inlineStr">
+        <is>
+          <t>ID.SC-1
+Supply chain risk</t>
+        </is>
+      </c>
       <c r="I55" s="74" t="n"/>
       <c r="J55" s="74" t="n"/>
       <c r="K55" s="74" t="n"/>
     </row>
     <row r="56" ht="25" customHeight="1">
-      <c r="B56" s="114" t="inlineStr">
-        <is>
-          <t>• Color-coded by framework for quick identification of coverage gaps</t>
-        </is>
-      </c>
-      <c r="C56" s="112" t="n"/>
-      <c r="D56" s="112" t="n"/>
-      <c r="E56" s="112" t="n"/>
-      <c r="F56" s="74" t="n"/>
-      <c r="G56" s="74" t="n"/>
-      <c r="H56" s="74" t="n"/>
+      <c r="B56" s="131" t="inlineStr">
+        <is>
+          <t>Human Oversight</t>
+        </is>
+      </c>
+      <c r="C56" s="206" t="inlineStr">
+        <is>
+          <t>Annex A.6.2.3
+Human oversight</t>
+        </is>
+      </c>
+      <c r="D56" s="207" t="inlineStr">
+        <is>
+          <t>GOVERN 3.1
+Human-AI teaming</t>
+        </is>
+      </c>
+      <c r="E56" s="208" t="inlineStr">
+        <is>
+          <t>Art. 14
+Human oversight</t>
+        </is>
+      </c>
+      <c r="F56" s="122" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="G56" s="122" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="H56" s="122" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="I56" s="74" t="n"/>
       <c r="J56" s="74" t="n"/>
       <c r="K56" s="74" t="n"/>
     </row>
     <row r="57">
-      <c r="B57" s="74" t="n"/>
-      <c r="C57" s="74" t="n"/>
-      <c r="D57" s="74" t="n"/>
-      <c r="E57" s="74" t="n"/>
-      <c r="F57" s="74" t="n"/>
-      <c r="G57" s="74" t="n"/>
-      <c r="H57" s="74" t="n"/>
+      <c r="B57" s="131" t="inlineStr">
+        <is>
+          <t>Data Protection</t>
+        </is>
+      </c>
+      <c r="C57" s="206" t="inlineStr">
+        <is>
+          <t>Annex A.7.4
+Data management</t>
+        </is>
+      </c>
+      <c r="D57" s="207" t="inlineStr">
+        <is>
+          <t>MAP 3.1
+Data quality</t>
+        </is>
+      </c>
+      <c r="E57" s="208" t="inlineStr">
+        <is>
+          <t>Art. 10
+Data governance</t>
+        </is>
+      </c>
+      <c r="F57" s="209" t="inlineStr">
+        <is>
+          <t>CC6.1
+Data protection</t>
+        </is>
+      </c>
+      <c r="G57" s="210" t="inlineStr">
+        <is>
+          <t>AIS-07
+Data security</t>
+        </is>
+      </c>
+      <c r="H57" s="211" t="inlineStr">
+        <is>
+          <t>PR.DS-1
+Data protection</t>
+        </is>
+      </c>
       <c r="I57" s="74" t="n"/>
       <c r="J57" s="74" t="n"/>
       <c r="K57" s="74" t="n"/>
     </row>
     <row r="58" ht="18" customHeight="1">
-      <c r="B58" s="96" t="inlineStr">
+      <c r="B58" s="112" t="n"/>
+      <c r="C58" s="112" t="n"/>
+      <c r="D58" s="112" t="n"/>
+      <c r="E58" s="112" t="n"/>
+      <c r="F58" s="74" t="n"/>
+      <c r="G58" s="74" t="n"/>
+      <c r="H58" s="74" t="n"/>
+      <c r="I58" s="74" t="n"/>
+      <c r="J58" s="74" t="n"/>
+      <c r="K58" s="74" t="n"/>
+    </row>
+    <row r="59">
+      <c r="B59" s="113" t="inlineStr">
+        <is>
+          <t>Reading the Matrix:</t>
+        </is>
+      </c>
+      <c r="C59" s="112" t="n"/>
+      <c r="D59" s="112" t="n"/>
+      <c r="E59" s="112" t="n"/>
+      <c r="F59" s="74" t="n"/>
+      <c r="G59" s="74" t="n"/>
+      <c r="H59" s="74" t="n"/>
+      <c r="I59" s="74" t="n"/>
+      <c r="J59" s="74" t="n"/>
+      <c r="K59" s="74" t="n"/>
+    </row>
+    <row r="60" ht="30" customHeight="1">
+      <c r="B60" s="114" t="inlineStr">
+        <is>
+          <t>• Each cell shows the specific clause/control requiring that metric category</t>
+        </is>
+      </c>
+      <c r="C60" s="112" t="n"/>
+      <c r="D60" s="112" t="n"/>
+      <c r="E60" s="112" t="n"/>
+      <c r="F60" s="74" t="n"/>
+      <c r="G60" s="74" t="n"/>
+      <c r="H60" s="74" t="n"/>
+      <c r="I60" s="74" t="n"/>
+      <c r="J60" s="74" t="n"/>
+      <c r="K60" s="74" t="n"/>
+    </row>
+    <row r="61" ht="30" customHeight="1">
+      <c r="B61" s="114" t="inlineStr">
+        <is>
+          <t>• '—' indicates the framework does not explicitly require this metric</t>
+        </is>
+      </c>
+      <c r="C61" s="112" t="n"/>
+      <c r="D61" s="112" t="n"/>
+      <c r="E61" s="112" t="n"/>
+      <c r="F61" s="74" t="n"/>
+      <c r="G61" s="74" t="n"/>
+      <c r="H61" s="74" t="n"/>
+      <c r="I61" s="74" t="n"/>
+      <c r="J61" s="74" t="n"/>
+      <c r="K61" s="74" t="n"/>
+    </row>
+    <row r="62" ht="30" customHeight="1">
+      <c r="B62" s="114" t="inlineStr">
+        <is>
+          <t>• Color-coded by framework for quick identification of coverage gaps</t>
+        </is>
+      </c>
+      <c r="C62" s="112" t="n"/>
+      <c r="D62" s="112" t="n"/>
+      <c r="E62" s="112" t="n"/>
+      <c r="F62" s="74" t="n"/>
+      <c r="G62" s="74" t="n"/>
+      <c r="H62" s="74" t="n"/>
+      <c r="I62" s="74" t="n"/>
+      <c r="J62" s="74" t="n"/>
+      <c r="K62" s="74" t="n"/>
+    </row>
+    <row r="63" ht="30" customHeight="1">
+      <c r="B63" s="74" t="n"/>
+      <c r="C63" s="74" t="n"/>
+      <c r="D63" s="74" t="n"/>
+      <c r="E63" s="74" t="n"/>
+      <c r="F63" s="74" t="n"/>
+      <c r="G63" s="74" t="n"/>
+      <c r="H63" s="74" t="n"/>
+      <c r="I63" s="74" t="n"/>
+      <c r="J63" s="74" t="n"/>
+      <c r="K63" s="74" t="n"/>
+    </row>
+    <row r="64" ht="30" customHeight="1">
+      <c r="B64" s="96" t="inlineStr">
         <is>
           <t>5. Reporting Cadence</t>
         </is>
       </c>
     </row>
-    <row r="59">
-      <c r="B59" s="99" t="inlineStr">
+    <row r="65">
+      <c r="B65" s="99" t="inlineStr">
         <is>
           <t>Report</t>
         </is>
       </c>
-      <c r="C59" s="99" t="inlineStr">
+      <c r="C65" s="99" t="inlineStr">
         <is>
           <t>Audience</t>
         </is>
       </c>
-      <c r="D59" s="99" t="inlineStr">
+      <c r="D65" s="99" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="E59" s="99" t="inlineStr">
+      <c r="E65" s="99" t="inlineStr">
         <is>
           <t>Contents</t>
         </is>
       </c>
     </row>
-    <row r="60" ht="30" customHeight="1">
-      <c r="B60" s="130" t="inlineStr">
+    <row r="66">
+      <c r="B66" s="130" t="inlineStr">
         <is>
           <t>Executive Dashboard</t>
         </is>
       </c>
-      <c r="C60" s="130" t="inlineStr">
+      <c r="C66" s="130" t="inlineStr">
         <is>
           <t>CISO, Security Leadership</t>
         </is>
       </c>
-      <c r="D60" s="130" t="inlineStr">
+      <c r="D66" s="130" t="inlineStr">
         <is>
           <t>Monthly</t>
         </is>
       </c>
-      <c r="E60" s="130" t="inlineStr">
+      <c r="E66" s="130" t="inlineStr">
         <is>
           <t>KPI summary, SLO status, trend analysis, risk highlights</t>
         </is>
       </c>
     </row>
-    <row r="61" ht="30" customHeight="1">
-      <c r="B61" s="130" t="inlineStr">
+    <row r="67" ht="18" customHeight="1">
+      <c r="B67" s="130" t="inlineStr">
         <is>
           <t>Operational Report</t>
         </is>
       </c>
-      <c r="C61" s="130" t="inlineStr">
+      <c r="C67" s="130" t="inlineStr">
         <is>
           <t>Security Team, Tool Owners</t>
         </is>
       </c>
-      <c r="D61" s="130" t="inlineStr">
+      <c r="D67" s="130" t="inlineStr">
         <is>
           <t>Weekly</t>
         </is>
       </c>
-      <c r="E61" s="130" t="inlineStr">
+      <c r="E67" s="130" t="inlineStr">
         <is>
           <t>New tools, pending reviews, expiring exceptions, incidents</t>
         </is>
       </c>
     </row>
-    <row r="62" ht="30" customHeight="1">
-      <c r="B62" s="130" t="inlineStr">
+    <row r="68">
+      <c r="B68" s="130" t="inlineStr">
         <is>
           <t>Compliance Report</t>
         </is>
       </c>
-      <c r="C62" s="130" t="inlineStr">
+      <c r="C68" s="130" t="inlineStr">
         <is>
           <t>Compliance, Audit, Legal</t>
         </is>
       </c>
-      <c r="D62" s="130" t="inlineStr">
+      <c r="D68" s="130" t="inlineStr">
         <is>
           <t>Quarterly</t>
         </is>
       </c>
-      <c r="E62" s="130" t="inlineStr">
+      <c r="E68" s="130" t="inlineStr">
         <is>
           <t>Framework-specific metrics, evidence artifacts, gaps</t>
         </is>
       </c>
     </row>
-    <row r="63" ht="30" customHeight="1">
-      <c r="B63" s="130" t="inlineStr">
+    <row r="69">
+      <c r="B69" s="130" t="inlineStr">
         <is>
           <t>Board Summary</t>
         </is>
       </c>
-      <c r="C63" s="130" t="inlineStr">
+      <c r="C69" s="130" t="inlineStr">
         <is>
           <t>Board, Executive Committee</t>
         </is>
       </c>
-      <c r="D63" s="130" t="inlineStr">
+      <c r="D69" s="130" t="inlineStr">
         <is>
           <t>Quarterly</t>
         </is>
       </c>
-      <c r="E63" s="130" t="inlineStr">
+      <c r="E69" s="130" t="inlineStr">
         <is>
           <t>Program maturity, major risks, strategic recommendations</t>
         </is>
       </c>
     </row>
-    <row r="64" ht="30" customHeight="1">
-      <c r="B64" s="130" t="inlineStr">
+    <row r="70" ht="85" customHeight="1">
+      <c r="B70" s="130" t="inlineStr">
         <is>
           <t>Incident Report</t>
         </is>
       </c>
-      <c r="C64" s="130" t="inlineStr">
+      <c r="C70" s="130" t="inlineStr">
         <is>
           <t>Security Leadership</t>
         </is>
       </c>
-      <c r="D64" s="130" t="inlineStr">
+      <c r="D70" s="130" t="inlineStr">
         <is>
           <t>Per incident</t>
         </is>
       </c>
-      <c r="E64" s="130" t="inlineStr">
+      <c r="E70" s="130" t="inlineStr">
         <is>
           <t>Root cause, impact, remediation, lessons learned</t>
         </is>
       </c>
     </row>
-    <row r="67" ht="18" customHeight="1">
-      <c r="B67" s="103" t="inlineStr">
+    <row r="71" ht="85" customHeight="1"/>
+    <row r="72" ht="85" customHeight="1"/>
+    <row r="73" ht="85" customHeight="1">
+      <c r="B73" s="103" t="inlineStr">
         <is>
           <t>6. Program Maturity Model (CMM-Aligned)</t>
         </is>
       </c>
-      <c r="C67" s="74" t="n"/>
-      <c r="D67" s="74" t="n"/>
-      <c r="E67" s="74" t="n"/>
-      <c r="F67" s="74" t="n"/>
-      <c r="G67" s="74" t="n"/>
-      <c r="H67" s="74" t="n"/>
-      <c r="I67" s="74" t="n"/>
-    </row>
-    <row r="68">
-      <c r="B68" s="104" t="inlineStr">
+      <c r="C73" s="74" t="n"/>
+      <c r="D73" s="74" t="n"/>
+      <c r="E73" s="74" t="n"/>
+      <c r="F73" s="74" t="n"/>
+      <c r="G73" s="74" t="n"/>
+      <c r="H73" s="74" t="n"/>
+      <c r="I73" s="74" t="n"/>
+    </row>
+    <row r="74" ht="85" customHeight="1">
+      <c r="B74" s="104" t="inlineStr">
         <is>
           <t>Based on Carnegie Mellon's Capability Maturity Model. Use this to assess current state, set improvement goals, and communicate progress to leadership.</t>
         </is>
       </c>
-      <c r="C68" s="74" t="n"/>
-      <c r="D68" s="74" t="n"/>
-      <c r="E68" s="74" t="n"/>
-      <c r="F68" s="74" t="n"/>
-      <c r="G68" s="74" t="n"/>
-      <c r="H68" s="74" t="n"/>
-      <c r="I68" s="74" t="n"/>
-    </row>
-    <row r="69">
-      <c r="B69" s="105" t="inlineStr">
+      <c r="C74" s="74" t="n"/>
+      <c r="D74" s="74" t="n"/>
+      <c r="E74" s="74" t="n"/>
+      <c r="F74" s="74" t="n"/>
+      <c r="G74" s="74" t="n"/>
+      <c r="H74" s="74" t="n"/>
+      <c r="I74" s="74" t="n"/>
+    </row>
+    <row r="75">
+      <c r="B75" s="105" t="inlineStr">
         <is>
           <t>Level</t>
         </is>
       </c>
-      <c r="C69" s="105" t="inlineStr">
+      <c r="C75" s="105" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="D69" s="105" t="inlineStr">
+      <c r="D75" s="105" t="inlineStr">
         <is>
           <t>CMM Alignment</t>
         </is>
       </c>
-      <c r="E69" s="105" t="inlineStr">
+      <c r="E75" s="105" t="inlineStr">
         <is>
           <t>Characteristics</t>
         </is>
       </c>
-      <c r="F69" s="105" t="inlineStr">
+      <c r="F75" s="105" t="inlineStr">
         <is>
           <t>Key Actions at This Level</t>
         </is>
       </c>
-      <c r="G69" s="105" t="inlineStr">
+      <c r="G75" s="105" t="inlineStr">
         <is>
           <t>Tabs to Use</t>
         </is>
       </c>
-      <c r="H69" s="105" t="inlineStr">
+      <c r="H75" s="105" t="inlineStr">
         <is>
           <t>How to Advance</t>
         </is>
       </c>
-      <c r="I69" s="74" t="n"/>
-    </row>
-    <row r="70" ht="85" customHeight="1">
-      <c r="B70" s="115" t="n">
+      <c r="I75" s="74" t="n"/>
+    </row>
+    <row r="76">
+      <c r="B76" s="115" t="n">
         <v>1</v>
       </c>
-      <c r="C70" s="132" t="inlineStr">
+      <c r="C76" s="132" t="inlineStr">
         <is>
           <t>Initial</t>
         </is>
       </c>
-      <c r="D70" s="195" t="inlineStr">
+      <c r="D76" s="195" t="inlineStr">
         <is>
           <t>Ad-hoc, unpredictable, reactive. Success depends on individual effort.</t>
         </is>
       </c>
-      <c r="E70" s="195" t="inlineStr">
+      <c r="E76" s="195" t="inlineStr">
         <is>
           <t>• No formal AI inventory
 • Shadow AI prevalent
@@ -6750,7 +6966,7 @@
 • Decisions made case-by-case</t>
         </is>
       </c>
-      <c r="F70" s="195" t="inlineStr">
+      <c r="F76" s="195" t="inlineStr">
         <is>
           <t>• Acknowledge the problem
 • Identify key stakeholders
@@ -6759,13 +6975,13 @@
 • Establish basic communication</t>
         </is>
       </c>
-      <c r="G70" s="195" t="inlineStr">
+      <c r="G76" s="195" t="inlineStr">
         <is>
           <t>Overview
 User Guide</t>
         </is>
       </c>
-      <c r="H70" s="195" t="inlineStr">
+      <c r="H76" s="195" t="inlineStr">
         <is>
           <t>• Establish governance committee
 • Create initial tool inventory
@@ -6774,23 +6990,23 @@
 • Set up basic intake process</t>
         </is>
       </c>
-      <c r="I70" s="74" t="n"/>
-    </row>
-    <row r="71" ht="85" customHeight="1">
-      <c r="B71" s="116" t="n">
+      <c r="I76" s="74" t="n"/>
+    </row>
+    <row r="77">
+      <c r="B77" s="116" t="n">
         <v>2</v>
       </c>
-      <c r="C71" s="133" t="inlineStr">
+      <c r="C77" s="133" t="inlineStr">
         <is>
           <t>Managed</t>
         </is>
       </c>
-      <c r="D71" s="195" t="inlineStr">
+      <c r="D77" s="195" t="inlineStr">
         <is>
           <t>Processes planned, documented at project level. Basic controls exist but inconsistent.</t>
         </is>
       </c>
-      <c r="E71" s="195" t="inlineStr">
+      <c r="E77" s="195" t="inlineStr">
         <is>
           <t>• Partial tool inventory (50-75%)
 • Basic intake process exists
@@ -6799,7 +7015,7 @@
 • Inconsistent enforcement</t>
         </is>
       </c>
-      <c r="F71" s="195" t="inlineStr">
+      <c r="F77" s="195" t="inlineStr">
         <is>
           <t>• Maintain tool registry
 • Process intake requests
@@ -6808,14 +7024,14 @@
 • Respond to incidents</t>
         </is>
       </c>
-      <c r="G71" s="195" t="inlineStr">
+      <c r="G77" s="195" t="inlineStr">
         <is>
           <t>Tool Registry
 Intake Form
 Governance Guide</t>
         </is>
       </c>
-      <c r="H71" s="195" t="inlineStr">
+      <c r="H77" s="195" t="inlineStr">
         <is>
           <t>• Standardize all processes
 • Document guardrail requirements
@@ -6824,23 +7040,23 @@
 • Train all stakeholders</t>
         </is>
       </c>
-      <c r="I71" s="74" t="n"/>
-    </row>
-    <row r="72" ht="85" customHeight="1">
-      <c r="B72" s="117" t="n">
+      <c r="I77" s="74" t="n"/>
+    </row>
+    <row r="78">
+      <c r="B78" s="117" t="n">
         <v>3</v>
       </c>
-      <c r="C72" s="134" t="inlineStr">
+      <c r="C78" s="134" t="inlineStr">
         <is>
           <t>Defined</t>
         </is>
       </c>
-      <c r="D72" s="195" t="inlineStr">
+      <c r="D78" s="195" t="inlineStr">
         <is>
           <t>Standard process for organization. Processes documented, understood, and followed.</t>
         </is>
       </c>
-      <c r="E72" s="195" t="inlineStr">
+      <c r="E78" s="195" t="inlineStr">
         <is>
           <t>• Complete inventory (75-90%)
 • Standardized workflows
@@ -6850,7 +7066,7 @@
 • Regular review cadence</t>
         </is>
       </c>
-      <c r="F72" s="195" t="inlineStr">
+      <c r="F78" s="195" t="inlineStr">
         <is>
           <t>• Follow defined workflows
 • Verify all guardrails
@@ -6859,7 +7075,7 @@
 • Generate compliance reports</t>
         </is>
       </c>
-      <c r="G72" s="195" t="inlineStr">
+      <c r="G78" s="195" t="inlineStr">
         <is>
           <t>All tabs
 Guardrail Checklist
@@ -6867,7 +7083,7 @@
 Compliance Mapping</t>
         </is>
       </c>
-      <c r="H72" s="195" t="inlineStr">
+      <c r="H78" s="195" t="inlineStr">
         <is>
           <t>• Implement metrics program
 • Establish SLO targets
@@ -6876,23 +7092,23 @@
 • Begin predictive analytics</t>
         </is>
       </c>
-      <c r="I72" s="74" t="n"/>
-    </row>
-    <row r="73" ht="85" customHeight="1">
-      <c r="B73" s="118" t="n">
+      <c r="I78" s="74" t="n"/>
+    </row>
+    <row r="79">
+      <c r="B79" s="118" t="n">
         <v>4</v>
       </c>
-      <c r="C73" s="135" t="inlineStr">
+      <c r="C79" s="135" t="inlineStr">
         <is>
           <t>Quantitatively Managed</t>
         </is>
       </c>
-      <c r="D73" s="195" t="inlineStr">
+      <c r="D79" s="195" t="inlineStr">
         <is>
           <t>Process measured and controlled. Quality and performance understood statistically.</t>
         </is>
       </c>
-      <c r="E73" s="195" t="inlineStr">
+      <c r="E79" s="195" t="inlineStr">
         <is>
           <t>• High coverage (&gt;90%)
 • SLOs consistently met
@@ -6902,7 +7118,7 @@
 • Predictable outcomes</t>
         </is>
       </c>
-      <c r="F73" s="195" t="inlineStr">
+      <c r="F79" s="195" t="inlineStr">
         <is>
           <t>• Monitor KPIs continuously
 • Enforce SLO compliance
@@ -6911,14 +7127,14 @@
 • Report to leadership</t>
         </is>
       </c>
-      <c r="G73" s="195" t="inlineStr">
+      <c r="G79" s="195" t="inlineStr">
         <is>
           <t>Program Metrics
 Compliance Mapping
 Tool Registry</t>
         </is>
       </c>
-      <c r="H73" s="195" t="inlineStr">
+      <c r="H79" s="195" t="inlineStr">
         <is>
           <t>• Focus on optimization
 • Implement AI for AI security
@@ -6927,23 +7143,23 @@
 • Pursue certifications</t>
         </is>
       </c>
-      <c r="I73" s="74" t="n"/>
-    </row>
-    <row r="74" ht="85" customHeight="1">
-      <c r="B74" s="119" t="n">
+      <c r="I79" s="74" t="n"/>
+    </row>
+    <row r="80">
+      <c r="B80" s="119" t="n">
         <v>5</v>
       </c>
-      <c r="C74" s="136" t="inlineStr">
+      <c r="C80" s="136" t="inlineStr">
         <is>
           <t>Optimizing</t>
         </is>
       </c>
-      <c r="D74" s="195" t="inlineStr">
+      <c r="D80" s="195" t="inlineStr">
         <is>
           <t>Focus on continuous improvement. Process improvement embedded in operations.</t>
         </is>
       </c>
-      <c r="E74" s="195" t="inlineStr">
+      <c r="E80" s="195" t="inlineStr">
         <is>
           <t>• Near-complete coverage (&gt;95%)
 • Leading-edge practices
@@ -6953,7 +7169,7 @@
 • Predictive risk management</t>
         </is>
       </c>
-      <c r="F74" s="195" t="inlineStr">
+      <c r="F80" s="195" t="inlineStr">
         <is>
           <t>• Optimize processes continuously
 • Lead industry initiatives
@@ -6962,13 +7178,13 @@
 • Publish thought leadership</t>
         </is>
       </c>
-      <c r="G74" s="195" t="inlineStr">
+      <c r="G80" s="195" t="inlineStr">
         <is>
           <t>All tabs (as templates)
 Program Metrics</t>
         </is>
       </c>
-      <c r="H74" s="195" t="inlineStr">
+      <c r="H80" s="195" t="inlineStr">
         <is>
           <t>Maintain excellence:
 • Regular framework updates
@@ -6977,346 +7193,346 @@
 • Innovation investment</t>
         </is>
       </c>
-      <c r="I74" s="74" t="n"/>
-    </row>
-    <row r="76">
-      <c r="B76" s="120" t="inlineStr">
-        <is>
-          <t>Assessment Guide:</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="B77" s="121" t="inlineStr">
-        <is>
-          <t>• Score each dimension: Inventory, Process, Controls, Monitoring, Compliance (1-5 each)</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" s="121" t="inlineStr">
-        <is>
-          <t>• Average score determines overall maturity level</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="B79" s="121" t="inlineStr">
-        <is>
-          <t>• Target: Advance one level every 6-12 months</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="B80" s="121" t="inlineStr">
-        <is>
-          <t>• Most organizations should aim for Level 3-4; Level 5 is for industry leaders</t>
-        </is>
-      </c>
+      <c r="I80" s="74" t="n"/>
     </row>
     <row r="82">
       <c r="B82" s="120" t="inlineStr">
         <is>
+          <t>Assessment Guide:</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" s="121" t="inlineStr">
+        <is>
+          <t>• Score each dimension: Inventory, Process, Controls, Monitoring, Compliance (1-5 each)</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" s="121" t="inlineStr">
+        <is>
+          <t>• Average score determines overall maturity level</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" s="121" t="inlineStr">
+        <is>
+          <t>• Target: Advance one level every 6-12 months</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" s="121" t="inlineStr">
+        <is>
+          <t>• Most organizations should aim for Level 3-4; Level 5 is for industry leaders</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" s="120" t="inlineStr">
+        <is>
           <t>KPI Benchmarks by Maturity Level:</t>
         </is>
       </c>
     </row>
-    <row r="83">
-      <c r="B83" s="105" t="inlineStr">
+    <row r="89">
+      <c r="B89" s="105" t="inlineStr">
         <is>
           <t>KPI</t>
         </is>
       </c>
-      <c r="C83" s="105" t="inlineStr">
+      <c r="C89" s="105" t="inlineStr">
         <is>
           <t>Level 1</t>
         </is>
       </c>
-      <c r="D83" s="105" t="inlineStr">
+      <c r="D89" s="105" t="inlineStr">
         <is>
           <t>Level 2</t>
         </is>
       </c>
-      <c r="E83" s="105" t="inlineStr">
+      <c r="E89" s="105" t="inlineStr">
         <is>
           <t>Level 3</t>
         </is>
       </c>
-      <c r="F83" s="105" t="inlineStr">
+      <c r="F89" s="105" t="inlineStr">
         <is>
           <t>Level 4</t>
         </is>
       </c>
-      <c r="G83" s="105" t="inlineStr">
+      <c r="G89" s="105" t="inlineStr">
         <is>
           <t>Level 5</t>
         </is>
       </c>
     </row>
-    <row r="84">
-      <c r="B84" s="122" t="inlineStr">
+    <row r="90">
+      <c r="B90" s="122" t="inlineStr">
         <is>
           <t>Tool Inventory Coverage</t>
         </is>
       </c>
-      <c r="C84" s="123" t="inlineStr">
+      <c r="C90" s="123" t="inlineStr">
         <is>
           <t>&lt;50%</t>
         </is>
       </c>
-      <c r="D84" s="124" t="inlineStr">
+      <c r="D90" s="124" t="inlineStr">
         <is>
           <t>50-75%</t>
         </is>
       </c>
-      <c r="E84" s="125" t="inlineStr">
+      <c r="E90" s="125" t="inlineStr">
         <is>
           <t>75-90%</t>
         </is>
       </c>
-      <c r="F84" s="126" t="inlineStr">
+      <c r="F90" s="126" t="inlineStr">
         <is>
           <t>90-95%</t>
         </is>
       </c>
-      <c r="G84" s="127" t="inlineStr">
+      <c r="G90" s="127" t="inlineStr">
         <is>
           <t>&gt;95%</t>
         </is>
       </c>
     </row>
-    <row r="85">
-      <c r="B85" s="122" t="inlineStr">
+    <row r="91" ht="18" customHeight="1">
+      <c r="B91" s="122" t="inlineStr">
         <is>
           <t>Review Completion Rate</t>
         </is>
       </c>
-      <c r="C85" s="123" t="inlineStr">
+      <c r="C91" s="123" t="inlineStr">
         <is>
           <t>&lt;50%</t>
         </is>
       </c>
-      <c r="D85" s="124" t="inlineStr">
+      <c r="D91" s="124" t="inlineStr">
         <is>
           <t>50-75%</t>
         </is>
       </c>
-      <c r="E85" s="125" t="inlineStr">
+      <c r="E91" s="125" t="inlineStr">
         <is>
           <t>75-90%</t>
         </is>
       </c>
-      <c r="F85" s="126" t="inlineStr">
+      <c r="F91" s="126" t="inlineStr">
         <is>
           <t>90-95%</t>
         </is>
       </c>
-      <c r="G85" s="127" t="inlineStr">
+      <c r="G91" s="127" t="inlineStr">
         <is>
           <t>&gt;95%</t>
         </is>
       </c>
     </row>
-    <row r="86">
-      <c r="B86" s="122" t="inlineStr">
+    <row r="92" ht="32" customHeight="1">
+      <c r="B92" s="122" t="inlineStr">
         <is>
           <t>Guardrail Verification</t>
         </is>
       </c>
-      <c r="C86" s="123" t="inlineStr">
+      <c r="C92" s="123" t="inlineStr">
         <is>
           <t>&lt;25%</t>
         </is>
       </c>
-      <c r="D86" s="124" t="inlineStr">
+      <c r="D92" s="124" t="inlineStr">
         <is>
           <t>25-50%</t>
         </is>
       </c>
-      <c r="E86" s="125" t="inlineStr">
+      <c r="E92" s="125" t="inlineStr">
         <is>
           <t>50-80%</t>
         </is>
       </c>
-      <c r="F86" s="126" t="inlineStr">
+      <c r="F92" s="126" t="inlineStr">
         <is>
           <t>80-95%</t>
         </is>
       </c>
-      <c r="G86" s="127" t="inlineStr">
+      <c r="G92" s="127" t="inlineStr">
         <is>
           <t>95-100%</t>
         </is>
       </c>
     </row>
-    <row r="87">
-      <c r="B87" s="122" t="inlineStr">
+    <row r="93" ht="16" customHeight="1">
+      <c r="B93" s="122" t="inlineStr">
         <is>
           <t>Non-Compliance Rate</t>
         </is>
       </c>
-      <c r="C87" s="123" t="inlineStr">
+      <c r="C93" s="123" t="inlineStr">
         <is>
           <t>&gt;20%</t>
         </is>
       </c>
-      <c r="D87" s="124" t="inlineStr">
+      <c r="D93" s="124" t="inlineStr">
         <is>
           <t>10-20%</t>
         </is>
       </c>
-      <c r="E87" s="125" t="inlineStr">
+      <c r="E93" s="125" t="inlineStr">
         <is>
           <t>5-10%</t>
         </is>
       </c>
-      <c r="F87" s="126" t="inlineStr">
+      <c r="F93" s="126" t="inlineStr">
         <is>
           <t>2-5%</t>
         </is>
       </c>
-      <c r="G87" s="127" t="inlineStr">
+      <c r="G93" s="127" t="inlineStr">
         <is>
           <t>&lt;2%</t>
         </is>
       </c>
     </row>
-    <row r="88">
-      <c r="B88" s="122" t="inlineStr">
+    <row r="94" ht="16" customHeight="1">
+      <c r="B94" s="122" t="inlineStr">
         <is>
           <t>Mean Time to Approval</t>
         </is>
       </c>
-      <c r="C88" s="123" t="inlineStr">
+      <c r="C94" s="123" t="inlineStr">
         <is>
           <t>&gt;20 days</t>
         </is>
       </c>
-      <c r="D88" s="124" t="inlineStr">
+      <c r="D94" s="124" t="inlineStr">
         <is>
           <t>10-20 days</t>
         </is>
       </c>
-      <c r="E88" s="125" t="inlineStr">
+      <c r="E94" s="125" t="inlineStr">
         <is>
           <t>5-10 days</t>
         </is>
       </c>
-      <c r="F88" s="126" t="inlineStr">
+      <c r="F94" s="126" t="inlineStr">
         <is>
           <t>3-5 days</t>
         </is>
       </c>
-      <c r="G88" s="127" t="inlineStr">
+      <c r="G94" s="127" t="inlineStr">
         <is>
           <t>&lt;3 days</t>
         </is>
       </c>
     </row>
-    <row r="89">
-      <c r="B89" s="122" t="inlineStr">
+    <row r="95" ht="32" customHeight="1">
+      <c r="B95" s="122" t="inlineStr">
         <is>
           <t>Exception Rate</t>
         </is>
       </c>
-      <c r="C89" s="123" t="inlineStr">
+      <c r="C95" s="123" t="inlineStr">
         <is>
           <t>&gt;30%</t>
         </is>
       </c>
-      <c r="D89" s="124" t="inlineStr">
+      <c r="D95" s="124" t="inlineStr">
         <is>
           <t>15-30%</t>
         </is>
       </c>
-      <c r="E89" s="125" t="inlineStr">
+      <c r="E95" s="125" t="inlineStr">
         <is>
           <t>8-15%</t>
         </is>
       </c>
-      <c r="F89" s="126" t="inlineStr">
+      <c r="F95" s="126" t="inlineStr">
         <is>
           <t>3-8%</t>
         </is>
       </c>
-      <c r="G89" s="127" t="inlineStr">
+      <c r="G95" s="127" t="inlineStr">
         <is>
           <t>&lt;3%</t>
         </is>
       </c>
     </row>
-    <row r="90">
-      <c r="B90" s="74" t="n"/>
-      <c r="C90" s="74" t="n"/>
-      <c r="D90" s="74" t="n"/>
-      <c r="E90" s="74" t="n"/>
-      <c r="F90" s="74" t="n"/>
-      <c r="G90" s="74" t="n"/>
-      <c r="H90" s="74" t="n"/>
-      <c r="I90" s="74" t="n"/>
-    </row>
-    <row r="91" ht="18" customHeight="1">
-      <c r="B91" s="96" t="inlineStr">
+    <row r="96" ht="32" customHeight="1">
+      <c r="B96" s="74" t="n"/>
+      <c r="C96" s="74" t="n"/>
+      <c r="D96" s="74" t="n"/>
+      <c r="E96" s="74" t="n"/>
+      <c r="F96" s="74" t="n"/>
+      <c r="G96" s="74" t="n"/>
+      <c r="H96" s="74" t="n"/>
+      <c r="I96" s="74" t="n"/>
+    </row>
+    <row r="97">
+      <c r="B97" s="96" t="inlineStr">
         <is>
           <t>7. Workbook Cross-References</t>
         </is>
       </c>
     </row>
-    <row r="92" ht="32" customHeight="1">
-      <c r="B92" s="137" t="inlineStr">
+    <row r="98">
+      <c r="B98" s="137" t="inlineStr">
         <is>
           <t>Governance Guide</t>
         </is>
       </c>
-      <c r="C92" s="130" t="inlineStr">
+      <c r="C98" s="130" t="inlineStr">
         <is>
           <t>Committee structure, approval workflow, enforcement procedures</t>
         </is>
       </c>
     </row>
-    <row r="93" ht="16" customHeight="1">
-      <c r="B93" s="137" t="inlineStr">
+    <row r="99">
+      <c r="B99" s="137" t="inlineStr">
         <is>
           <t>Tool Registry</t>
         </is>
       </c>
-      <c r="C93" s="130" t="inlineStr">
+      <c r="C99" s="130" t="inlineStr">
         <is>
           <t>Source data for inventory and status metrics</t>
         </is>
       </c>
     </row>
-    <row r="94" ht="16" customHeight="1">
-      <c r="B94" s="137" t="inlineStr">
+    <row r="100">
+      <c r="B100" s="137" t="inlineStr">
         <is>
           <t>Guardrail Checklist</t>
         </is>
       </c>
-      <c r="C94" s="130" t="inlineStr">
+      <c r="C100" s="130" t="inlineStr">
         <is>
           <t>Source data for verification rate metrics</t>
         </is>
       </c>
     </row>
-    <row r="95" ht="32" customHeight="1">
-      <c r="B95" s="137" t="inlineStr">
+    <row r="101">
+      <c r="B101" s="137" t="inlineStr">
         <is>
           <t>Exception Tracker</t>
         </is>
       </c>
-      <c r="C95" s="130" t="inlineStr">
+      <c r="C101" s="130" t="inlineStr">
         <is>
           <t>Source data for exception rate and renewal metrics</t>
         </is>
       </c>
     </row>
-    <row r="96" ht="32" customHeight="1">
-      <c r="B96" s="137" t="inlineStr">
+    <row r="102">
+      <c r="B102" s="137" t="inlineStr">
         <is>
           <t>Compliance Mapping</t>
         </is>
       </c>
-      <c r="C96" s="130" t="inlineStr">
+      <c r="C102" s="130" t="inlineStr">
         <is>
           <t>Framework requirements that drive metric selection</t>
         </is>
@@ -9759,7 +9975,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:F70"/>
+  <dimension ref="B2:F68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="20" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
@@ -10932,74 +11148,74 @@
       </c>
     </row>
     <row r="56" ht="24" customHeight="1">
-      <c r="B56" s="258" t="inlineStr">
+      <c r="B56" s="197" t="inlineStr">
+        <is>
+          <t>RAG/Vector Database</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Access controls, encryption, audit logging</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Knostic, Cyera, Wiz</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Data Protection, AI Supply Chain</t>
+        </is>
+      </c>
+    </row>
+    <row r="57" ht="40" customHeight="1">
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>MCP Server Integration</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>System prompt protection, tool verification, input validation</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Lakera, Prompt Armor, Straiker</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Runtime Protection, NHI &amp; Agentic Access</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" ht="40" customHeight="1">
+      <c r="B58" s="258" t="inlineStr">
         <is>
           <t>SEVERE RISK — CISO/executive approval; comprehensive controls required</t>
         </is>
       </c>
-      <c r="C56" s="251" t="n"/>
-      <c r="D56" s="251" t="n"/>
-      <c r="E56" s="251" t="n"/>
-      <c r="F56" s="26" t="n"/>
-    </row>
-    <row r="57" ht="40" customHeight="1">
-      <c r="B57" s="8" t="inlineStr">
-        <is>
-          <t>Autonomous web browsing</t>
-        </is>
-      </c>
-      <c r="C57" s="14" t="inlineStr">
-        <is>
-          <t>Severe</t>
-        </is>
-      </c>
-      <c r="D57" s="8" t="inlineStr">
-        <is>
-          <t>Requires formal security exception; high risk of unauthorized data collection</t>
-        </is>
-      </c>
-      <c r="E57" s="8" t="inlineStr">
-        <is>
-          <t>Full stack required + formal review</t>
-        </is>
-      </c>
-      <c r="F57" s="8" t="inlineStr">
-        <is>
-          <t>All 7 families</t>
-        </is>
-      </c>
-    </row>
-    <row r="58" ht="40" customHeight="1">
-      <c r="B58" s="8" t="inlineStr">
-        <is>
-          <t>Log analysis containing PII/sensitive data</t>
-        </is>
-      </c>
-      <c r="C58" s="14" t="inlineStr">
-        <is>
-          <t>Severe</t>
-        </is>
-      </c>
-      <c r="D58" s="8" t="inlineStr">
-        <is>
-          <t>Subject to security review; sensitive data must be masked or redacted</t>
-        </is>
-      </c>
-      <c r="E58" s="8" t="inlineStr">
-        <is>
-          <t>Cyera + Datadog + security review</t>
-        </is>
-      </c>
-      <c r="F58" s="8" t="inlineStr">
-        <is>
-          <t>Data Protection, Observability</t>
-        </is>
-      </c>
+      <c r="C58" s="251" t="n"/>
+      <c r="D58" s="251" t="n"/>
+      <c r="E58" s="251" t="n"/>
+      <c r="F58" s="26" t="n"/>
     </row>
     <row r="59" ht="40" customHeight="1">
       <c r="B59" s="8" t="inlineStr">
         <is>
-          <t>Privileged system automation</t>
+          <t>Autonomous web browsing</t>
         </is>
       </c>
       <c r="C59" s="14" t="inlineStr">
@@ -11009,24 +11225,24 @@
       </c>
       <c r="D59" s="8" t="inlineStr">
         <is>
-          <t>Prohibited by default; formal security approval and documented risk mitigation required</t>
+          <t>Requires formal security exception; high risk of unauthorized data collection</t>
         </is>
       </c>
       <c r="E59" s="8" t="inlineStr">
         <is>
-          <t>Silverfort, Astrix, Oasis + full stack</t>
+          <t>Full stack required + formal review</t>
         </is>
       </c>
       <c r="F59" s="8" t="inlineStr">
         <is>
-          <t>NHI, AI Posture</t>
+          <t>All 7 families</t>
         </is>
       </c>
     </row>
     <row r="60" ht="40" customHeight="1">
       <c r="B60" s="8" t="inlineStr">
         <is>
-          <t>Unrestricted code execution</t>
+          <t>Log analysis containing PII/sensitive data</t>
         </is>
       </c>
       <c r="C60" s="14" t="inlineStr">
@@ -11036,24 +11252,24 @@
       </c>
       <c r="D60" s="8" t="inlineStr">
         <is>
-          <t>Blocked by default; exceptions require strict containment strategies and oversight</t>
+          <t>Subject to security review; sensitive data must be masked or redacted</t>
         </is>
       </c>
       <c r="E60" s="8" t="inlineStr">
         <is>
-          <t>Full stack + mandatory sandbox</t>
+          <t>Cyera + Datadog + security review</t>
         </is>
       </c>
       <c r="F60" s="8" t="inlineStr">
         <is>
-          <t>All 7 families</t>
+          <t>Data Protection, Observability</t>
         </is>
       </c>
     </row>
     <row r="61" ht="40" customHeight="1">
       <c r="B61" s="8" t="inlineStr">
         <is>
-          <t>Model fine-tuning with production data</t>
+          <t>Privileged system automation</t>
         </is>
       </c>
       <c r="C61" s="14" t="inlineStr">
@@ -11063,24 +11279,24 @@
       </c>
       <c r="D61" s="8" t="inlineStr">
         <is>
-          <t>Data governance review required; IP protection; formal approval with time limit</t>
+          <t>Prohibited by default; formal security approval and documented risk mitigation required</t>
         </is>
       </c>
       <c r="E61" s="8" t="inlineStr">
         <is>
-          <t>Noma, HiddenLayer, Cyera, BigID</t>
+          <t>Silverfort, Astrix, Oasis + full stack</t>
         </is>
       </c>
       <c r="F61" s="8" t="inlineStr">
         <is>
-          <t>AI Supply Chain, Data Protection</t>
+          <t>NHI, AI Posture</t>
         </is>
       </c>
     </row>
     <row r="62" ht="40" customHeight="1">
       <c r="B62" s="8" t="inlineStr">
         <is>
-          <t>Infrastructure automation (Terraform, K8s)</t>
+          <t>Unrestricted code execution</t>
         </is>
       </c>
       <c r="C62" s="14" t="inlineStr">
@@ -11090,24 +11306,24 @@
       </c>
       <c r="D62" s="8" t="inlineStr">
         <is>
-          <t>Prohibited by default; requires full security review; admin rights must be scoped</t>
+          <t>Blocked by default; exceptions require strict containment strategies and oversight</t>
         </is>
       </c>
       <c r="E62" s="8" t="inlineStr">
         <is>
-          <t>Silverfort, Astrix + full review</t>
+          <t>Full stack + mandatory sandbox</t>
         </is>
       </c>
       <c r="F62" s="8" t="inlineStr">
         <is>
-          <t>NHI, AI Posture</t>
+          <t>All 7 families</t>
         </is>
       </c>
     </row>
     <row r="63" ht="40" customHeight="1">
       <c r="B63" s="8" t="inlineStr">
         <is>
-          <t>Autonomous agent with unrestricted API access</t>
+          <t>Model fine-tuning with production data</t>
         </is>
       </c>
       <c r="C63" s="14" t="inlineStr">
@@ -11117,24 +11333,24 @@
       </c>
       <c r="D63" s="8" t="inlineStr">
         <is>
-          <t>Prohibited by default; formal exception with strict monitoring and kill switch</t>
+          <t>Data governance review required; IP protection; formal approval with time limit</t>
         </is>
       </c>
       <c r="E63" s="8" t="inlineStr">
         <is>
-          <t>Full stack + continuous monitoring</t>
+          <t>Noma, HiddenLayer, Cyera, BigID</t>
         </is>
       </c>
       <c r="F63" s="8" t="inlineStr">
         <is>
-          <t>All 7 families</t>
+          <t>AI Supply Chain, Data Protection</t>
         </is>
       </c>
     </row>
     <row r="64" ht="40" customHeight="1">
       <c r="B64" s="8" t="inlineStr">
         <is>
-          <t>Multi-agent orchestration (autonomous)</t>
+          <t>Infrastructure automation (Terraform, K8s)</t>
         </is>
       </c>
       <c r="C64" s="14" t="inlineStr">
@@ -11144,12 +11360,12 @@
       </c>
       <c r="D64" s="8" t="inlineStr">
         <is>
-          <t>Prohibited by default; requires agent inventory, communication controls, kill switches</t>
+          <t>Prohibited by default; requires full security review; admin rights must be scoped</t>
         </is>
       </c>
       <c r="E64" s="8" t="inlineStr">
         <is>
-          <t>Zenity, Oasis, Astrix + full stack</t>
+          <t>Silverfort, Astrix + full review</t>
         </is>
       </c>
       <c r="F64" s="8" t="inlineStr">
@@ -11161,7 +11377,7 @@
     <row r="65" ht="40" customHeight="1">
       <c r="B65" s="8" t="inlineStr">
         <is>
-          <t>Agent task delegation / spawning</t>
+          <t>Autonomous agent with unrestricted API access</t>
         </is>
       </c>
       <c r="C65" s="14" t="inlineStr">
@@ -11171,160 +11387,105 @@
       </c>
       <c r="D65" s="8" t="inlineStr">
         <is>
-          <t>Prohibited by default; limit spawn depth; enforce resource quotas; audit lineage</t>
+          <t>Prohibited by default; formal exception with strict monitoring and kill switch</t>
         </is>
       </c>
       <c r="E65" s="8" t="inlineStr">
         <is>
-          <t>Zenity, Noma, Oasis Security</t>
+          <t>Full stack + continuous monitoring</t>
         </is>
       </c>
       <c r="F65" s="8" t="inlineStr">
         <is>
-          <t>NHI, AI Posture</t>
+          <t>All 7 families</t>
         </is>
       </c>
     </row>
     <row r="66" ht="40" customHeight="1">
       <c r="B66" s="8" t="inlineStr">
         <is>
+          <t>Multi-agent orchestration (autonomous)</t>
+        </is>
+      </c>
+      <c r="C66" s="14" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+      <c r="D66" s="8" t="inlineStr">
+        <is>
+          <t>Prohibited by default; requires agent inventory, communication controls, kill switches</t>
+        </is>
+      </c>
+      <c r="E66" s="8" t="inlineStr">
+        <is>
+          <t>Zenity, Oasis, Astrix + full stack</t>
+        </is>
+      </c>
+      <c r="F66" s="8" t="inlineStr">
+        <is>
+          <t>NHI, AI Posture</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" s="8" t="inlineStr">
+        <is>
+          <t>Agent task delegation / spawning</t>
+        </is>
+      </c>
+      <c r="C67" s="14" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+      <c r="D67" s="8" t="inlineStr">
+        <is>
+          <t>Prohibited by default; limit spawn depth; enforce resource quotas; audit lineage</t>
+        </is>
+      </c>
+      <c r="E67" s="8" t="inlineStr">
+        <is>
+          <t>Zenity, Noma, Oasis Security</t>
+        </is>
+      </c>
+      <c r="F67" s="8" t="inlineStr">
+        <is>
+          <t>NHI, AI Posture</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" s="8" t="inlineStr">
+        <is>
           <t>Autonomous decision-making (no human review)</t>
         </is>
       </c>
-      <c r="C66" s="14" t="inlineStr">
+      <c r="C68" s="14" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D66" s="8" t="inlineStr">
+      <c r="D68" s="8" t="inlineStr">
         <is>
           <t>Prohibited for consequential decisions; requires formal exception and audit trail</t>
         </is>
       </c>
-      <c r="E66" s="8" t="inlineStr">
+      <c r="E68" s="8" t="inlineStr">
         <is>
           <t>Full stack + mandatory logging</t>
         </is>
       </c>
-      <c r="F66" s="8" t="inlineStr">
+      <c r="F68" s="8" t="inlineStr">
         <is>
           <t>All 7 families</t>
         </is>
       </c>
     </row>
-    <row r="67">
-      <c r="B67" s="259" t="inlineStr">
-        <is>
-          <t>Multi-Agent Orchestration</t>
-        </is>
-      </c>
-      <c r="C67" s="259" t="inlineStr">
-        <is>
-          <t>Severe</t>
-        </is>
-      </c>
-      <c r="D67" s="259" t="inlineStr">
-        <is>
-          <t>Agentic boundary controls, Tool authorization, Autonomous action limits</t>
-        </is>
-      </c>
-      <c r="E67" s="259" t="inlineStr">
-        <is>
-          <t>Straiker, Zenity, Invariant Labs</t>
-        </is>
-      </c>
-      <c r="F67" s="259" t="inlineStr">
-        <is>
-          <t>NHI &amp; Agentic Access, Runtime Protection</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="B68" s="259" t="inlineStr">
-        <is>
-          <t>RAG/Vector Database</t>
-        </is>
-      </c>
-      <c r="C68" s="259" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="D68" s="259" t="inlineStr">
-        <is>
-          <t>Vector store security, Embedding integrity, Data classification</t>
-        </is>
-      </c>
-      <c r="E68" s="259" t="inlineStr">
-        <is>
-          <t>Cyera, BigID, Wiz</t>
-        </is>
-      </c>
-      <c r="F68" s="259" t="inlineStr">
-        <is>
-          <t>Data Protection for AI, AI Supply Chain</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="B69" s="259" t="inlineStr">
-        <is>
-          <t>Autonomous Code Execution</t>
-        </is>
-      </c>
-      <c r="C69" s="259" t="inlineStr">
-        <is>
-          <t>Severe</t>
-        </is>
-      </c>
-      <c r="D69" s="259" t="inlineStr">
-        <is>
-          <t>Tool authorization, Sandbox isolation, Audit logging</t>
-        </is>
-      </c>
-      <c r="E69" s="259" t="inlineStr">
-        <is>
-          <t>Zenity, Straiker, Spec</t>
-        </is>
-      </c>
-      <c r="F69" s="259" t="inlineStr">
-        <is>
-          <t>NHI &amp; Agentic Access, Runtime Protection</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="B70" s="259" t="inlineStr">
-        <is>
-          <t>MCP Server Integration</t>
-        </is>
-      </c>
-      <c r="C70" s="259" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="D70" s="259" t="inlineStr">
-        <is>
-          <t>System prompt protection, Tool authorization, Input validation</t>
-        </is>
-      </c>
-      <c r="E70" s="259" t="inlineStr">
-        <is>
-          <t>Lakera, Prompt Armor, Straiker</t>
-        </is>
-      </c>
-      <c r="F70" s="259" t="inlineStr">
-        <is>
-          <t>Runtime Protection, NHI &amp; Agentic Access</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B27:F27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11337,7 +11498,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D74"/>
+  <dimension ref="B2:D74"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD15"/>
@@ -11351,7 +11512,6 @@
     <col width="20" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1"/>
     <row r="2" ht="21" customHeight="1">
       <c r="B2" s="9" t="inlineStr">
         <is>
@@ -11359,7 +11519,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4" ht="28" customHeight="1">
       <c r="B4" s="15" t="inlineStr">
         <is>
@@ -11452,8 +11611,6 @@
         </is>
       </c>
     </row>
-    <row r="10"/>
-    <row r="11"/>
     <row r="12" ht="19" customHeight="1">
       <c r="B12" s="31" t="inlineStr">
         <is>
@@ -11492,7 +11649,6 @@
       </c>
       <c r="C16" s="23" t="n"/>
     </row>
-    <row r="17"/>
     <row r="18" ht="28" customHeight="1">
       <c r="B18" s="4" t="inlineStr">
         <is>
@@ -11539,7 +11695,6 @@
         </is>
       </c>
     </row>
-    <row r="22"/>
     <row r="23" ht="28" customHeight="1">
       <c r="B23" s="4" t="inlineStr">
         <is>
@@ -11580,7 +11735,6 @@
         </is>
       </c>
     </row>
-    <row r="27"/>
     <row r="28" ht="17" customHeight="1">
       <c r="B28" s="4" t="inlineStr">
         <is>
@@ -11677,7 +11831,6 @@
         </is>
       </c>
     </row>
-    <row r="36"/>
     <row r="37" ht="17" customHeight="1">
       <c r="B37" s="4" t="inlineStr">
         <is>
@@ -11734,7 +11887,6 @@
         </is>
       </c>
     </row>
-    <row r="42"/>
     <row r="43">
       <c r="B43" s="33" t="inlineStr">
         <is>
@@ -11742,7 +11894,6 @@
         </is>
       </c>
     </row>
-    <row r="44"/>
     <row r="45" ht="19" customHeight="1">
       <c r="B45" s="34" t="inlineStr">
         <is>
@@ -11750,7 +11901,6 @@
         </is>
       </c>
     </row>
-    <row r="46"/>
     <row r="47" ht="17" customHeight="1">
       <c r="B47" s="4" t="inlineStr">
         <is>
@@ -11847,7 +11997,6 @@
         </is>
       </c>
     </row>
-    <row r="55"/>
     <row r="56">
       <c r="B56" s="21" t="inlineStr">
         <is>
@@ -11860,7 +12009,6 @@
         </is>
       </c>
     </row>
-    <row r="57"/>
     <row r="58" ht="17" customHeight="1">
       <c r="B58" s="4" t="inlineStr">
         <is>
@@ -11952,7 +12100,6 @@
         </is>
       </c>
     </row>
-    <row r="66"/>
     <row r="67">
       <c r="B67" s="21" t="inlineStr">
         <is>
@@ -11974,7 +12121,6 @@
         </is>
       </c>
     </row>
-    <row r="69"/>
     <row r="70" ht="17" customHeight="1">
       <c r="B70" s="4" t="inlineStr">
         <is>
@@ -14925,34 +15071,34 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="10" t="inlineStr">
+      <c r="B7" s="290" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="C7" s="10" t="inlineStr">
+      <c r="C7" s="290" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="D7" s="10" t="inlineStr">
+      <c r="D7" s="290" t="inlineStr">
         <is>
           <t>Approval Required</t>
         </is>
       </c>
-      <c r="E7" s="10" t="inlineStr">
+      <c r="E7" s="290" t="inlineStr">
         <is>
           <t>Max Duration</t>
         </is>
       </c>
-      <c r="F7" s="10" t="inlineStr">
+      <c r="F7" s="290" t="inlineStr">
         <is>
           <t>Renewal</t>
         </is>
       </c>
     </row>
     <row r="8" ht="25" customHeight="1">
-      <c r="B8" s="90" t="inlineStr">
+      <c r="B8" s="291" t="inlineStr">
         <is>
           <t>Severe Tool</t>
         </is>
@@ -14979,7 +15125,7 @@
       </c>
     </row>
     <row r="9" ht="25" customHeight="1">
-      <c r="B9" s="91" t="inlineStr">
+      <c r="B9" s="292" t="inlineStr">
         <is>
           <t>Guardrail Bypass</t>
         </is>
@@ -15006,7 +15152,7 @@
       </c>
     </row>
     <row r="10" ht="25" customHeight="1">
-      <c r="B10" s="92" t="inlineStr">
+      <c r="B10" s="293" t="inlineStr">
         <is>
           <t>Vendor Risk</t>
         </is>
@@ -15033,7 +15179,7 @@
       </c>
     </row>
     <row r="11" ht="25" customHeight="1">
-      <c r="B11" s="173" t="inlineStr">
+      <c r="B11" s="294" t="inlineStr">
         <is>
           <t>Compliance Gap</t>
         </is>
@@ -15060,7 +15206,7 @@
       </c>
     </row>
     <row r="12" ht="25" customHeight="1">
-      <c r="B12" s="93" t="inlineStr">
+      <c r="B12" s="295" t="inlineStr">
         <is>
           <t>Emergency Use</t>
         </is>
@@ -15105,7 +15251,7 @@
       <c r="F14" s="149" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="174" t="inlineStr">
+      <c r="B15" s="296" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -15120,7 +15266,7 @@
       <c r="F15" s="149" t="n"/>
     </row>
     <row r="16">
-      <c r="B16" s="176" t="inlineStr">
+      <c r="B16" s="297" t="inlineStr">
         <is>
           <t>Renewal Due</t>
         </is>
@@ -15135,7 +15281,7 @@
       <c r="F16" s="149" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="177" t="inlineStr">
+      <c r="B17" s="298" t="inlineStr">
         <is>
           <t>Expired</t>
         </is>
@@ -15150,7 +15296,7 @@
       <c r="F17" s="149" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="178" t="inlineStr">
+      <c r="B18" s="299" t="inlineStr">
         <is>
           <t>Closed</t>
         </is>
@@ -15172,42 +15318,42 @@
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="10" t="inlineStr">
+      <c r="B23" s="290" t="inlineStr">
         <is>
           <t>Exception ID</t>
         </is>
       </c>
-      <c r="C23" s="10" t="inlineStr">
+      <c r="C23" s="290" t="inlineStr">
         <is>
           <t>Tool Name</t>
         </is>
       </c>
-      <c r="D23" s="10" t="inlineStr">
+      <c r="D23" s="290" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E23" s="10" t="inlineStr">
+      <c r="E23" s="290" t="inlineStr">
         <is>
           <t>Risk Level</t>
         </is>
       </c>
-      <c r="F23" s="10" t="inlineStr">
+      <c r="F23" s="290" t="inlineStr">
         <is>
           <t>Guardrails Affected</t>
         </is>
       </c>
-      <c r="G23" s="10" t="inlineStr">
+      <c r="G23" s="290" t="inlineStr">
         <is>
           <t>Business Justification</t>
         </is>
       </c>
-      <c r="H23" s="10" t="inlineStr">
+      <c r="H23" s="290" t="inlineStr">
         <is>
           <t>Compensating Controls</t>
         </is>
       </c>
-      <c r="I23" s="10" t="inlineStr">
+      <c r="I23" s="290" t="inlineStr">
         <is>
           <t>Requestor</t>
         </is>
@@ -15254,7 +15400,7 @@
           <t>Autonomous Agent X</t>
         </is>
       </c>
-      <c r="D24" s="90" t="inlineStr">
+      <c r="D24" s="291" t="inlineStr">
         <is>
           <t>Severe Tool</t>
         </is>
@@ -15326,7 +15472,7 @@
           <t>Custom ML Pipeline</t>
         </is>
       </c>
-      <c r="D25" s="91" t="inlineStr">
+      <c r="D25" s="292" t="inlineStr">
         <is>
           <t>Guardrail Bypass</t>
         </is>
@@ -15398,7 +15544,7 @@
           <t>Vendor AI Tool Y</t>
         </is>
       </c>
-      <c r="D26" s="92" t="inlineStr">
+      <c r="D26" s="293" t="inlineStr">
         <is>
           <t>Vendor Risk</t>
         </is>
@@ -15470,7 +15616,7 @@
           <t>Emergency Chatbot</t>
         </is>
       </c>
-      <c r="D27" s="93" t="inlineStr">
+      <c r="D27" s="295" t="inlineStr">
         <is>
           <t>Emergency Use</t>
         </is>

</xml_diff>

<commit_message>
Fix Program Metrics SLOs, clean up Tool Landscape data
Program Metrics:
- Moved Agentic AI SLOs to correct section (after existing SLOs)

AI Security Tool Landscape:
- Fixed corrupted Status values for Sonatype, Chainguard, JFrog, Snyk, Cycode
- Removed duplicate Wiz entry
- Updated Wiz status to "Pending Acquisition" (Google $32B deal)
- Updated SentinelOne summary to include Observo AI acquisition
- Updated acquisitions note with 2024-2026 deals

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/AI_Security_Risk_Draft1.xlsx
+++ b/AI_Security_Risk_Draft1.xlsx
@@ -5796,256 +5796,254 @@
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Agent Inventory Coverage</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
+    <row r="26" ht="25" customHeight="1">
+      <c r="B26" s="96" t="inlineStr">
+        <is>
+          <t>3. Service Level Objectives (SLOs)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="25" customHeight="1">
+      <c r="B27" s="98" t="inlineStr">
+        <is>
+          <t>Performance targets that the AI security program commits to meeting.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="25" customHeight="1">
+      <c r="B28" s="99" t="inlineStr">
+        <is>
+          <t>SLO</t>
+        </is>
+      </c>
+      <c r="C28" s="99" t="inlineStr">
+        <is>
+          <t>Target</t>
+        </is>
+      </c>
+      <c r="D28" s="99" t="inlineStr">
+        <is>
+          <t>Threshold</t>
+        </is>
+      </c>
+      <c r="E28" s="99" t="inlineStr">
+        <is>
+          <t>Escalation</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="25" customHeight="1">
+      <c r="B29" s="130" t="inlineStr">
+        <is>
+          <t>Tool Inventory Coverage</t>
+        </is>
+      </c>
+      <c r="C29" s="130" t="inlineStr">
         <is>
           <t>≥ 95%</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D29" s="130" t="inlineStr">
         <is>
           <t>&lt; 90% triggers audit</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="E29" s="130" t="inlineStr">
         <is>
           <t>Security Lead → CISO</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Autonomous Action Rate</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>&lt; 20% for High-risk agents</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>&gt; 30% triggers review</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
+    <row r="30" ht="25" customHeight="1">
+      <c r="B30" s="130" t="inlineStr">
+        <is>
+          <t>Review Completion Rate</t>
+        </is>
+      </c>
+      <c r="C30" s="130" t="inlineStr">
+        <is>
+          <t>≥ 95%</t>
+        </is>
+      </c>
+      <c r="D30" s="130" t="inlineStr">
+        <is>
+          <t>&lt; 85% triggers remediation</t>
+        </is>
+      </c>
+      <c r="E30" s="130" t="inlineStr">
         <is>
           <t>Security Lead</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="25" customHeight="1">
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Agent Incident Rate</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>&lt; 2 per quarter</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>&gt; 3 triggers program review</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Committee</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" ht="25" customHeight="1"/>
-    <row r="28" ht="25" customHeight="1"/>
-    <row r="29" ht="25" customHeight="1">
-      <c r="B29" s="96" t="inlineStr">
-        <is>
-          <t>3. Service Level Objectives (SLOs)</t>
-        </is>
-      </c>
-    </row>
-    <row r="30" ht="25" customHeight="1">
-      <c r="B30" s="98" t="inlineStr">
-        <is>
-          <t>Performance targets that the AI security program commits to meeting.</t>
-        </is>
-      </c>
-    </row>
     <row r="31" ht="25" customHeight="1">
-      <c r="B31" s="99" t="inlineStr">
-        <is>
-          <t>SLO</t>
-        </is>
-      </c>
-      <c r="C31" s="99" t="inlineStr">
-        <is>
-          <t>Target</t>
-        </is>
-      </c>
-      <c r="D31" s="99" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="E31" s="99" t="inlineStr">
-        <is>
-          <t>Escalation</t>
+      <c r="B31" s="130" t="inlineStr">
+        <is>
+          <t>Low Risk Approval Time</t>
+        </is>
+      </c>
+      <c r="C31" s="130" t="inlineStr">
+        <is>
+          <t>≤ 2 business days</t>
+        </is>
+      </c>
+      <c r="D31" s="130" t="inlineStr">
+        <is>
+          <t>&gt; 3 days escalates</t>
+        </is>
+      </c>
+      <c r="E31" s="130" t="inlineStr">
+        <is>
+          <t>Security Team</t>
         </is>
       </c>
     </row>
     <row r="32" ht="25" customHeight="1">
       <c r="B32" s="130" t="inlineStr">
         <is>
-          <t>Tool Inventory Coverage</t>
+          <t>Medium Risk Approval Time</t>
         </is>
       </c>
       <c r="C32" s="130" t="inlineStr">
         <is>
-          <t>≥ 95%</t>
+          <t>≤ 5 business days</t>
         </is>
       </c>
       <c r="D32" s="130" t="inlineStr">
         <is>
-          <t>&lt; 90% triggers audit</t>
+          <t>&gt; 7 days escalates</t>
         </is>
       </c>
       <c r="E32" s="130" t="inlineStr">
         <is>
-          <t>Security Lead → CISO</t>
+          <t>Security Lead</t>
         </is>
       </c>
     </row>
     <row r="33" ht="25" customHeight="1">
       <c r="B33" s="130" t="inlineStr">
         <is>
-          <t>Review Completion Rate</t>
+          <t>High Risk Approval Time</t>
         </is>
       </c>
       <c r="C33" s="130" t="inlineStr">
         <is>
-          <t>≥ 95%</t>
+          <t>≤ 10 business days</t>
         </is>
       </c>
       <c r="D33" s="130" t="inlineStr">
         <is>
-          <t>&lt; 85% triggers remediation</t>
+          <t>&gt; 14 days escalates</t>
         </is>
       </c>
       <c r="E33" s="130" t="inlineStr">
         <is>
-          <t>Security Lead</t>
+          <t>Committee Chair</t>
         </is>
       </c>
     </row>
     <row r="34" ht="25" customHeight="1">
       <c r="B34" s="130" t="inlineStr">
         <is>
-          <t>Low Risk Approval Time</t>
+          <t>Severe Risk Exception Review</t>
         </is>
       </c>
       <c r="C34" s="130" t="inlineStr">
         <is>
-          <t>≤ 2 business days</t>
+          <t>≤ 15 business days</t>
         </is>
       </c>
       <c r="D34" s="130" t="inlineStr">
         <is>
-          <t>&gt; 3 days escalates</t>
+          <t>&gt; 20 days escalates</t>
         </is>
       </c>
       <c r="E34" s="130" t="inlineStr">
         <is>
-          <t>Security Team</t>
+          <t>CISO</t>
         </is>
       </c>
     </row>
     <row r="35" ht="25" customHeight="1">
       <c r="B35" s="130" t="inlineStr">
         <is>
-          <t>Medium Risk Approval Time</t>
+          <t>Guardrail Verification Rate</t>
         </is>
       </c>
       <c r="C35" s="130" t="inlineStr">
         <is>
-          <t>≤ 5 business days</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="D35" s="130" t="inlineStr">
         <is>
-          <t>&gt; 7 days escalates</t>
+          <t>&lt; 95% blocks activation</t>
         </is>
       </c>
       <c r="E35" s="130" t="inlineStr">
         <is>
-          <t>Security Lead</t>
+          <t>Security Team</t>
         </is>
       </c>
     </row>
     <row r="36" ht="25" customHeight="1">
       <c r="B36" s="130" t="inlineStr">
         <is>
-          <t>High Risk Approval Time</t>
+          <t>Tier 1 (Kill Switch) Response</t>
         </is>
       </c>
       <c r="C36" s="130" t="inlineStr">
         <is>
-          <t>≤ 10 business days</t>
+          <t>&lt; 15 minutes</t>
         </is>
       </c>
       <c r="D36" s="130" t="inlineStr">
         <is>
-          <t>&gt; 14 days escalates</t>
+          <t>Immediate escalation</t>
         </is>
       </c>
       <c r="E36" s="130" t="inlineStr">
         <is>
-          <t>Committee Chair</t>
+          <t>On-call Security</t>
         </is>
       </c>
     </row>
     <row r="37" ht="25" customHeight="1">
       <c r="B37" s="130" t="inlineStr">
         <is>
-          <t>Severe Risk Exception Review</t>
+          <t>Tier 2 (Rapid Response) Time</t>
         </is>
       </c>
       <c r="C37" s="130" t="inlineStr">
         <is>
-          <t>≤ 15 business days</t>
+          <t>&lt; 4 hours</t>
         </is>
       </c>
       <c r="D37" s="130" t="inlineStr">
         <is>
-          <t>&gt; 20 days escalates</t>
+          <t>&gt; 6 hours escalates</t>
         </is>
       </c>
       <c r="E37" s="130" t="inlineStr">
         <is>
-          <t>CISO</t>
+          <t>Security Lead</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="130" t="inlineStr">
         <is>
-          <t>Guardrail Verification Rate</t>
+          <t>Tier 3 (Accelerated Review) Time</t>
         </is>
       </c>
       <c r="C38" s="130" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>&lt; 24 hours</t>
         </is>
       </c>
       <c r="D38" s="130" t="inlineStr">
         <is>
-          <t>&lt; 95% blocks activation</t>
+          <t>&gt; 48 hours escalates</t>
         </is>
       </c>
       <c r="E38" s="130" t="inlineStr">
@@ -6057,110 +6055,110 @@
     <row r="39">
       <c r="B39" s="130" t="inlineStr">
         <is>
-          <t>Tier 1 (Kill Switch) Response</t>
+          <t>Non-Compliance Rate</t>
         </is>
       </c>
       <c r="C39" s="130" t="inlineStr">
         <is>
-          <t>&lt; 15 minutes</t>
+          <t>&lt; 5%</t>
         </is>
       </c>
       <c r="D39" s="130" t="inlineStr">
         <is>
-          <t>Immediate escalation</t>
+          <t>&gt; 10% triggers program review</t>
         </is>
       </c>
       <c r="E39" s="130" t="inlineStr">
         <is>
-          <t>On-call Security</t>
+          <t>Committee</t>
         </is>
       </c>
     </row>
     <row r="40" ht="18" customHeight="1">
       <c r="B40" s="130" t="inlineStr">
         <is>
-          <t>Tier 2 (Rapid Response) Time</t>
+          <t>Exception Renewal Processing</t>
         </is>
       </c>
       <c r="C40" s="130" t="inlineStr">
         <is>
-          <t>&lt; 4 hours</t>
+          <t>≤ 5 business days before expiry</t>
         </is>
       </c>
       <c r="D40" s="130" t="inlineStr">
         <is>
-          <t>&gt; 6 hours escalates</t>
+          <t>Auto-suspend if missed</t>
         </is>
       </c>
       <c r="E40" s="130" t="inlineStr">
         <is>
+          <t>Exception Owner</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Agent Inventory Coverage</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>≥ 95%</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>&lt; 90% triggers audit</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Security Lead → CISO</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Autonomous Action Rate</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>&lt; 20% for High-risk agents</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>&gt; 30% triggers review</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
           <t>Security Lead</t>
         </is>
       </c>
     </row>
-    <row r="41">
-      <c r="B41" s="130" t="inlineStr">
-        <is>
-          <t>Tier 3 (Accelerated Review) Time</t>
-        </is>
-      </c>
-      <c r="C41" s="130" t="inlineStr">
-        <is>
-          <t>&lt; 24 hours</t>
-        </is>
-      </c>
-      <c r="D41" s="130" t="inlineStr">
-        <is>
-          <t>&gt; 48 hours escalates</t>
-        </is>
-      </c>
-      <c r="E41" s="130" t="inlineStr">
-        <is>
-          <t>Security Team</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" s="130" t="inlineStr">
-        <is>
-          <t>Non-Compliance Rate</t>
-        </is>
-      </c>
-      <c r="C42" s="130" t="inlineStr">
-        <is>
-          <t>&lt; 5%</t>
-        </is>
-      </c>
-      <c r="D42" s="130" t="inlineStr">
-        <is>
-          <t>&gt; 10% triggers program review</t>
-        </is>
-      </c>
-      <c r="E42" s="130" t="inlineStr">
+    <row r="43" ht="40" customHeight="1">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Agent Incident Rate</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>&lt; 2 per quarter</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>&gt; 3 triggers program review</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>Committee</t>
-        </is>
-      </c>
-    </row>
-    <row r="43" ht="40" customHeight="1">
-      <c r="B43" s="130" t="inlineStr">
-        <is>
-          <t>Exception Renewal Processing</t>
-        </is>
-      </c>
-      <c r="C43" s="130" t="inlineStr">
-        <is>
-          <t>≤ 5 business days before expiry</t>
-        </is>
-      </c>
-      <c r="D43" s="130" t="inlineStr">
-        <is>
-          <t>Auto-suspend if missed</t>
-        </is>
-      </c>
-      <c r="E43" s="130" t="inlineStr">
-        <is>
-          <t>Exception Owner</t>
         </is>
       </c>
     </row>
@@ -15992,7 +15990,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H158"/>
+  <dimension ref="B2:H157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
@@ -16167,10 +16165,11 @@
         </is>
       </c>
     </row>
+    <row r="14"/>
     <row r="15">
       <c r="B15" s="260" t="inlineStr">
         <is>
-          <t>Note: Major 2024-2025 acquisitions include Wiz ($32B by Google), Lakera ($300M by Check Point), CalypsoAI ($180M by F5), Prompt Security (by SentinelOne)</t>
+          <t>Note: Major 2024-2026 acquisitions include Google/Wiz ($32B pending), Palo Alto/Protect AI ($700M), CrowdStrike/Pangea ($260M), Check Point/Lakera ($300M), SentinelOne/Prompt Security, F5/CalypsoAI, Cato/AIM Security</t>
         </is>
       </c>
     </row>
@@ -16330,7 +16329,7 @@
       </c>
       <c r="C20" s="262" t="inlineStr">
         <is>
-          <t>Independent</t>
+          <t>Pending Acquisition</t>
         </is>
       </c>
       <c r="D20" s="276" t="inlineStr">
@@ -16350,7 +16349,7 @@
       </c>
       <c r="G20" s="262" t="inlineStr">
         <is>
-          <t>CNAPP-native AI-SPM: agentless discovery, risk prioritization, compliance mapping</t>
+          <t>CNAPP-native AI-SPM: agentless discovery, risk prioritization, attack path analysis. Google $32B acquisition pending EU approval (Feb 2026); would be Google's largest acquisition ever</t>
         </is>
       </c>
       <c r="H20" s="262" t="inlineStr">
@@ -17090,7 +17089,7 @@
       </c>
       <c r="G40" s="262" t="inlineStr">
         <is>
-          <t>Purple AI + Prompt Security acquisition: GenAI visibility, runtime protection</t>
+          <t>Purple AI + Prompt Security acquisition: GenAI visibility, runtime guardrails, data protection. Also acquired Observo AI ($225M) for AI-native telemetry pipeline</t>
         </is>
       </c>
       <c r="H40" s="262" t="inlineStr">
@@ -18143,7 +18142,7 @@
       </c>
       <c r="C69" s="262" t="inlineStr">
         <is>
-          <t>sonatype.com</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D69" s="277" t="inlineStr">
@@ -18176,7 +18175,7 @@
       </c>
       <c r="C70" s="262" t="inlineStr">
         <is>
-          <t>chainguard.dev</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D70" s="277" t="inlineStr">
@@ -18209,7 +18208,7 @@
       </c>
       <c r="C71" s="262" t="inlineStr">
         <is>
-          <t>jfrog.com</t>
+          <t>Platform</t>
         </is>
       </c>
       <c r="D71" s="277" t="inlineStr">
@@ -18242,7 +18241,7 @@
       </c>
       <c r="C72" s="262" t="inlineStr">
         <is>
-          <t>snyk.io</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D72" s="277" t="inlineStr">
@@ -18270,12 +18269,12 @@
     <row r="73" ht="40" customHeight="1">
       <c r="B73" s="262" t="inlineStr">
         <is>
-          <t>Wiz</t>
+          <t>Cycode</t>
         </is>
       </c>
       <c r="C73" s="262" t="inlineStr">
         <is>
-          <t>wiz.io</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D73" s="276" t="inlineStr">
@@ -18283,60 +18282,64 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E73" s="281" t="inlineStr">
-        <is>
-          <t>Data Protection for AI</t>
-        </is>
-      </c>
-      <c r="F73" s="277" t="inlineStr">
+      <c r="E73" s="277" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
+      <c r="F73" s="280" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
+        </is>
+      </c>
       <c r="G73" s="262" t="inlineStr">
         <is>
-          <t>AI-SPM leader: training data exposure, model pipeline security, DSPM for AI, attack path analysis to models</t>
+          <t>ASPM platform: AI-native code security, Risk Intelligence Graph, pipeline security, secrets detection</t>
         </is>
       </c>
       <c r="H73" s="259" t="n"/>
     </row>
     <row r="74" ht="40" customHeight="1">
-      <c r="B74" s="262" t="inlineStr">
-        <is>
-          <t>Cycode</t>
-        </is>
-      </c>
-      <c r="C74" s="262" t="inlineStr">
-        <is>
-          <t>cycode.com</t>
-        </is>
-      </c>
-      <c r="D74" s="276" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
-        </is>
-      </c>
-      <c r="E74" s="277" t="inlineStr">
-        <is>
-          <t>AI Supply Chain</t>
-        </is>
-      </c>
-      <c r="F74" s="280" t="inlineStr">
+      <c r="B74" s="259" t="inlineStr">
+        <is>
+          <t>Straiker Defend AI</t>
+        </is>
+      </c>
+      <c r="C74" s="259" t="inlineStr">
+        <is>
+          <t>Independent</t>
+        </is>
+      </c>
+      <c r="D74" s="283" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="G74" s="262" t="inlineStr">
-        <is>
-          <t>ASPM platform: AI-native code security, Risk Intelligence Graph, pipeline security, secrets detection</t>
-        </is>
-      </c>
-      <c r="H74" s="259" t="n"/>
+      <c r="E74" s="284" t="inlineStr">
+        <is>
+          <t>NHI &amp; Agentic Access</t>
+        </is>
+      </c>
+      <c r="F74" s="285" t="inlineStr">
+        <is>
+          <t>Observability &amp; Evaluation</t>
+        </is>
+      </c>
+      <c r="G74" s="259" t="inlineStr">
+        <is>
+          <t>Agentic AI runtime security ($21M Series A, Lightspeed): fast context-aware guardrails; inspects prompts, reasoning steps, tool calls; stops prompt injection, data leaks, agent manipulation.</t>
+        </is>
+      </c>
+      <c r="H74" s="259" t="inlineStr">
+        <is>
+          <t>Production agentic AI; real-time agent security</t>
+        </is>
+      </c>
     </row>
     <row r="75" ht="40" customHeight="1">
       <c r="B75" s="259" t="inlineStr">
         <is>
-          <t>Straiker Defend AI</t>
+          <t>Maxim AI</t>
         </is>
       </c>
       <c r="C75" s="259" t="inlineStr">
@@ -18344,36 +18347,36 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D75" s="283" t="inlineStr">
+      <c r="D75" s="285" t="inlineStr">
+        <is>
+          <t>Observability &amp; Evaluation</t>
+        </is>
+      </c>
+      <c r="E75" s="286" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
+        </is>
+      </c>
+      <c r="F75" s="283" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E75" s="284" t="inlineStr">
-        <is>
-          <t>NHI &amp; Agentic Access</t>
-        </is>
-      </c>
-      <c r="F75" s="285" t="inlineStr">
-        <is>
-          <t>Observability &amp; Evaluation</t>
-        </is>
-      </c>
       <c r="G75" s="259" t="inlineStr">
         <is>
-          <t>Agentic AI runtime security ($21M Series A, Lightspeed): fast context-aware guardrails; inspects prompts, reasoning steps, tool calls; stops prompt injection, data leaks, agent manipulation.</t>
+          <t>End-to-end AI agent lifecycle platform: experimentation, simulation, evaluation, production observability; unified workflow replacing multiple point tools.</t>
         </is>
       </c>
       <c r="H75" s="259" t="inlineStr">
         <is>
-          <t>Production agentic AI; real-time agent security</t>
+          <t>Agent development teams; unified agent lifecycle</t>
         </is>
       </c>
     </row>
     <row r="76" ht="40" customHeight="1">
       <c r="B76" s="259" t="inlineStr">
         <is>
-          <t>Maxim AI</t>
+          <t>Braintrust</t>
         </is>
       </c>
       <c r="C76" s="259" t="inlineStr">
@@ -18391,26 +18394,26 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F76" s="283" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
+      <c r="F76" s="259" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
       <c r="G76" s="259" t="inlineStr">
         <is>
-          <t>End-to-end AI agent lifecycle platform: experimentation, simulation, evaluation, production observability; unified workflow replacing multiple point tools.</t>
+          <t>End-to-end LLM platform connecting observability to improvement: production traces become eval cases; results on PRs; unified PM/engineer interface.</t>
         </is>
       </c>
       <c r="H76" s="259" t="inlineStr">
         <is>
-          <t>Agent development teams; unified agent lifecycle</t>
+          <t>LLM app teams; iterative improvement workflows</t>
         </is>
       </c>
     </row>
     <row r="77" ht="40" customHeight="1">
       <c r="B77" s="259" t="inlineStr">
         <is>
-          <t>Braintrust</t>
+          <t>LangFuse</t>
         </is>
       </c>
       <c r="C77" s="259" t="inlineStr">
@@ -18435,19 +18438,19 @@
       </c>
       <c r="G77" s="259" t="inlineStr">
         <is>
-          <t>End-to-end LLM platform connecting observability to improvement: production traces become eval cases; results on PRs; unified PM/engineer interface.</t>
+          <t>Open-source LLM observability: distributed tracing, prompt management, evaluation; self-hosted or cloud; growing ecosystem.</t>
         </is>
       </c>
       <c r="H77" s="259" t="inlineStr">
         <is>
-          <t>LLM app teams; iterative improvement workflows</t>
+          <t>OSS-first teams; cost-conscious LLM monitoring</t>
         </is>
       </c>
     </row>
     <row r="78" ht="40" customHeight="1">
       <c r="B78" s="259" t="inlineStr">
         <is>
-          <t>LangFuse</t>
+          <t>Comet Opik</t>
         </is>
       </c>
       <c r="C78" s="259" t="inlineStr">
@@ -18460,9 +18463,9 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E78" s="286" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
+      <c r="E78" s="283" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="F78" s="259" t="inlineStr">
@@ -18472,19 +18475,19 @@
       </c>
       <c r="G78" s="259" t="inlineStr">
         <is>
-          <t>Open-source LLM observability: distributed tracing, prompt management, evaluation; self-hosted or cloud; growing ecosystem.</t>
+          <t>LLM evaluation and monitoring platform: tracks AI model quality, performance drift; integrates with major LLM providers.</t>
         </is>
       </c>
       <c r="H78" s="259" t="inlineStr">
         <is>
-          <t>OSS-first teams; cost-conscious LLM monitoring</t>
+          <t>ML teams; model quality assurance</t>
         </is>
       </c>
     </row>
     <row r="79" ht="40" customHeight="1">
       <c r="B79" s="259" t="inlineStr">
         <is>
-          <t>Comet Opik</t>
+          <t>Spectra Assure</t>
         </is>
       </c>
       <c r="C79" s="259" t="inlineStr">
@@ -18492,41 +18495,41 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D79" s="285" t="inlineStr">
-        <is>
-          <t>Observability &amp; Evaluation</t>
-        </is>
-      </c>
-      <c r="E79" s="283" t="inlineStr">
+      <c r="D79" s="287" t="inlineStr">
+        <is>
+          <t>AI Supply Chain</t>
+        </is>
+      </c>
+      <c r="E79" s="286" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
+        </is>
+      </c>
+      <c r="F79" s="283" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F79" s="259" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
       <c r="G79" s="259" t="inlineStr">
         <is>
-          <t>LLM evaluation and monitoring platform: tracks AI model quality, performance drift; integrates with major LLM providers.</t>
+          <t>Software supply chain security: SAFE reports for AI/ML artifacts; flags poisoning risks; CycloneDX export; NIST/ISO 42001 compliant.</t>
         </is>
       </c>
       <c r="H79" s="259" t="inlineStr">
         <is>
-          <t>ML teams; model quality assurance</t>
+          <t>Regulated industries; AI supply chain compliance</t>
         </is>
       </c>
     </row>
     <row r="80" ht="40" customHeight="1">
       <c r="B80" s="259" t="inlineStr">
         <is>
-          <t>Spectra Assure</t>
+          <t>OpenSSF Model Signing</t>
         </is>
       </c>
       <c r="C80" s="259" t="inlineStr">
         <is>
-          <t>Independent</t>
+          <t>Open Standard</t>
         </is>
       </c>
       <c r="D80" s="287" t="inlineStr">
@@ -18534,68 +18537,68 @@
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E80" s="286" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
-        </is>
-      </c>
-      <c r="F80" s="283" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
+      <c r="E80" s="259" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F80" s="259" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
       <c r="G80" s="259" t="inlineStr">
         <is>
-          <t>Software supply chain security: SAFE reports for AI/ML artifacts; flags poisoning risks; CycloneDX export; NIST/ISO 42001 compliant.</t>
+          <t>Open Source Security Foundation: model signing specification for cryptographically verifying AI model origin and integrity.</t>
         </is>
       </c>
       <c r="H80" s="259" t="inlineStr">
         <is>
-          <t>Regulated industries; AI supply chain compliance</t>
+          <t>OSS model consumers; provenance verification</t>
         </is>
       </c>
     </row>
     <row r="81" ht="40" customHeight="1">
       <c r="B81" s="259" t="inlineStr">
         <is>
-          <t>OpenSSF Model Signing</t>
+          <t>Torq</t>
         </is>
       </c>
       <c r="C81" s="259" t="inlineStr">
         <is>
-          <t>Open Standard</t>
-        </is>
-      </c>
-      <c r="D81" s="287" t="inlineStr">
-        <is>
-          <t>AI Supply Chain</t>
-        </is>
-      </c>
-      <c r="E81" s="259" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F81" s="259" t="inlineStr">
-        <is>
-          <t>—</t>
+          <t>Independent</t>
+        </is>
+      </c>
+      <c r="D81" s="285" t="inlineStr">
+        <is>
+          <t>Observability &amp; Evaluation</t>
+        </is>
+      </c>
+      <c r="E81" s="284" t="inlineStr">
+        <is>
+          <t>NHI &amp; Agentic Access</t>
+        </is>
+      </c>
+      <c r="F81" s="286" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
         </is>
       </c>
       <c r="G81" s="259" t="inlineStr">
         <is>
-          <t>Open Source Security Foundation: model signing specification for cryptographically verifying AI model origin and integrity.</t>
+          <t>AI-native security hyperautomation ($1.2B valuation): 300% revenue growth; customers include Marriott, PepsiCo, Siemens, Uber.</t>
         </is>
       </c>
       <c r="H81" s="259" t="inlineStr">
         <is>
-          <t>OSS model consumers; provenance verification</t>
+          <t>Security automation; enterprise SOC</t>
         </is>
       </c>
     </row>
     <row r="82" ht="40" customHeight="1">
       <c r="B82" s="259" t="inlineStr">
         <is>
-          <t>Torq</t>
+          <t>Radiant Security</t>
         </is>
       </c>
       <c r="C82" s="259" t="inlineStr">
@@ -18608,31 +18611,31 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E82" s="284" t="inlineStr">
-        <is>
-          <t>NHI &amp; Agentic Access</t>
-        </is>
-      </c>
-      <c r="F82" s="286" t="inlineStr">
+      <c r="E82" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
+      <c r="F82" s="283" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
+        </is>
+      </c>
       <c r="G82" s="259" t="inlineStr">
         <is>
-          <t>AI-native security hyperautomation ($1.2B valuation): 300% revenue growth; customers include Marriott, PepsiCo, Siemens, Uber.</t>
+          <t>Agentic AI SOC platform: handles 100% of alerts; 90% false positive reduction; integrates 100+ data sources; autonomous triage.</t>
         </is>
       </c>
       <c r="H82" s="259" t="inlineStr">
         <is>
-          <t>Security automation; enterprise SOC</t>
+          <t>SOC teams; alert fatigue reduction</t>
         </is>
       </c>
     </row>
     <row r="83" ht="40" customHeight="1">
       <c r="B83" s="259" t="inlineStr">
         <is>
-          <t>Radiant Security</t>
+          <t>Stellar Cyber</t>
         </is>
       </c>
       <c r="C83" s="259" t="inlineStr">
@@ -18650,26 +18653,26 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F83" s="283" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
+      <c r="F83" s="288" t="inlineStr">
+        <is>
+          <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
       <c r="G83" s="259" t="inlineStr">
         <is>
-          <t>Agentic AI SOC platform: handles 100% of alerts; 90% false positive reduction; integrates 100+ data sources; autonomous triage.</t>
+          <t>Open XDR with agentic AI: multi-agent architecture (detection, correlation, scoring, response); 50M+ data points across endpoints/network/cloud.</t>
         </is>
       </c>
       <c r="H83" s="259" t="inlineStr">
         <is>
-          <t>SOC teams; alert fatigue reduction</t>
+          <t>Mid-market; unified security operations</t>
         </is>
       </c>
     </row>
     <row r="84" ht="40" customHeight="1">
       <c r="B84" s="259" t="inlineStr">
         <is>
-          <t>Stellar Cyber</t>
+          <t>Strata Identity</t>
         </is>
       </c>
       <c r="C84" s="259" t="inlineStr">
@@ -18677,9 +18680,9 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D84" s="285" t="inlineStr">
-        <is>
-          <t>Observability &amp; Evaluation</t>
+      <c r="D84" s="284" t="inlineStr">
+        <is>
+          <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
       <c r="E84" s="286" t="inlineStr">
@@ -18687,41 +18690,41 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F84" s="288" t="inlineStr">
-        <is>
-          <t>Shadow AI &amp; Usage Discovery</t>
+      <c r="F84" s="259" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
       <c r="G84" s="259" t="inlineStr">
         <is>
-          <t>Open XDR with agentic AI: multi-agent architecture (detection, correlation, scoring, response); 50M+ data points across endpoints/network/cloud.</t>
+          <t>Agentic identity management: dynamic, autonomous NHI governance; distinct from static machine identities; policy-based agent permissions.</t>
         </is>
       </c>
       <c r="H84" s="259" t="inlineStr">
         <is>
-          <t>Mid-market; unified security operations</t>
+          <t>Agentic AI identity; dynamic access control</t>
         </is>
       </c>
     </row>
     <row r="85" ht="40" customHeight="1">
       <c r="B85" s="259" t="inlineStr">
         <is>
-          <t>Strata Identity</t>
+          <t>NVIDIA NeMo Guardrails</t>
         </is>
       </c>
       <c r="C85" s="259" t="inlineStr">
         <is>
-          <t>Independent</t>
-        </is>
-      </c>
-      <c r="D85" s="284" t="inlineStr">
-        <is>
-          <t>NHI &amp; Agentic Access</t>
-        </is>
-      </c>
-      <c r="E85" s="286" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
+          <t>Platform</t>
+        </is>
+      </c>
+      <c r="D85" s="283" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
+        </is>
+      </c>
+      <c r="E85" s="285" t="inlineStr">
+        <is>
+          <t>Observability &amp; Evaluation</t>
         </is>
       </c>
       <c r="F85" s="259" t="inlineStr">
@@ -18731,29 +18734,29 @@
       </c>
       <c r="G85" s="259" t="inlineStr">
         <is>
-          <t>Agentic identity management: dynamic, autonomous NHI governance; distinct from static machine identities; policy-based agent permissions.</t>
+          <t>Inference microservices (GA Jan 2025): programmable guardrails for LLMs; safety, security, control for AI applications.</t>
         </is>
       </c>
       <c r="H85" s="259" t="inlineStr">
         <is>
-          <t>Agentic AI identity; dynamic access control</t>
+          <t>NVIDIA ecosystem; custom guardrail logic</t>
         </is>
       </c>
     </row>
     <row r="86" ht="40" customHeight="1">
       <c r="B86" s="259" t="inlineStr">
         <is>
-          <t>NVIDIA NeMo Guardrails</t>
+          <t>Holistic AI</t>
         </is>
       </c>
       <c r="C86" s="259" t="inlineStr">
         <is>
-          <t>Platform</t>
-        </is>
-      </c>
-      <c r="D86" s="283" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
+          <t>Independent</t>
+        </is>
+      </c>
+      <c r="D86" s="286" t="inlineStr">
+        <is>
+          <t>AI Posture &amp; Governance</t>
         </is>
       </c>
       <c r="E86" s="285" t="inlineStr">
@@ -18768,19 +18771,19 @@
       </c>
       <c r="G86" s="259" t="inlineStr">
         <is>
-          <t>Inference microservices (GA Jan 2025): programmable guardrails for LLMs; safety, security, control for AI applications.</t>
+          <t>End-to-end AI risk management: live AI system inventory; EU AI Act alignment; bias auditing; regulatory compliance focus.</t>
         </is>
       </c>
       <c r="H86" s="259" t="inlineStr">
         <is>
-          <t>NVIDIA ecosystem; custom guardrail logic</t>
+          <t>EU AI Act compliance; risk management</t>
         </is>
       </c>
     </row>
     <row r="87" ht="40" customHeight="1">
       <c r="B87" s="259" t="inlineStr">
         <is>
-          <t>Holistic AI</t>
+          <t>Airia</t>
         </is>
       </c>
       <c r="C87" s="259" t="inlineStr">
@@ -18793,31 +18796,31 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E87" s="285" t="inlineStr">
-        <is>
-          <t>Observability &amp; Evaluation</t>
-        </is>
-      </c>
-      <c r="F87" s="259" t="inlineStr">
-        <is>
-          <t>—</t>
+      <c r="E87" s="284" t="inlineStr">
+        <is>
+          <t>NHI &amp; Agentic Access</t>
+        </is>
+      </c>
+      <c r="F87" s="283" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="G87" s="259" t="inlineStr">
         <is>
-          <t>End-to-end AI risk management: live AI system inventory; EU AI Act alignment; bias auditing; regulatory compliance focus.</t>
+          <t>Three-pillar platform (Q1 2026): AI Security, AI Governance, Agent Orchestration; unified enterprise AI management.</t>
         </is>
       </c>
       <c r="H87" s="259" t="inlineStr">
         <is>
-          <t>EU AI Act compliance; risk management</t>
+          <t>Enterprises needing unified AI governance</t>
         </is>
       </c>
     </row>
     <row r="88" ht="40" customHeight="1">
       <c r="B88" s="259" t="inlineStr">
         <is>
-          <t>Airia</t>
+          <t>Adri</t>
         </is>
       </c>
       <c r="C88" s="259" t="inlineStr">
@@ -18825,36 +18828,36 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D88" s="286" t="inlineStr">
+      <c r="D88" s="288" t="inlineStr">
+        <is>
+          <t>Shadow AI &amp; Usage Discovery</t>
+        </is>
+      </c>
+      <c r="E88" s="289" t="inlineStr">
+        <is>
+          <t>Data Protection for AI</t>
+        </is>
+      </c>
+      <c r="F88" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E88" s="284" t="inlineStr">
-        <is>
-          <t>NHI &amp; Agentic Access</t>
-        </is>
-      </c>
-      <c r="F88" s="283" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
       <c r="G88" s="259" t="inlineStr">
         <is>
-          <t>Three-pillar platform (Q1 2026): AI Security, AI Governance, Agent Orchestration; unified enterprise AI management.</t>
+          <t>Y Combinator-backed: patented technology monitoring AI vendor infrastructure; detects intentional/accidental misuse of proprietary data.</t>
         </is>
       </c>
       <c r="H88" s="259" t="inlineStr">
         <is>
-          <t>Enterprises needing unified AI governance</t>
+          <t>IP protection; AI vendor monitoring</t>
         </is>
       </c>
     </row>
     <row r="89" ht="40" customHeight="1">
       <c r="B89" s="259" t="inlineStr">
         <is>
-          <t>Adri</t>
+          <t>Prophet Security</t>
         </is>
       </c>
       <c r="C89" s="259" t="inlineStr">
@@ -18862,36 +18865,36 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D89" s="288" t="inlineStr">
-        <is>
-          <t>Shadow AI &amp; Usage Discovery</t>
-        </is>
-      </c>
-      <c r="E89" s="289" t="inlineStr">
-        <is>
-          <t>Data Protection for AI</t>
-        </is>
-      </c>
-      <c r="F89" s="286" t="inlineStr">
+      <c r="D89" s="285" t="inlineStr">
+        <is>
+          <t>Observability &amp; Evaluation</t>
+        </is>
+      </c>
+      <c r="E89" s="286" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
+      <c r="F89" s="259" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="G89" s="259" t="inlineStr">
         <is>
-          <t>Y Combinator-backed: patented technology monitoring AI vendor infrastructure; detects intentional/accidental misuse of proprietary data.</t>
+          <t>Agentic SOC: autonomous security investigation; AI-driven threat response; reduces analyst burden.</t>
         </is>
       </c>
       <c r="H89" s="259" t="inlineStr">
         <is>
-          <t>IP protection; AI vendor monitoring</t>
+          <t>SOC teams; autonomous investigation</t>
         </is>
       </c>
     </row>
     <row r="90" ht="40" customHeight="1">
       <c r="B90" s="259" t="inlineStr">
         <is>
-          <t>Prophet Security</t>
+          <t>Hex Security</t>
         </is>
       </c>
       <c r="C90" s="259" t="inlineStr">
@@ -18899,9 +18902,9 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D90" s="285" t="inlineStr">
-        <is>
-          <t>Observability &amp; Evaluation</t>
+      <c r="D90" s="283" t="inlineStr">
+        <is>
+          <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
       <c r="E90" s="286" t="inlineStr">
@@ -18916,51 +18919,22 @@
       </c>
       <c r="G90" s="259" t="inlineStr">
         <is>
-          <t>Agentic SOC: autonomous security investigation; AI-driven threat response; reduces analyst burden.</t>
+          <t>Y Combinator-backed: AI agents running continuous pen tests; 24/7 vulnerability discovery and verification.</t>
         </is>
       </c>
       <c r="H90" s="259" t="inlineStr">
         <is>
-          <t>SOC teams; autonomous investigation</t>
+          <t>Continuous security testing; red team automation</t>
         </is>
       </c>
     </row>
     <row r="91" ht="40" customHeight="1">
-      <c r="B91" s="259" t="inlineStr">
-        <is>
-          <t>Hex Security</t>
-        </is>
-      </c>
-      <c r="C91" s="259" t="inlineStr">
-        <is>
-          <t>Independent</t>
-        </is>
-      </c>
-      <c r="D91" s="283" t="inlineStr">
-        <is>
-          <t>Runtime Protection &amp; Guardrails</t>
-        </is>
-      </c>
-      <c r="E91" s="286" t="inlineStr">
-        <is>
-          <t>AI Posture &amp; Governance</t>
-        </is>
-      </c>
-      <c r="F91" s="259" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="G91" s="259" t="inlineStr">
-        <is>
-          <t>Y Combinator-backed: AI agents running continuous pen tests; 24/7 vulnerability discovery and verification.</t>
-        </is>
-      </c>
-      <c r="H91" s="259" t="inlineStr">
-        <is>
-          <t>Continuous security testing; red team automation</t>
-        </is>
-      </c>
+      <c r="C91" s="190" t="n"/>
+      <c r="D91" s="190" t="n"/>
+      <c r="E91" s="190" t="n"/>
+      <c r="F91" s="190" t="n"/>
+      <c r="G91" s="190" t="n"/>
+      <c r="H91" s="190" t="n"/>
     </row>
     <row r="92">
       <c r="C92" s="190" t="n"/>
@@ -19490,14 +19464,6 @@
       <c r="G157" s="190" t="n"/>
       <c r="H157" s="190" t="n"/>
     </row>
-    <row r="158">
-      <c r="C158" s="190" t="n"/>
-      <c r="D158" s="190" t="n"/>
-      <c r="E158" s="190" t="n"/>
-      <c r="F158" s="190" t="n"/>
-      <c r="G158" s="190" t="n"/>
-      <c r="H158" s="190" t="n"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix Tool Landscape family column colors (D, E, F only)
Applied correct family colors to Primary/Secondary/Tertiary columns:
- AI Posture & Governance = light green (E2EFDA)
- Runtime Protection & Guardrails = light orange (FCE4D6)
- Shadow AI & Usage Discovery = light blue (DDEBF7)
- Observability & Evaluation = light yellow (FFF2CC)
- Data Protection for AI = light purple (E4DFEC)
- NHI & Agentic Access = blue (B4C6E7)
- AI Supply Chain = salmon (F8CBAD)

Each cell is now colored based on the family it contains.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/AI_Security_Risk_Draft1.xlsx
+++ b/AI_Security_Risk_Draft1.xlsx
@@ -329,7 +329,7 @@
       <color rgb="FFFFFFFF"/>
     </font>
   </fonts>
-  <fills count="58">
+  <fills count="60">
     <fill>
       <patternFill/>
     </fill>
@@ -645,6 +645,18 @@
         <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CBAD"/>
+        <bgColor rgb="FFF8CBAD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FFB4C6E7"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -766,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6"/>
   </cellStyleXfs>
-  <cellXfs count="300">
+  <cellXfs count="314">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1554,6 +1566,48 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="57" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="30" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="58" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="34" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="31" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="32" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="33" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="59" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="32" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="59" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="34" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="30" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="58" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="31" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="33" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -16165,7 +16219,6 @@
         </is>
       </c>
     </row>
-    <row r="14"/>
     <row r="15">
       <c r="B15" s="260" t="inlineStr">
         <is>
@@ -16221,17 +16274,17 @@
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D17" s="276" t="inlineStr">
+      <c r="D17" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E17" s="277" t="inlineStr">
+      <c r="E17" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F17" s="278" t="inlineStr">
+      <c r="F17" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -16258,17 +16311,17 @@
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D18" s="276" t="inlineStr">
+      <c r="D18" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E18" s="277" t="inlineStr">
+      <c r="E18" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F18" s="279" t="inlineStr">
+      <c r="F18" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
@@ -16295,17 +16348,17 @@
           <t>Platform</t>
         </is>
       </c>
-      <c r="D19" s="276" t="inlineStr">
+      <c r="D19" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E19" s="280" t="inlineStr">
+      <c r="E19" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F19" s="281" t="inlineStr">
+      <c r="F19" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
@@ -16332,17 +16385,17 @@
           <t>Pending Acquisition</t>
         </is>
       </c>
-      <c r="D20" s="276" t="inlineStr">
+      <c r="D20" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E20" s="279" t="inlineStr">
+      <c r="E20" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F20" s="278" t="inlineStr">
+      <c r="F20" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -16369,17 +16422,17 @@
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D21" s="276" t="inlineStr">
+      <c r="D21" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E21" s="280" t="inlineStr">
+      <c r="E21" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F21" s="277" t="inlineStr">
+      <c r="F21" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16406,17 +16459,17 @@
           <t>Platform</t>
         </is>
       </c>
-      <c r="D22" s="276" t="inlineStr">
+      <c r="D22" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E22" s="278" t="inlineStr">
+      <c r="E22" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F22" s="282" t="inlineStr">
+      <c r="F22" s="306" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -16443,17 +16496,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D23" s="277" t="inlineStr">
+      <c r="D23" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E23" s="280" t="inlineStr">
+      <c r="E23" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F23" s="276" t="inlineStr">
+      <c r="F23" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -16480,17 +16533,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D24" s="276" t="inlineStr">
+      <c r="D24" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E24" s="277" t="inlineStr">
+      <c r="E24" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F24" s="278" t="inlineStr">
+      <c r="F24" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -16517,17 +16570,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D25" s="276" t="inlineStr">
+      <c r="D25" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E25" s="278" t="inlineStr">
+      <c r="E25" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F25" s="277" t="inlineStr">
+      <c r="F25" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16554,17 +16607,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D26" s="276" t="inlineStr">
+      <c r="D26" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E26" s="279" t="inlineStr">
+      <c r="E26" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F26" s="280" t="inlineStr">
+      <c r="F26" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -16591,17 +16644,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D27" s="276" t="inlineStr">
+      <c r="D27" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E27" s="281" t="inlineStr">
+      <c r="E27" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F27" s="279" t="inlineStr">
+      <c r="F27" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
@@ -16628,17 +16681,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D28" s="276" t="inlineStr">
+      <c r="D28" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E28" s="282" t="inlineStr">
+      <c r="E28" s="306" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F28" s="280" t="inlineStr">
+      <c r="F28" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -16665,17 +16718,17 @@
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D29" s="276" t="inlineStr">
+      <c r="D29" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E29" s="280" t="inlineStr">
+      <c r="E29" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F29" s="279" t="inlineStr">
+      <c r="F29" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
@@ -16702,17 +16755,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D30" s="277" t="inlineStr">
+      <c r="D30" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E30" s="276" t="inlineStr">
+      <c r="E30" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F30" s="280" t="inlineStr">
+      <c r="F30" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -16739,17 +16792,17 @@
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D31" s="280" t="inlineStr">
+      <c r="D31" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E31" s="276" t="inlineStr">
+      <c r="E31" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F31" s="277" t="inlineStr">
+      <c r="F31" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16776,17 +16829,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D32" s="280" t="inlineStr">
+      <c r="D32" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E32" s="277" t="inlineStr">
+      <c r="E32" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F32" s="278" t="inlineStr">
+      <c r="F32" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -16813,17 +16866,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D33" s="280" t="inlineStr">
+      <c r="D33" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E33" s="278" t="inlineStr">
+      <c r="E33" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F33" s="276" t="inlineStr">
+      <c r="F33" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -16850,17 +16903,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D34" s="280" t="inlineStr">
+      <c r="D34" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E34" s="278" t="inlineStr">
+      <c r="E34" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F34" s="277" t="inlineStr">
+      <c r="F34" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16887,17 +16940,17 @@
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D35" s="280" t="inlineStr">
+      <c r="D35" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E35" s="278" t="inlineStr">
+      <c r="E35" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F35" s="277" t="inlineStr">
+      <c r="F35" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16924,12 +16977,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D36" s="280" t="inlineStr">
+      <c r="D36" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E36" s="278" t="inlineStr">
+      <c r="E36" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -16961,12 +17014,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D37" s="280" t="inlineStr">
+      <c r="D37" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E37" s="281" t="inlineStr">
+      <c r="E37" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
@@ -16998,17 +17051,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D38" s="280" t="inlineStr">
+      <c r="D38" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E38" s="281" t="inlineStr">
+      <c r="E38" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F38" s="278" t="inlineStr">
+      <c r="F38" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -17035,17 +17088,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D39" s="280" t="inlineStr">
+      <c r="D39" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E39" s="282" t="inlineStr">
+      <c r="E39" s="306" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F39" s="278" t="inlineStr">
+      <c r="F39" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -17072,17 +17125,17 @@
           <t>Acquired</t>
         </is>
       </c>
-      <c r="D40" s="279" t="inlineStr">
+      <c r="D40" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E40" s="280" t="inlineStr">
+      <c r="E40" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F40" s="281" t="inlineStr">
+      <c r="F40" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
@@ -17109,17 +17162,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D41" s="279" t="inlineStr">
+      <c r="D41" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E41" s="281" t="inlineStr">
+      <c r="E41" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F41" s="276" t="inlineStr">
+      <c r="F41" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17146,17 +17199,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D42" s="279" t="inlineStr">
+      <c r="D42" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E42" s="281" t="inlineStr">
+      <c r="E42" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F42" s="280" t="inlineStr">
+      <c r="F42" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -17183,17 +17236,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D43" s="279" t="inlineStr">
+      <c r="D43" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E43" s="281" t="inlineStr">
+      <c r="E43" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F43" s="276" t="inlineStr">
+      <c r="F43" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17220,17 +17273,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D44" s="278" t="inlineStr">
+      <c r="D44" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E44" s="276" t="inlineStr">
+      <c r="E44" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F44" s="280" t="inlineStr">
+      <c r="F44" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -17257,17 +17310,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D45" s="278" t="inlineStr">
+      <c r="D45" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E45" s="280" t="inlineStr">
+      <c r="E45" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F45" s="276" t="inlineStr">
+      <c r="F45" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17294,17 +17347,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D46" s="278" t="inlineStr">
+      <c r="D46" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E46" s="276" t="inlineStr">
+      <c r="E46" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F46" s="281" t="inlineStr">
+      <c r="F46" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
@@ -17331,12 +17384,12 @@
           <t>Platform</t>
         </is>
       </c>
-      <c r="D47" s="278" t="inlineStr">
+      <c r="D47" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E47" s="276" t="inlineStr">
+      <c r="E47" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17368,12 +17421,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D48" s="278" t="inlineStr">
+      <c r="D48" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E48" s="276" t="inlineStr">
+      <c r="E48" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17405,12 +17458,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D49" s="278" t="inlineStr">
+      <c r="D49" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E49" s="276" t="inlineStr">
+      <c r="E49" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17442,17 +17495,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D50" s="278" t="inlineStr">
+      <c r="D50" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E50" s="280" t="inlineStr">
+      <c r="E50" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F50" s="281" t="inlineStr">
+      <c r="F50" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
@@ -17479,17 +17532,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D51" s="278" t="inlineStr">
+      <c r="D51" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E51" s="280" t="inlineStr">
+      <c r="E51" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F51" s="276" t="inlineStr">
+      <c r="F51" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17516,12 +17569,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D52" s="278" t="inlineStr">
+      <c r="D52" s="302" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E52" s="276" t="inlineStr">
+      <c r="E52" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17553,17 +17606,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D53" s="281" t="inlineStr">
+      <c r="D53" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E53" s="276" t="inlineStr">
+      <c r="E53" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F53" s="279" t="inlineStr">
+      <c r="F53" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
@@ -17590,17 +17643,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D54" s="281" t="inlineStr">
+      <c r="D54" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E54" s="276" t="inlineStr">
+      <c r="E54" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F54" s="279" t="inlineStr">
+      <c r="F54" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
@@ -17627,17 +17680,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D55" s="281" t="inlineStr">
+      <c r="D55" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E55" s="279" t="inlineStr">
+      <c r="E55" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F55" s="280" t="inlineStr">
+      <c r="F55" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -17664,17 +17717,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D56" s="281" t="inlineStr">
+      <c r="D56" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E56" s="279" t="inlineStr">
+      <c r="E56" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F56" s="280" t="inlineStr">
+      <c r="F56" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -17701,17 +17754,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D57" s="281" t="inlineStr">
+      <c r="D57" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E57" s="279" t="inlineStr">
+      <c r="E57" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F57" s="276" t="inlineStr">
+      <c r="F57" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17738,17 +17791,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D58" s="281" t="inlineStr">
+      <c r="D58" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E58" s="276" t="inlineStr">
+      <c r="E58" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F58" s="280" t="inlineStr">
+      <c r="F58" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -17775,12 +17828,12 @@
           <t>Platform</t>
         </is>
       </c>
-      <c r="D59" s="281" t="inlineStr">
+      <c r="D59" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E59" s="280" t="inlineStr">
+      <c r="E59" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -17812,12 +17865,12 @@
           <t>Platform</t>
         </is>
       </c>
-      <c r="D60" s="281" t="inlineStr">
+      <c r="D60" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="E60" s="280" t="inlineStr">
+      <c r="E60" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -17849,17 +17902,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D61" s="282" t="inlineStr">
+      <c r="D61" s="306" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E61" s="279" t="inlineStr">
+      <c r="E61" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F61" s="276" t="inlineStr">
+      <c r="F61" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17886,17 +17939,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D62" s="282" t="inlineStr">
+      <c r="D62" s="306" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E62" s="279" t="inlineStr">
+      <c r="E62" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F62" s="276" t="inlineStr">
+      <c r="F62" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17923,17 +17976,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D63" s="282" t="inlineStr">
+      <c r="D63" s="306" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E63" s="279" t="inlineStr">
+      <c r="E63" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F63" s="276" t="inlineStr">
+      <c r="F63" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -17960,17 +18013,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D64" s="282" t="inlineStr">
+      <c r="D64" s="306" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E64" s="279" t="inlineStr">
+      <c r="E64" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F64" s="281" t="inlineStr">
+      <c r="F64" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
@@ -17997,17 +18050,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D65" s="282" t="inlineStr">
+      <c r="D65" s="306" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E65" s="279" t="inlineStr">
+      <c r="E65" s="303" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="F65" s="276" t="inlineStr">
+      <c r="F65" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18034,17 +18087,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D66" s="282" t="inlineStr">
+      <c r="D66" s="306" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E66" s="276" t="inlineStr">
+      <c r="E66" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F66" s="281" t="inlineStr">
+      <c r="F66" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
@@ -18071,12 +18124,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D67" s="282" t="inlineStr">
+      <c r="D67" s="306" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E67" s="281" t="inlineStr">
+      <c r="E67" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
@@ -18108,17 +18161,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D68" s="282" t="inlineStr">
+      <c r="D68" s="306" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E68" s="280" t="inlineStr">
+      <c r="E68" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F68" s="276" t="inlineStr">
+      <c r="F68" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18145,12 +18198,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D69" s="277" t="inlineStr">
+      <c r="D69" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E69" s="276" t="inlineStr">
+      <c r="E69" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18178,12 +18231,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D70" s="277" t="inlineStr">
+      <c r="D70" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E70" s="281" t="inlineStr">
+      <c r="E70" s="305" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
@@ -18211,12 +18264,12 @@
           <t>Platform</t>
         </is>
       </c>
-      <c r="D71" s="277" t="inlineStr">
+      <c r="D71" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E71" s="276" t="inlineStr">
+      <c r="E71" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18244,17 +18297,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D72" s="277" t="inlineStr">
+      <c r="D72" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E72" s="280" t="inlineStr">
+      <c r="E72" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F72" s="276" t="inlineStr">
+      <c r="F72" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18277,17 +18330,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D73" s="276" t="inlineStr">
+      <c r="D73" s="300" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E73" s="277" t="inlineStr">
+      <c r="E73" s="301" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="F73" s="280" t="inlineStr">
+      <c r="F73" s="304" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -18310,17 +18363,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D74" s="283" t="inlineStr">
+      <c r="D74" s="307" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E74" s="284" t="inlineStr">
+      <c r="E74" s="308" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F74" s="285" t="inlineStr">
+      <c r="F74" s="309" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -18347,17 +18400,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D75" s="285" t="inlineStr">
+      <c r="D75" s="309" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E75" s="286" t="inlineStr">
+      <c r="E75" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F75" s="283" t="inlineStr">
+      <c r="F75" s="307" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -18384,12 +18437,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D76" s="285" t="inlineStr">
+      <c r="D76" s="309" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E76" s="286" t="inlineStr">
+      <c r="E76" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18421,12 +18474,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D77" s="285" t="inlineStr">
+      <c r="D77" s="309" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E77" s="286" t="inlineStr">
+      <c r="E77" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18458,12 +18511,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D78" s="285" t="inlineStr">
+      <c r="D78" s="309" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E78" s="283" t="inlineStr">
+      <c r="E78" s="307" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -18495,17 +18548,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D79" s="287" t="inlineStr">
+      <c r="D79" s="311" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
       </c>
-      <c r="E79" s="286" t="inlineStr">
+      <c r="E79" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F79" s="283" t="inlineStr">
+      <c r="F79" s="307" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -18532,7 +18585,7 @@
           <t>Open Standard</t>
         </is>
       </c>
-      <c r="D80" s="287" t="inlineStr">
+      <c r="D80" s="311" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -18569,17 +18622,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D81" s="285" t="inlineStr">
+      <c r="D81" s="309" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E81" s="284" t="inlineStr">
+      <c r="E81" s="308" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F81" s="286" t="inlineStr">
+      <c r="F81" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18606,17 +18659,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D82" s="285" t="inlineStr">
+      <c r="D82" s="309" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E82" s="286" t="inlineStr">
+      <c r="E82" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F82" s="283" t="inlineStr">
+      <c r="F82" s="307" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -18643,17 +18696,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D83" s="285" t="inlineStr">
+      <c r="D83" s="309" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E83" s="286" t="inlineStr">
+      <c r="E83" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F83" s="288" t="inlineStr">
+      <c r="F83" s="312" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
@@ -18680,12 +18733,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D84" s="284" t="inlineStr">
+      <c r="D84" s="308" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="E84" s="286" t="inlineStr">
+      <c r="E84" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18717,12 +18770,12 @@
           <t>Platform</t>
         </is>
       </c>
-      <c r="D85" s="283" t="inlineStr">
+      <c r="D85" s="307" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E85" s="285" t="inlineStr">
+      <c r="E85" s="309" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -18754,12 +18807,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D86" s="286" t="inlineStr">
+      <c r="D86" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E86" s="285" t="inlineStr">
+      <c r="E86" s="309" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
@@ -18791,17 +18844,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D87" s="286" t="inlineStr">
+      <c r="D87" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E87" s="284" t="inlineStr">
+      <c r="E87" s="308" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
       </c>
-      <c r="F87" s="283" t="inlineStr">
+      <c r="F87" s="307" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
@@ -18828,17 +18881,17 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D88" s="288" t="inlineStr">
+      <c r="D88" s="312" t="inlineStr">
         <is>
           <t>Shadow AI &amp; Usage Discovery</t>
         </is>
       </c>
-      <c r="E88" s="289" t="inlineStr">
+      <c r="E88" s="313" t="inlineStr">
         <is>
           <t>Data Protection for AI</t>
         </is>
       </c>
-      <c r="F88" s="286" t="inlineStr">
+      <c r="F88" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18865,12 +18918,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D89" s="285" t="inlineStr">
+      <c r="D89" s="309" t="inlineStr">
         <is>
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E89" s="286" t="inlineStr">
+      <c r="E89" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>
@@ -18902,12 +18955,12 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D90" s="283" t="inlineStr">
+      <c r="D90" s="307" t="inlineStr">
         <is>
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E90" s="286" t="inlineStr">
+      <c r="E90" s="310" t="inlineStr">
         <is>
           <t>AI Posture &amp; Governance</t>
         </is>

</xml_diff>

<commit_message>
Fix Tool Landscape D/E/F colors to match Quick Reference
Corrected NHI & Agentic Access and AI Supply Chain colors:
- NHI & Agentic Access = salmon (F8CBAD) - matches row 12
- AI Supply Chain = blue (B4C6E7) - matches row 13

Colors now match the Quick Reference: Product Families section exactly.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/AI_Security_Risk_Draft1.xlsx
+++ b/AI_Security_Risk_Draft1.xlsx
@@ -16279,7 +16279,7 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E17" s="301" t="inlineStr">
+      <c r="E17" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16316,7 +16316,7 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E18" s="301" t="inlineStr">
+      <c r="E18" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16432,7 +16432,7 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="F21" s="301" t="inlineStr">
+      <c r="F21" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16469,7 +16469,7 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F22" s="306" t="inlineStr">
+      <c r="F22" s="301" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -16496,7 +16496,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D23" s="301" t="inlineStr">
+      <c r="D23" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16538,7 +16538,7 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E24" s="301" t="inlineStr">
+      <c r="E24" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16580,7 +16580,7 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F25" s="301" t="inlineStr">
+      <c r="F25" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16686,7 +16686,7 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E28" s="306" t="inlineStr">
+      <c r="E28" s="301" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -16755,7 +16755,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D30" s="301" t="inlineStr">
+      <c r="D30" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16802,7 +16802,7 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="F31" s="301" t="inlineStr">
+      <c r="F31" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16834,7 +16834,7 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E32" s="301" t="inlineStr">
+      <c r="E32" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16913,7 +16913,7 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F34" s="301" t="inlineStr">
+      <c r="F34" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -16950,7 +16950,7 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="F35" s="301" t="inlineStr">
+      <c r="F35" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -17093,7 +17093,7 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E39" s="306" t="inlineStr">
+      <c r="E39" s="301" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -17902,7 +17902,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D61" s="306" t="inlineStr">
+      <c r="D61" s="301" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -17939,7 +17939,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D62" s="306" t="inlineStr">
+      <c r="D62" s="301" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -17976,7 +17976,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D63" s="306" t="inlineStr">
+      <c r="D63" s="301" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -18013,7 +18013,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D64" s="306" t="inlineStr">
+      <c r="D64" s="301" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -18050,7 +18050,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D65" s="306" t="inlineStr">
+      <c r="D65" s="301" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -18087,7 +18087,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D66" s="306" t="inlineStr">
+      <c r="D66" s="301" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -18124,7 +18124,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D67" s="306" t="inlineStr">
+      <c r="D67" s="301" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -18161,7 +18161,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D68" s="306" t="inlineStr">
+      <c r="D68" s="301" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -18198,7 +18198,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D69" s="301" t="inlineStr">
+      <c r="D69" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -18231,7 +18231,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D70" s="301" t="inlineStr">
+      <c r="D70" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -18264,7 +18264,7 @@
           <t>Platform</t>
         </is>
       </c>
-      <c r="D71" s="301" t="inlineStr">
+      <c r="D71" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -18297,7 +18297,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D72" s="301" t="inlineStr">
+      <c r="D72" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -18335,7 +18335,7 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E73" s="301" t="inlineStr">
+      <c r="E73" s="306" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -18368,7 +18368,7 @@
           <t>Runtime Protection &amp; Guardrails</t>
         </is>
       </c>
-      <c r="E74" s="308" t="inlineStr">
+      <c r="E74" s="311" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -18548,7 +18548,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D79" s="311" t="inlineStr">
+      <c r="D79" s="308" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -18585,7 +18585,7 @@
           <t>Open Standard</t>
         </is>
       </c>
-      <c r="D80" s="311" t="inlineStr">
+      <c r="D80" s="308" t="inlineStr">
         <is>
           <t>AI Supply Chain</t>
         </is>
@@ -18627,7 +18627,7 @@
           <t>Observability &amp; Evaluation</t>
         </is>
       </c>
-      <c r="E81" s="308" t="inlineStr">
+      <c r="E81" s="311" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -18733,7 +18733,7 @@
           <t>Independent</t>
         </is>
       </c>
-      <c r="D84" s="308" t="inlineStr">
+      <c r="D84" s="311" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>
@@ -18849,7 +18849,7 @@
           <t>AI Posture &amp; Governance</t>
         </is>
       </c>
-      <c r="E87" s="308" t="inlineStr">
+      <c r="E87" s="311" t="inlineStr">
         <is>
           <t>NHI &amp; Agentic Access</t>
         </is>

</xml_diff>